<commit_message>
std variables nearly done, added geocode eng
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="267">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -203,12 +203,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>worker_status</t>
-  </si>
-  <si>
-    <t>worker</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -221,9 +215,6 @@
     <t>student_status</t>
   </si>
   <si>
-    <t>student</t>
-  </si>
-  <si>
     <t>non-student</t>
   </si>
   <si>
@@ -474,6 +465,366 @@
   </si>
   <si>
     <t>number_transfers_alight_dest</t>
+  </si>
+  <si>
+    <t>full- or part-time</t>
+  </si>
+  <si>
+    <t>fare_medium</t>
+  </si>
+  <si>
+    <t>PAY_MODE_CODE</t>
+  </si>
+  <si>
+    <t>pass (24-hr)</t>
+  </si>
+  <si>
+    <t>pass (go)</t>
+  </si>
+  <si>
+    <t>ticket (one-way)</t>
+  </si>
+  <si>
+    <t>clipper (e-cash)</t>
+  </si>
+  <si>
+    <t>clipper (8-ride)</t>
+  </si>
+  <si>
+    <t>clipper (monthly)</t>
+  </si>
+  <si>
+    <t>FARE_TYPE_CODE</t>
+  </si>
+  <si>
+    <t>fare_category</t>
+  </si>
+  <si>
+    <t>adult</t>
+  </si>
+  <si>
+    <t>senior</t>
+  </si>
+  <si>
+    <t>youth</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>HISP_LATINO_SPANISH_CODE</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>hispanic</t>
+  </si>
+  <si>
+    <t>HISPANIC/LATINO OR OF SPANISH ORIGIN</t>
+  </si>
+  <si>
+    <t>NOT HISPANIC/LATINO OR OF SPANISH ORIGIN</t>
+  </si>
+  <si>
+    <t>RACE_AMERICANINDIAN_ALASKANNATIVE</t>
+  </si>
+  <si>
+    <t>race_dmy_ind</t>
+  </si>
+  <si>
+    <t>RACE_ASIAN</t>
+  </si>
+  <si>
+    <t>race_dmy_asn</t>
+  </si>
+  <si>
+    <t>RACE_BLACK_AFRICANAM</t>
+  </si>
+  <si>
+    <t>race_dmy_blk</t>
+  </si>
+  <si>
+    <t>RACE_NATHAWAIIAN_PACISLAND</t>
+  </si>
+  <si>
+    <t>race_dmy_hwi</t>
+  </si>
+  <si>
+    <t>RACE_WHITE</t>
+  </si>
+  <si>
+    <t>race_dmy_wht</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY_OTHER</t>
+  </si>
+  <si>
+    <t>race_other_string</t>
+  </si>
+  <si>
+    <t>LANG_OTHER_THAN_ENG</t>
+  </si>
+  <si>
+    <t>ENGLISH ONLY</t>
+  </si>
+  <si>
+    <t>language_at_home_binary</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
+    <t>OTHER_LANG_CODE</t>
+  </si>
+  <si>
+    <t>language_at_home_detail</t>
+  </si>
+  <si>
+    <t>CHINESE (MANDARIN)</t>
+  </si>
+  <si>
+    <t>FRENCH</t>
+  </si>
+  <si>
+    <t>SPANISH</t>
+  </si>
+  <si>
+    <t>KOREAN</t>
+  </si>
+  <si>
+    <t>POLISH</t>
+  </si>
+  <si>
+    <t>PORTUGUESE</t>
+  </si>
+  <si>
+    <t>RUSSIAN</t>
+  </si>
+  <si>
+    <t>FRENCH CREOLE</t>
+  </si>
+  <si>
+    <t>CHINESE (CANTONESE)</t>
+  </si>
+  <si>
+    <t>TAGALOG</t>
+  </si>
+  <si>
+    <t>CHINESE</t>
+  </si>
+  <si>
+    <t>AFRIKAANS</t>
+  </si>
+  <si>
+    <t>AMHARIC</t>
+  </si>
+  <si>
+    <t>ARABIC</t>
+  </si>
+  <si>
+    <t>ARMENIAN</t>
+  </si>
+  <si>
+    <t>BENGALI</t>
+  </si>
+  <si>
+    <t>BOSNIAN</t>
+  </si>
+  <si>
+    <t>CUBUANO</t>
+  </si>
+  <si>
+    <t>DUTCH</t>
+  </si>
+  <si>
+    <t>FARSI</t>
+  </si>
+  <si>
+    <t>GERMAN</t>
+  </si>
+  <si>
+    <t>GREEK</t>
+  </si>
+  <si>
+    <t>HINDI</t>
+  </si>
+  <si>
+    <t>HUNGARIAN</t>
+  </si>
+  <si>
+    <t>INDONESIAN</t>
+  </si>
+  <si>
+    <t>ITALIAN</t>
+  </si>
+  <si>
+    <t>JAPANESE</t>
+  </si>
+  <si>
+    <t>LATIN</t>
+  </si>
+  <si>
+    <t>MONGOLIAN</t>
+  </si>
+  <si>
+    <t>NORWEGIAN</t>
+  </si>
+  <si>
+    <t>PERSIAN</t>
+  </si>
+  <si>
+    <t>PIDGIN-NIGERIAN</t>
+  </si>
+  <si>
+    <t>PUNJABI</t>
+  </si>
+  <si>
+    <t>ROMANIAN</t>
+  </si>
+  <si>
+    <t>SWEDISH</t>
+  </si>
+  <si>
+    <t>TELUGU</t>
+  </si>
+  <si>
+    <t>THAI</t>
+  </si>
+  <si>
+    <t>TONGAN</t>
+  </si>
+  <si>
+    <t>TURKISH</t>
+  </si>
+  <si>
+    <t>URDU</t>
+  </si>
+  <si>
+    <t>VIETNAMESE</t>
+  </si>
+  <si>
+    <t>HAWAIIAN</t>
+  </si>
+  <si>
+    <t>FILIPINO</t>
+  </si>
+  <si>
+    <t>SIGN LANGUAGE</t>
+  </si>
+  <si>
+    <t>MICRONESIAN</t>
+  </si>
+  <si>
+    <t>SOMOAN</t>
+  </si>
+  <si>
+    <t>SWAHILI</t>
+  </si>
+  <si>
+    <t>HH_INCOME_CODE</t>
+  </si>
+  <si>
+    <t>household_income</t>
+  </si>
+  <si>
+    <t>under $10,000</t>
+  </si>
+  <si>
+    <t>$10,000 to $25,000</t>
+  </si>
+  <si>
+    <t>$25,000 to $35,000</t>
+  </si>
+  <si>
+    <t>$35,000 to $50,000</t>
+  </si>
+  <si>
+    <t>$50,000 to $75,000</t>
+  </si>
+  <si>
+    <t>$75,000 to $100,000</t>
+  </si>
+  <si>
+    <t>$100,000 to $150,000</t>
+  </si>
+  <si>
+    <t>$150,000 or higher</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>RESP_GENDER_CODE</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>ENGLISH_FLUENCY_CODE</t>
+  </si>
+  <si>
+    <t>VERY WELL</t>
+  </si>
+  <si>
+    <t>WELL</t>
+  </si>
+  <si>
+    <t>NOT WELL</t>
+  </si>
+  <si>
+    <t>NOT AT ALL</t>
+  </si>
+  <si>
+    <t>eng_proficient</t>
+  </si>
+  <si>
+    <t>DIRECTION</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>NORTHBOUND</t>
+  </si>
+  <si>
+    <t>SOUTHBOUND</t>
+  </si>
+  <si>
+    <t>work_status</t>
+  </si>
+  <si>
+    <t>TIME_LAST_LEFT_HOME_CODE</t>
+  </si>
+  <si>
+    <t>depart_hour</t>
+  </si>
+  <si>
+    <t>TIME_RETURN_HOME_CODE</t>
+  </si>
+  <si>
+    <t>return_hour</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>date_string</t>
   </si>
 </sst>
 </file>
@@ -891,11 +1242,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -904,7 +1255,7 @@
     <col min="2" max="2" width="35.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -929,13 +1280,13 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -946,13 +1297,13 @@
         <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -963,16 +1314,16 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -980,16 +1331,16 @@
         <v>40</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -997,16 +1348,16 @@
         <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1014,16 +1365,16 @@
         <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1031,16 +1382,16 @@
         <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,16 +1399,16 @@
         <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C9" s="1">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1065,16 +1416,16 @@
         <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C10" s="1">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,16 +1433,16 @@
         <v>40</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C11" s="1">
         <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1099,16 +1450,16 @@
         <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C12" s="1">
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1116,16 +1467,16 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1133,16 +1484,16 @@
         <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1150,16 +1501,16 @@
         <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1167,16 +1518,16 @@
         <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,13 +1535,13 @@
         <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>4</v>
@@ -1201,13 +1552,13 @@
         <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>4</v>
@@ -1473,16 +1824,16 @@
         <v>40</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>115</v>
+        <v>254</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>4</v>
+        <v>255</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>116</v>
+        <v>257</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>4</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1490,16 +1841,16 @@
         <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>117</v>
+        <v>254</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>4</v>
+        <v>256</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>118</v>
+        <v>257</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1507,16 +1858,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1</v>
+        <v>112</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>142</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1524,16 +1875,16 @@
         <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C37" s="1">
-        <v>2</v>
+        <v>114</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>143</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1541,16 +1892,16 @@
         <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C38" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1558,16 +1909,16 @@
         <v>40</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C39" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1575,16 +1926,16 @@
         <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C40" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1592,16 +1943,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C41" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1609,16 +1960,16 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C42" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1626,16 +1977,16 @@
         <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1643,16 +1994,16 @@
         <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C44" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1660,16 +2011,16 @@
         <v>40</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>61</v>
+        <v>143</v>
+      </c>
+      <c r="C45" s="1">
+        <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1677,16 +2028,16 @@
         <v>40</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>58</v>
+        <v>143</v>
+      </c>
+      <c r="C46" s="1">
+        <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>59</v>
+        <v>144</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1694,16 +2045,16 @@
         <v>40</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="1">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>16</v>
+        <v>260</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1711,16 +2062,16 @@
         <v>40</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>16</v>
+        <v>260</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1731,13 +2082,13 @@
         <v>26</v>
       </c>
       <c r="C49" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1748,13 +2099,13 @@
         <v>26</v>
       </c>
       <c r="C50" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,13 +2116,13 @@
         <v>26</v>
       </c>
       <c r="C51" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1782,13 +2133,13 @@
         <v>26</v>
       </c>
       <c r="C52" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1799,13 +2150,13 @@
         <v>26</v>
       </c>
       <c r="C53" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1813,16 +2164,16 @@
         <v>40</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="C54" s="1">
+        <v>5</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,16 +2181,16 @@
         <v>40</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="C55" s="1">
+        <v>6</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,16 +2198,16 @@
         <v>40</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>4</v>
+        <v>248</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>104</v>
+        <v>253</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>4</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1864,16 +2215,16 @@
         <v>40</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>4</v>
+        <v>248</v>
+      </c>
+      <c r="C57" s="1">
+        <v>2</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>105</v>
+        <v>253</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>4</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1881,16 +2232,16 @@
         <v>40</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>4</v>
+        <v>248</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>4</v>
+        <v>251</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1898,16 +2249,16 @@
         <v>40</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C59" s="1">
         <v>4</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>124</v>
+        <v>253</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>4</v>
+        <v>252</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1915,13 +2266,13 @@
         <v>40</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>4</v>
@@ -1932,13 +2283,13 @@
         <v>40</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>4</v>
@@ -1949,16 +2300,16 @@
         <v>40</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1966,16 +2317,16 @@
         <v>40</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>73</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1983,13 +2334,13 @@
         <v>40</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>4</v>
@@ -2000,13 +2351,13 @@
         <v>40</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>4</v>
@@ -2017,13 +2368,13 @@
         <v>40</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>4</v>
@@ -2034,13 +2385,13 @@
         <v>40</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>4</v>
@@ -2051,16 +2402,16 @@
         <v>40</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>4</v>
+        <v>156</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>4</v>
+        <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,16 +2419,16 @@
         <v>40</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="C69" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2085,16 +2436,16 @@
         <v>40</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="C70" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2102,16 +2453,16 @@
         <v>40</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="C71" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2119,16 +2470,16 @@
         <v>40</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C72" s="1">
-        <v>4</v>
+        <v>68</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,16 +2487,16 @@
         <v>40</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C73" s="1">
-        <v>5</v>
+        <v>68</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2153,16 +2504,16 @@
         <v>40</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C74" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>48</v>
+        <v>234</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,16 +2521,16 @@
         <v>40</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C75" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>51</v>
+        <v>234</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2187,16 +2538,16 @@
         <v>40</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C76" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>49</v>
+        <v>234</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2204,16 +2555,16 @@
         <v>40</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C77" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>52</v>
+        <v>234</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2221,16 +2572,16 @@
         <v>40</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C78" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>50</v>
+        <v>234</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2238,16 +2589,16 @@
         <v>40</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C79" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>51</v>
+        <v>234</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,16 +2606,16 @@
         <v>40</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C80" s="1">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>52</v>
+        <v>234</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2272,16 +2623,16 @@
         <v>40</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C81" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>52</v>
+        <v>234</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2289,16 +2640,16 @@
         <v>40</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C82" s="1">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>42</v>
+        <v>234</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>52</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,16 +2657,16 @@
         <v>40</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="C83" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>42</v>
+        <v>234</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>52</v>
+        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2323,16 +2674,16 @@
         <v>40</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>28</v>
+        <v>233</v>
+      </c>
+      <c r="C84" s="1">
+        <v>88</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>38</v>
+        <v>234</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>14</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,16 +2691,16 @@
         <v>40</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>37</v>
+        <v>233</v>
+      </c>
+      <c r="C85" s="1">
+        <v>99</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>38</v>
+        <v>234</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,16 +2708,16 @@
         <v>40</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>11</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,16 +2725,16 @@
         <v>40</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>27</v>
+        <v>162</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>30</v>
+        <v>163</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>12</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,16 +2742,16 @@
         <v>40</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,16 +2759,16 @@
         <v>40</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2425,16 +2776,16 @@
         <v>40</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,16 +2793,16 @@
         <v>40</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2459,16 +2810,16 @@
         <v>40</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>23</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2476,16 +2827,16 @@
         <v>40</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,13 +2844,13 @@
         <v>40</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>4</v>
@@ -2510,16 +2861,16 @@
         <v>40</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C95" s="1">
+        <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2527,16 +2878,16 @@
         <v>40</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2544,16 +2895,16 @@
         <v>40</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>58</v>
+        <v>41</v>
+      </c>
+      <c r="C97" s="1">
+        <v>3</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,16 +2912,16 @@
         <v>40</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C98" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C98" s="1">
         <v>4</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,16 +2929,16 @@
         <v>40</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C99" s="1">
+        <v>5</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>131</v>
+        <v>42</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2595,16 +2946,16 @@
         <v>40</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C100" s="1">
+        <v>6</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2612,16 +2963,16 @@
         <v>40</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="C101" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E101" s="1">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,16 +2980,16 @@
         <v>40</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="C102" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E102" s="1">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2646,16 +2997,16 @@
         <v>40</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="C103" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E103" s="1">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2663,16 +3014,16 @@
         <v>40</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>126</v>
+        <v>41</v>
+      </c>
+      <c r="C104" s="1">
+        <v>10</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E104" s="1">
-        <v>3</v>
+        <v>42</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,16 +3031,16 @@
         <v>40</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C105" s="1">
+        <v>11</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2697,16 +3048,16 @@
         <v>40</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C106" s="1">
+        <v>12</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>138</v>
+        <v>42</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,16 +3065,16 @@
         <v>40</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="C107" s="1">
+        <v>13</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2731,16 +3082,16 @@
         <v>40</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="C108" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E108" s="1">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2748,16 +3099,16 @@
         <v>40</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="C109" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E109" s="1">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2765,16 +3116,16 @@
         <v>40</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="C110" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E110" s="1">
-        <v>2</v>
+        <v>185</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,16 +3133,16 @@
         <v>40</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>126</v>
+        <v>184</v>
+      </c>
+      <c r="C111" s="1">
+        <v>11</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E111" s="1">
-        <v>3</v>
+        <v>185</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2799,16 +3150,16 @@
         <v>40</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C112" s="3">
-        <v>1</v>
+        <v>184</v>
+      </c>
+      <c r="C112" s="1">
+        <v>13</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>14</v>
+        <v>199</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2816,16 +3167,16 @@
         <v>40</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C113" s="3">
-        <v>2</v>
+        <v>184</v>
+      </c>
+      <c r="C113" s="1">
+        <v>17</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2833,16 +3184,16 @@
         <v>40</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C114" s="3">
-        <v>3</v>
+        <v>184</v>
+      </c>
+      <c r="C114" s="1">
+        <v>18</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -2850,16 +3201,16 @@
         <v>40</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>21</v>
+        <v>184</v>
+      </c>
+      <c r="C115" s="1">
+        <v>37</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>15</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -2867,16 +3218,16 @@
         <v>40</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>20</v>
+        <v>184</v>
+      </c>
+      <c r="C116" s="1">
+        <v>45</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>9</v>
+        <v>185</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>10</v>
+        <v>202</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2884,16 +3235,16 @@
         <v>40</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>61</v>
+        <v>184</v>
+      </c>
+      <c r="C117" s="1">
+        <v>56</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2901,16 +3252,16 @@
         <v>40</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>58</v>
+        <v>184</v>
+      </c>
+      <c r="C118" s="1">
+        <v>63</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2918,16 +3269,16 @@
         <v>40</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>4</v>
+        <v>184</v>
+      </c>
+      <c r="C119" s="1">
+        <v>84</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>86</v>
+        <v>185</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>4</v>
+        <v>204</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2935,16 +3286,16 @@
         <v>40</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>4</v>
+        <v>184</v>
+      </c>
+      <c r="C120" s="1">
+        <v>102</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>90</v>
+        <v>185</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>4</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,23 +3303,2335 @@
         <v>40</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C121" s="1">
+        <v>111</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C122" s="1">
+        <v>129</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C123" s="1">
+        <v>135</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C124" s="1">
+        <v>143</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C125" s="1">
+        <v>146</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C126" s="1">
+        <v>148</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C127" s="1">
+        <v>152</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C128" s="1">
+        <v>156</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C129" s="1">
+        <v>159</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C130" s="1">
+        <v>208</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C131" s="1">
+        <v>220</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C132" s="1">
+        <v>279</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C133" s="1">
+        <v>297</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C134" s="1">
+        <v>321</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C135" s="1">
+        <v>325</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C136" s="1">
+        <v>351</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C137" s="1">
+        <v>351</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C138" s="1">
+        <v>356</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C139" s="1">
+        <v>358</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C140" s="1">
+        <v>378</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C141" s="1">
+        <v>385</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C142" s="1">
+        <v>408</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C143" s="1">
+        <v>426</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C144" s="1">
+        <v>432</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C145" s="1">
+        <v>441</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C146" s="1">
+        <v>443</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C147" s="1">
+        <v>446</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C148" s="1">
+        <v>448</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C149" s="1">
+        <v>456</v>
+      </c>
+      <c r="D149" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C150" s="1">
+        <v>465</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C151" s="1">
+        <v>488</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C152" s="1">
+        <v>489</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C153" s="1">
+        <v>490</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E153" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C154" s="1">
+        <v>491</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C155" s="1">
+        <v>498</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C156" s="1">
+        <v>501</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C157" s="1">
+        <v>502</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C158" s="1">
+        <v>503</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C159" s="1">
+        <v>504</v>
+      </c>
+      <c r="D159" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C160" s="1">
+        <v>1</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C161" s="1">
+        <v>2</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C162" s="1">
+        <v>3</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C163" s="1">
+        <v>4</v>
+      </c>
+      <c r="D163" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E163" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C164" s="1">
+        <v>5</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C165" s="1">
         <v>6</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D121" s="1" t="s">
+      <c r="D165" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E176" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E177" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E178" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E179" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E181" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E183" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E185" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E186" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C187" s="1">
+        <v>1</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C188" s="1">
+        <v>2</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C194" s="1">
+        <v>1</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E194" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C195" s="1">
+        <v>2</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E195" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C196" s="1">
+        <v>3</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E196" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C197" s="1">
+        <v>4</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E197" s="1">
         <v>7</v>
       </c>
-      <c r="E121" s="1" t="s">
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C198" s="1">
+        <v>5</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E198" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C199" s="1">
+        <v>6</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E199" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C200" s="1">
+        <v>7</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E200" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C201" s="1">
+        <v>8</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E201" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C202" s="1">
+        <v>9</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E202" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C203" s="1">
+        <v>10</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E203" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C204" s="1">
+        <v>11</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E204" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C205" s="1">
+        <v>12</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E205" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C206" s="1">
+        <v>13</v>
+      </c>
+      <c r="D206" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E206" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C207" s="1">
+        <v>14</v>
+      </c>
+      <c r="D207" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E207" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C208" s="1">
+        <v>15</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E208" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C209" s="1">
+        <v>16</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E209" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C210" s="1">
+        <v>17</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E210" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C211" s="1">
+        <v>18</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E211" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C212" s="1">
+        <v>19</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E212" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C213" s="1">
+        <v>20</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E213" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C214" s="1">
+        <v>1</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E214" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C215" s="1">
+        <v>2</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E215" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C216" s="1">
+        <v>3</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E216" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C217" s="1">
+        <v>4</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E217" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C218" s="1">
+        <v>5</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E218" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C219" s="1">
+        <v>6</v>
+      </c>
+      <c r="D219" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E219" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C220" s="1">
+        <v>7</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E220" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C221" s="1">
+        <v>8</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E221" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C222" s="1">
+        <v>9</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E222" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C223" s="1">
+        <v>10</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E223" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C224" s="1">
+        <v>11</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E224" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C225" s="1">
+        <v>12</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E225" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C226" s="1">
+        <v>13</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E226" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C227" s="1">
+        <v>14</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E227" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C228" s="1">
+        <v>15</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E228" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C229" s="1">
+        <v>16</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E229" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B230" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C230" s="1">
+        <v>17</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E230" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C231" s="1">
+        <v>18</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E231" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C232" s="1">
+        <v>19</v>
+      </c>
+      <c r="D232" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E232" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C233" s="1">
+        <v>20</v>
+      </c>
+      <c r="D233" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E233" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B234" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D234" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D235" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D236" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C240" s="1">
+        <v>0</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E240" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C241" s="1">
+        <v>1</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E241" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C242" s="1">
+        <v>2</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E242" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E243" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C244" s="1">
+        <v>0</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E244" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C245" s="1">
+        <v>1</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E245" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C246" s="1">
+        <v>2</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E246" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E247" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C248" s="3">
+        <v>1</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C249" s="3">
+        <v>2</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C250" s="3">
+        <v>3</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E257" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E587">
-    <sortCondition ref="A2:A587"/>
-    <sortCondition ref="B2:B587"/>
-    <sortCondition ref="C2:C587"/>
+  <sortState ref="A2:E257">
+    <sortCondition ref="A2:A257"/>
+    <sortCondition ref="B2:B257"/>
+    <sortCondition ref="C2:C257"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
good pass at standard, legacy needs testing
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -1245,8 +1245,8 @@
   <dimension ref="A1:E257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new caltrain data; all tableau but last
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2355" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="362">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1049,21 +1049,9 @@
     <t>exempt (employee, law enforcement)</t>
   </si>
   <si>
-    <t>SURVEYMODE_PLACEHOLDER</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>on_off_dummy</t>
   </si>
   <si>
-    <t>SURVEYLANGUAGE_PLACEHOLDER</t>
-  </si>
-  <si>
-    <t>UNLNKD_WGT_FCTR_BtoA</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -1098,6 +1086,30 @@
   </si>
   <si>
     <t>WEEKEND</t>
+  </si>
+  <si>
+    <t>SURVEY_TYPE</t>
+  </si>
+  <si>
+    <t>Tablet</t>
+  </si>
+  <si>
+    <t>SURVEY_LANGUAGE</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Korean</t>
+  </si>
+  <si>
+    <t>Vietnamese</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>MTC_WEIGHT</t>
   </si>
 </sst>
 </file>
@@ -1530,11 +1542,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E579"/>
+  <dimension ref="A1:E580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E234" sqref="E234"/>
+      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5535,7 +5547,7 @@
         <v>4</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E235" s="1" t="s">
         <v>4</v>
@@ -6634,10 +6646,10 @@
         <v>296</v>
       </c>
       <c r="B300" s="5" t="s">
-        <v>341</v>
+        <v>354</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>283</v>
+        <v>355</v>
       </c>
       <c r="D300" s="5" t="s">
         <v>284</v>
@@ -6651,16 +6663,16 @@
         <v>296</v>
       </c>
       <c r="B301" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="C301" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="C301" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="D301" s="5" t="s">
         <v>284</v>
       </c>
       <c r="E301" s="5" t="s">
-        <v>286</v>
+        <v>341</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -6668,16 +6680,16 @@
         <v>296</v>
       </c>
       <c r="B302" s="5" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="C302" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D302" s="5" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E302" s="5" t="s">
-        <v>287</v>
+        <v>360</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -6685,16 +6697,16 @@
         <v>296</v>
       </c>
       <c r="B303" s="5" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
       <c r="C303" s="5" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
       <c r="D303" s="5" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E303" s="5" t="s">
-        <v>343</v>
+        <v>187</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -6702,16 +6714,16 @@
         <v>296</v>
       </c>
       <c r="B304" s="5" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="C304" s="5" t="s">
-        <v>261</v>
+        <v>293</v>
       </c>
       <c r="D304" s="5" t="s">
         <v>291</v>
       </c>
       <c r="E304" s="5" t="s">
-        <v>292</v>
+        <v>179</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -6719,33 +6731,33 @@
         <v>296</v>
       </c>
       <c r="B305" s="5" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="C305" s="5" t="s">
-        <v>259</v>
+        <v>358</v>
       </c>
       <c r="D305" s="5" t="s">
         <v>291</v>
       </c>
       <c r="E305" s="5" t="s">
-        <v>293</v>
+        <v>180</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A306" s="5" t="s">
+      <c r="A306" s="1" t="s">
         <v>296</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>294</v>
+        <v>356</v>
       </c>
       <c r="C306" s="5" t="s">
-        <v>4</v>
+        <v>359</v>
       </c>
       <c r="D306" s="5" t="s">
-        <v>110</v>
+        <v>291</v>
       </c>
       <c r="E306" s="5" t="s">
-        <v>4</v>
+        <v>217</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -6753,13 +6765,13 @@
         <v>296</v>
       </c>
       <c r="B307" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C307" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D307" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E307" s="5" t="s">
         <v>4</v>
@@ -6770,13 +6782,13 @@
         <v>296</v>
       </c>
       <c r="B308" s="5" t="s">
-        <v>266</v>
+        <v>295</v>
       </c>
       <c r="C308" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D308" s="5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E308" s="5" t="s">
         <v>4</v>
@@ -6787,13 +6799,13 @@
         <v>296</v>
       </c>
       <c r="B309" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C309" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D309" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E309" s="5" t="s">
         <v>4</v>
@@ -6804,16 +6816,16 @@
         <v>296</v>
       </c>
       <c r="B310" s="5" t="s">
-        <v>352</v>
+        <v>267</v>
       </c>
       <c r="C310" s="5" t="s">
-        <v>353</v>
+        <v>4</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>354</v>
+        <v>109</v>
       </c>
       <c r="E310" s="5" t="s">
-        <v>355</v>
+        <v>4</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -6821,16 +6833,16 @@
         <v>296</v>
       </c>
       <c r="B311" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C311" s="5" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E311" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -6838,32 +6850,32 @@
         <v>296</v>
       </c>
       <c r="B312" s="5" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C312" s="5" t="s">
-        <v>4</v>
+        <v>352</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="E312" s="5" t="s">
-        <v>4</v>
+        <v>353</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A313" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B313" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="C313" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D313" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E313" s="4" t="s">
+      <c r="A313" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B313" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C313" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D313" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E313" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -6872,13 +6884,13 @@
         <v>257</v>
       </c>
       <c r="B314" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C314" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D314" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E314" s="4" t="s">
         <v>4</v>
@@ -6889,16 +6901,16 @@
         <v>257</v>
       </c>
       <c r="B315" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C315" s="4">
-        <v>1</v>
+        <v>295</v>
+      </c>
+      <c r="C315" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D315" s="4" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E315" s="4" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -6909,13 +6921,13 @@
         <v>128</v>
       </c>
       <c r="C316" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D316" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E316" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -6926,13 +6938,13 @@
         <v>128</v>
       </c>
       <c r="C317" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D317" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E317" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
@@ -6943,7 +6955,7 @@
         <v>128</v>
       </c>
       <c r="C318" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D318" s="4" t="s">
         <v>129</v>
@@ -6960,7 +6972,7 @@
         <v>128</v>
       </c>
       <c r="C319" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D319" s="4" t="s">
         <v>129</v>
@@ -6977,7 +6989,7 @@
         <v>128</v>
       </c>
       <c r="C320" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D320" s="4" t="s">
         <v>129</v>
@@ -6994,13 +7006,13 @@
         <v>128</v>
       </c>
       <c r="C321" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D321" s="4" t="s">
         <v>129</v>
       </c>
       <c r="E321" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
@@ -7011,7 +7023,7 @@
         <v>128</v>
       </c>
       <c r="C322" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D322" s="4" t="s">
         <v>129</v>
@@ -7028,7 +7040,7 @@
         <v>128</v>
       </c>
       <c r="C323" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D323" s="4" t="s">
         <v>129</v>
@@ -7042,16 +7054,16 @@
         <v>257</v>
       </c>
       <c r="B324" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C324" s="4" t="s">
-        <v>57</v>
+        <v>128</v>
+      </c>
+      <c r="C324" s="4">
+        <v>9</v>
       </c>
       <c r="D324" s="4" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="E324" s="4" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
@@ -7062,13 +7074,13 @@
         <v>70</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D325" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E325" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -7076,16 +7088,16 @@
         <v>257</v>
       </c>
       <c r="B326" s="4" t="s">
-        <v>258</v>
+        <v>70</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D326" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E326" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -7096,13 +7108,13 @@
         <v>258</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D327" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E327" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -7110,16 +7122,16 @@
         <v>257</v>
       </c>
       <c r="B328" s="4" t="s">
-        <v>90</v>
+        <v>258</v>
       </c>
       <c r="C328" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D328" s="4" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="E328" s="4" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -7127,13 +7139,13 @@
         <v>257</v>
       </c>
       <c r="B329" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C329" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D329" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E329" s="4" t="s">
         <v>4</v>
@@ -7144,16 +7156,16 @@
         <v>257</v>
       </c>
       <c r="B330" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C330" s="4">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="C330" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D330" s="4" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="E330" s="4" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -7164,13 +7176,13 @@
         <v>51</v>
       </c>
       <c r="C331" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D331" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E331" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -7181,13 +7193,13 @@
         <v>51</v>
       </c>
       <c r="C332" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D332" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E332" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -7198,13 +7210,13 @@
         <v>51</v>
       </c>
       <c r="C333" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D333" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E333" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -7215,13 +7227,13 @@
         <v>51</v>
       </c>
       <c r="C334" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D334" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E334" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -7232,13 +7244,13 @@
         <v>51</v>
       </c>
       <c r="C335" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D335" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E335" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -7249,13 +7261,13 @@
         <v>51</v>
       </c>
       <c r="C336" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D336" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E336" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -7266,13 +7278,13 @@
         <v>51</v>
       </c>
       <c r="C337" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D337" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E337" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -7283,13 +7295,13 @@
         <v>51</v>
       </c>
       <c r="C338" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D338" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E338" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -7300,13 +7312,13 @@
         <v>51</v>
       </c>
       <c r="C339" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D339" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E339" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -7317,13 +7329,13 @@
         <v>51</v>
       </c>
       <c r="C340" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D340" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E340" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
@@ -7334,13 +7346,13 @@
         <v>51</v>
       </c>
       <c r="C341" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D341" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E341" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
@@ -7351,13 +7363,13 @@
         <v>51</v>
       </c>
       <c r="C342" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D342" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E342" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
@@ -7368,13 +7380,13 @@
         <v>51</v>
       </c>
       <c r="C343" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D343" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E343" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -7385,13 +7397,13 @@
         <v>51</v>
       </c>
       <c r="C344" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D344" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E344" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
@@ -7399,16 +7411,16 @@
         <v>257</v>
       </c>
       <c r="B345" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C345" s="4" t="s">
-        <v>155</v>
+        <v>51</v>
+      </c>
+      <c r="C345" s="4">
+        <v>15</v>
       </c>
       <c r="D345" s="4" t="s">
-        <v>246</v>
+        <v>52</v>
       </c>
       <c r="E345" s="4" t="s">
-        <v>247</v>
+        <v>54</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -7419,13 +7431,13 @@
         <v>245</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>259</v>
+        <v>155</v>
       </c>
       <c r="D346" s="4" t="s">
         <v>246</v>
       </c>
       <c r="E346" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -7436,13 +7448,13 @@
         <v>245</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D347" s="4" t="s">
         <v>246</v>
       </c>
       <c r="E347" s="4" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -7453,13 +7465,13 @@
         <v>245</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D348" s="4" t="s">
         <v>246</v>
       </c>
       <c r="E348" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -7470,13 +7482,13 @@
         <v>245</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D349" s="4" t="s">
         <v>246</v>
       </c>
       <c r="E349" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -7484,16 +7496,16 @@
         <v>257</v>
       </c>
       <c r="B350" s="4" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>4</v>
+        <v>262</v>
       </c>
       <c r="D350" s="4" t="s">
-        <v>108</v>
+        <v>246</v>
       </c>
       <c r="E350" s="4" t="s">
-        <v>4</v>
+        <v>265</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -7501,13 +7513,13 @@
         <v>257</v>
       </c>
       <c r="B351" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C351" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D351" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E351" s="4" t="s">
         <v>4</v>
@@ -7518,16 +7530,16 @@
         <v>257</v>
       </c>
       <c r="B352" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C352" s="4">
-        <v>1</v>
+        <v>267</v>
+      </c>
+      <c r="C352" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D352" s="4" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="E352" s="4" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
@@ -7538,13 +7550,13 @@
         <v>134</v>
       </c>
       <c r="C353" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D353" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E353" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
@@ -7555,13 +7567,13 @@
         <v>134</v>
       </c>
       <c r="C354" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D354" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E354" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -7572,7 +7584,7 @@
         <v>134</v>
       </c>
       <c r="C355" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D355" s="4" t="s">
         <v>135</v>
@@ -7589,7 +7601,7 @@
         <v>134</v>
       </c>
       <c r="C356" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D356" s="4" t="s">
         <v>135</v>
@@ -7606,7 +7618,7 @@
         <v>134</v>
       </c>
       <c r="C357" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D357" s="4" t="s">
         <v>135</v>
@@ -7623,13 +7635,13 @@
         <v>134</v>
       </c>
       <c r="C358" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D358" s="4" t="s">
         <v>135</v>
       </c>
       <c r="E358" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
@@ -7640,7 +7652,7 @@
         <v>134</v>
       </c>
       <c r="C359" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D359" s="4" t="s">
         <v>135</v>
@@ -7657,7 +7669,7 @@
         <v>134</v>
       </c>
       <c r="C360" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D360" s="4" t="s">
         <v>135</v>
@@ -7671,16 +7683,16 @@
         <v>257</v>
       </c>
       <c r="B361" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C361" s="4" t="s">
-        <v>57</v>
+        <v>134</v>
+      </c>
+      <c r="C361" s="4">
+        <v>9</v>
       </c>
       <c r="D361" s="4" t="s">
-        <v>249</v>
+        <v>135</v>
       </c>
       <c r="E361" s="4" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -7691,13 +7703,13 @@
         <v>55</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D362" s="4" t="s">
         <v>249</v>
       </c>
       <c r="E362" s="4" t="s">
-        <v>138</v>
+        <v>58</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -7705,16 +7717,16 @@
         <v>257</v>
       </c>
       <c r="B363" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C363" s="4">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="C363" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D363" s="4" t="s">
-        <v>16</v>
+        <v>249</v>
       </c>
       <c r="E363" s="4" t="s">
-        <v>10</v>
+        <v>138</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -7725,13 +7737,13 @@
         <v>25</v>
       </c>
       <c r="C364" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D364" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E364" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
@@ -7742,13 +7754,13 @@
         <v>25</v>
       </c>
       <c r="C365" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D365" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E365" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -7759,13 +7771,13 @@
         <v>25</v>
       </c>
       <c r="C366" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D366" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E366" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -7776,13 +7788,13 @@
         <v>25</v>
       </c>
       <c r="C367" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D367" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E367" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -7793,13 +7805,13 @@
         <v>25</v>
       </c>
       <c r="C368" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D368" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E368" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -7810,13 +7822,13 @@
         <v>25</v>
       </c>
       <c r="C369" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D369" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E369" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -7824,16 +7836,16 @@
         <v>257</v>
       </c>
       <c r="B370" s="4" t="s">
-        <v>239</v>
+        <v>25</v>
       </c>
       <c r="C370" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D370" s="4" t="s">
-        <v>244</v>
+        <v>16</v>
       </c>
       <c r="E370" s="4" t="s">
-        <v>240</v>
+        <v>24</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -7844,13 +7856,13 @@
         <v>239</v>
       </c>
       <c r="C371" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D371" s="4" t="s">
         <v>244</v>
       </c>
       <c r="E371" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -7861,13 +7873,13 @@
         <v>239</v>
       </c>
       <c r="C372" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D372" s="4" t="s">
         <v>244</v>
       </c>
       <c r="E372" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -7878,13 +7890,13 @@
         <v>239</v>
       </c>
       <c r="C373" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D373" s="4" t="s">
         <v>244</v>
       </c>
       <c r="E373" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
@@ -7892,16 +7904,16 @@
         <v>257</v>
       </c>
       <c r="B374" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C374" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C374" s="4">
         <v>4</v>
       </c>
       <c r="D374" s="4" t="s">
-        <v>99</v>
+        <v>244</v>
       </c>
       <c r="E374" s="4" t="s">
-        <v>4</v>
+        <v>243</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
@@ -7909,13 +7921,13 @@
         <v>257</v>
       </c>
       <c r="B375" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C375" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E375" s="4" t="s">
         <v>4</v>
@@ -7926,13 +7938,13 @@
         <v>257</v>
       </c>
       <c r="B376" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C376" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E376" s="4" t="s">
         <v>4</v>
@@ -7943,13 +7955,13 @@
         <v>257</v>
       </c>
       <c r="B377" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C377" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D377" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E377" s="4" t="s">
         <v>4</v>
@@ -7960,16 +7972,16 @@
         <v>257</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C378" s="4">
-        <v>1</v>
+        <v>271</v>
+      </c>
+      <c r="C378" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D378" s="4" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="E378" s="4" t="s">
-        <v>149</v>
+        <v>4</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
@@ -7980,13 +7992,13 @@
         <v>147</v>
       </c>
       <c r="C379" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D379" s="4" t="s">
         <v>148</v>
       </c>
       <c r="E379" s="4" t="s">
-        <v>272</v>
+        <v>149</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
@@ -7997,13 +8009,13 @@
         <v>147</v>
       </c>
       <c r="C380" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D380" s="4" t="s">
         <v>148</v>
       </c>
       <c r="E380" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
@@ -8011,16 +8023,16 @@
         <v>257</v>
       </c>
       <c r="B381" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C381" s="4" t="s">
-        <v>57</v>
+        <v>147</v>
+      </c>
+      <c r="C381" s="4">
+        <v>3</v>
       </c>
       <c r="D381" s="4" t="s">
-        <v>67</v>
+        <v>148</v>
       </c>
       <c r="E381" s="4" t="s">
-        <v>69</v>
+        <v>273</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
@@ -8031,13 +8043,13 @@
         <v>274</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D382" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E382" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -8045,16 +8057,16 @@
         <v>257</v>
       </c>
       <c r="B383" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C383" s="4">
-        <v>1</v>
+        <v>274</v>
+      </c>
+      <c r="C383" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="D383" s="4" t="s">
-        <v>225</v>
+        <v>67</v>
       </c>
       <c r="E383" s="4" t="s">
-        <v>226</v>
+        <v>68</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
@@ -8065,13 +8077,13 @@
         <v>224</v>
       </c>
       <c r="C384" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D384" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E384" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
@@ -8082,13 +8094,13 @@
         <v>224</v>
       </c>
       <c r="C385" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D385" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E385" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
@@ -8099,13 +8111,13 @@
         <v>224</v>
       </c>
       <c r="C386" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D386" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E386" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -8116,7 +8128,7 @@
         <v>224</v>
       </c>
       <c r="C387" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D387" s="4" t="s">
         <v>225</v>
@@ -8133,13 +8145,13 @@
         <v>224</v>
       </c>
       <c r="C388" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D388" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E388" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
@@ -8150,7 +8162,7 @@
         <v>224</v>
       </c>
       <c r="C389" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D389" s="4" t="s">
         <v>225</v>
@@ -8167,13 +8179,13 @@
         <v>224</v>
       </c>
       <c r="C390" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D390" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E390" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="391" spans="1:5" x14ac:dyDescent="0.25">
@@ -8184,13 +8196,13 @@
         <v>224</v>
       </c>
       <c r="C391" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D391" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E391" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
@@ -8201,13 +8213,13 @@
         <v>224</v>
       </c>
       <c r="C392" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D392" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E392" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="393" spans="1:5" x14ac:dyDescent="0.25">
@@ -8218,13 +8230,13 @@
         <v>224</v>
       </c>
       <c r="C393" s="4">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="D393" s="4" t="s">
         <v>225</v>
       </c>
       <c r="E393" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="394" spans="1:5" x14ac:dyDescent="0.25">
@@ -8235,7 +8247,7 @@
         <v>224</v>
       </c>
       <c r="C394" s="4">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D394" s="4" t="s">
         <v>225</v>
@@ -8249,16 +8261,16 @@
         <v>257</v>
       </c>
       <c r="B395" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C395" s="4" t="s">
-        <v>155</v>
+        <v>224</v>
+      </c>
+      <c r="C395" s="4">
+        <v>99</v>
       </c>
       <c r="D395" s="4" t="s">
-        <v>156</v>
+        <v>225</v>
       </c>
       <c r="E395" s="4" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
@@ -8269,13 +8281,13 @@
         <v>153</v>
       </c>
       <c r="C396" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D396" s="4" t="s">
         <v>156</v>
       </c>
       <c r="E396" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
@@ -8283,16 +8295,16 @@
         <v>257</v>
       </c>
       <c r="B397" s="4" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>4</v>
+        <v>154</v>
       </c>
       <c r="D397" s="4" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="E397" s="4" t="s">
-        <v>4</v>
+        <v>157</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
@@ -8300,13 +8312,13 @@
         <v>257</v>
       </c>
       <c r="B398" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C398" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D398" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E398" s="4" t="s">
         <v>4</v>
@@ -8317,13 +8329,13 @@
         <v>257</v>
       </c>
       <c r="B399" s="4" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="C399" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D399" s="4" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="E399" s="4" t="s">
         <v>4</v>
@@ -8334,16 +8346,16 @@
         <v>257</v>
       </c>
       <c r="B400" s="4" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="C400" s="4" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D400" s="4" t="s">
-        <v>173</v>
+        <v>5</v>
       </c>
       <c r="E400" s="4" t="s">
-        <v>172</v>
+        <v>4</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
@@ -8354,13 +8366,13 @@
         <v>171</v>
       </c>
       <c r="C401" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D401" s="4" t="s">
         <v>173</v>
       </c>
       <c r="E401" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
@@ -8368,16 +8380,16 @@
         <v>257</v>
       </c>
       <c r="B402" s="4" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D402" s="4" t="s">
-        <v>95</v>
+        <v>173</v>
       </c>
       <c r="E402" s="4" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
@@ -8385,13 +8397,13 @@
         <v>257</v>
       </c>
       <c r="B403" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C403" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D403" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E403" s="4" t="s">
         <v>4</v>
@@ -8402,16 +8414,16 @@
         <v>257</v>
       </c>
       <c r="B404" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C404" s="4">
-        <v>1</v>
+        <v>96</v>
+      </c>
+      <c r="C404" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D404" s="4" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="E404" s="4" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
@@ -8422,13 +8434,13 @@
         <v>39</v>
       </c>
       <c r="C405" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D405" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E405" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
@@ -8439,13 +8451,13 @@
         <v>39</v>
       </c>
       <c r="C406" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D406" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E406" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
@@ -8456,13 +8468,13 @@
         <v>39</v>
       </c>
       <c r="C407" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D407" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E407" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -8473,13 +8485,13 @@
         <v>39</v>
       </c>
       <c r="C408" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D408" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E408" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
@@ -8490,13 +8502,13 @@
         <v>39</v>
       </c>
       <c r="C409" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D409" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E409" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
@@ -8507,13 +8519,13 @@
         <v>39</v>
       </c>
       <c r="C410" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D410" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E410" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
@@ -8524,13 +8536,13 @@
         <v>39</v>
       </c>
       <c r="C411" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D411" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E411" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
@@ -8541,13 +8553,13 @@
         <v>39</v>
       </c>
       <c r="C412" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D412" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E412" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
@@ -8558,13 +8570,13 @@
         <v>39</v>
       </c>
       <c r="C413" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D413" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E413" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
@@ -8575,13 +8587,13 @@
         <v>39</v>
       </c>
       <c r="C414" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D414" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E414" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
@@ -8592,13 +8604,13 @@
         <v>39</v>
       </c>
       <c r="C415" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D415" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E415" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
@@ -8609,7 +8621,7 @@
         <v>39</v>
       </c>
       <c r="C416" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D416" s="4" t="s">
         <v>40</v>
@@ -8626,7 +8638,7 @@
         <v>39</v>
       </c>
       <c r="C417" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D417" s="4" t="s">
         <v>40</v>
@@ -8643,13 +8655,13 @@
         <v>39</v>
       </c>
       <c r="C418" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D418" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E418" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
@@ -8657,16 +8669,16 @@
         <v>257</v>
       </c>
       <c r="B419" s="4" t="s">
-        <v>175</v>
+        <v>39</v>
       </c>
       <c r="C419" s="4">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D419" s="4" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="E419" s="4" t="s">
-        <v>188</v>
+        <v>54</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
@@ -8677,13 +8689,13 @@
         <v>175</v>
       </c>
       <c r="C420" s="4">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D420" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E420" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -8694,13 +8706,13 @@
         <v>175</v>
       </c>
       <c r="C421" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D421" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E421" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
@@ -8711,13 +8723,13 @@
         <v>175</v>
       </c>
       <c r="C422" s="4">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D422" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E422" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -8728,7 +8740,7 @@
         <v>175</v>
       </c>
       <c r="C423" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D423" s="4" t="s">
         <v>176</v>
@@ -8745,13 +8757,13 @@
         <v>175</v>
       </c>
       <c r="C424" s="4">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D424" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E424" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
@@ -8762,13 +8774,13 @@
         <v>175</v>
       </c>
       <c r="C425" s="4">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D425" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E425" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -8779,13 +8791,13 @@
         <v>175</v>
       </c>
       <c r="C426" s="4">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D426" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E426" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
@@ -8796,13 +8808,13 @@
         <v>175</v>
       </c>
       <c r="C427" s="4">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D427" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E427" s="4" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
@@ -8813,13 +8825,13 @@
         <v>175</v>
       </c>
       <c r="C428" s="4">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D428" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E428" s="4" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -8830,13 +8842,13 @@
         <v>175</v>
       </c>
       <c r="C429" s="4">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="D429" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E429" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -8847,13 +8859,13 @@
         <v>175</v>
       </c>
       <c r="C430" s="4">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D430" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E430" s="4" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
@@ -8864,13 +8876,13 @@
         <v>175</v>
       </c>
       <c r="C431" s="4">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D431" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E431" s="4" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
@@ -8881,13 +8893,13 @@
         <v>175</v>
       </c>
       <c r="C432" s="4">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D432" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E432" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.25">
@@ -8898,13 +8910,13 @@
         <v>175</v>
       </c>
       <c r="C433" s="4">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D433" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E433" s="4" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
@@ -8915,13 +8927,13 @@
         <v>175</v>
       </c>
       <c r="C434" s="4">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D434" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E434" s="4" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
@@ -8932,13 +8944,13 @@
         <v>175</v>
       </c>
       <c r="C435" s="4">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D435" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E435" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.25">
@@ -8949,13 +8961,13 @@
         <v>175</v>
       </c>
       <c r="C436" s="4">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D436" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E436" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
@@ -8966,13 +8978,13 @@
         <v>175</v>
       </c>
       <c r="C437" s="4">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D437" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E437" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -8983,13 +8995,13 @@
         <v>175</v>
       </c>
       <c r="C438" s="4">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D438" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E438" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
@@ -9000,13 +9012,13 @@
         <v>175</v>
       </c>
       <c r="C439" s="4">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="D439" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E439" s="4" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
@@ -9017,13 +9029,13 @@
         <v>175</v>
       </c>
       <c r="C440" s="4">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="D440" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E440" s="4" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
@@ -9034,13 +9046,13 @@
         <v>175</v>
       </c>
       <c r="C441" s="4">
-        <v>279</v>
+        <v>220</v>
       </c>
       <c r="D441" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E441" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
@@ -9051,13 +9063,13 @@
         <v>175</v>
       </c>
       <c r="C442" s="4">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="D442" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E442" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
@@ -9068,13 +9080,13 @@
         <v>175</v>
       </c>
       <c r="C443" s="4">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="D443" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E443" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
@@ -9085,13 +9097,13 @@
         <v>175</v>
       </c>
       <c r="C444" s="4">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D444" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E444" s="4" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
@@ -9102,13 +9114,13 @@
         <v>175</v>
       </c>
       <c r="C445" s="4">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="D445" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E445" s="4" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -9125,7 +9137,7 @@
         <v>176</v>
       </c>
       <c r="E446" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.25">
@@ -9136,13 +9148,13 @@
         <v>175</v>
       </c>
       <c r="C447" s="4">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="D447" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E447" s="4" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -9153,13 +9165,13 @@
         <v>175</v>
       </c>
       <c r="C448" s="4">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D448" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E448" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -9170,13 +9182,13 @@
         <v>175</v>
       </c>
       <c r="C449" s="4">
-        <v>378</v>
+        <v>358</v>
       </c>
       <c r="D449" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E449" s="4" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -9187,13 +9199,13 @@
         <v>175</v>
       </c>
       <c r="C450" s="4">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D450" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E450" s="4" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
@@ -9204,13 +9216,13 @@
         <v>175</v>
       </c>
       <c r="C451" s="4">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="D451" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E451" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
@@ -9221,13 +9233,13 @@
         <v>175</v>
       </c>
       <c r="C452" s="4">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="D452" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E452" s="4" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
@@ -9238,13 +9250,13 @@
         <v>175</v>
       </c>
       <c r="C453" s="4">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D453" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E453" s="4" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
@@ -9255,13 +9267,13 @@
         <v>175</v>
       </c>
       <c r="C454" s="4">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D454" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E454" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
@@ -9272,13 +9284,13 @@
         <v>175</v>
       </c>
       <c r="C455" s="4">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D455" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E455" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.25">
@@ -9289,13 +9301,13 @@
         <v>175</v>
       </c>
       <c r="C456" s="4">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D456" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E456" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
@@ -9306,13 +9318,13 @@
         <v>175</v>
       </c>
       <c r="C457" s="4">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D457" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E457" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
@@ -9323,13 +9335,13 @@
         <v>175</v>
       </c>
       <c r="C458" s="4">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D458" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E458" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -9340,13 +9352,13 @@
         <v>175</v>
       </c>
       <c r="C459" s="4">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="D459" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E459" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
@@ -9357,13 +9369,13 @@
         <v>175</v>
       </c>
       <c r="C460" s="4">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="D460" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E460" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
@@ -9374,13 +9386,13 @@
         <v>175</v>
       </c>
       <c r="C461" s="4">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D461" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E461" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
@@ -9391,13 +9403,13 @@
         <v>175</v>
       </c>
       <c r="C462" s="4">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D462" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E462" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">
@@ -9408,13 +9420,13 @@
         <v>175</v>
       </c>
       <c r="C463" s="4">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D463" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E463" s="4" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
@@ -9425,13 +9437,13 @@
         <v>175</v>
       </c>
       <c r="C464" s="4">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="D464" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E464" s="4" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.25">
@@ -9442,13 +9454,13 @@
         <v>175</v>
       </c>
       <c r="C465" s="4">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D465" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E465" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.25">
@@ -9459,13 +9471,13 @@
         <v>175</v>
       </c>
       <c r="C466" s="4">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D466" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E466" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
@@ -9476,13 +9488,13 @@
         <v>175</v>
       </c>
       <c r="C467" s="4">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D467" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E467" s="4" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
@@ -9493,13 +9505,13 @@
         <v>175</v>
       </c>
       <c r="C468" s="4">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D468" s="4" t="s">
         <v>176</v>
       </c>
       <c r="E468" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
@@ -9507,16 +9519,16 @@
         <v>257</v>
       </c>
       <c r="B469" s="4" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="C469" s="4">
-        <v>1</v>
+        <v>504</v>
       </c>
       <c r="D469" s="4" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="E469" s="4" t="s">
-        <v>275</v>
+        <v>187</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
@@ -9527,13 +9539,13 @@
         <v>140</v>
       </c>
       <c r="C470" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D470" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E470" s="4" t="s">
-        <v>141</v>
+        <v>275</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
@@ -9544,13 +9556,13 @@
         <v>140</v>
       </c>
       <c r="C471" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D471" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E471" s="4" t="s">
-        <v>276</v>
+        <v>141</v>
       </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.25">
@@ -9561,13 +9573,13 @@
         <v>140</v>
       </c>
       <c r="C472" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D472" s="4" t="s">
         <v>139</v>
       </c>
       <c r="E472" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.25">
@@ -9575,16 +9587,16 @@
         <v>257</v>
       </c>
       <c r="B473" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C473" s="4" t="s">
-        <v>27</v>
+        <v>140</v>
+      </c>
+      <c r="C473" s="4">
+        <v>4</v>
       </c>
       <c r="D473" s="4" t="s">
-        <v>37</v>
+        <v>139</v>
       </c>
       <c r="E473" s="4" t="s">
-        <v>14</v>
+        <v>277</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
@@ -9595,13 +9607,13 @@
         <v>26</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D474" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E474" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
@@ -9612,13 +9624,13 @@
         <v>26</v>
       </c>
       <c r="C475" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D475" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E475" s="4" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
@@ -9629,13 +9641,13 @@
         <v>26</v>
       </c>
       <c r="C476" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D476" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E476" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
@@ -9646,13 +9658,13 @@
         <v>26</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D477" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E477" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.25">
@@ -9663,13 +9675,13 @@
         <v>26</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D478" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E478" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
@@ -9680,13 +9692,13 @@
         <v>26</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D479" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E479" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
@@ -9697,13 +9709,13 @@
         <v>26</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D480" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E480" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.25">
@@ -9714,13 +9726,13 @@
         <v>26</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D481" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E481" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.25">
@@ -9731,13 +9743,13 @@
         <v>26</v>
       </c>
       <c r="C482" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D482" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E482" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
@@ -9745,16 +9757,16 @@
         <v>257</v>
       </c>
       <c r="B483" s="4" t="s">
-        <v>159</v>
+        <v>26</v>
       </c>
       <c r="C483" s="4" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D483" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E483" s="4">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="E483" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
@@ -9765,13 +9777,13 @@
         <v>159</v>
       </c>
       <c r="C484" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D484" s="4" t="s">
         <v>160</v>
       </c>
       <c r="E484" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
@@ -9779,16 +9791,16 @@
         <v>257</v>
       </c>
       <c r="B485" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C485" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D485" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E485" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
@@ -9799,13 +9811,13 @@
         <v>161</v>
       </c>
       <c r="C486" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D486" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E486" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
@@ -9813,16 +9825,16 @@
         <v>257</v>
       </c>
       <c r="B487" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C487" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D487" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E487" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
@@ -9833,13 +9845,13 @@
         <v>163</v>
       </c>
       <c r="C488" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D488" s="4" t="s">
         <v>164</v>
       </c>
       <c r="E488" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.25">
@@ -9847,16 +9859,16 @@
         <v>257</v>
       </c>
       <c r="B489" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C489" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E489" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.25">
@@ -9867,13 +9879,13 @@
         <v>165</v>
       </c>
       <c r="C490" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D490" s="4" t="s">
         <v>166</v>
       </c>
       <c r="E490" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
@@ -9881,16 +9893,16 @@
         <v>257</v>
       </c>
       <c r="B491" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C491" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D491" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E491" s="4" t="s">
-        <v>4</v>
+        <v>166</v>
+      </c>
+      <c r="E491" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
@@ -9898,16 +9910,16 @@
         <v>257</v>
       </c>
       <c r="B492" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C492" s="4" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E492" s="4">
-        <v>0</v>
+        <v>170</v>
+      </c>
+      <c r="E492" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">
@@ -9918,13 +9930,13 @@
         <v>167</v>
       </c>
       <c r="C493" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D493" s="4" t="s">
         <v>168</v>
       </c>
       <c r="E493" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
@@ -9932,16 +9944,16 @@
         <v>257</v>
       </c>
       <c r="B494" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C494" s="4">
+        <v>167</v>
+      </c>
+      <c r="C494" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D494" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E494" s="4">
         <v>1</v>
-      </c>
-      <c r="D494" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E494" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
@@ -9952,13 +9964,13 @@
         <v>278</v>
       </c>
       <c r="C495" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D495" s="4" t="s">
         <v>236</v>
       </c>
       <c r="E495" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
@@ -9966,16 +9978,16 @@
         <v>257</v>
       </c>
       <c r="B496" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C496" s="4" t="s">
-        <v>4</v>
+        <v>278</v>
+      </c>
+      <c r="C496" s="4">
+        <v>2</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>87</v>
+        <v>236</v>
       </c>
       <c r="E496" s="4" t="s">
-        <v>4</v>
+        <v>238</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -9983,13 +9995,13 @@
         <v>257</v>
       </c>
       <c r="B497" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C497" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E497" s="4" t="s">
         <v>4</v>
@@ -10000,16 +10012,16 @@
         <v>257</v>
       </c>
       <c r="B498" s="4" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="C498" s="4" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="E498" s="4" t="s">
-        <v>61</v>
+        <v>4</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.25">
@@ -10020,13 +10032,13 @@
         <v>59</v>
       </c>
       <c r="C499" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D499" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E499" s="4" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
@@ -10034,16 +10046,16 @@
         <v>257</v>
       </c>
       <c r="B500" s="4" t="s">
-        <v>279</v>
+        <v>59</v>
       </c>
       <c r="C500" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D500" s="4" t="s">
-        <v>255</v>
+        <v>60</v>
       </c>
       <c r="E500" s="4" t="s">
-        <v>4</v>
+        <v>138</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.25">
@@ -10051,15 +10063,15 @@
         <v>257</v>
       </c>
       <c r="B501" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C501" s="4">
-        <v>1</v>
+        <v>279</v>
+      </c>
+      <c r="C501" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="E501" s="4">
+        <v>255</v>
+      </c>
+      <c r="E501" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -10071,13 +10083,13 @@
         <v>280</v>
       </c>
       <c r="C502" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D502" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E502" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.25">
@@ -10088,13 +10100,13 @@
         <v>280</v>
       </c>
       <c r="C503" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D503" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E503" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
@@ -10105,13 +10117,13 @@
         <v>280</v>
       </c>
       <c r="C504" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D504" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E504" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
@@ -10122,13 +10134,13 @@
         <v>280</v>
       </c>
       <c r="C505" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D505" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E505" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
@@ -10139,13 +10151,13 @@
         <v>280</v>
       </c>
       <c r="C506" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D506" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E506" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
@@ -10156,13 +10168,13 @@
         <v>280</v>
       </c>
       <c r="C507" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D507" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E507" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -10173,13 +10185,13 @@
         <v>280</v>
       </c>
       <c r="C508" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D508" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E508" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
@@ -10190,13 +10202,13 @@
         <v>280</v>
       </c>
       <c r="C509" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D509" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E509" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
@@ -10207,13 +10219,13 @@
         <v>280</v>
       </c>
       <c r="C510" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D510" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E510" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
@@ -10224,13 +10236,13 @@
         <v>280</v>
       </c>
       <c r="C511" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D511" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E511" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
@@ -10241,13 +10253,13 @@
         <v>280</v>
       </c>
       <c r="C512" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D512" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E512" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
@@ -10258,13 +10270,13 @@
         <v>280</v>
       </c>
       <c r="C513" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D513" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E513" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
@@ -10275,13 +10287,13 @@
         <v>280</v>
       </c>
       <c r="C514" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D514" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E514" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
@@ -10292,13 +10304,13 @@
         <v>280</v>
       </c>
       <c r="C515" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D515" s="4" t="s">
         <v>251</v>
       </c>
       <c r="E515" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
@@ -10306,16 +10318,16 @@
         <v>257</v>
       </c>
       <c r="B516" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C516" s="4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D516" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E516" s="4">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
@@ -10326,13 +10338,13 @@
         <v>281</v>
       </c>
       <c r="C517" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D517" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E517" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
@@ -10343,13 +10355,13 @@
         <v>281</v>
       </c>
       <c r="C518" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D518" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E518" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
@@ -10360,13 +10372,13 @@
         <v>281</v>
       </c>
       <c r="C519" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D519" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E519" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
@@ -10377,13 +10389,13 @@
         <v>281</v>
       </c>
       <c r="C520" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D520" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E520" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
@@ -10394,13 +10406,13 @@
         <v>281</v>
       </c>
       <c r="C521" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D521" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E521" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
@@ -10411,13 +10423,13 @@
         <v>281</v>
       </c>
       <c r="C522" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D522" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E522" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
@@ -10428,13 +10440,13 @@
         <v>281</v>
       </c>
       <c r="C523" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D523" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E523" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
@@ -10445,13 +10457,13 @@
         <v>281</v>
       </c>
       <c r="C524" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D524" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E524" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
@@ -10462,13 +10474,13 @@
         <v>281</v>
       </c>
       <c r="C525" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D525" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E525" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
@@ -10479,13 +10491,13 @@
         <v>281</v>
       </c>
       <c r="C526" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D526" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E526" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
@@ -10496,13 +10508,13 @@
         <v>281</v>
       </c>
       <c r="C527" s="4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D527" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E527" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
@@ -10513,13 +10525,13 @@
         <v>281</v>
       </c>
       <c r="C528" s="4">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D528" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E528" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
@@ -10530,13 +10542,13 @@
         <v>281</v>
       </c>
       <c r="C529" s="4">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D529" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E529" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -10547,13 +10559,13 @@
         <v>281</v>
       </c>
       <c r="C530" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D530" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E530" s="4">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -10564,13 +10576,13 @@
         <v>281</v>
       </c>
       <c r="C531" s="4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D531" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E531" s="4">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.25">
@@ -10578,16 +10590,16 @@
         <v>257</v>
       </c>
       <c r="B532" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C532" s="4" t="s">
-        <v>4</v>
+        <v>281</v>
+      </c>
+      <c r="C532" s="4">
+        <v>20</v>
       </c>
       <c r="D532" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E532" s="4" t="s">
-        <v>4</v>
+        <v>253</v>
+      </c>
+      <c r="E532" s="4">
+        <v>23</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -10595,13 +10607,13 @@
         <v>257</v>
       </c>
       <c r="B533" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C533" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D533" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E533" s="4" t="s">
         <v>4</v>
@@ -10612,13 +10624,13 @@
         <v>257</v>
       </c>
       <c r="B534" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C534" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D534" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E534" s="4" t="s">
         <v>4</v>
@@ -10629,13 +10641,13 @@
         <v>257</v>
       </c>
       <c r="B535" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C535" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D535" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E535" s="4" t="s">
         <v>4</v>
@@ -10646,13 +10658,13 @@
         <v>257</v>
       </c>
       <c r="B536" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C536" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D536" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E536" s="4" t="s">
         <v>4</v>
@@ -10663,13 +10675,13 @@
         <v>257</v>
       </c>
       <c r="B537" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C537" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D537" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E537" s="4" t="s">
         <v>4</v>
@@ -10680,16 +10692,16 @@
         <v>257</v>
       </c>
       <c r="B538" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C538" s="4">
-        <v>0</v>
+        <v>125</v>
+      </c>
+      <c r="C538" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D538" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E538" s="4">
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="E538" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
@@ -10700,13 +10712,13 @@
         <v>114</v>
       </c>
       <c r="C539" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D539" s="4" t="s">
         <v>136</v>
       </c>
       <c r="E539" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
@@ -10717,13 +10729,13 @@
         <v>114</v>
       </c>
       <c r="C540" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D540" s="4" t="s">
         <v>136</v>
       </c>
       <c r="E540" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
@@ -10734,13 +10746,13 @@
         <v>114</v>
       </c>
       <c r="C541" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D541" s="4" t="s">
         <v>136</v>
       </c>
       <c r="E541" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -10748,16 +10760,16 @@
         <v>257</v>
       </c>
       <c r="B542" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C542" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D542" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E542" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
@@ -10768,13 +10780,13 @@
         <v>115</v>
       </c>
       <c r="C543" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D543" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E543" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -10785,13 +10797,13 @@
         <v>115</v>
       </c>
       <c r="C544" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D544" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E544" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.25">
@@ -10802,13 +10814,13 @@
         <v>115</v>
       </c>
       <c r="C545" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D545" s="4" t="s">
         <v>137</v>
       </c>
       <c r="E545" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="546" spans="1:5" x14ac:dyDescent="0.25">
@@ -10816,16 +10828,16 @@
         <v>257</v>
       </c>
       <c r="B546" s="4" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="C546" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D546" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E546" s="4" t="s">
-        <v>14</v>
+        <v>137</v>
+      </c>
+      <c r="E546" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
@@ -10836,13 +10848,13 @@
         <v>8</v>
       </c>
       <c r="C547" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D547" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E547" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
@@ -10853,13 +10865,13 @@
         <v>8</v>
       </c>
       <c r="C548" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D548" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E548" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.25">
@@ -10869,14 +10881,14 @@
       <c r="B549" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C549" s="4" t="s">
-        <v>20</v>
+      <c r="C549" s="4">
+        <v>3</v>
       </c>
       <c r="D549" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E549" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
@@ -10887,13 +10899,13 @@
         <v>8</v>
       </c>
       <c r="C550" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D550" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E550" s="4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
@@ -10901,16 +10913,16 @@
         <v>257</v>
       </c>
       <c r="B551" s="4" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="C551" s="4" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D551" s="4" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="E551" s="4" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
@@ -10921,13 +10933,13 @@
         <v>77</v>
       </c>
       <c r="C552" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D552" s="4" t="s">
         <v>72</v>
       </c>
       <c r="E552" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
@@ -10935,16 +10947,16 @@
         <v>257</v>
       </c>
       <c r="B553" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C553" s="4" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D553" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E553" s="4" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
@@ -10952,13 +10964,13 @@
         <v>257</v>
       </c>
       <c r="B554" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C554" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D554" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E554" s="4" t="s">
         <v>4</v>
@@ -10969,13 +10981,13 @@
         <v>257</v>
       </c>
       <c r="B555" s="4" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="C555" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D555" s="4" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E555" s="4" t="s">
         <v>4</v>
@@ -10986,16 +10998,16 @@
         <v>257</v>
       </c>
       <c r="B556" s="4" t="s">
-        <v>282</v>
+        <v>6</v>
       </c>
       <c r="C556" s="4" t="s">
-        <v>283</v>
+        <v>4</v>
       </c>
       <c r="D556" s="4" t="s">
-        <v>284</v>
+        <v>7</v>
       </c>
       <c r="E556" s="4" t="s">
-        <v>285</v>
+        <v>4</v>
       </c>
     </row>
     <row r="557" spans="1:5" x14ac:dyDescent="0.25">
@@ -11006,13 +11018,13 @@
         <v>282</v>
       </c>
       <c r="C557" s="4" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D557" s="4" t="s">
         <v>284</v>
       </c>
       <c r="E557" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="558" spans="1:5" x14ac:dyDescent="0.25">
@@ -11023,13 +11035,13 @@
         <v>282</v>
       </c>
       <c r="C558" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D558" s="4" t="s">
         <v>284</v>
       </c>
       <c r="E558" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
@@ -11037,16 +11049,16 @@
         <v>257</v>
       </c>
       <c r="B559" s="4" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="C559" s="4" t="s">
-        <v>261</v>
+        <v>289</v>
       </c>
       <c r="D559" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E559" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.25">
@@ -11057,13 +11069,13 @@
         <v>290</v>
       </c>
       <c r="C560" s="4" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D560" s="4" t="s">
         <v>291</v>
       </c>
       <c r="E560" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
@@ -11071,16 +11083,16 @@
         <v>257</v>
       </c>
       <c r="B561" s="4" t="s">
-        <v>347</v>
+        <v>290</v>
       </c>
       <c r="C561" s="4" t="s">
-        <v>4</v>
+        <v>259</v>
       </c>
       <c r="D561" s="4" t="s">
-        <v>346</v>
+        <v>291</v>
       </c>
       <c r="E561" s="4" t="s">
-        <v>4</v>
+        <v>293</v>
       </c>
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.25">
@@ -11088,13 +11100,13 @@
         <v>257</v>
       </c>
       <c r="B562" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C562" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D562" s="4" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E562" s="4" t="s">
         <v>4</v>
@@ -11105,16 +11117,16 @@
         <v>257</v>
       </c>
       <c r="B563" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="C563" s="4">
-        <v>1</v>
+        <v>344</v>
+      </c>
+      <c r="C563" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="D563" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E563" s="6">
-        <v>0.22916666666666666</v>
+        <v>345</v>
+      </c>
+      <c r="E563" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
@@ -11122,16 +11134,16 @@
         <v>257</v>
       </c>
       <c r="B564" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C564" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D564" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E564" s="6">
-        <v>0.27083333333333331</v>
+        <v>0.22916666666666666</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
@@ -11139,16 +11151,16 @@
         <v>257</v>
       </c>
       <c r="B565" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C565" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D565" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E565" s="6">
-        <v>0.3125</v>
+        <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
@@ -11156,16 +11168,16 @@
         <v>257</v>
       </c>
       <c r="B566" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C566" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D566" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E566" s="6">
-        <v>0.35416666666666669</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
@@ -11173,16 +11185,16 @@
         <v>257</v>
       </c>
       <c r="B567" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C567" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D567" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E567" s="6">
-        <v>0.39583333333333331</v>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
@@ -11190,16 +11202,16 @@
         <v>257</v>
       </c>
       <c r="B568" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C568" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D568" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E568" s="6">
-        <v>0.4375</v>
+        <v>0.39583333333333331</v>
       </c>
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.25">
@@ -11207,16 +11219,16 @@
         <v>257</v>
       </c>
       <c r="B569" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C569" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D569" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E569" s="6">
-        <v>0.47916666666666669</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.25">
@@ -11224,16 +11236,16 @@
         <v>257</v>
       </c>
       <c r="B570" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C570" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D570" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E570" s="6">
-        <v>0.52083333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.25">
@@ -11241,16 +11253,16 @@
         <v>257</v>
       </c>
       <c r="B571" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C571" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D571" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E571" s="6">
-        <v>0.5625</v>
+        <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
@@ -11258,16 +11270,16 @@
         <v>257</v>
       </c>
       <c r="B572" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C572" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D572" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E572" s="6">
-        <v>0.60416666666666663</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.25">
@@ -11275,16 +11287,16 @@
         <v>257</v>
       </c>
       <c r="B573" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C573" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D573" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E573" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
@@ -11292,16 +11304,16 @@
         <v>257</v>
       </c>
       <c r="B574" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C574" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D574" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E574" s="6">
-        <v>0.6875</v>
+        <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.25">
@@ -11309,16 +11321,16 @@
         <v>257</v>
       </c>
       <c r="B575" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C575" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D575" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E575" s="6">
-        <v>0.72916666666666663</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.25">
@@ -11326,16 +11338,16 @@
         <v>257</v>
       </c>
       <c r="B576" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C576" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D576" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E576" s="6">
-        <v>0.77083333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
@@ -11343,16 +11355,16 @@
         <v>257</v>
       </c>
       <c r="B577" s="4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C577" s="4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D577" s="4" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E577" s="6">
-        <v>0.8125</v>
+        <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
@@ -11360,16 +11372,16 @@
         <v>257</v>
       </c>
       <c r="B578" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C578" s="4" t="s">
-        <v>353</v>
+        <v>346</v>
+      </c>
+      <c r="C578" s="4">
+        <v>15</v>
       </c>
       <c r="D578" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="E578" s="6" t="s">
-        <v>355</v>
+        <v>347</v>
+      </c>
+      <c r="E578" s="6">
+        <v>0.8125</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
@@ -11377,16 +11389,33 @@
         <v>257</v>
       </c>
       <c r="B579" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C579" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="D579" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E579" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="580" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A580" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B580" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C580" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="C579" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D579" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="E579" s="6" t="s">
-        <v>357</v>
+      <c r="D580" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E580" s="6" t="s">
+        <v>353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting in on BART
early days, data not yet final
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Dictionary" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -53,12 +53,204 @@
         </r>
       </text>
     </comment>
+    <comment ref="A582" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A583" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A584" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A585" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A586" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A587" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A588" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A589" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+BART interim variables listed as a check that we have everything.  Need to update and check all values when real data comes in.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="404">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1149,61 +1341,127 @@
     <t>BART Interim</t>
   </si>
   <si>
-    <t>DE_PLACE_TYPE_CODE</t>
-  </si>
-  <si>
-    <t>DE_ADDRESS_LAT</t>
-  </si>
-  <si>
-    <t>DE_ADDRESS_LONG</t>
-  </si>
-  <si>
-    <t>EGRESS_TO_1ST_RTE_CODE</t>
-  </si>
-  <si>
-    <t>ACCESS_TO_1ST_RTE_CODE</t>
-  </si>
-  <si>
-    <t>ADULTS_IN_HH_CODE</t>
-  </si>
-  <si>
     <t>FIRST_ENTERED_BART</t>
   </si>
   <si>
     <t>BART_EXIT_STATION</t>
   </si>
   <si>
-    <t>CLIPPER_REG_ADULT_CODE</t>
-  </si>
-  <si>
-    <t>HOME_ADDRESS_LAT</t>
-  </si>
-  <si>
-    <t>HOME_ADDRESS_LONG</t>
-  </si>
-  <si>
-    <t>OR_ADDRESS_LAT</t>
-  </si>
-  <si>
-    <t>OR_ADDRESS_LON</t>
-  </si>
-  <si>
-    <t>OR_PLACE_TYPE_CODE</t>
-  </si>
-  <si>
-    <t>HOW_PAID_FARE_CODE</t>
-  </si>
-  <si>
-    <t>SCHOOL_NAME_ADDRESS_LAT</t>
-  </si>
-  <si>
-    <t>SCHOOL_NAME_ADDRESS_LONG</t>
-  </si>
-  <si>
-    <t>DATE_STARTED</t>
-  </si>
-  <si>
-    <t>START_TIME_HHMM</t>
+    <t>BART</t>
+  </si>
+  <si>
+    <t>ACCESS_TO_1ST_RTE.Code.</t>
+  </si>
+  <si>
+    <t>DE_ADDRESS..LAT.</t>
+  </si>
+  <si>
+    <t>DE_ADDRESS..LONG.</t>
+  </si>
+  <si>
+    <t>DE_PLACE_TYPE.Code.</t>
+  </si>
+  <si>
+    <t>EGRESS_TO_1ST_RTE.Code.</t>
+  </si>
+  <si>
+    <t>ADULTS_IN_HH.Code.</t>
+  </si>
+  <si>
+    <t>ENGLISH_FLUENCY.Code.</t>
+  </si>
+  <si>
+    <t>CLIPPER_REG_ADULT.Code.</t>
+  </si>
+  <si>
+    <t>HH_INCOME.Code.</t>
+  </si>
+  <si>
+    <t>HISP_LATINO_SPANISH.Code.</t>
+  </si>
+  <si>
+    <t>HOME_ADDRESS..LAT.</t>
+  </si>
+  <si>
+    <t>HOME_ADDRESS..LONG.</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>OR_ADDRESS..LAT.</t>
+  </si>
+  <si>
+    <t>OR_ADDRESS..LONG.</t>
+  </si>
+  <si>
+    <t>OR_PLACE_TYPE.Code.</t>
+  </si>
+  <si>
+    <t>OTHER_LANG.Code.</t>
+  </si>
+  <si>
+    <t>HOW_PAID_FARE.Code.</t>
+  </si>
+  <si>
+    <t>PPL_IN_HH.Code.</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY..ASIAN.</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY..BLACK.</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY..AMALA.</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY..HAWPI.</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY..WHITE.</t>
+  </si>
+  <si>
+    <t>RESP_GENDER.Code.</t>
+  </si>
+  <si>
+    <t>SCHOOL_NAME_ADDRESS..LAT.</t>
+  </si>
+  <si>
+    <t>SCHOOL_NAME_ADDRESS..LONG.</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>TRIP_START_TIME2.Code.</t>
+  </si>
+  <si>
+    <t>FROM_TRNSFR_LIST1</t>
+  </si>
+  <si>
+    <t>FROM_TRNSFR_LIST2</t>
+  </si>
+  <si>
+    <t>FROM_TRNSFR_LIST3</t>
+  </si>
+  <si>
+    <t>TO_TRNSFR_LIST1</t>
+  </si>
+  <si>
+    <t>TO_TRNSFR_LIST2</t>
+  </si>
+  <si>
+    <t>TO_TRNSFR_LIST3</t>
+  </si>
+  <si>
+    <t>WORKP_NAME_ADDRESS..LAT.</t>
+  </si>
+  <si>
+    <t>WORKP_NAME_ADDRESS..LONG.</t>
+  </si>
+  <si>
+    <t>YEAR_BORN..Year.</t>
   </si>
 </sst>
 </file>
@@ -1262,7 +1520,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1272,6 +1530,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,7 +1556,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1313,6 +1577,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1661,8 +1928,8 @@
   <dimension ref="A1:E890"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A567" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A581" sqref="A581"/>
+      <pane ySplit="1" topLeftCell="A560" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A884" sqref="A884:E890"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11536,10 +11803,10 @@
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A581" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B581" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C581" s="1">
         <v>1</v>
@@ -11553,10 +11820,10 @@
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A582" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B582" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C582" s="1">
         <v>2</v>
@@ -11570,10 +11837,10 @@
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A583" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B583" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C583" s="1">
         <v>3</v>
@@ -11587,10 +11854,10 @@
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A584" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B584" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C584" s="1">
         <v>4</v>
@@ -11604,10 +11871,10 @@
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A585" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B585" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C585" s="1">
         <v>5</v>
@@ -11621,10 +11888,10 @@
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A586" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B586" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C586" s="1">
         <v>6</v>
@@ -11638,10 +11905,10 @@
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A587" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B587" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C587" s="1">
         <v>7</v>
@@ -11655,10 +11922,10 @@
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A588" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B588" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C588" s="1">
         <v>8</v>
@@ -11672,10 +11939,10 @@
     </row>
     <row r="589" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A589" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B589" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C589" s="1">
         <v>9</v>
@@ -11689,7 +11956,7 @@
     </row>
     <row r="590" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A590" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B590" s="1" t="s">
         <v>70</v>
@@ -11706,7 +11973,7 @@
     </row>
     <row r="591" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A591" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B591" s="1" t="s">
         <v>70</v>
@@ -11723,7 +11990,7 @@
     </row>
     <row r="592" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A592" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B592" s="1" t="s">
         <v>258</v>
@@ -11740,7 +12007,7 @@
     </row>
     <row r="593" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A593" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B593" s="1" t="s">
         <v>258</v>
@@ -11757,10 +12024,10 @@
     </row>
     <row r="594" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A594" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C594" s="1" t="s">
         <v>4</v>
@@ -11774,10 +12041,10 @@
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A595" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C595" s="1" t="s">
         <v>4</v>
@@ -11791,10 +12058,10 @@
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A596" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C596" s="1">
         <v>1</v>
@@ -11808,10 +12075,10 @@
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A597" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C597" s="1">
         <v>2</v>
@@ -11825,10 +12092,10 @@
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A598" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C598" s="1">
         <v>3</v>
@@ -11842,10 +12109,10 @@
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A599" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C599" s="1">
         <v>4</v>
@@ -11859,10 +12126,10 @@
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A600" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C600" s="1">
         <v>5</v>
@@ -11876,10 +12143,10 @@
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A601" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C601" s="1">
         <v>6</v>
@@ -11893,10 +12160,10 @@
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A602" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C602" s="1">
         <v>7</v>
@@ -11910,10 +12177,10 @@
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A603" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C603" s="1">
         <v>8</v>
@@ -11927,10 +12194,10 @@
     </row>
     <row r="604" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A604" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C604" s="1">
         <v>9</v>
@@ -11944,10 +12211,10 @@
     </row>
     <row r="605" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A605" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C605" s="1">
         <v>10</v>
@@ -11961,10 +12228,10 @@
     </row>
     <row r="606" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A606" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C606" s="1">
         <v>11</v>
@@ -11978,10 +12245,10 @@
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A607" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C607" s="1">
         <v>12</v>
@@ -11995,10 +12262,10 @@
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A608" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C608" s="1">
         <v>13</v>
@@ -12012,10 +12279,10 @@
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A609" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C609" s="1">
         <v>14</v>
@@ -12029,10 +12296,10 @@
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A610" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C610" s="1">
         <v>15</v>
@@ -12046,10 +12313,10 @@
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A611" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="C611" s="1">
         <v>16</v>
@@ -12063,10 +12330,10 @@
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A612" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C612" s="1">
         <v>1</v>
@@ -12080,10 +12347,10 @@
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A613" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C613" s="1">
         <v>2</v>
@@ -12097,10 +12364,10 @@
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A614" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C614" s="1">
         <v>3</v>
@@ -12114,10 +12381,10 @@
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A615" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C615" s="1">
         <v>4</v>
@@ -12131,10 +12398,10 @@
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A616" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C616" s="1">
         <v>5</v>
@@ -12148,10 +12415,10 @@
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A617" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C617" s="1">
         <v>6</v>
@@ -12165,10 +12432,10 @@
     </row>
     <row r="618" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A618" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C618" s="1">
         <v>7</v>
@@ -12182,10 +12449,10 @@
     </row>
     <row r="619" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A619" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C619" s="1">
         <v>8</v>
@@ -12199,10 +12466,10 @@
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A620" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C620" s="1">
         <v>9</v>
@@ -12216,7 +12483,7 @@
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A621" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B621" s="1" t="s">
         <v>55</v>
@@ -12233,7 +12500,7 @@
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A622" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B622" s="1" t="s">
         <v>55</v>
@@ -12250,10 +12517,10 @@
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A623" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B623" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C623" s="1">
         <v>0</v>
@@ -12267,10 +12534,10 @@
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A624" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C624" s="1">
         <v>1</v>
@@ -12284,10 +12551,10 @@
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A625" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C625" s="1">
         <v>2</v>
@@ -12301,10 +12568,10 @@
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A626" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C626" s="1">
         <v>3</v>
@@ -12318,10 +12585,10 @@
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A627" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C627" s="1">
         <v>4</v>
@@ -12335,10 +12602,10 @@
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A628" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C628" s="1">
         <v>5</v>
@@ -12352,10 +12619,10 @@
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A629" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C629" s="1">
         <v>6</v>
@@ -12369,10 +12636,10 @@
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A630" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>239</v>
+        <v>372</v>
       </c>
       <c r="C630" s="1">
         <v>1</v>
@@ -12386,10 +12653,10 @@
     </row>
     <row r="631" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A631" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>239</v>
+        <v>372</v>
       </c>
       <c r="C631" s="1">
         <v>2</v>
@@ -12403,10 +12670,10 @@
     </row>
     <row r="632" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A632" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>239</v>
+        <v>372</v>
       </c>
       <c r="C632" s="1">
         <v>3</v>
@@ -12420,10 +12687,10 @@
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A633" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>239</v>
+        <v>372</v>
       </c>
       <c r="C633" s="1">
         <v>4</v>
@@ -12437,10 +12704,10 @@
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A634" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B634" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C634" s="1" t="s">
         <v>4</v>
@@ -12453,45 +12720,45 @@
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A635" s="1" t="s">
+      <c r="A635" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B635" s="1" t="s">
+      <c r="B635" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C635" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D635" s="1" t="s">
+      <c r="C635" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D635" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E635" s="1" t="s">
+      <c r="E635" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="636" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A636" s="1" t="s">
+      <c r="A636" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B636" s="1" t="s">
+      <c r="B636" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C636" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D636" s="1" t="s">
+      <c r="C636" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D636" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E636" s="1" t="s">
+      <c r="E636" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A637" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B637" s="1" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C637" s="1" t="s">
         <v>4</v>
@@ -12504,45 +12771,45 @@
       </c>
     </row>
     <row r="638" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A638" s="1" t="s">
+      <c r="A638" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B638" s="1" t="s">
+      <c r="B638" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C638" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D638" s="1" t="s">
+      <c r="C638" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D638" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E638" s="1" t="s">
+      <c r="E638" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="639" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A639" s="1" t="s">
+      <c r="A639" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B639" s="1" t="s">
+      <c r="B639" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="C639" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D639" s="1" t="s">
+      <c r="C639" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D639" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E639" s="1" t="s">
+      <c r="E639" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="640" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A640" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C640" s="1">
         <v>1</v>
@@ -12556,10 +12823,10 @@
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A641" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C641" s="1">
         <v>2</v>
@@ -12573,10 +12840,10 @@
     </row>
     <row r="642" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A642" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C642" s="1">
         <v>3</v>
@@ -12590,10 +12857,10 @@
     </row>
     <row r="643" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A643" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C643" s="1">
         <v>4</v>
@@ -12607,10 +12874,10 @@
     </row>
     <row r="644" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A644" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C644" s="1">
         <v>5</v>
@@ -12624,7 +12891,7 @@
     </row>
     <row r="645" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A645" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B645" s="1" t="s">
         <v>274</v>
@@ -12641,7 +12908,7 @@
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A646" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B646" s="1" t="s">
         <v>274</v>
@@ -12658,10 +12925,10 @@
     </row>
     <row r="647" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A647" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C647" s="1">
         <v>1</v>
@@ -12675,10 +12942,10 @@
     </row>
     <row r="648" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A648" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C648" s="1">
         <v>2</v>
@@ -12692,10 +12959,10 @@
     </row>
     <row r="649" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A649" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B649" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C649" s="1">
         <v>3</v>
@@ -12709,10 +12976,10 @@
     </row>
     <row r="650" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A650" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C650" s="1">
         <v>4</v>
@@ -12726,10 +12993,10 @@
     </row>
     <row r="651" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A651" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C651" s="1">
         <v>5</v>
@@ -12743,10 +13010,10 @@
     </row>
     <row r="652" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A652" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C652" s="1">
         <v>6</v>
@@ -12760,10 +13027,10 @@
     </row>
     <row r="653" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A653" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C653" s="1">
         <v>7</v>
@@ -12777,10 +13044,10 @@
     </row>
     <row r="654" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A654" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B654" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C654" s="1">
         <v>8</v>
@@ -12794,10 +13061,10 @@
     </row>
     <row r="655" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A655" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C655" s="1">
         <v>9</v>
@@ -12811,10 +13078,10 @@
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A656" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C656" s="1">
         <v>10</v>
@@ -12828,10 +13095,10 @@
     </row>
     <row r="657" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A657" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B657" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C657" s="1">
         <v>88</v>
@@ -12845,10 +13112,10 @@
     </row>
     <row r="658" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A658" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="C658" s="1">
         <v>99</v>
@@ -12862,10 +13129,10 @@
     </row>
     <row r="659" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A659" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>153</v>
+        <v>375</v>
       </c>
       <c r="C659" s="1" t="s">
         <v>155</v>
@@ -12879,10 +13146,10 @@
     </row>
     <row r="660" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A660" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>153</v>
+        <v>375</v>
       </c>
       <c r="C660" s="1" t="s">
         <v>154</v>
@@ -12896,10 +13163,10 @@
     </row>
     <row r="661" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A661" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C661" s="1" t="s">
         <v>4</v>
@@ -12913,10 +13180,10 @@
     </row>
     <row r="662" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A662" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C662" s="1" t="s">
         <v>4</v>
@@ -12930,10 +13197,10 @@
     </row>
     <row r="663" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A663" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>5</v>
+        <v>378</v>
       </c>
       <c r="C663" s="1" t="s">
         <v>4</v>
@@ -12947,7 +13214,7 @@
     </row>
     <row r="664" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A664" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B664" s="1" t="s">
         <v>171</v>
@@ -12964,7 +13231,7 @@
     </row>
     <row r="665" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A665" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B665" s="1" t="s">
         <v>171</v>
@@ -12981,10 +13248,10 @@
     </row>
     <row r="666" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A666" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="C666" s="1" t="s">
         <v>4</v>
@@ -12998,10 +13265,10 @@
     </row>
     <row r="667" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A667" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C667" s="1" t="s">
         <v>4</v>
@@ -13015,10 +13282,10 @@
     </row>
     <row r="668" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A668" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C668" s="1">
         <v>1</v>
@@ -13032,10 +13299,10 @@
     </row>
     <row r="669" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A669" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C669" s="1">
         <v>2</v>
@@ -13049,10 +13316,10 @@
     </row>
     <row r="670" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A670" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C670" s="1">
         <v>3</v>
@@ -13066,10 +13333,10 @@
     </row>
     <row r="671" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A671" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C671" s="1">
         <v>4</v>
@@ -13083,10 +13350,10 @@
     </row>
     <row r="672" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A672" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C672" s="1">
         <v>5</v>
@@ -13100,10 +13367,10 @@
     </row>
     <row r="673" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A673" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C673" s="1">
         <v>6</v>
@@ -13117,10 +13384,10 @@
     </row>
     <row r="674" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A674" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C674" s="1">
         <v>7</v>
@@ -13134,10 +13401,10 @@
     </row>
     <row r="675" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A675" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C675" s="1">
         <v>8</v>
@@ -13151,10 +13418,10 @@
     </row>
     <row r="676" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A676" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C676" s="1">
         <v>9</v>
@@ -13168,10 +13435,10 @@
     </row>
     <row r="677" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A677" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C677" s="1">
         <v>10</v>
@@ -13185,10 +13452,10 @@
     </row>
     <row r="678" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A678" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C678" s="1">
         <v>11</v>
@@ -13202,10 +13469,10 @@
     </row>
     <row r="679" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A679" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C679" s="1">
         <v>12</v>
@@ -13219,10 +13486,10 @@
     </row>
     <row r="680" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A680" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C680" s="1">
         <v>13</v>
@@ -13236,10 +13503,10 @@
     </row>
     <row r="681" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A681" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C681" s="1">
         <v>14</v>
@@ -13253,10 +13520,10 @@
     </row>
     <row r="682" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A682" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C682" s="1">
         <v>15</v>
@@ -13270,10 +13537,10 @@
     </row>
     <row r="683" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A683" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="C683" s="1">
         <v>16</v>
@@ -13287,10 +13554,10 @@
     </row>
     <row r="684" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A684" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C684" s="1">
         <v>3</v>
@@ -13304,10 +13571,10 @@
     </row>
     <row r="685" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A685" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C685" s="1">
         <v>7</v>
@@ -13321,10 +13588,10 @@
     </row>
     <row r="686" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A686" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C686" s="1">
         <v>11</v>
@@ -13338,10 +13605,10 @@
     </row>
     <row r="687" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A687" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C687" s="1">
         <v>13</v>
@@ -13355,10 +13622,10 @@
     </row>
     <row r="688" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A688" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C688" s="1">
         <v>17</v>
@@ -13372,10 +13639,10 @@
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A689" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C689" s="1">
         <v>18</v>
@@ -13389,10 +13656,10 @@
     </row>
     <row r="690" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A690" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C690" s="1">
         <v>20</v>
@@ -13406,10 +13673,10 @@
     </row>
     <row r="691" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A691" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C691" s="1">
         <v>30</v>
@@ -13423,10 +13690,10 @@
     </row>
     <row r="692" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A692" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C692" s="1">
         <v>33</v>
@@ -13440,10 +13707,10 @@
     </row>
     <row r="693" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A693" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C693" s="1">
         <v>34</v>
@@ -13457,10 +13724,10 @@
     </row>
     <row r="694" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A694" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C694" s="1">
         <v>35</v>
@@ -13474,10 +13741,10 @@
     </row>
     <row r="695" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A695" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C695" s="1">
         <v>37</v>
@@ -13491,10 +13758,10 @@
     </row>
     <row r="696" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A696" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C696" s="1">
         <v>45</v>
@@ -13508,10 +13775,10 @@
     </row>
     <row r="697" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A697" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C697" s="1">
         <v>51</v>
@@ -13525,10 +13792,10 @@
     </row>
     <row r="698" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A698" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C698" s="1">
         <v>56</v>
@@ -13542,10 +13809,10 @@
     </row>
     <row r="699" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A699" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B699" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C699" s="1">
         <v>58</v>
@@ -13559,10 +13826,10 @@
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A700" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B700" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C700" s="1">
         <v>61</v>
@@ -13576,10 +13843,10 @@
     </row>
     <row r="701" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A701" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B701" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C701" s="1">
         <v>63</v>
@@ -13593,10 +13860,10 @@
     </row>
     <row r="702" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A702" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C702" s="1">
         <v>80</v>
@@ -13610,10 +13877,10 @@
     </row>
     <row r="703" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A703" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C703" s="1">
         <v>84</v>
@@ -13627,10 +13894,10 @@
     </row>
     <row r="704" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A704" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C704" s="1">
         <v>86</v>
@@ -13644,10 +13911,10 @@
     </row>
     <row r="705" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A705" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C705" s="1">
         <v>95</v>
@@ -13661,10 +13928,10 @@
     </row>
     <row r="706" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A706" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C706" s="1">
         <v>102</v>
@@ -13678,10 +13945,10 @@
     </row>
     <row r="707" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A707" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B707" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C707" s="1">
         <v>104</v>
@@ -13695,10 +13962,10 @@
     </row>
     <row r="708" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A708" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C708" s="1">
         <v>111</v>
@@ -13712,10 +13979,10 @@
     </row>
     <row r="709" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A709" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B709" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C709" s="1">
         <v>129</v>
@@ -13729,10 +13996,10 @@
     </row>
     <row r="710" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A710" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C710" s="1">
         <v>135</v>
@@ -13746,10 +14013,10 @@
     </row>
     <row r="711" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A711" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C711" s="1">
         <v>138</v>
@@ -13763,10 +14030,10 @@
     </row>
     <row r="712" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A712" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B712" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C712" s="1">
         <v>142</v>
@@ -13780,10 +14047,10 @@
     </row>
     <row r="713" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A713" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C713" s="1">
         <v>143</v>
@@ -13797,10 +14064,10 @@
     </row>
     <row r="714" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A714" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C714" s="1">
         <v>144</v>
@@ -13814,10 +14081,10 @@
     </row>
     <row r="715" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A715" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C715" s="1">
         <v>146</v>
@@ -13831,10 +14098,10 @@
     </row>
     <row r="716" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A716" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C716" s="1">
         <v>148</v>
@@ -13848,10 +14115,10 @@
     </row>
     <row r="717" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A717" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B717" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C717" s="1">
         <v>150</v>
@@ -13865,10 +14132,10 @@
     </row>
     <row r="718" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A718" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C718" s="1">
         <v>151</v>
@@ -13882,10 +14149,10 @@
     </row>
     <row r="719" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A719" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C719" s="1">
         <v>152</v>
@@ -13899,10 +14166,10 @@
     </row>
     <row r="720" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A720" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C720" s="1">
         <v>154</v>
@@ -13916,10 +14183,10 @@
     </row>
     <row r="721" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A721" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C721" s="1">
         <v>156</v>
@@ -13933,10 +14200,10 @@
     </row>
     <row r="722" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A722" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C722" s="1">
         <v>159</v>
@@ -13950,10 +14217,10 @@
     </row>
     <row r="723" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A723" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C723" s="1">
         <v>161</v>
@@ -13967,10 +14234,10 @@
     </row>
     <row r="724" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A724" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C724" s="1">
         <v>174</v>
@@ -13984,10 +14251,10 @@
     </row>
     <row r="725" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A725" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C725" s="1">
         <v>175</v>
@@ -14001,10 +14268,10 @@
     </row>
     <row r="726" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A726" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C726" s="1">
         <v>186</v>
@@ -14018,10 +14285,10 @@
     </row>
     <row r="727" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A727" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C727" s="1">
         <v>200</v>
@@ -14035,10 +14302,10 @@
     </row>
     <row r="728" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A728" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B728" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C728" s="1">
         <v>208</v>
@@ -14052,10 +14319,10 @@
     </row>
     <row r="729" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A729" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C729" s="1">
         <v>220</v>
@@ -14069,10 +14336,10 @@
     </row>
     <row r="730" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A730" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C730" s="1">
         <v>237</v>
@@ -14086,10 +14353,10 @@
     </row>
     <row r="731" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A731" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C731" s="1">
         <v>238</v>
@@ -14103,10 +14370,10 @@
     </row>
     <row r="732" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A732" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C732" s="1">
         <v>243</v>
@@ -14120,10 +14387,10 @@
     </row>
     <row r="733" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A733" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C733" s="1">
         <v>279</v>
@@ -14137,10 +14404,10 @@
     </row>
     <row r="734" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A734" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C734" s="1">
         <v>288</v>
@@ -14154,10 +14421,10 @@
     </row>
     <row r="735" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A735" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C735" s="1">
         <v>297</v>
@@ -14171,10 +14438,10 @@
     </row>
     <row r="736" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A736" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C736" s="1">
         <v>321</v>
@@ -14188,10 +14455,10 @@
     </row>
     <row r="737" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A737" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C737" s="1">
         <v>325</v>
@@ -14205,10 +14472,10 @@
     </row>
     <row r="738" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A738" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C738" s="1">
         <v>351</v>
@@ -14222,10 +14489,10 @@
     </row>
     <row r="739" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A739" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C739" s="1">
         <v>351</v>
@@ -14239,10 +14506,10 @@
     </row>
     <row r="740" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A740" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C740" s="1">
         <v>356</v>
@@ -14256,10 +14523,10 @@
     </row>
     <row r="741" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A741" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C741" s="1">
         <v>358</v>
@@ -14273,10 +14540,10 @@
     </row>
     <row r="742" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A742" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C742" s="1">
         <v>368</v>
@@ -14290,10 +14557,10 @@
     </row>
     <row r="743" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A743" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B743" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C743" s="1">
         <v>378</v>
@@ -14307,10 +14574,10 @@
     </row>
     <row r="744" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A744" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C744" s="1">
         <v>385</v>
@@ -14324,10 +14591,10 @@
     </row>
     <row r="745" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A745" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B745" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C745" s="1">
         <v>393</v>
@@ -14341,10 +14608,10 @@
     </row>
     <row r="746" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A746" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B746" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C746" s="1">
         <v>408</v>
@@ -14358,10 +14625,10 @@
     </row>
     <row r="747" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A747" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C747" s="1">
         <v>426</v>
@@ -14375,10 +14642,10 @@
     </row>
     <row r="748" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A748" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C748" s="1">
         <v>410</v>
@@ -14392,10 +14659,10 @@
     </row>
     <row r="749" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A749" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B749" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C749" s="1">
         <v>419</v>
@@ -14409,10 +14676,10 @@
     </row>
     <row r="750" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A750" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B750" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C750" s="1">
         <v>421</v>
@@ -14426,10 +14693,10 @@
     </row>
     <row r="751" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A751" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C751" s="1">
         <v>432</v>
@@ -14443,10 +14710,10 @@
     </row>
     <row r="752" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A752" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B752" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C752" s="1">
         <v>436</v>
@@ -14460,10 +14727,10 @@
     </row>
     <row r="753" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A753" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B753" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C753" s="1">
         <v>441</v>
@@ -14477,10 +14744,10 @@
     </row>
     <row r="754" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A754" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B754" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C754" s="1">
         <v>443</v>
@@ -14494,10 +14761,10 @@
     </row>
     <row r="755" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A755" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B755" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C755" s="1">
         <v>446</v>
@@ -14511,10 +14778,10 @@
     </row>
     <row r="756" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A756" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B756" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C756" s="1">
         <v>448</v>
@@ -14528,10 +14795,10 @@
     </row>
     <row r="757" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A757" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B757" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C757" s="1">
         <v>452</v>
@@ -14545,10 +14812,10 @@
     </row>
     <row r="758" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A758" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B758" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C758" s="1">
         <v>456</v>
@@ -14562,10 +14829,10 @@
     </row>
     <row r="759" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A759" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B759" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C759" s="1">
         <v>465</v>
@@ -14579,10 +14846,10 @@
     </row>
     <row r="760" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A760" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B760" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C760" s="1">
         <v>488</v>
@@ -14596,10 +14863,10 @@
     </row>
     <row r="761" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A761" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B761" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C761" s="1">
         <v>489</v>
@@ -14613,10 +14880,10 @@
     </row>
     <row r="762" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A762" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B762" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C762" s="1">
         <v>490</v>
@@ -14630,10 +14897,10 @@
     </row>
     <row r="763" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A763" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B763" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C763" s="1">
         <v>491</v>
@@ -14647,10 +14914,10 @@
     </row>
     <row r="764" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A764" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B764" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C764" s="1">
         <v>493</v>
@@ -14664,10 +14931,10 @@
     </row>
     <row r="765" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A765" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B765" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C765" s="1">
         <v>498</v>
@@ -14681,10 +14948,10 @@
     </row>
     <row r="766" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A766" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B766" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C766" s="1">
         <v>499</v>
@@ -14698,10 +14965,10 @@
     </row>
     <row r="767" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A767" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B767" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C767" s="1">
         <v>501</v>
@@ -14715,10 +14982,10 @@
     </row>
     <row r="768" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A768" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C768" s="1">
         <v>502</v>
@@ -14732,10 +14999,10 @@
     </row>
     <row r="769" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A769" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B769" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C769" s="1">
         <v>503</v>
@@ -14749,10 +15016,10 @@
     </row>
     <row r="770" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A770" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B770" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C770" s="1">
         <v>504</v>
@@ -14766,10 +15033,10 @@
     </row>
     <row r="771" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A771" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B771" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C771" s="1">
         <v>600</v>
@@ -14783,10 +15050,10 @@
     </row>
     <row r="772" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A772" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B772" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C772" s="1">
         <v>601</v>
@@ -14800,10 +15067,10 @@
     </row>
     <row r="773" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A773" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B773" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C773" s="1">
         <v>602</v>
@@ -14817,10 +15084,10 @@
     </row>
     <row r="774" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A774" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B774" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C774" s="1">
         <v>603</v>
@@ -14834,10 +15101,10 @@
     </row>
     <row r="775" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A775" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B775" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C775" s="1">
         <v>604</v>
@@ -14851,10 +15118,10 @@
     </row>
     <row r="776" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A776" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B776" s="1" t="s">
-        <v>175</v>
+        <v>382</v>
       </c>
       <c r="C776" s="1">
         <v>605</v>
@@ -14868,10 +15135,10 @@
     </row>
     <row r="777" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A777" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B777" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C777" s="1">
         <v>1</v>
@@ -14885,10 +15152,10 @@
     </row>
     <row r="778" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A778" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C778" s="1">
         <v>2</v>
@@ -14902,10 +15169,10 @@
     </row>
     <row r="779" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A779" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B779" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C779" s="1">
         <v>3</v>
@@ -14919,10 +15186,10 @@
     </row>
     <row r="780" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A780" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B780" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C780" s="1">
         <v>4</v>
@@ -14936,10 +15203,10 @@
     </row>
     <row r="781" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A781" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B781" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C781" s="1">
         <v>5</v>
@@ -14953,10 +15220,10 @@
     </row>
     <row r="782" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A782" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B782" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C782" s="1">
         <v>6</v>
@@ -14970,10 +15237,10 @@
     </row>
     <row r="783" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A783" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B783" s="1" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="C783" s="1">
         <v>7</v>
@@ -14987,10 +15254,10 @@
     </row>
     <row r="784" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A784" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B784" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C784" s="1" t="s">
         <v>27</v>
@@ -15004,10 +15271,10 @@
     </row>
     <row r="785" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A785" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C785" s="1" t="s">
         <v>36</v>
@@ -15021,10 +15288,10 @@
     </row>
     <row r="786" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A786" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B786" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C786" s="1" t="s">
         <v>28</v>
@@ -15038,10 +15305,10 @@
     </row>
     <row r="787" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A787" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B787" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C787" s="1" t="s">
         <v>29</v>
@@ -15055,10 +15322,10 @@
     </row>
     <row r="788" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A788" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B788" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C788" s="1" t="s">
         <v>30</v>
@@ -15072,10 +15339,10 @@
     </row>
     <row r="789" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A789" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B789" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C789" s="1" t="s">
         <v>31</v>
@@ -15089,10 +15356,10 @@
     </row>
     <row r="790" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A790" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B790" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C790" s="1" t="s">
         <v>32</v>
@@ -15106,10 +15373,10 @@
     </row>
     <row r="791" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A791" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C791" s="1" t="s">
         <v>33</v>
@@ -15123,10 +15390,10 @@
     </row>
     <row r="792" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A792" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C792" s="1" t="s">
         <v>34</v>
@@ -15140,10 +15407,10 @@
     </row>
     <row r="793" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A793" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>26</v>
+        <v>384</v>
       </c>
       <c r="C793" s="1" t="s">
         <v>35</v>
@@ -15157,10 +15424,10 @@
     </row>
     <row r="794" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A794" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B794" s="1" t="s">
-        <v>159</v>
+        <v>387</v>
       </c>
       <c r="C794" s="1" t="s">
         <v>57</v>
@@ -15174,10 +15441,10 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>159</v>
+        <v>387</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>56</v>
@@ -15191,10 +15458,10 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>161</v>
+        <v>385</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>57</v>
@@ -15208,10 +15475,10 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>161</v>
+        <v>385</v>
       </c>
       <c r="C797" s="1" t="s">
         <v>56</v>
@@ -15225,10 +15492,10 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>163</v>
+        <v>386</v>
       </c>
       <c r="C798" s="1" t="s">
         <v>57</v>
@@ -15242,10 +15509,10 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>163</v>
+        <v>386</v>
       </c>
       <c r="C799" s="1" t="s">
         <v>56</v>
@@ -15259,10 +15526,10 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>165</v>
+        <v>388</v>
       </c>
       <c r="C800" s="1" t="s">
         <v>57</v>
@@ -15276,10 +15543,10 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>165</v>
+        <v>388</v>
       </c>
       <c r="C801" s="1" t="s">
         <v>56</v>
@@ -15293,7 +15560,7 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B802" s="1" t="s">
         <v>169</v>
@@ -15310,10 +15577,10 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>167</v>
+        <v>389</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>57</v>
@@ -15327,10 +15594,10 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>167</v>
+        <v>389</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>56</v>
@@ -15344,10 +15611,10 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>235</v>
+        <v>390</v>
       </c>
       <c r="C805" s="1">
         <v>1</v>
@@ -15361,10 +15628,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>235</v>
+        <v>390</v>
       </c>
       <c r="C806" s="1">
         <v>2</v>
@@ -15378,10 +15645,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -15395,10 +15662,10 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="C808" s="1" t="s">
         <v>4</v>
@@ -15412,7 +15679,7 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B809" s="1" t="s">
         <v>59</v>
@@ -15429,7 +15696,7 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B810" s="1" t="s">
         <v>59</v>
@@ -15445,28 +15712,28 @@
       </c>
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A811" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B811" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C811" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D811" s="1" t="s">
+      <c r="A811" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B811" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="C811" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D811" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="E811" s="1" t="s">
+      <c r="E811" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="C812" s="1" t="s">
         <v>4</v>
@@ -15479,28 +15746,28 @@
       </c>
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A813" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="B813" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C813" s="1">
+      <c r="A813" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="B813" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="C813" s="8">
         <v>1</v>
       </c>
-      <c r="D813" s="1" t="s">
+      <c r="D813" s="8" t="s">
         <v>251</v>
       </c>
-      <c r="E813" s="1">
+      <c r="E813" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C814" s="1">
         <v>2</v>
@@ -15514,10 +15781,10 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C815" s="1">
         <v>3</v>
@@ -15531,10 +15798,10 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C816" s="1">
         <v>4</v>
@@ -15548,10 +15815,10 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C817" s="1">
         <v>5</v>
@@ -15565,10 +15832,10 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C818" s="1">
         <v>6</v>
@@ -15582,10 +15849,10 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C819" s="1">
         <v>7</v>
@@ -15599,10 +15866,10 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C820" s="1">
         <v>8</v>
@@ -15616,10 +15883,10 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C821" s="1">
         <v>9</v>
@@ -15633,10 +15900,10 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C822" s="1">
         <v>10</v>
@@ -15650,10 +15917,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C823" s="1">
         <v>11</v>
@@ -15667,10 +15934,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C824" s="1">
         <v>12</v>
@@ -15684,10 +15951,10 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C825" s="1">
         <v>13</v>
@@ -15701,10 +15968,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C826" s="1">
         <v>14</v>
@@ -15718,10 +15985,10 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C827" s="1">
         <v>15</v>
@@ -15735,10 +16002,10 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C828" s="1">
         <v>16</v>
@@ -15752,10 +16019,10 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C829" s="1">
         <v>17</v>
@@ -15769,10 +16036,10 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C830" s="1">
         <v>18</v>
@@ -15786,10 +16053,10 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C831" s="1">
         <v>19</v>
@@ -15803,10 +16070,10 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>250</v>
+        <v>394</v>
       </c>
       <c r="C832" s="1">
         <v>20</v>
@@ -15819,351 +16086,351 @@
       </c>
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A833" s="1" t="s">
+      <c r="A833" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B833" s="1" t="s">
+      <c r="B833" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C833" s="1">
+      <c r="C833" s="8">
         <v>1</v>
       </c>
-      <c r="D833" s="1" t="s">
+      <c r="D833" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E833" s="1">
+      <c r="E833" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A834" s="1" t="s">
+      <c r="A834" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B834" s="1" t="s">
+      <c r="B834" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C834" s="1">
+      <c r="C834" s="8">
         <v>2</v>
       </c>
-      <c r="D834" s="1" t="s">
+      <c r="D834" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E834" s="1">
+      <c r="E834" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A835" s="1" t="s">
+      <c r="A835" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B835" s="1" t="s">
+      <c r="B835" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C835" s="1">
+      <c r="C835" s="8">
         <v>3</v>
       </c>
-      <c r="D835" s="1" t="s">
+      <c r="D835" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E835" s="1">
+      <c r="E835" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A836" s="1" t="s">
+      <c r="A836" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B836" s="1" t="s">
+      <c r="B836" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C836" s="1">
-        <v>4</v>
-      </c>
-      <c r="D836" s="1" t="s">
+      <c r="C836" s="8">
+        <v>4</v>
+      </c>
+      <c r="D836" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E836" s="1">
+      <c r="E836" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A837" s="1" t="s">
+      <c r="A837" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B837" s="1" t="s">
+      <c r="B837" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C837" s="1">
+      <c r="C837" s="8">
         <v>5</v>
       </c>
-      <c r="D837" s="1" t="s">
+      <c r="D837" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E837" s="1">
+      <c r="E837" s="8">
         <v>8</v>
       </c>
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A838" s="1" t="s">
+      <c r="A838" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B838" s="1" t="s">
+      <c r="B838" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C838" s="1">
+      <c r="C838" s="8">
         <v>6</v>
       </c>
-      <c r="D838" s="1" t="s">
+      <c r="D838" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E838" s="1">
+      <c r="E838" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A839" s="1" t="s">
+      <c r="A839" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B839" s="1" t="s">
+      <c r="B839" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C839" s="1">
+      <c r="C839" s="8">
         <v>7</v>
       </c>
-      <c r="D839" s="1" t="s">
+      <c r="D839" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E839" s="1">
+      <c r="E839" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A840" s="1" t="s">
+      <c r="A840" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B840" s="1" t="s">
+      <c r="B840" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C840" s="1">
+      <c r="C840" s="8">
         <v>8</v>
       </c>
-      <c r="D840" s="1" t="s">
+      <c r="D840" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E840" s="1">
+      <c r="E840" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A841" s="1" t="s">
+      <c r="A841" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B841" s="1" t="s">
+      <c r="B841" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C841" s="1">
+      <c r="C841" s="8">
         <v>9</v>
       </c>
-      <c r="D841" s="1" t="s">
+      <c r="D841" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E841" s="1">
+      <c r="E841" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A842" s="1" t="s">
+      <c r="A842" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B842" s="1" t="s">
+      <c r="B842" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C842" s="1">
+      <c r="C842" s="8">
         <v>10</v>
       </c>
-      <c r="D842" s="1" t="s">
+      <c r="D842" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E842" s="1">
+      <c r="E842" s="8">
         <v>13</v>
       </c>
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A843" s="1" t="s">
+      <c r="A843" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B843" s="1" t="s">
+      <c r="B843" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C843" s="1">
+      <c r="C843" s="8">
         <v>11</v>
       </c>
-      <c r="D843" s="1" t="s">
+      <c r="D843" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E843" s="1">
+      <c r="E843" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A844" s="1" t="s">
+      <c r="A844" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B844" s="1" t="s">
+      <c r="B844" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C844" s="1">
+      <c r="C844" s="8">
         <v>12</v>
       </c>
-      <c r="D844" s="1" t="s">
+      <c r="D844" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E844" s="1">
+      <c r="E844" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A845" s="1" t="s">
+      <c r="A845" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B845" s="1" t="s">
+      <c r="B845" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C845" s="1">
+      <c r="C845" s="8">
         <v>13</v>
       </c>
-      <c r="D845" s="1" t="s">
+      <c r="D845" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E845" s="1">
+      <c r="E845" s="8">
         <v>16</v>
       </c>
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A846" s="1" t="s">
+      <c r="A846" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B846" s="1" t="s">
+      <c r="B846" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C846" s="1">
+      <c r="C846" s="8">
         <v>14</v>
       </c>
-      <c r="D846" s="1" t="s">
+      <c r="D846" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E846" s="1">
+      <c r="E846" s="8">
         <v>17</v>
       </c>
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A847" s="1" t="s">
+      <c r="A847" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B847" s="1" t="s">
+      <c r="B847" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C847" s="1">
+      <c r="C847" s="8">
         <v>15</v>
       </c>
-      <c r="D847" s="1" t="s">
+      <c r="D847" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E847" s="1">
+      <c r="E847" s="8">
         <v>18</v>
       </c>
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A848" s="1" t="s">
+      <c r="A848" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B848" s="1" t="s">
+      <c r="B848" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C848" s="1">
+      <c r="C848" s="8">
         <v>16</v>
       </c>
-      <c r="D848" s="1" t="s">
+      <c r="D848" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E848" s="1">
+      <c r="E848" s="8">
         <v>19</v>
       </c>
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A849" s="1" t="s">
+      <c r="A849" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B849" s="1" t="s">
+      <c r="B849" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C849" s="1">
+      <c r="C849" s="8">
         <v>17</v>
       </c>
-      <c r="D849" s="1" t="s">
+      <c r="D849" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E849" s="1">
+      <c r="E849" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A850" s="1" t="s">
+      <c r="A850" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B850" s="1" t="s">
+      <c r="B850" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C850" s="1">
+      <c r="C850" s="8">
         <v>18</v>
       </c>
-      <c r="D850" s="1" t="s">
+      <c r="D850" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E850" s="1">
+      <c r="E850" s="8">
         <v>21</v>
       </c>
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A851" s="1" t="s">
+      <c r="A851" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B851" s="1" t="s">
+      <c r="B851" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C851" s="1">
+      <c r="C851" s="8">
         <v>19</v>
       </c>
-      <c r="D851" s="1" t="s">
+      <c r="D851" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E851" s="1">
+      <c r="E851" s="8">
         <v>22</v>
       </c>
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A852" s="1" t="s">
+      <c r="A852" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B852" s="1" t="s">
+      <c r="B852" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="C852" s="1">
+      <c r="C852" s="8">
         <v>20</v>
       </c>
-      <c r="D852" s="1" t="s">
+      <c r="D852" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="E852" s="1">
+      <c r="E852" s="8">
         <v>23</v>
       </c>
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>116</v>
+        <v>395</v>
       </c>
       <c r="C853" s="1" t="s">
         <v>4</v>
@@ -16177,10 +16444,10 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>118</v>
+        <v>396</v>
       </c>
       <c r="C854" s="1" t="s">
         <v>4</v>
@@ -16194,10 +16461,10 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>120</v>
+        <v>397</v>
       </c>
       <c r="C855" s="1" t="s">
         <v>4</v>
@@ -16211,10 +16478,10 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B856" s="1" t="s">
-        <v>122</v>
+        <v>398</v>
       </c>
       <c r="C856" s="1" t="s">
         <v>4</v>
@@ -16228,10 +16495,10 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B857" s="1" t="s">
-        <v>124</v>
+        <v>399</v>
       </c>
       <c r="C857" s="1" t="s">
         <v>4</v>
@@ -16245,10 +16512,10 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>125</v>
+        <v>400</v>
       </c>
       <c r="C858" s="1" t="s">
         <v>4</v>
@@ -16261,144 +16528,144 @@
       </c>
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A859" s="1" t="s">
+      <c r="A859" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B859" s="1" t="s">
+      <c r="B859" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C859" s="1">
+      <c r="C859" s="8">
         <v>0</v>
       </c>
-      <c r="D859" s="1" t="s">
+      <c r="D859" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E859" s="1">
+      <c r="E859" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A860" s="1" t="s">
+      <c r="A860" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B860" s="1" t="s">
+      <c r="B860" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C860" s="1">
+      <c r="C860" s="8">
         <v>1</v>
       </c>
-      <c r="D860" s="1" t="s">
+      <c r="D860" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E860" s="1">
+      <c r="E860" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A861" s="1" t="s">
+      <c r="A861" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B861" s="1" t="s">
+      <c r="B861" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C861" s="1">
+      <c r="C861" s="8">
         <v>2</v>
       </c>
-      <c r="D861" s="1" t="s">
+      <c r="D861" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E861" s="1">
+      <c r="E861" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A862" s="1" t="s">
+      <c r="A862" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B862" s="1" t="s">
+      <c r="B862" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C862" s="1">
+      <c r="C862" s="8">
         <v>3</v>
       </c>
-      <c r="D862" s="1" t="s">
+      <c r="D862" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="E862" s="1">
+      <c r="E862" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A863" s="1" t="s">
+      <c r="A863" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B863" s="1" t="s">
+      <c r="B863" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C863" s="1">
+      <c r="C863" s="8">
         <v>0</v>
       </c>
-      <c r="D863" s="1" t="s">
+      <c r="D863" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E863" s="1">
+      <c r="E863" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A864" s="1" t="s">
+      <c r="A864" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B864" s="1" t="s">
+      <c r="B864" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C864" s="1">
+      <c r="C864" s="8">
         <v>1</v>
       </c>
-      <c r="D864" s="1" t="s">
+      <c r="D864" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E864" s="1">
+      <c r="E864" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A865" s="1" t="s">
+      <c r="A865" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B865" s="1" t="s">
+      <c r="B865" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C865" s="1">
+      <c r="C865" s="8">
         <v>2</v>
       </c>
-      <c r="D865" s="1" t="s">
+      <c r="D865" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E865" s="1">
+      <c r="E865" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A866" s="1" t="s">
+      <c r="A866" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B866" s="1" t="s">
+      <c r="B866" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C866" s="1">
+      <c r="C866" s="8">
         <v>3</v>
       </c>
-      <c r="D866" s="1" t="s">
+      <c r="D866" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E866" s="1">
+      <c r="E866" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B867" s="1" t="s">
         <v>8</v>
@@ -16415,7 +16682,7 @@
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B868" s="1" t="s">
         <v>8</v>
@@ -16432,7 +16699,7 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B869" s="1" t="s">
         <v>8</v>
@@ -16449,7 +16716,7 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B870" s="1" t="s">
         <v>8</v>
@@ -16466,7 +16733,7 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B871" s="1" t="s">
         <v>8</v>
@@ -16483,7 +16750,7 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B872" s="1" t="s">
         <v>77</v>
@@ -16500,7 +16767,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>77</v>
@@ -16517,10 +16784,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>80</v>
+        <v>401</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>4</v>
@@ -16534,10 +16801,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>84</v>
+        <v>402</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>4</v>
@@ -16551,10 +16818,10 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>6</v>
+        <v>403</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
@@ -16567,240 +16834,240 @@
       </c>
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A877" s="1" t="s">
+      <c r="A877" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B877" s="1" t="s">
+      <c r="B877" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C877" s="1" t="s">
+      <c r="C877" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="D877" s="1" t="s">
+      <c r="D877" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="E877" s="1" t="s">
+      <c r="E877" s="8" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A878" s="1" t="s">
+      <c r="A878" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B878" s="1" t="s">
+      <c r="B878" s="8" t="s">
         <v>354</v>
       </c>
-      <c r="C878" s="1" t="s">
+      <c r="C878" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="D878" s="1" t="s">
+      <c r="D878" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="E878" s="1" t="s">
+      <c r="E878" s="8" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A879" s="1" t="s">
+      <c r="A879" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B879" s="1" t="s">
+      <c r="B879" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C879" s="1" t="s">
+      <c r="C879" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="D879" s="1" t="s">
+      <c r="D879" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="E879" s="1" t="s">
+      <c r="E879" s="8" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A880" s="1" t="s">
+      <c r="A880" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B880" s="1" t="s">
+      <c r="B880" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C880" s="1" t="s">
+      <c r="C880" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="D880" s="1" t="s">
+      <c r="D880" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="E880" s="1" t="s">
+      <c r="E880" s="8" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A881" s="1" t="s">
+      <c r="A881" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B881" s="1" t="s">
+      <c r="B881" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C881" s="1" t="s">
+      <c r="C881" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="D881" s="1" t="s">
+      <c r="D881" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="E881" s="1" t="s">
+      <c r="E881" s="8" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A882" s="1" t="s">
+      <c r="A882" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B882" s="1" t="s">
+      <c r="B882" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C882" s="1" t="s">
+      <c r="C882" s="8" t="s">
         <v>358</v>
       </c>
-      <c r="D882" s="1" t="s">
+      <c r="D882" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="E882" s="1" t="s">
+      <c r="E882" s="8" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A883" s="1" t="s">
+      <c r="A883" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B883" s="1" t="s">
+      <c r="B883" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C883" s="1" t="s">
+      <c r="C883" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="D883" s="1" t="s">
+      <c r="D883" s="8" t="s">
         <v>291</v>
       </c>
-      <c r="E883" s="1" t="s">
+      <c r="E883" s="8" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A884" s="1" t="s">
+      <c r="A884" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B884" s="1" t="s">
+      <c r="B884" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C884" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D884" s="1" t="s">
+      <c r="C884" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D884" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E884" s="1" t="s">
+      <c r="E884" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A885" s="1" t="s">
+      <c r="A885" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B885" s="1" t="s">
+      <c r="B885" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="C885" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D885" s="1" t="s">
+      <c r="C885" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D885" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E885" s="1" t="s">
+      <c r="E885" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A886" s="1" t="s">
+      <c r="A886" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B886" s="1" t="s">
+      <c r="B886" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="C886" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D886" s="1" t="s">
+      <c r="C886" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D886" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="E886" s="1" t="s">
+      <c r="E886" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A887" s="1" t="s">
+      <c r="A887" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B887" s="1" t="s">
+      <c r="B887" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="C887" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D887" s="1" t="s">
+      <c r="C887" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D887" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E887" s="1" t="s">
+      <c r="E887" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A888" s="1" t="s">
+      <c r="A888" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B888" s="1" t="s">
+      <c r="B888" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="C888" s="1" t="s">
+      <c r="C888" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="D888" s="1" t="s">
+      <c r="D888" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="E888" s="1" t="s">
+      <c r="E888" s="8" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A889" s="1" t="s">
+      <c r="A889" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B889" s="1" t="s">
+      <c r="B889" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="C889" s="1" t="s">
+      <c r="C889" s="8" t="s">
         <v>352</v>
       </c>
-      <c r="D889" s="1" t="s">
+      <c r="D889" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="E889" s="1" t="s">
+      <c r="E889" s="8" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A890" s="1" t="s">
+      <c r="A890" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="B890" s="1" t="s">
+      <c r="B890" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="C890" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D890" s="1" t="s">
+      <c r="C890" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D890" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="E890" s="1" t="s">
+      <c r="E890" s="8" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lil' progress on BART debugging
wait for real data to finish
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3621" uniqueCount="405">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1350,9 +1350,6 @@
     <t>BART</t>
   </si>
   <si>
-    <t>ACCESS_TO_1ST_RTE.Code.</t>
-  </si>
-  <si>
     <t>DE_ADDRESS..LAT.</t>
   </si>
   <si>
@@ -1362,9 +1359,6 @@
     <t>DE_PLACE_TYPE.Code.</t>
   </si>
   <si>
-    <t>EGRESS_TO_1ST_RTE.Code.</t>
-  </si>
-  <si>
     <t>ADULTS_IN_HH.Code.</t>
   </si>
   <si>
@@ -1386,9 +1380,6 @@
     <t>HOME_ADDRESS..LONG.</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>OR_ADDRESS..LAT.</t>
   </si>
   <si>
@@ -1462,6 +1453,18 @@
   </si>
   <si>
     <t>YEAR_BORN..Year.</t>
+  </si>
+  <si>
+    <t>TRIP_END_TIME2.Code.</t>
+  </si>
+  <si>
+    <t>RACE_OR_ETHNICITY..Other.</t>
+  </si>
+  <si>
+    <t>OR_TRANSPORT.Code.</t>
+  </si>
+  <si>
+    <t>DE_TRANSPORT.Code.</t>
   </si>
 </sst>
 </file>
@@ -1928,8 +1931,8 @@
   <dimension ref="A1:E890"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A560" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A884" sqref="A884:E890"/>
+      <pane ySplit="1" topLeftCell="A862" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A878" sqref="A878"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11806,7 +11809,7 @@
         <v>365</v>
       </c>
       <c r="B581" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C581" s="1">
         <v>1</v>
@@ -11823,7 +11826,7 @@
         <v>365</v>
       </c>
       <c r="B582" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C582" s="1">
         <v>2</v>
@@ -11840,7 +11843,7 @@
         <v>365</v>
       </c>
       <c r="B583" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C583" s="1">
         <v>3</v>
@@ -11857,7 +11860,7 @@
         <v>365</v>
       </c>
       <c r="B584" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C584" s="1">
         <v>4</v>
@@ -11874,7 +11877,7 @@
         <v>365</v>
       </c>
       <c r="B585" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C585" s="1">
         <v>5</v>
@@ -11891,7 +11894,7 @@
         <v>365</v>
       </c>
       <c r="B586" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C586" s="1">
         <v>6</v>
@@ -11908,7 +11911,7 @@
         <v>365</v>
       </c>
       <c r="B587" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C587" s="1">
         <v>7</v>
@@ -11925,7 +11928,7 @@
         <v>365</v>
       </c>
       <c r="B588" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C588" s="1">
         <v>8</v>
@@ -11942,7 +11945,7 @@
         <v>365</v>
       </c>
       <c r="B589" s="7" t="s">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="C589" s="1">
         <v>9</v>
@@ -12027,7 +12030,7 @@
         <v>365</v>
       </c>
       <c r="B594" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C594" s="1" t="s">
         <v>4</v>
@@ -12044,7 +12047,7 @@
         <v>365</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C595" s="1" t="s">
         <v>4</v>
@@ -12061,7 +12064,7 @@
         <v>365</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C596" s="1">
         <v>1</v>
@@ -12078,7 +12081,7 @@
         <v>365</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C597" s="1">
         <v>2</v>
@@ -12095,7 +12098,7 @@
         <v>365</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C598" s="1">
         <v>3</v>
@@ -12112,7 +12115,7 @@
         <v>365</v>
       </c>
       <c r="B599" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C599" s="1">
         <v>4</v>
@@ -12129,7 +12132,7 @@
         <v>365</v>
       </c>
       <c r="B600" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C600" s="1">
         <v>5</v>
@@ -12146,7 +12149,7 @@
         <v>365</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C601" s="1">
         <v>6</v>
@@ -12163,7 +12166,7 @@
         <v>365</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C602" s="1">
         <v>7</v>
@@ -12180,7 +12183,7 @@
         <v>365</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C603" s="1">
         <v>8</v>
@@ -12197,7 +12200,7 @@
         <v>365</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C604" s="1">
         <v>9</v>
@@ -12214,7 +12217,7 @@
         <v>365</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C605" s="1">
         <v>10</v>
@@ -12231,7 +12234,7 @@
         <v>365</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C606" s="1">
         <v>11</v>
@@ -12248,7 +12251,7 @@
         <v>365</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C607" s="1">
         <v>12</v>
@@ -12265,7 +12268,7 @@
         <v>365</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C608" s="1">
         <v>13</v>
@@ -12282,7 +12285,7 @@
         <v>365</v>
       </c>
       <c r="B609" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C609" s="1">
         <v>14</v>
@@ -12299,7 +12302,7 @@
         <v>365</v>
       </c>
       <c r="B610" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C610" s="1">
         <v>15</v>
@@ -12316,7 +12319,7 @@
         <v>365</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C611" s="1">
         <v>16</v>
@@ -12333,7 +12336,7 @@
         <v>365</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C612" s="1">
         <v>1</v>
@@ -12350,7 +12353,7 @@
         <v>365</v>
       </c>
       <c r="B613" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C613" s="1">
         <v>2</v>
@@ -12367,7 +12370,7 @@
         <v>365</v>
       </c>
       <c r="B614" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C614" s="1">
         <v>3</v>
@@ -12384,7 +12387,7 @@
         <v>365</v>
       </c>
       <c r="B615" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C615" s="1">
         <v>4</v>
@@ -12401,7 +12404,7 @@
         <v>365</v>
       </c>
       <c r="B616" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C616" s="1">
         <v>5</v>
@@ -12418,7 +12421,7 @@
         <v>365</v>
       </c>
       <c r="B617" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C617" s="1">
         <v>6</v>
@@ -12435,7 +12438,7 @@
         <v>365</v>
       </c>
       <c r="B618" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C618" s="1">
         <v>7</v>
@@ -12452,7 +12455,7 @@
         <v>365</v>
       </c>
       <c r="B619" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C619" s="1">
         <v>8</v>
@@ -12469,7 +12472,7 @@
         <v>365</v>
       </c>
       <c r="B620" s="1" t="s">
-        <v>370</v>
+        <v>404</v>
       </c>
       <c r="C620" s="1">
         <v>9</v>
@@ -12520,7 +12523,7 @@
         <v>365</v>
       </c>
       <c r="B623" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C623" s="1">
         <v>0</v>
@@ -12537,7 +12540,7 @@
         <v>365</v>
       </c>
       <c r="B624" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C624" s="1">
         <v>1</v>
@@ -12554,7 +12557,7 @@
         <v>365</v>
       </c>
       <c r="B625" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C625" s="1">
         <v>2</v>
@@ -12571,7 +12574,7 @@
         <v>365</v>
       </c>
       <c r="B626" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C626" s="1">
         <v>3</v>
@@ -12588,7 +12591,7 @@
         <v>365</v>
       </c>
       <c r="B627" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C627" s="1">
         <v>4</v>
@@ -12605,7 +12608,7 @@
         <v>365</v>
       </c>
       <c r="B628" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C628" s="1">
         <v>5</v>
@@ -12622,7 +12625,7 @@
         <v>365</v>
       </c>
       <c r="B629" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C629" s="1">
         <v>6</v>
@@ -12639,7 +12642,7 @@
         <v>365</v>
       </c>
       <c r="B630" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C630" s="1">
         <v>1</v>
@@ -12656,7 +12659,7 @@
         <v>365</v>
       </c>
       <c r="B631" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C631" s="1">
         <v>2</v>
@@ -12673,7 +12676,7 @@
         <v>365</v>
       </c>
       <c r="B632" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C632" s="1">
         <v>3</v>
@@ -12690,7 +12693,7 @@
         <v>365</v>
       </c>
       <c r="B633" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C633" s="1">
         <v>4</v>
@@ -12809,7 +12812,7 @@
         <v>365</v>
       </c>
       <c r="B640" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C640" s="1">
         <v>1</v>
@@ -12826,7 +12829,7 @@
         <v>365</v>
       </c>
       <c r="B641" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C641" s="1">
         <v>2</v>
@@ -12843,7 +12846,7 @@
         <v>365</v>
       </c>
       <c r="B642" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C642" s="1">
         <v>3</v>
@@ -12860,7 +12863,7 @@
         <v>365</v>
       </c>
       <c r="B643" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C643" s="1">
         <v>4</v>
@@ -12877,7 +12880,7 @@
         <v>365</v>
       </c>
       <c r="B644" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C644" s="1">
         <v>5</v>
@@ -12928,7 +12931,7 @@
         <v>365</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C647" s="1">
         <v>1</v>
@@ -12945,7 +12948,7 @@
         <v>365</v>
       </c>
       <c r="B648" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C648" s="1">
         <v>2</v>
@@ -12962,7 +12965,7 @@
         <v>365</v>
       </c>
       <c r="B649" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C649" s="1">
         <v>3</v>
@@ -12979,7 +12982,7 @@
         <v>365</v>
       </c>
       <c r="B650" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C650" s="1">
         <v>4</v>
@@ -12996,7 +12999,7 @@
         <v>365</v>
       </c>
       <c r="B651" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C651" s="1">
         <v>5</v>
@@ -13013,7 +13016,7 @@
         <v>365</v>
       </c>
       <c r="B652" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C652" s="1">
         <v>6</v>
@@ -13030,7 +13033,7 @@
         <v>365</v>
       </c>
       <c r="B653" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C653" s="1">
         <v>7</v>
@@ -13047,7 +13050,7 @@
         <v>365</v>
       </c>
       <c r="B654" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C654" s="1">
         <v>8</v>
@@ -13064,7 +13067,7 @@
         <v>365</v>
       </c>
       <c r="B655" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C655" s="1">
         <v>9</v>
@@ -13081,7 +13084,7 @@
         <v>365</v>
       </c>
       <c r="B656" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C656" s="1">
         <v>10</v>
@@ -13098,7 +13101,7 @@
         <v>365</v>
       </c>
       <c r="B657" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C657" s="1">
         <v>88</v>
@@ -13115,7 +13118,7 @@
         <v>365</v>
       </c>
       <c r="B658" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C658" s="1">
         <v>99</v>
@@ -13132,7 +13135,7 @@
         <v>365</v>
       </c>
       <c r="B659" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C659" s="1" t="s">
         <v>155</v>
@@ -13149,7 +13152,7 @@
         <v>365</v>
       </c>
       <c r="B660" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C660" s="1" t="s">
         <v>154</v>
@@ -13166,7 +13169,7 @@
         <v>365</v>
       </c>
       <c r="B661" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C661" s="1" t="s">
         <v>4</v>
@@ -13183,7 +13186,7 @@
         <v>365</v>
       </c>
       <c r="B662" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C662" s="1" t="s">
         <v>4</v>
@@ -13200,7 +13203,7 @@
         <v>365</v>
       </c>
       <c r="B663" s="1" t="s">
-        <v>378</v>
+        <v>5</v>
       </c>
       <c r="C663" s="1" t="s">
         <v>4</v>
@@ -13251,7 +13254,7 @@
         <v>365</v>
       </c>
       <c r="B666" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C666" s="1" t="s">
         <v>4</v>
@@ -13268,7 +13271,7 @@
         <v>365</v>
       </c>
       <c r="B667" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C667" s="1" t="s">
         <v>4</v>
@@ -13285,7 +13288,7 @@
         <v>365</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C668" s="1">
         <v>1</v>
@@ -13302,7 +13305,7 @@
         <v>365</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C669" s="1">
         <v>2</v>
@@ -13319,7 +13322,7 @@
         <v>365</v>
       </c>
       <c r="B670" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C670" s="1">
         <v>3</v>
@@ -13336,7 +13339,7 @@
         <v>365</v>
       </c>
       <c r="B671" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C671" s="1">
         <v>4</v>
@@ -13353,7 +13356,7 @@
         <v>365</v>
       </c>
       <c r="B672" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C672" s="1">
         <v>5</v>
@@ -13370,7 +13373,7 @@
         <v>365</v>
       </c>
       <c r="B673" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C673" s="1">
         <v>6</v>
@@ -13387,7 +13390,7 @@
         <v>365</v>
       </c>
       <c r="B674" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C674" s="1">
         <v>7</v>
@@ -13404,7 +13407,7 @@
         <v>365</v>
       </c>
       <c r="B675" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C675" s="1">
         <v>8</v>
@@ -13421,7 +13424,7 @@
         <v>365</v>
       </c>
       <c r="B676" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C676" s="1">
         <v>9</v>
@@ -13438,7 +13441,7 @@
         <v>365</v>
       </c>
       <c r="B677" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C677" s="1">
         <v>10</v>
@@ -13455,7 +13458,7 @@
         <v>365</v>
       </c>
       <c r="B678" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C678" s="1">
         <v>11</v>
@@ -13472,7 +13475,7 @@
         <v>365</v>
       </c>
       <c r="B679" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C679" s="1">
         <v>12</v>
@@ -13489,7 +13492,7 @@
         <v>365</v>
       </c>
       <c r="B680" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C680" s="1">
         <v>13</v>
@@ -13506,7 +13509,7 @@
         <v>365</v>
       </c>
       <c r="B681" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C681" s="1">
         <v>14</v>
@@ -13523,7 +13526,7 @@
         <v>365</v>
       </c>
       <c r="B682" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C682" s="1">
         <v>15</v>
@@ -13540,7 +13543,7 @@
         <v>365</v>
       </c>
       <c r="B683" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C683" s="1">
         <v>16</v>
@@ -13557,7 +13560,7 @@
         <v>365</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C684" s="1">
         <v>3</v>
@@ -13574,7 +13577,7 @@
         <v>365</v>
       </c>
       <c r="B685" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C685" s="1">
         <v>7</v>
@@ -13591,7 +13594,7 @@
         <v>365</v>
       </c>
       <c r="B686" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C686" s="1">
         <v>11</v>
@@ -13608,7 +13611,7 @@
         <v>365</v>
       </c>
       <c r="B687" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C687" s="1">
         <v>13</v>
@@ -13625,7 +13628,7 @@
         <v>365</v>
       </c>
       <c r="B688" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C688" s="1">
         <v>17</v>
@@ -13642,7 +13645,7 @@
         <v>365</v>
       </c>
       <c r="B689" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C689" s="1">
         <v>18</v>
@@ -13659,7 +13662,7 @@
         <v>365</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C690" s="1">
         <v>20</v>
@@ -13676,7 +13679,7 @@
         <v>365</v>
       </c>
       <c r="B691" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C691" s="1">
         <v>30</v>
@@ -13693,7 +13696,7 @@
         <v>365</v>
       </c>
       <c r="B692" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C692" s="1">
         <v>33</v>
@@ -13710,7 +13713,7 @@
         <v>365</v>
       </c>
       <c r="B693" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C693" s="1">
         <v>34</v>
@@ -13727,7 +13730,7 @@
         <v>365</v>
       </c>
       <c r="B694" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C694" s="1">
         <v>35</v>
@@ -13744,7 +13747,7 @@
         <v>365</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C695" s="1">
         <v>37</v>
@@ -13761,7 +13764,7 @@
         <v>365</v>
       </c>
       <c r="B696" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C696" s="1">
         <v>45</v>
@@ -13778,7 +13781,7 @@
         <v>365</v>
       </c>
       <c r="B697" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C697" s="1">
         <v>51</v>
@@ -13795,7 +13798,7 @@
         <v>365</v>
       </c>
       <c r="B698" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C698" s="1">
         <v>56</v>
@@ -13812,7 +13815,7 @@
         <v>365</v>
       </c>
       <c r="B699" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C699" s="1">
         <v>58</v>
@@ -13829,7 +13832,7 @@
         <v>365</v>
       </c>
       <c r="B700" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C700" s="1">
         <v>61</v>
@@ -13846,7 +13849,7 @@
         <v>365</v>
       </c>
       <c r="B701" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C701" s="1">
         <v>63</v>
@@ -13863,7 +13866,7 @@
         <v>365</v>
       </c>
       <c r="B702" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C702" s="1">
         <v>80</v>
@@ -13880,7 +13883,7 @@
         <v>365</v>
       </c>
       <c r="B703" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C703" s="1">
         <v>84</v>
@@ -13897,7 +13900,7 @@
         <v>365</v>
       </c>
       <c r="B704" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C704" s="1">
         <v>86</v>
@@ -13914,7 +13917,7 @@
         <v>365</v>
       </c>
       <c r="B705" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C705" s="1">
         <v>95</v>
@@ -13931,7 +13934,7 @@
         <v>365</v>
       </c>
       <c r="B706" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C706" s="1">
         <v>102</v>
@@ -13948,7 +13951,7 @@
         <v>365</v>
       </c>
       <c r="B707" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C707" s="1">
         <v>104</v>
@@ -13965,7 +13968,7 @@
         <v>365</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C708" s="1">
         <v>111</v>
@@ -13982,7 +13985,7 @@
         <v>365</v>
       </c>
       <c r="B709" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C709" s="1">
         <v>129</v>
@@ -13999,7 +14002,7 @@
         <v>365</v>
       </c>
       <c r="B710" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C710" s="1">
         <v>135</v>
@@ -14016,7 +14019,7 @@
         <v>365</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C711" s="1">
         <v>138</v>
@@ -14033,7 +14036,7 @@
         <v>365</v>
       </c>
       <c r="B712" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C712" s="1">
         <v>142</v>
@@ -14050,7 +14053,7 @@
         <v>365</v>
       </c>
       <c r="B713" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C713" s="1">
         <v>143</v>
@@ -14067,7 +14070,7 @@
         <v>365</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C714" s="1">
         <v>144</v>
@@ -14084,7 +14087,7 @@
         <v>365</v>
       </c>
       <c r="B715" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C715" s="1">
         <v>146</v>
@@ -14101,7 +14104,7 @@
         <v>365</v>
       </c>
       <c r="B716" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C716" s="1">
         <v>148</v>
@@ -14118,7 +14121,7 @@
         <v>365</v>
       </c>
       <c r="B717" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C717" s="1">
         <v>150</v>
@@ -14135,7 +14138,7 @@
         <v>365</v>
       </c>
       <c r="B718" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C718" s="1">
         <v>151</v>
@@ -14152,7 +14155,7 @@
         <v>365</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C719" s="1">
         <v>152</v>
@@ -14169,7 +14172,7 @@
         <v>365</v>
       </c>
       <c r="B720" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C720" s="1">
         <v>154</v>
@@ -14186,7 +14189,7 @@
         <v>365</v>
       </c>
       <c r="B721" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C721" s="1">
         <v>156</v>
@@ -14203,7 +14206,7 @@
         <v>365</v>
       </c>
       <c r="B722" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C722" s="1">
         <v>159</v>
@@ -14220,7 +14223,7 @@
         <v>365</v>
       </c>
       <c r="B723" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C723" s="1">
         <v>161</v>
@@ -14237,7 +14240,7 @@
         <v>365</v>
       </c>
       <c r="B724" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C724" s="1">
         <v>174</v>
@@ -14254,7 +14257,7 @@
         <v>365</v>
       </c>
       <c r="B725" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C725" s="1">
         <v>175</v>
@@ -14271,7 +14274,7 @@
         <v>365</v>
       </c>
       <c r="B726" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C726" s="1">
         <v>186</v>
@@ -14288,7 +14291,7 @@
         <v>365</v>
       </c>
       <c r="B727" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C727" s="1">
         <v>200</v>
@@ -14305,7 +14308,7 @@
         <v>365</v>
       </c>
       <c r="B728" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C728" s="1">
         <v>208</v>
@@ -14322,7 +14325,7 @@
         <v>365</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C729" s="1">
         <v>220</v>
@@ -14339,7 +14342,7 @@
         <v>365</v>
       </c>
       <c r="B730" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C730" s="1">
         <v>237</v>
@@ -14356,7 +14359,7 @@
         <v>365</v>
       </c>
       <c r="B731" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C731" s="1">
         <v>238</v>
@@ -14373,7 +14376,7 @@
         <v>365</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C732" s="1">
         <v>243</v>
@@ -14390,7 +14393,7 @@
         <v>365</v>
       </c>
       <c r="B733" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C733" s="1">
         <v>279</v>
@@ -14407,7 +14410,7 @@
         <v>365</v>
       </c>
       <c r="B734" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C734" s="1">
         <v>288</v>
@@ -14424,7 +14427,7 @@
         <v>365</v>
       </c>
       <c r="B735" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C735" s="1">
         <v>297</v>
@@ -14441,7 +14444,7 @@
         <v>365</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C736" s="1">
         <v>321</v>
@@ -14458,7 +14461,7 @@
         <v>365</v>
       </c>
       <c r="B737" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C737" s="1">
         <v>325</v>
@@ -14475,7 +14478,7 @@
         <v>365</v>
       </c>
       <c r="B738" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C738" s="1">
         <v>351</v>
@@ -14492,7 +14495,7 @@
         <v>365</v>
       </c>
       <c r="B739" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C739" s="1">
         <v>351</v>
@@ -14509,7 +14512,7 @@
         <v>365</v>
       </c>
       <c r="B740" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C740" s="1">
         <v>356</v>
@@ -14526,7 +14529,7 @@
         <v>365</v>
       </c>
       <c r="B741" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C741" s="1">
         <v>358</v>
@@ -14543,7 +14546,7 @@
         <v>365</v>
       </c>
       <c r="B742" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C742" s="1">
         <v>368</v>
@@ -14560,7 +14563,7 @@
         <v>365</v>
       </c>
       <c r="B743" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C743" s="1">
         <v>378</v>
@@ -14577,7 +14580,7 @@
         <v>365</v>
       </c>
       <c r="B744" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C744" s="1">
         <v>385</v>
@@ -14594,7 +14597,7 @@
         <v>365</v>
       </c>
       <c r="B745" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C745" s="1">
         <v>393</v>
@@ -14611,7 +14614,7 @@
         <v>365</v>
       </c>
       <c r="B746" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C746" s="1">
         <v>408</v>
@@ -14628,7 +14631,7 @@
         <v>365</v>
       </c>
       <c r="B747" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C747" s="1">
         <v>426</v>
@@ -14645,7 +14648,7 @@
         <v>365</v>
       </c>
       <c r="B748" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C748" s="1">
         <v>410</v>
@@ -14662,7 +14665,7 @@
         <v>365</v>
       </c>
       <c r="B749" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C749" s="1">
         <v>419</v>
@@ -14679,7 +14682,7 @@
         <v>365</v>
       </c>
       <c r="B750" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C750" s="1">
         <v>421</v>
@@ -14696,7 +14699,7 @@
         <v>365</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C751" s="1">
         <v>432</v>
@@ -14713,7 +14716,7 @@
         <v>365</v>
       </c>
       <c r="B752" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C752" s="1">
         <v>436</v>
@@ -14730,7 +14733,7 @@
         <v>365</v>
       </c>
       <c r="B753" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C753" s="1">
         <v>441</v>
@@ -14747,7 +14750,7 @@
         <v>365</v>
       </c>
       <c r="B754" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C754" s="1">
         <v>443</v>
@@ -14764,7 +14767,7 @@
         <v>365</v>
       </c>
       <c r="B755" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C755" s="1">
         <v>446</v>
@@ -14781,7 +14784,7 @@
         <v>365</v>
       </c>
       <c r="B756" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C756" s="1">
         <v>448</v>
@@ -14798,7 +14801,7 @@
         <v>365</v>
       </c>
       <c r="B757" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C757" s="1">
         <v>452</v>
@@ -14815,7 +14818,7 @@
         <v>365</v>
       </c>
       <c r="B758" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C758" s="1">
         <v>456</v>
@@ -14832,7 +14835,7 @@
         <v>365</v>
       </c>
       <c r="B759" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C759" s="1">
         <v>465</v>
@@ -14849,7 +14852,7 @@
         <v>365</v>
       </c>
       <c r="B760" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C760" s="1">
         <v>488</v>
@@ -14866,7 +14869,7 @@
         <v>365</v>
       </c>
       <c r="B761" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C761" s="1">
         <v>489</v>
@@ -14883,7 +14886,7 @@
         <v>365</v>
       </c>
       <c r="B762" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C762" s="1">
         <v>490</v>
@@ -14900,7 +14903,7 @@
         <v>365</v>
       </c>
       <c r="B763" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C763" s="1">
         <v>491</v>
@@ -14917,7 +14920,7 @@
         <v>365</v>
       </c>
       <c r="B764" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C764" s="1">
         <v>493</v>
@@ -14934,7 +14937,7 @@
         <v>365</v>
       </c>
       <c r="B765" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C765" s="1">
         <v>498</v>
@@ -14951,7 +14954,7 @@
         <v>365</v>
       </c>
       <c r="B766" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C766" s="1">
         <v>499</v>
@@ -14968,7 +14971,7 @@
         <v>365</v>
       </c>
       <c r="B767" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C767" s="1">
         <v>501</v>
@@ -14985,7 +14988,7 @@
         <v>365</v>
       </c>
       <c r="B768" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C768" s="1">
         <v>502</v>
@@ -15002,7 +15005,7 @@
         <v>365</v>
       </c>
       <c r="B769" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C769" s="1">
         <v>503</v>
@@ -15019,7 +15022,7 @@
         <v>365</v>
       </c>
       <c r="B770" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C770" s="1">
         <v>504</v>
@@ -15036,7 +15039,7 @@
         <v>365</v>
       </c>
       <c r="B771" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C771" s="1">
         <v>600</v>
@@ -15053,7 +15056,7 @@
         <v>365</v>
       </c>
       <c r="B772" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C772" s="1">
         <v>601</v>
@@ -15070,7 +15073,7 @@
         <v>365</v>
       </c>
       <c r="B773" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C773" s="1">
         <v>602</v>
@@ -15087,7 +15090,7 @@
         <v>365</v>
       </c>
       <c r="B774" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C774" s="1">
         <v>603</v>
@@ -15104,7 +15107,7 @@
         <v>365</v>
       </c>
       <c r="B775" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C775" s="1">
         <v>604</v>
@@ -15121,7 +15124,7 @@
         <v>365</v>
       </c>
       <c r="B776" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C776" s="1">
         <v>605</v>
@@ -15138,7 +15141,7 @@
         <v>365</v>
       </c>
       <c r="B777" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C777" s="1">
         <v>1</v>
@@ -15155,7 +15158,7 @@
         <v>365</v>
       </c>
       <c r="B778" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C778" s="1">
         <v>2</v>
@@ -15172,7 +15175,7 @@
         <v>365</v>
       </c>
       <c r="B779" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C779" s="1">
         <v>3</v>
@@ -15189,7 +15192,7 @@
         <v>365</v>
       </c>
       <c r="B780" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C780" s="1">
         <v>4</v>
@@ -15206,7 +15209,7 @@
         <v>365</v>
       </c>
       <c r="B781" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C781" s="1">
         <v>5</v>
@@ -15223,7 +15226,7 @@
         <v>365</v>
       </c>
       <c r="B782" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C782" s="1">
         <v>6</v>
@@ -15240,7 +15243,7 @@
         <v>365</v>
       </c>
       <c r="B783" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C783" s="1">
         <v>7</v>
@@ -15257,7 +15260,7 @@
         <v>365</v>
       </c>
       <c r="B784" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C784" s="1" t="s">
         <v>27</v>
@@ -15274,7 +15277,7 @@
         <v>365</v>
       </c>
       <c r="B785" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C785" s="1" t="s">
         <v>36</v>
@@ -15291,7 +15294,7 @@
         <v>365</v>
       </c>
       <c r="B786" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C786" s="1" t="s">
         <v>28</v>
@@ -15308,7 +15311,7 @@
         <v>365</v>
       </c>
       <c r="B787" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C787" s="1" t="s">
         <v>29</v>
@@ -15325,7 +15328,7 @@
         <v>365</v>
       </c>
       <c r="B788" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C788" s="1" t="s">
         <v>30</v>
@@ -15342,7 +15345,7 @@
         <v>365</v>
       </c>
       <c r="B789" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C789" s="1" t="s">
         <v>31</v>
@@ -15359,7 +15362,7 @@
         <v>365</v>
       </c>
       <c r="B790" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C790" s="1" t="s">
         <v>32</v>
@@ -15376,7 +15379,7 @@
         <v>365</v>
       </c>
       <c r="B791" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C791" s="1" t="s">
         <v>33</v>
@@ -15393,7 +15396,7 @@
         <v>365</v>
       </c>
       <c r="B792" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C792" s="1" t="s">
         <v>34</v>
@@ -15410,7 +15413,7 @@
         <v>365</v>
       </c>
       <c r="B793" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C793" s="1" t="s">
         <v>35</v>
@@ -15427,7 +15430,7 @@
         <v>365</v>
       </c>
       <c r="B794" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C794" s="1" t="s">
         <v>57</v>
@@ -15444,7 +15447,7 @@
         <v>365</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>56</v>
@@ -15461,7 +15464,7 @@
         <v>365</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>57</v>
@@ -15478,7 +15481,7 @@
         <v>365</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C797" s="1" t="s">
         <v>56</v>
@@ -15495,7 +15498,7 @@
         <v>365</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C798" s="1" t="s">
         <v>57</v>
@@ -15512,7 +15515,7 @@
         <v>365</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C799" s="1" t="s">
         <v>56</v>
@@ -15529,7 +15532,7 @@
         <v>365</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C800" s="1" t="s">
         <v>57</v>
@@ -15546,7 +15549,7 @@
         <v>365</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C801" s="1" t="s">
         <v>56</v>
@@ -15563,7 +15566,7 @@
         <v>365</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>169</v>
+        <v>402</v>
       </c>
       <c r="C802" s="1" t="s">
         <v>4</v>
@@ -15580,7 +15583,7 @@
         <v>365</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>57</v>
@@ -15597,7 +15600,7 @@
         <v>365</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>56</v>
@@ -15614,7 +15617,7 @@
         <v>365</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C805" s="1">
         <v>1</v>
@@ -15631,7 +15634,7 @@
         <v>365</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C806" s="1">
         <v>2</v>
@@ -15648,7 +15651,7 @@
         <v>365</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -15665,7 +15668,7 @@
         <v>365</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C808" s="1" t="s">
         <v>4</v>
@@ -15716,7 +15719,7 @@
         <v>365</v>
       </c>
       <c r="B811" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C811" s="8" t="s">
         <v>4</v>
@@ -15733,7 +15736,7 @@
         <v>365</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C812" s="1" t="s">
         <v>4</v>
@@ -15746,19 +15749,19 @@
       </c>
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A813" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="B813" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="C813" s="8">
+      <c r="A813" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B813" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C813" s="5">
         <v>1</v>
       </c>
-      <c r="D813" s="8" t="s">
+      <c r="D813" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="E813" s="8">
+      <c r="E813" s="5">
         <v>4</v>
       </c>
     </row>
@@ -15767,7 +15770,7 @@
         <v>365</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C814" s="1">
         <v>2</v>
@@ -15784,7 +15787,7 @@
         <v>365</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C815" s="1">
         <v>3</v>
@@ -15801,7 +15804,7 @@
         <v>365</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C816" s="1">
         <v>4</v>
@@ -15818,7 +15821,7 @@
         <v>365</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C817" s="1">
         <v>5</v>
@@ -15835,7 +15838,7 @@
         <v>365</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C818" s="1">
         <v>6</v>
@@ -15852,7 +15855,7 @@
         <v>365</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C819" s="1">
         <v>7</v>
@@ -15869,7 +15872,7 @@
         <v>365</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C820" s="1">
         <v>8</v>
@@ -15886,7 +15889,7 @@
         <v>365</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C821" s="1">
         <v>9</v>
@@ -15903,7 +15906,7 @@
         <v>365</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C822" s="1">
         <v>10</v>
@@ -15920,7 +15923,7 @@
         <v>365</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C823" s="1">
         <v>11</v>
@@ -15937,7 +15940,7 @@
         <v>365</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C824" s="1">
         <v>12</v>
@@ -15954,7 +15957,7 @@
         <v>365</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C825" s="1">
         <v>13</v>
@@ -15971,7 +15974,7 @@
         <v>365</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C826" s="1">
         <v>14</v>
@@ -15988,7 +15991,7 @@
         <v>365</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C827" s="1">
         <v>15</v>
@@ -16005,7 +16008,7 @@
         <v>365</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C828" s="1">
         <v>16</v>
@@ -16022,7 +16025,7 @@
         <v>365</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C829" s="1">
         <v>17</v>
@@ -16039,7 +16042,7 @@
         <v>365</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C830" s="1">
         <v>18</v>
@@ -16056,7 +16059,7 @@
         <v>365</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C831" s="1">
         <v>19</v>
@@ -16073,7 +16076,7 @@
         <v>365</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C832" s="1">
         <v>20</v>
@@ -16086,342 +16089,342 @@
       </c>
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A833" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B833" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C833" s="8">
+      <c r="A833" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B833" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C833" s="5">
         <v>1</v>
       </c>
-      <c r="D833" s="8" t="s">
+      <c r="D833" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E833" s="8">
+      <c r="E833" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A834" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B834" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C834" s="8">
+      <c r="A834" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B834" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C834" s="5">
         <v>2</v>
       </c>
-      <c r="D834" s="8" t="s">
+      <c r="D834" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E834" s="8">
+      <c r="E834" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A835" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B835" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C835" s="8">
+      <c r="A835" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B835" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C835" s="5">
         <v>3</v>
       </c>
-      <c r="D835" s="8" t="s">
+      <c r="D835" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E835" s="8">
+      <c r="E835" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A836" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B836" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C836" s="8">
-        <v>4</v>
-      </c>
-      <c r="D836" s="8" t="s">
+      <c r="A836" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B836" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C836" s="5">
+        <v>4</v>
+      </c>
+      <c r="D836" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E836" s="8">
+      <c r="E836" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A837" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B837" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C837" s="8">
+      <c r="A837" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B837" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C837" s="5">
         <v>5</v>
       </c>
-      <c r="D837" s="8" t="s">
+      <c r="D837" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E837" s="8">
+      <c r="E837" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A838" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B838" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C838" s="8">
+      <c r="A838" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B838" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C838" s="5">
         <v>6</v>
       </c>
-      <c r="D838" s="8" t="s">
+      <c r="D838" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E838" s="8">
+      <c r="E838" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A839" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B839" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C839" s="8">
+      <c r="A839" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B839" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C839" s="5">
         <v>7</v>
       </c>
-      <c r="D839" s="8" t="s">
+      <c r="D839" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E839" s="8">
+      <c r="E839" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A840" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B840" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C840" s="8">
+      <c r="A840" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B840" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C840" s="5">
         <v>8</v>
       </c>
-      <c r="D840" s="8" t="s">
+      <c r="D840" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E840" s="8">
+      <c r="E840" s="5">
         <v>11</v>
       </c>
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A841" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B841" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C841" s="8">
+      <c r="A841" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B841" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C841" s="5">
         <v>9</v>
       </c>
-      <c r="D841" s="8" t="s">
+      <c r="D841" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E841" s="8">
+      <c r="E841" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A842" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B842" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C842" s="8">
+      <c r="A842" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B842" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C842" s="5">
         <v>10</v>
       </c>
-      <c r="D842" s="8" t="s">
+      <c r="D842" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E842" s="8">
+      <c r="E842" s="5">
         <v>13</v>
       </c>
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A843" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B843" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C843" s="8">
+      <c r="A843" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B843" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C843" s="5">
         <v>11</v>
       </c>
-      <c r="D843" s="8" t="s">
+      <c r="D843" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E843" s="8">
+      <c r="E843" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A844" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B844" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C844" s="8">
+      <c r="A844" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B844" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C844" s="5">
         <v>12</v>
       </c>
-      <c r="D844" s="8" t="s">
+      <c r="D844" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E844" s="8">
+      <c r="E844" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A845" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B845" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C845" s="8">
+      <c r="A845" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B845" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C845" s="5">
         <v>13</v>
       </c>
-      <c r="D845" s="8" t="s">
+      <c r="D845" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E845" s="8">
+      <c r="E845" s="5">
         <v>16</v>
       </c>
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A846" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B846" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C846" s="8">
+      <c r="A846" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B846" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C846" s="5">
         <v>14</v>
       </c>
-      <c r="D846" s="8" t="s">
+      <c r="D846" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E846" s="8">
+      <c r="E846" s="5">
         <v>17</v>
       </c>
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A847" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B847" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C847" s="8">
+      <c r="A847" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B847" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C847" s="5">
         <v>15</v>
       </c>
-      <c r="D847" s="8" t="s">
+      <c r="D847" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E847" s="8">
+      <c r="E847" s="5">
         <v>18</v>
       </c>
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A848" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B848" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C848" s="8">
+      <c r="A848" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B848" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C848" s="5">
         <v>16</v>
       </c>
-      <c r="D848" s="8" t="s">
+      <c r="D848" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E848" s="8">
+      <c r="E848" s="5">
         <v>19</v>
       </c>
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A849" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B849" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C849" s="8">
+      <c r="A849" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B849" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C849" s="5">
         <v>17</v>
       </c>
-      <c r="D849" s="8" t="s">
+      <c r="D849" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E849" s="8">
+      <c r="E849" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A850" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B850" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C850" s="8">
+      <c r="A850" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B850" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C850" s="5">
         <v>18</v>
       </c>
-      <c r="D850" s="8" t="s">
+      <c r="D850" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E850" s="8">
+      <c r="E850" s="5">
         <v>21</v>
       </c>
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A851" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B851" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C851" s="8">
+      <c r="A851" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B851" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C851" s="5">
         <v>19</v>
       </c>
-      <c r="D851" s="8" t="s">
+      <c r="D851" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E851" s="8">
+      <c r="E851" s="5">
         <v>22</v>
       </c>
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A852" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="B852" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C852" s="8">
+      <c r="A852" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B852" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C852" s="5">
         <v>20</v>
       </c>
-      <c r="D852" s="8" t="s">
+      <c r="D852" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E852" s="8">
+      <c r="E852" s="5">
         <v>23</v>
       </c>
     </row>
@@ -16430,7 +16433,7 @@
         <v>365</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C853" s="1" t="s">
         <v>4</v>
@@ -16447,7 +16450,7 @@
         <v>365</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C854" s="1" t="s">
         <v>4</v>
@@ -16464,7 +16467,7 @@
         <v>365</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C855" s="1" t="s">
         <v>4</v>
@@ -16481,7 +16484,7 @@
         <v>365</v>
       </c>
       <c r="B856" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C856" s="1" t="s">
         <v>4</v>
@@ -16498,7 +16501,7 @@
         <v>365</v>
       </c>
       <c r="B857" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C857" s="1" t="s">
         <v>4</v>
@@ -16515,7 +16518,7 @@
         <v>365</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C858" s="1" t="s">
         <v>4</v>
@@ -16787,7 +16790,7 @@
         <v>365</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>4</v>
@@ -16804,7 +16807,7 @@
         <v>365</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>4</v>
@@ -16821,7 +16824,7 @@
         <v>365</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
bit of progress on variables
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3930" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4006" uniqueCount="463">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1537,6 +1537,108 @@
   </si>
   <si>
     <t>WORKED_BEFORE_TRIP</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>DESTIN_ADDRESS..LAT.</t>
+  </si>
+  <si>
+    <t>DESTIN_ADDRESS..LONG.</t>
+  </si>
+  <si>
+    <t>DESTIN_PLACE_TYPE.Code.</t>
+  </si>
+  <si>
+    <t>Walk all the way</t>
+  </si>
+  <si>
+    <t>Be picked up by Uber or similar service</t>
+  </si>
+  <si>
+    <t>Be picked up by someone (Not a service)</t>
+  </si>
+  <si>
+    <t>Get in a parked vehicle and drive alone</t>
+  </si>
+  <si>
+    <t>Get in a parked vehicle and drive with others</t>
+  </si>
+  <si>
+    <t>DESTIN_TRANSPORT</t>
+  </si>
+  <si>
+    <t>STATUS_EMPLOYMENT</t>
+  </si>
+  <si>
+    <t>COUNT_EMPLOYED_HH.Code.</t>
+  </si>
+  <si>
+    <t>ENGLISH_ABILITY.Code.</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Senior</t>
+  </si>
+  <si>
+    <t>Free Muni for People with Disabilities</t>
+  </si>
+  <si>
+    <t>Low Income (Lifeline) Pass</t>
+  </si>
+  <si>
+    <t>Disabled/Medicare Card Holder</t>
+  </si>
+  <si>
+    <t>Free Muni for Seniors</t>
+  </si>
+  <si>
+    <t>Youth</t>
+  </si>
+  <si>
+    <t>Free Muni for Youth</t>
+  </si>
+  <si>
+    <t>FARE_CATEGORY</t>
+  </si>
+  <si>
+    <t>Under $10,000</t>
+  </si>
+  <si>
+    <t>$10,000 to $24,999</t>
+  </si>
+  <si>
+    <t>$25,000 to $34,999</t>
+  </si>
+  <si>
+    <t>$35,000 - $49,999</t>
+  </si>
+  <si>
+    <t>$50,000 - $64,999</t>
+  </si>
+  <si>
+    <t>$65,000 - $74,999</t>
+  </si>
+  <si>
+    <t>$75,000 - $84,999</t>
+  </si>
+  <si>
+    <t>$85,000 - $99,999</t>
+  </si>
+  <si>
+    <t>$100,000 - $124,999</t>
+  </si>
+  <si>
+    <t>$125,000 - $149,999</t>
+  </si>
+  <si>
+    <t>$150,000 OR OVER</t>
+  </si>
+  <si>
+    <t>INCOME</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2010,18 +2112,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1006"/>
+  <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A796" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A806" sqref="A806"/>
+      <pane ySplit="1" topLeftCell="A862" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A868" sqref="A868"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.375" style="1" customWidth="1"/>
   </cols>
@@ -15712,9 +15814,11 @@
       </c>
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A806" s="10"/>
+      <c r="A806" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B806" s="1" t="s">
-        <v>369</v>
+        <v>430</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -15727,8 +15831,11 @@
       </c>
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A807" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B807" s="1" t="s">
-        <v>370</v>
+        <v>431</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -15741,8 +15848,11 @@
       </c>
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A808" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B808" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C808" s="1">
         <v>1</v>
@@ -15755,8 +15865,11 @@
       </c>
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A809" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B809" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C809" s="1">
         <v>2</v>
@@ -15769,8 +15882,11 @@
       </c>
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A810" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B810" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C810" s="1">
         <v>3</v>
@@ -15783,8 +15899,11 @@
       </c>
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A811" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B811" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C811" s="1">
         <v>4</v>
@@ -15797,8 +15916,11 @@
       </c>
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A812" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B812" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C812" s="1">
         <v>5</v>
@@ -15811,8 +15933,11 @@
       </c>
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A813" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B813" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C813" s="1">
         <v>6</v>
@@ -15825,8 +15950,11 @@
       </c>
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A814" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B814" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C814" s="1">
         <v>7</v>
@@ -15839,8 +15967,11 @@
       </c>
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A815" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B815" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C815" s="1">
         <v>8</v>
@@ -15853,8 +15984,11 @@
       </c>
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A816" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B816" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C816" s="1">
         <v>9</v>
@@ -15866,9 +16000,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="817" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A817" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B817" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C817" s="1">
         <v>10</v>
@@ -15880,9 +16017,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="818" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A818" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B818" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C818" s="1">
         <v>11</v>
@@ -15894,9 +16034,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="819" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A819" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B819" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C819" s="1">
         <v>12</v>
@@ -15908,9 +16051,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="820" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A820" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B820" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C820" s="1">
         <v>13</v>
@@ -15922,9 +16068,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="821" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A821" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B821" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C821" s="1">
         <v>14</v>
@@ -15936,9 +16085,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="822" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A822" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B822" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C822" s="1">
         <v>15</v>
@@ -15950,9 +16102,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="823" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A823" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B823" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C823" s="1">
         <v>16</v>
@@ -15964,9 +16119,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="824" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A824" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B824" s="1" t="s">
-        <v>371</v>
+        <v>432</v>
       </c>
       <c r="C824" s="1">
         <v>17</v>
@@ -15978,12 +16136,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="825" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A825" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B825" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C825" s="1">
-        <v>1</v>
+        <v>438</v>
+      </c>
+      <c r="C825" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>135</v>
@@ -15992,82 +16153,100 @@
         <v>130</v>
       </c>
     </row>
-    <row r="826" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A826" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B826" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C826" s="1">
-        <v>2</v>
+        <v>438</v>
+      </c>
+      <c r="C826" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D826" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E826" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="827" spans="2:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A827" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B827" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C827" s="1">
-        <v>3</v>
+        <v>438</v>
+      </c>
+      <c r="C827" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E827" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="828" spans="2:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A828" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B828" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C828" s="1">
-        <v>4</v>
+        <v>438</v>
+      </c>
+      <c r="C828" s="1" t="s">
+        <v>422</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E828" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="829" spans="2:5" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A829" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B829" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C829" s="1">
-        <v>5</v>
+        <v>438</v>
+      </c>
+      <c r="C829" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E829" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="830" spans="2:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A830" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B830" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C830" s="1">
-        <v>6</v>
+        <v>438</v>
+      </c>
+      <c r="C830" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E830" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="831" spans="2:5" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A831" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B831" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C831" s="1">
-        <v>7</v>
+        <v>438</v>
+      </c>
+      <c r="C831" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>135</v>
@@ -16076,37 +16255,46 @@
         <v>133</v>
       </c>
     </row>
-    <row r="832" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A832" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B832" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C832" s="1">
-        <v>8</v>
+        <v>438</v>
+      </c>
+      <c r="C832" s="1" t="s">
+        <v>436</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E832" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="833" spans="2:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A833" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B833" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C833" s="1">
-        <v>9</v>
+        <v>438</v>
+      </c>
+      <c r="C833" s="1" t="s">
+        <v>437</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E833" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="834" spans="2:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A834" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B834" s="1" t="s">
-        <v>55</v>
+        <v>439</v>
       </c>
       <c r="C834" s="1" t="s">
         <v>57</v>
@@ -16118,9 +16306,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="835" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A835" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B835" s="1" t="s">
-        <v>55</v>
+        <v>439</v>
       </c>
       <c r="C835" s="1" t="s">
         <v>56</v>
@@ -16132,9 +16323,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="836" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A836" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B836" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C836" s="1">
         <v>0</v>
@@ -16146,9 +16340,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="837" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A837" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B837" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C837" s="1">
         <v>1</v>
@@ -16160,9 +16357,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="838" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A838" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B838" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C838" s="1">
         <v>2</v>
@@ -16174,9 +16374,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="839" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A839" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B839" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C839" s="1">
         <v>3</v>
@@ -16188,9 +16391,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="840" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A840" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B840" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C840" s="1">
         <v>4</v>
@@ -16202,9 +16408,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="841" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A841" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B841" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C841" s="1">
         <v>5</v>
@@ -16216,9 +16425,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="842" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A842" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B842" s="1" t="s">
-        <v>373</v>
+        <v>440</v>
       </c>
       <c r="C842" s="1">
         <v>6</v>
@@ -16230,9 +16442,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="843" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A843" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B843" s="1" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="C843" s="1">
         <v>1</v>
@@ -16244,9 +16459,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="844" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A844" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B844" s="1" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="C844" s="1">
         <v>2</v>
@@ -16258,9 +16476,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="845" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A845" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B845" s="1" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="C845" s="1">
         <v>3</v>
@@ -16272,9 +16493,12 @@
         <v>242</v>
       </c>
     </row>
-    <row r="846" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A846" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B846" s="1" t="s">
-        <v>239</v>
+        <v>441</v>
       </c>
       <c r="C846" s="1">
         <v>4</v>
@@ -16286,54 +16510,66 @@
         <v>243</v>
       </c>
     </row>
-    <row r="847" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A847" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B847" s="1" t="s">
-        <v>374</v>
+        <v>450</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>4</v>
+        <v>442</v>
       </c>
       <c r="D847" s="1" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="E847" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="848" spans="2:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="848" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A848" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B848" s="1" t="s">
-        <v>375</v>
+        <v>450</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>4</v>
+        <v>446</v>
       </c>
       <c r="D848" s="1" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="E848" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="849" spans="2:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="849" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A849" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B849" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C849" s="1">
-        <v>1</v>
+        <v>450</v>
+      </c>
+      <c r="C849" s="1" t="s">
+        <v>444</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E849" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="850" spans="2:5" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="850" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A850" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B850" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C850" s="1">
-        <v>2</v>
+        <v>450</v>
+      </c>
+      <c r="C850" s="1" t="s">
+        <v>447</v>
       </c>
       <c r="D850" s="1" t="s">
         <v>148</v>
@@ -16342,12 +16578,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="851" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A851" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B851" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C851" s="1">
-        <v>3</v>
+        <v>450</v>
+      </c>
+      <c r="C851" s="1" t="s">
+        <v>449</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>148</v>
@@ -16356,410 +16595,469 @@
         <v>151</v>
       </c>
     </row>
-    <row r="852" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="852" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A852" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B852" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C852" s="1">
-        <v>4</v>
+        <v>450</v>
+      </c>
+      <c r="C852" s="1" t="s">
+        <v>445</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E852" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="853" spans="2:5" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="853" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A853" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B853" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C853" s="1">
-        <v>1</v>
+        <v>450</v>
+      </c>
+      <c r="C853" s="1" t="s">
+        <v>443</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E853" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="854" spans="2:5" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="854" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A854" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B854" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C854" s="1">
-        <v>2</v>
+        <v>450</v>
+      </c>
+      <c r="C854" s="1" t="s">
+        <v>448</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E854" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="855" spans="2:5" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="855" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A855" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B855" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C855" s="1">
-        <v>3</v>
+        <v>274</v>
+      </c>
+      <c r="C855" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D855" s="1" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="E855" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="856" spans="2:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="856" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A856" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B856" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C856" s="1">
-        <v>4</v>
+        <v>274</v>
+      </c>
+      <c r="C856" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D856" s="1" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="E856" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="857" spans="2:5" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="857" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A857" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B857" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C857" s="1">
-        <v>5</v>
+        <v>462</v>
+      </c>
+      <c r="C857" s="1" t="s">
+        <v>451</v>
       </c>
       <c r="D857" s="1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="E857" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="858" spans="2:5" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+      <c r="F857" s="1"/>
+    </row>
+    <row r="858" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A858" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B858" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C858" s="1">
-        <v>6</v>
+        <v>462</v>
+      </c>
+      <c r="C858" s="1" t="s">
+        <v>452</v>
       </c>
       <c r="D858" s="1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="E858" s="1" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="859" spans="2:5" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+      <c r="F858" s="1"/>
+    </row>
+    <row r="859" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A859" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B859" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C859" s="1">
-        <v>7</v>
+        <v>462</v>
+      </c>
+      <c r="C859" s="1" t="s">
+        <v>453</v>
       </c>
       <c r="D859" s="1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="E859" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="860" spans="2:5" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="F859" s="1"/>
+    </row>
+    <row r="860" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A860" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B860" s="1" t="s">
-        <v>274</v>
+        <v>462</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>57</v>
+        <v>454</v>
       </c>
       <c r="D860" s="1" t="s">
-        <v>67</v>
+        <v>225</v>
       </c>
       <c r="E860" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="861" spans="2:5" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="F860" s="1"/>
+    </row>
+    <row r="861" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A861" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B861" s="1" t="s">
-        <v>274</v>
+        <v>462</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>56</v>
+        <v>455</v>
       </c>
       <c r="D861" s="1" t="s">
-        <v>67</v>
+        <v>225</v>
       </c>
       <c r="E861" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="862" spans="2:5" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="F861" s="1"/>
+    </row>
+    <row r="862" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A862" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B862" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C862" s="1">
-        <v>1</v>
+        <v>462</v>
+      </c>
+      <c r="C862" s="1" t="s">
+        <v>456</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E862" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="863" spans="2:5" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="F862" s="1"/>
+    </row>
+    <row r="863" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A863" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B863" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C863" s="1">
-        <v>2</v>
+        <v>462</v>
+      </c>
+      <c r="C863" s="1" t="s">
+        <v>457</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E863" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="864" spans="2:5" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="F863" s="1"/>
+    </row>
+    <row r="864" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A864" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B864" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C864" s="1">
-        <v>3</v>
+        <v>462</v>
+      </c>
+      <c r="C864" s="1" t="s">
+        <v>458</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E864" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="865" spans="2:5" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="F864" s="1"/>
+    </row>
+    <row r="865" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A865" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B865" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C865" s="1">
-        <v>4</v>
+        <v>462</v>
+      </c>
+      <c r="C865" s="1" t="s">
+        <v>459</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E865" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="866" spans="2:5" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="F865" s="1"/>
+    </row>
+    <row r="866" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A866" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B866" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C866" s="1">
-        <v>5</v>
+        <v>462</v>
+      </c>
+      <c r="C866" s="1" t="s">
+        <v>460</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E866" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="867" spans="2:5" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="F866" s="1"/>
+    </row>
+    <row r="867" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A867" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B867" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C867" s="1">
-        <v>6</v>
-      </c>
-      <c r="D867" s="1" t="s">
-        <v>225</v>
+        <v>462</v>
+      </c>
+      <c r="C867" s="1" t="s">
+        <v>461</v>
       </c>
       <c r="E867" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="868" spans="2:5" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="868" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A868" s="10"/>
       <c r="B868" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C868" s="1">
-        <v>7</v>
+        <v>153</v>
+      </c>
+      <c r="C868" s="1" t="s">
+        <v>412</v>
       </c>
       <c r="D868" s="1" t="s">
-        <v>225</v>
+        <v>156</v>
       </c>
       <c r="E868" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="869" spans="2:5" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="869" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B869" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C869" s="1">
-        <v>8</v>
+        <v>153</v>
+      </c>
+      <c r="C869" s="1" t="s">
+        <v>413</v>
       </c>
       <c r="D869" s="1" t="s">
-        <v>225</v>
+        <v>156</v>
       </c>
       <c r="E869" s="1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="870" spans="2:5" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="870" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B870" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C870" s="1">
-        <v>9</v>
+        <v>376</v>
+      </c>
+      <c r="C870" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D870" s="1" t="s">
-        <v>225</v>
+        <v>82</v>
       </c>
       <c r="E870" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="871" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="871" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B871" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C871" s="1">
-        <v>10</v>
+        <v>377</v>
+      </c>
+      <c r="C871" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D871" s="1" t="s">
-        <v>225</v>
+        <v>83</v>
       </c>
       <c r="E871" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="872" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="872" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A872" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="B872" s="1" t="s">
-        <v>153</v>
+        <v>429</v>
       </c>
       <c r="C872" s="1" t="s">
-        <v>412</v>
+        <v>4</v>
       </c>
       <c r="D872" s="1" t="s">
-        <v>156</v>
+        <v>5</v>
       </c>
       <c r="E872" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="873" spans="2:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="873" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B873" s="1" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C873" s="1" t="s">
-        <v>413</v>
+        <v>57</v>
       </c>
       <c r="D873" s="1" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="E873" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="874" spans="2:5" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="874" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B874" s="1" t="s">
-        <v>376</v>
+        <v>171</v>
       </c>
       <c r="C874" s="1" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="D874" s="1" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
       <c r="E874" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="875" spans="2:5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="875" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B875" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D875" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E875" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="876" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B876" s="1" t="s">
-        <v>5</v>
+        <v>379</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D876" s="1" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="E876" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="877" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B877" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C877" s="1" t="s">
-        <v>57</v>
+        <v>380</v>
+      </c>
+      <c r="C877" s="1">
+        <v>1</v>
       </c>
       <c r="D877" s="1" t="s">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="E877" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="878" spans="2:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="878" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B878" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C878" s="1" t="s">
-        <v>56</v>
+        <v>380</v>
+      </c>
+      <c r="C878" s="1">
+        <v>2</v>
       </c>
       <c r="D878" s="1" t="s">
-        <v>173</v>
+        <v>40</v>
       </c>
       <c r="E878" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="879" spans="2:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="879" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B879" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C879" s="1" t="s">
-        <v>4</v>
+        <v>380</v>
+      </c>
+      <c r="C879" s="1">
+        <v>3</v>
       </c>
       <c r="D879" s="1" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="E879" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="880" spans="2:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="880" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B880" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C880" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C880" s="1">
         <v>4</v>
       </c>
       <c r="D880" s="1" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="E880" s="1" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
     <row r="881" spans="2:5" x14ac:dyDescent="0.25">
@@ -16767,13 +17065,13 @@
         <v>380</v>
       </c>
       <c r="C881" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E881" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="882" spans="2:5" x14ac:dyDescent="0.25">
@@ -16781,13 +17079,13 @@
         <v>380</v>
       </c>
       <c r="C882" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E882" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="883" spans="2:5" x14ac:dyDescent="0.25">
@@ -16795,13 +17093,13 @@
         <v>380</v>
       </c>
       <c r="C883" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E883" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="884" spans="2:5" x14ac:dyDescent="0.25">
@@ -16809,13 +17107,13 @@
         <v>380</v>
       </c>
       <c r="C884" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E884" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="885" spans="2:5" x14ac:dyDescent="0.25">
@@ -16823,13 +17121,13 @@
         <v>380</v>
       </c>
       <c r="C885" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E885" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="886" spans="2:5" x14ac:dyDescent="0.25">
@@ -16837,13 +17135,13 @@
         <v>380</v>
       </c>
       <c r="C886" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E886" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="887" spans="2:5" x14ac:dyDescent="0.25">
@@ -16851,7 +17149,7 @@
         <v>380</v>
       </c>
       <c r="C887" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
@@ -16865,13 +17163,13 @@
         <v>380</v>
       </c>
       <c r="C888" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E888" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="889" spans="2:5" x14ac:dyDescent="0.25">
@@ -16879,7 +17177,7 @@
         <v>380</v>
       </c>
       <c r="C889" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
@@ -16893,13 +17191,13 @@
         <v>380</v>
       </c>
       <c r="C890" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E890" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="891" spans="2:5" x14ac:dyDescent="0.25">
@@ -16907,13 +17205,13 @@
         <v>380</v>
       </c>
       <c r="C891" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D891" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E891" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="892" spans="2:5" x14ac:dyDescent="0.25">
@@ -16921,13 +17219,13 @@
         <v>380</v>
       </c>
       <c r="C892" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="893" spans="2:5" x14ac:dyDescent="0.25">
@@ -16935,83 +17233,83 @@
         <v>380</v>
       </c>
       <c r="C893" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="894" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B894" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C894" s="1">
-        <v>14</v>
+        <v>381</v>
+      </c>
+      <c r="C894" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D894" s="1" t="s">
-        <v>40</v>
+        <v>176</v>
       </c>
       <c r="E894" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
     </row>
     <row r="895" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B895" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C895" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D895" s="1" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="E895" s="1" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
     </row>
     <row r="896" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B896" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C896" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D896" s="1" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="E896" s="1" t="s">
-        <v>53</v>
+        <v>383</v>
       </c>
     </row>
     <row r="897" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B897" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C897" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D897" s="1" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="E897" s="1" t="s">
-        <v>49</v>
+        <v>340</v>
       </c>
     </row>
     <row r="898" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B898" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C898" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C898" s="1">
         <v>4</v>
       </c>
       <c r="D898" s="1" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="E898" s="1" t="s">
-        <v>4</v>
+        <v>340</v>
       </c>
     </row>
     <row r="899" spans="2:5" x14ac:dyDescent="0.25">
@@ -17019,69 +17317,69 @@
         <v>382</v>
       </c>
       <c r="C899" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E899" s="1" t="s">
-        <v>144</v>
+        <v>340</v>
       </c>
     </row>
     <row r="900" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B900" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C900" s="1">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="C900" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D900" s="1" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="E900" s="1" t="s">
-        <v>383</v>
+        <v>14</v>
       </c>
     </row>
     <row r="901" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B901" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C901" s="1">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="C901" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D901" s="1" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="E901" s="1" t="s">
-        <v>340</v>
+        <v>38</v>
       </c>
     </row>
     <row r="902" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B902" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C902" s="1">
-        <v>4</v>
+        <v>26</v>
+      </c>
+      <c r="C902" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="D902" s="1" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="E902" s="1" t="s">
-        <v>340</v>
+        <v>11</v>
       </c>
     </row>
     <row r="903" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B903" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C903" s="1">
-        <v>5</v>
+        <v>26</v>
+      </c>
+      <c r="C903" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D903" s="1" t="s">
-        <v>139</v>
+        <v>37</v>
       </c>
       <c r="E903" s="1" t="s">
-        <v>340</v>
+        <v>12</v>
       </c>
     </row>
     <row r="904" spans="2:5" x14ac:dyDescent="0.25">
@@ -17089,13 +17387,13 @@
         <v>26</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E904" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="905" spans="2:5" x14ac:dyDescent="0.25">
@@ -17103,13 +17401,13 @@
         <v>26</v>
       </c>
       <c r="C905" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D905" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E905" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="906" spans="2:5" x14ac:dyDescent="0.25">
@@ -17117,13 +17415,13 @@
         <v>26</v>
       </c>
       <c r="C906" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D906" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E906" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="907" spans="2:5" x14ac:dyDescent="0.25">
@@ -17131,13 +17429,13 @@
         <v>26</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E907" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="908" spans="2:5" x14ac:dyDescent="0.25">
@@ -17145,13 +17443,13 @@
         <v>26</v>
       </c>
       <c r="C908" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D908" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E908" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="909" spans="2:5" x14ac:dyDescent="0.25">
@@ -17159,80 +17457,80 @@
         <v>26</v>
       </c>
       <c r="C909" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D909" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E909" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="910" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B910" s="1" t="s">
-        <v>26</v>
+        <v>365</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="D910" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E910" s="1" t="s">
-        <v>18</v>
+        <v>160</v>
+      </c>
+      <c r="E910" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="911" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B911" s="1" t="s">
-        <v>26</v>
+        <v>365</v>
       </c>
       <c r="C911" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D911" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E911" s="1" t="s">
-        <v>21</v>
+        <v>160</v>
+      </c>
+      <c r="E911" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="912" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B912" s="1" t="s">
-        <v>26</v>
+        <v>363</v>
       </c>
       <c r="C912" s="1" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D912" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E912" s="1" t="s">
-        <v>22</v>
+        <v>162</v>
+      </c>
+      <c r="E912" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="913" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B913" s="1" t="s">
-        <v>26</v>
+        <v>363</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="D913" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E913" s="1" t="s">
-        <v>23</v>
+        <v>162</v>
+      </c>
+      <c r="E913" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="914" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B914" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D914" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E914" s="1">
         <v>0</v>
@@ -17240,13 +17538,13 @@
     </row>
     <row r="915" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B915" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D915" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E915" s="1">
         <v>1</v>
@@ -17254,13 +17552,13 @@
     </row>
     <row r="916" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B916" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C916" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D916" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E916" s="1">
         <v>0</v>
@@ -17268,13 +17566,13 @@
     </row>
     <row r="917" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B917" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D917" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E917" s="1">
         <v>1</v>
@@ -17282,139 +17580,139 @@
     </row>
     <row r="918" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B918" s="1" t="s">
-        <v>364</v>
+        <v>403</v>
       </c>
       <c r="C918" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D918" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E918" s="1">
-        <v>0</v>
+        <v>170</v>
+      </c>
+      <c r="E918" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="919" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B919" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D919" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E919" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="920" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B920" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C920" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D920" s="1" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E920" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="921" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B921" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C921" s="1" t="s">
-        <v>56</v>
+        <v>235</v>
+      </c>
+      <c r="C921" s="1">
+        <v>1</v>
       </c>
       <c r="D921" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E921" s="1">
-        <v>1</v>
+        <v>236</v>
+      </c>
+      <c r="E921" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="922" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B922" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C922" s="1" t="s">
-        <v>4</v>
+        <v>235</v>
+      </c>
+      <c r="C922" s="1">
+        <v>2</v>
       </c>
       <c r="D922" s="1" t="s">
-        <v>170</v>
+        <v>236</v>
       </c>
       <c r="E922" s="1" t="s">
-        <v>4</v>
+        <v>238</v>
       </c>
     </row>
     <row r="923" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B923" s="1" t="s">
-        <v>367</v>
+        <v>384</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D923" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E923" s="1">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="E923" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="924" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B924" s="1" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
       <c r="C924" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D924" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E924" s="1">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="E924" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="925" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B925" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C925" s="1">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="C925" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D925" s="1" t="s">
-        <v>236</v>
+        <v>60</v>
       </c>
       <c r="E925" s="1" t="s">
-        <v>237</v>
+        <v>61</v>
       </c>
     </row>
     <row r="926" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B926" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C926" s="1">
-        <v>2</v>
+        <v>59</v>
+      </c>
+      <c r="C926" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D926" s="1" t="s">
-        <v>236</v>
+        <v>60</v>
       </c>
       <c r="E926" s="1" t="s">
-        <v>238</v>
+        <v>138</v>
       </c>
     </row>
     <row r="927" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B927" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C927" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D927" s="1" t="s">
-        <v>87</v>
+        <v>255</v>
       </c>
       <c r="E927" s="1" t="s">
         <v>4</v>
@@ -17422,13 +17720,13 @@
     </row>
     <row r="928" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B928" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C928" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D928" s="1" t="s">
-        <v>89</v>
+        <v>347</v>
       </c>
       <c r="E928" s="1" t="s">
         <v>4</v>
@@ -17436,58 +17734,58 @@
     </row>
     <row r="929" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B929" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C929" s="1" t="s">
-        <v>57</v>
+        <v>388</v>
+      </c>
+      <c r="C929" s="1">
+        <v>1</v>
       </c>
       <c r="D929" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E929" s="1" t="s">
-        <v>61</v>
+        <v>251</v>
+      </c>
+      <c r="E929" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="930" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B930" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C930" s="1" t="s">
-        <v>56</v>
+        <v>388</v>
+      </c>
+      <c r="C930" s="1">
+        <v>2</v>
       </c>
       <c r="D930" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E930" s="1" t="s">
-        <v>138</v>
+        <v>251</v>
+      </c>
+      <c r="E930" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="931" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B931" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="C931" s="1" t="s">
-        <v>4</v>
+        <v>388</v>
+      </c>
+      <c r="C931" s="1">
+        <v>3</v>
       </c>
       <c r="D931" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E931" s="1" t="s">
-        <v>4</v>
+        <v>251</v>
+      </c>
+      <c r="E931" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="932" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B932" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C932" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C932" s="1">
         <v>4</v>
       </c>
       <c r="D932" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="E932" s="1" t="s">
-        <v>4</v>
+        <v>251</v>
+      </c>
+      <c r="E932" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="933" spans="2:5" x14ac:dyDescent="0.25">
@@ -17495,13 +17793,13 @@
         <v>388</v>
       </c>
       <c r="C933" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D933" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E933" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="934" spans="2:5" x14ac:dyDescent="0.25">
@@ -17509,13 +17807,13 @@
         <v>388</v>
       </c>
       <c r="C934" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D934" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E934" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="935" spans="2:5" x14ac:dyDescent="0.25">
@@ -17523,13 +17821,13 @@
         <v>388</v>
       </c>
       <c r="C935" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E935" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="936" spans="2:5" x14ac:dyDescent="0.25">
@@ -17537,13 +17835,13 @@
         <v>388</v>
       </c>
       <c r="C936" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E936" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="937" spans="2:5" x14ac:dyDescent="0.25">
@@ -17551,13 +17849,13 @@
         <v>388</v>
       </c>
       <c r="C937" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E937" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="938" spans="2:5" x14ac:dyDescent="0.25">
@@ -17565,13 +17863,13 @@
         <v>388</v>
       </c>
       <c r="C938" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E938" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="939" spans="2:5" x14ac:dyDescent="0.25">
@@ -17579,13 +17877,13 @@
         <v>388</v>
       </c>
       <c r="C939" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E939" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="940" spans="2:5" x14ac:dyDescent="0.25">
@@ -17593,13 +17891,13 @@
         <v>388</v>
       </c>
       <c r="C940" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E940" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="941" spans="2:5" x14ac:dyDescent="0.25">
@@ -17607,13 +17905,13 @@
         <v>388</v>
       </c>
       <c r="C941" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E941" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="942" spans="2:5" x14ac:dyDescent="0.25">
@@ -17621,13 +17919,13 @@
         <v>388</v>
       </c>
       <c r="C942" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E942" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="943" spans="2:5" x14ac:dyDescent="0.25">
@@ -17635,13 +17933,13 @@
         <v>388</v>
       </c>
       <c r="C943" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E943" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="944" spans="2:5" x14ac:dyDescent="0.25">
@@ -17649,13 +17947,13 @@
         <v>388</v>
       </c>
       <c r="C944" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E944" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="945" spans="2:5" x14ac:dyDescent="0.25">
@@ -17663,13 +17961,13 @@
         <v>388</v>
       </c>
       <c r="C945" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E945" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="946" spans="2:5" x14ac:dyDescent="0.25">
@@ -17677,13 +17975,13 @@
         <v>388</v>
       </c>
       <c r="C946" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E946" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="947" spans="2:5" x14ac:dyDescent="0.25">
@@ -17691,13 +17989,13 @@
         <v>388</v>
       </c>
       <c r="C947" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E947" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="948" spans="2:5" x14ac:dyDescent="0.25">
@@ -17705,69 +18003,69 @@
         <v>388</v>
       </c>
       <c r="C948" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
       </c>
       <c r="E948" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="949" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B949" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C949" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D949" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E949" s="1">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="950" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B950" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C950" s="1">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D950" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E950" s="1">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="951" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B951" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C951" s="1">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D951" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E951" s="1">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="952" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B952" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C952" s="1">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D952" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E952" s="1">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="953" spans="2:5" x14ac:dyDescent="0.25">
@@ -17775,13 +18073,13 @@
         <v>389</v>
       </c>
       <c r="C953" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E953" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="954" spans="2:5" x14ac:dyDescent="0.25">
@@ -17789,13 +18087,13 @@
         <v>389</v>
       </c>
       <c r="C954" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E954" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="955" spans="2:5" x14ac:dyDescent="0.25">
@@ -17803,13 +18101,13 @@
         <v>389</v>
       </c>
       <c r="C955" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E955" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="956" spans="2:5" x14ac:dyDescent="0.25">
@@ -17817,13 +18115,13 @@
         <v>389</v>
       </c>
       <c r="C956" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E956" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="957" spans="2:5" x14ac:dyDescent="0.25">
@@ -17831,13 +18129,13 @@
         <v>389</v>
       </c>
       <c r="C957" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E957" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="958" spans="2:5" x14ac:dyDescent="0.25">
@@ -17845,13 +18143,13 @@
         <v>389</v>
       </c>
       <c r="C958" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E958" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="959" spans="2:5" x14ac:dyDescent="0.25">
@@ -17859,13 +18157,13 @@
         <v>389</v>
       </c>
       <c r="C959" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E959" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="960" spans="2:5" x14ac:dyDescent="0.25">
@@ -17873,13 +18171,13 @@
         <v>389</v>
       </c>
       <c r="C960" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E960" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="961" spans="2:5" x14ac:dyDescent="0.25">
@@ -17887,13 +18185,13 @@
         <v>389</v>
       </c>
       <c r="C961" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E961" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="962" spans="2:5" x14ac:dyDescent="0.25">
@@ -17901,13 +18199,13 @@
         <v>389</v>
       </c>
       <c r="C962" s="1">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E962" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="963" spans="2:5" x14ac:dyDescent="0.25">
@@ -17915,13 +18213,13 @@
         <v>389</v>
       </c>
       <c r="C963" s="1">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E963" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="964" spans="2:5" x14ac:dyDescent="0.25">
@@ -17929,13 +18227,13 @@
         <v>389</v>
       </c>
       <c r="C964" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E964" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="965" spans="2:5" x14ac:dyDescent="0.25">
@@ -17943,13 +18241,13 @@
         <v>389</v>
       </c>
       <c r="C965" s="1">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E965" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="966" spans="2:5" x14ac:dyDescent="0.25">
@@ -17957,13 +18255,13 @@
         <v>389</v>
       </c>
       <c r="C966" s="1">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E966" s="1">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="967" spans="2:5" x14ac:dyDescent="0.25">
@@ -17971,13 +18269,13 @@
         <v>389</v>
       </c>
       <c r="C967" s="1">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E967" s="1">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="968" spans="2:5" x14ac:dyDescent="0.25">
@@ -17985,80 +18283,80 @@
         <v>389</v>
       </c>
       <c r="C968" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
       </c>
       <c r="E968" s="1">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="969" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B969" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C969" s="1">
-        <v>17</v>
+        <v>390</v>
+      </c>
+      <c r="C969" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D969" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E969" s="1">
-        <v>20</v>
+        <v>117</v>
+      </c>
+      <c r="E969" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="970" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B970" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C970" s="1">
-        <v>18</v>
+        <v>391</v>
+      </c>
+      <c r="C970" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D970" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E970" s="1">
-        <v>21</v>
+        <v>119</v>
+      </c>
+      <c r="E970" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="971" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B971" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C971" s="1">
-        <v>19</v>
+        <v>404</v>
+      </c>
+      <c r="C971" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D971" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E971" s="1">
-        <v>22</v>
+        <v>121</v>
+      </c>
+      <c r="E971" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="972" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B972" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C972" s="1">
-        <v>20</v>
+        <v>392</v>
+      </c>
+      <c r="C972" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="D972" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="E972" s="1">
-        <v>23</v>
+        <v>123</v>
+      </c>
+      <c r="E972" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="973" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B973" s="1" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C973" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D973" s="1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="E973" s="1" t="s">
         <v>4</v>
@@ -18066,13 +18364,13 @@
     </row>
     <row r="974" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B974" s="1" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D974" s="1" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="E974" s="1" t="s">
         <v>4</v>
@@ -18080,254 +18378,254 @@
     </row>
     <row r="975" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B975" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="C975" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C975" s="1">
+        <v>1</v>
       </c>
       <c r="D975" s="1" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="E975" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="976" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B976" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C976" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C976" s="1">
+        <v>2</v>
       </c>
       <c r="D976" s="1" t="s">
-        <v>123</v>
+        <v>9</v>
       </c>
       <c r="E976" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="977" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B977" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C977" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C977" s="1">
+        <v>3</v>
       </c>
       <c r="D977" s="1" t="s">
-        <v>126</v>
+        <v>9</v>
       </c>
       <c r="E977" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="978" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B978" s="1" t="s">
-        <v>405</v>
+        <v>8</v>
       </c>
       <c r="C978" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D978" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="E978" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="979" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B979" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C979" s="1">
-        <v>1</v>
+      <c r="C979" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E979" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="980" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B980" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C980" s="1">
-        <v>2</v>
+        <v>77</v>
+      </c>
+      <c r="C980" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D980" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="E980" s="1" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
     <row r="981" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B981" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C981" s="1">
-        <v>3</v>
+        <v>77</v>
+      </c>
+      <c r="C981" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D981" s="1" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="E981" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
     </row>
     <row r="982" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B982" s="1" t="s">
-        <v>8</v>
+        <v>408</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D982" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="E982" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="983" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B983" s="1" t="s">
-        <v>8</v>
+        <v>409</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D983" s="1" t="s">
-        <v>9</v>
+        <v>85</v>
       </c>
       <c r="E983" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="984" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B984" s="1" t="s">
-        <v>77</v>
+        <v>6</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="D984" s="1" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E984" s="1" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="985" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B985" s="1" t="s">
-        <v>77</v>
+        <v>394</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>56</v>
+        <v>395</v>
       </c>
       <c r="D985" s="1" t="s">
-        <v>72</v>
+        <v>284</v>
       </c>
       <c r="E985" s="1" t="s">
-        <v>75</v>
+        <v>287</v>
       </c>
     </row>
     <row r="986" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B986" s="1" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>4</v>
+        <v>396</v>
       </c>
       <c r="D986" s="1" t="s">
-        <v>81</v>
+        <v>284</v>
       </c>
       <c r="E986" s="1" t="s">
-        <v>4</v>
+        <v>285</v>
       </c>
     </row>
     <row r="987" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B987" s="1" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>4</v>
+        <v>397</v>
       </c>
       <c r="D987" s="1" t="s">
-        <v>85</v>
+        <v>284</v>
       </c>
       <c r="E987" s="1" t="s">
-        <v>4</v>
+        <v>286</v>
       </c>
     </row>
     <row r="988" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B988" s="1" t="s">
-        <v>6</v>
+        <v>394</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>4</v>
+        <v>398</v>
       </c>
       <c r="D988" s="1" t="s">
-        <v>7</v>
+        <v>284</v>
       </c>
       <c r="E988" s="1" t="s">
-        <v>4</v>
+        <v>341</v>
       </c>
     </row>
     <row r="989" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B989" s="1" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>395</v>
+        <v>292</v>
       </c>
       <c r="D989" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E989" s="1" t="s">
-        <v>287</v>
+        <v>360</v>
       </c>
     </row>
     <row r="990" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B990" s="1" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="C990" s="1" t="s">
-        <v>396</v>
+        <v>357</v>
       </c>
       <c r="D990" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E990" s="1" t="s">
-        <v>285</v>
+        <v>187</v>
       </c>
     </row>
     <row r="991" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B991" s="1" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="C991" s="1" t="s">
-        <v>397</v>
+        <v>293</v>
       </c>
       <c r="D991" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E991" s="1" t="s">
-        <v>286</v>
+        <v>179</v>
       </c>
     </row>
     <row r="992" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B992" s="1" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="C992" s="1" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="D992" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E992" s="1" t="s">
-        <v>341</v>
+        <v>180</v>
       </c>
     </row>
     <row r="993" spans="2:5" x14ac:dyDescent="0.25">
@@ -18335,80 +18633,80 @@
         <v>399</v>
       </c>
       <c r="C993" s="1" t="s">
-        <v>292</v>
+        <v>359</v>
       </c>
       <c r="D993" s="1" t="s">
         <v>291</v>
       </c>
       <c r="E993" s="1" t="s">
-        <v>360</v>
+        <v>217</v>
       </c>
     </row>
     <row r="994" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B994" s="1" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="C994" s="1" t="s">
-        <v>357</v>
+        <v>4</v>
       </c>
       <c r="D994" s="1" t="s">
-        <v>291</v>
+        <v>110</v>
       </c>
       <c r="E994" s="1" t="s">
-        <v>187</v>
+        <v>4</v>
       </c>
     </row>
     <row r="995" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B995" s="1" t="s">
-        <v>399</v>
+        <v>407</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>293</v>
+        <v>4</v>
       </c>
       <c r="D995" s="1" t="s">
-        <v>291</v>
+        <v>111</v>
       </c>
       <c r="E995" s="1" t="s">
-        <v>179</v>
+        <v>4</v>
       </c>
     </row>
     <row r="996" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B996" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>358</v>
+        <v>4</v>
       </c>
       <c r="D996" s="1" t="s">
-        <v>291</v>
+        <v>108</v>
       </c>
       <c r="E996" s="1" t="s">
-        <v>180</v>
+        <v>4</v>
       </c>
     </row>
     <row r="997" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B997" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>359</v>
+        <v>4</v>
       </c>
       <c r="D997" s="1" t="s">
-        <v>291</v>
+        <v>109</v>
       </c>
       <c r="E997" s="1" t="s">
-        <v>217</v>
+        <v>4</v>
       </c>
     </row>
     <row r="998" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B998" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C998" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D998" s="1" t="s">
-        <v>110</v>
+        <v>342</v>
       </c>
       <c r="E998" s="1" t="s">
         <v>4</v>
@@ -18416,13 +18714,13 @@
     </row>
     <row r="999" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B999" s="1" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C999" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D999" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="E999" s="1" t="s">
         <v>4</v>
@@ -18430,13 +18728,13 @@
     </row>
     <row r="1000" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1000" s="1" t="s">
-        <v>400</v>
+        <v>415</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1000" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E1000" s="1" t="s">
         <v>4</v>
@@ -18444,13 +18742,13 @@
     </row>
     <row r="1001" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1001" s="1" t="s">
-        <v>401</v>
+        <v>416</v>
       </c>
       <c r="C1001" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1001" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E1001" s="1" t="s">
         <v>4</v>
@@ -18458,71 +18756,15 @@
     </row>
     <row r="1002" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1002" s="1" t="s">
-        <v>402</v>
+        <v>417</v>
       </c>
       <c r="C1002" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1002" s="1" t="s">
-        <v>342</v>
+        <v>107</v>
       </c>
       <c r="E1002" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1003" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1003" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C1003" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1003" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1003" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1004" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1004" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C1004" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1004" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1004" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1005" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1005" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="C1005" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1005" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1005" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1006" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1006" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C1006" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1006" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1006" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first pass through muni; updated tableau
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4302" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4302" uniqueCount="584">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1996,6 +1996,12 @@
   </si>
   <si>
     <t>ROUTE_SURVEYED</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>Not employed</t>
   </si>
 </sst>
 </file>
@@ -2465,8 +2471,8 @@
   <dimension ref="A1:E1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A978" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1016" sqref="A1016"/>
+      <pane ySplit="1" topLeftCell="A816" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C833" sqref="C833"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16596,7 +16602,7 @@
         <v>437</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>57</v>
+        <v>583</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16613,7 +16619,7 @@
         <v>437</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>56</v>
+        <v>582</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
rename Muni to Pilot
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -1506,9 +1506,6 @@
     <t>BART_EXIT_LON</t>
   </si>
   <si>
-    <t>SF Muni</t>
-  </si>
-  <si>
     <t>Walked all the way</t>
   </si>
   <si>
@@ -2002,6 +1999,9 @@
   </si>
   <si>
     <t>Not employed</t>
+  </si>
+  <si>
+    <t>SF Muni Pilot</t>
   </si>
 </sst>
 </file>
@@ -2471,8 +2471,8 @@
   <dimension ref="A1:E1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A816" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C833" sqref="C833"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15984,13 +15984,13 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="B795" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C795" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="B795" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="C795" s="1" t="s">
-        <v>419</v>
       </c>
       <c r="D795" s="1" t="s">
         <v>129</v>
@@ -16001,13 +16001,13 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D796" s="1" t="s">
         <v>129</v>
@@ -16018,13 +16018,13 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D797" s="1" t="s">
         <v>129</v>
@@ -16035,13 +16035,13 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D798" s="1" t="s">
         <v>129</v>
@@ -16052,13 +16052,13 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D799" s="1" t="s">
         <v>129</v>
@@ -16069,13 +16069,13 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D800" s="1" t="s">
         <v>129</v>
@@ -16086,13 +16086,13 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D801" s="1" t="s">
         <v>129</v>
@@ -16103,10 +16103,10 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C802" s="1" t="s">
         <v>57</v>
@@ -16120,10 +16120,10 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>56</v>
@@ -16137,10 +16137,10 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>57</v>
@@ -16154,10 +16154,10 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>56</v>
@@ -16171,10 +16171,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -16188,10 +16188,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -16205,13 +16205,13 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>52</v>
@@ -16222,13 +16222,13 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>52</v>
@@ -16239,13 +16239,13 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>52</v>
@@ -16256,13 +16256,13 @@
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>52</v>
@@ -16273,13 +16273,13 @@
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>52</v>
@@ -16290,13 +16290,13 @@
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>52</v>
@@ -16307,13 +16307,13 @@
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>52</v>
@@ -16324,13 +16324,13 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>52</v>
@@ -16341,13 +16341,13 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>52</v>
@@ -16358,13 +16358,13 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>52</v>
@@ -16375,13 +16375,13 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>52</v>
@@ -16392,13 +16392,13 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>52</v>
@@ -16409,13 +16409,13 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>52</v>
@@ -16426,13 +16426,13 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>52</v>
@@ -16443,13 +16443,13 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>135</v>
@@ -16460,10 +16460,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>50</v>
@@ -16477,10 +16477,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>50</v>
@@ -16494,13 +16494,13 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>135</v>
@@ -16511,10 +16511,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>50</v>
@@ -16528,13 +16528,13 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>135</v>
@@ -16545,13 +16545,13 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>135</v>
@@ -16562,13 +16562,13 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>135</v>
@@ -16579,13 +16579,13 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>135</v>
@@ -16596,13 +16596,13 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16613,13 +16613,13 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>
@@ -16630,13 +16630,13 @@
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>16</v>
@@ -16647,13 +16647,13 @@
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>16</v>
@@ -16664,13 +16664,13 @@
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>16</v>
@@ -16681,13 +16681,13 @@
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -16698,13 +16698,13 @@
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -16715,13 +16715,13 @@
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>16</v>
@@ -16732,13 +16732,13 @@
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>16</v>
@@ -16749,13 +16749,13 @@
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C840" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>16</v>
@@ -16766,13 +16766,13 @@
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>16</v>
@@ -16783,13 +16783,13 @@
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
@@ -16800,13 +16800,13 @@
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -16817,13 +16817,13 @@
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>244</v>
@@ -16834,13 +16834,13 @@
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>244</v>
@@ -16851,13 +16851,13 @@
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>244</v>
@@ -16868,13 +16868,13 @@
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>244</v>
@@ -16885,13 +16885,13 @@
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D848" s="1" t="s">
         <v>148</v>
@@ -16902,13 +16902,13 @@
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C849" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>148</v>
@@ -16919,13 +16919,13 @@
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D850" s="1" t="s">
         <v>148</v>
@@ -16936,13 +16936,13 @@
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>148</v>
@@ -16953,13 +16953,13 @@
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>148</v>
@@ -16970,13 +16970,13 @@
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>148</v>
@@ -16987,13 +16987,13 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>148</v>
@@ -17004,13 +17004,13 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D855" s="1" t="s">
         <v>148</v>
@@ -17021,7 +17021,7 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>274</v>
@@ -17038,7 +17038,7 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>274</v>
@@ -17055,13 +17055,13 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>225</v>
@@ -17072,13 +17072,13 @@
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A859" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>225</v>
@@ -17089,13 +17089,13 @@
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A860" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D860" s="1" t="s">
         <v>225</v>
@@ -17106,13 +17106,13 @@
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A861" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>225</v>
@@ -17123,13 +17123,13 @@
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
@@ -17140,13 +17140,13 @@
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A863" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
@@ -17157,13 +17157,13 @@
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A864" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
@@ -17174,13 +17174,13 @@
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
@@ -17191,13 +17191,13 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
@@ -17208,13 +17208,13 @@
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>225</v>
@@ -17225,13 +17225,13 @@
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D868" s="1" t="s">
         <v>225</v>
@@ -17242,10 +17242,10 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>57</v>
@@ -17259,10 +17259,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>56</v>
@@ -17276,10 +17276,10 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B871" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C871" s="1" t="s">
         <v>4</v>
@@ -17293,10 +17293,10 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B872" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C872" s="1" t="s">
         <v>4</v>
@@ -17310,7 +17310,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>5</v>
@@ -17327,10 +17327,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>57</v>
@@ -17344,10 +17344,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>56</v>
@@ -17361,10 +17361,10 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
@@ -17378,10 +17378,10 @@
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C877" s="1" t="s">
         <v>4</v>
@@ -17395,13 +17395,13 @@
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A878" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B878" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="C878" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="C878" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="D878" s="1" t="s">
         <v>40</v>
@@ -17412,13 +17412,13 @@
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>40</v>
@@ -17429,13 +17429,13 @@
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
@@ -17446,13 +17446,13 @@
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
@@ -17463,13 +17463,13 @@
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
@@ -17480,13 +17480,13 @@
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
@@ -17497,13 +17497,13 @@
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
@@ -17514,13 +17514,13 @@
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
@@ -17531,13 +17531,13 @@
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
@@ -17548,13 +17548,13 @@
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
@@ -17565,13 +17565,13 @@
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
@@ -17582,13 +17582,13 @@
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
@@ -17599,13 +17599,13 @@
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
@@ -17616,10 +17616,10 @@
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C891" s="1" t="s">
         <v>4</v>
@@ -17633,47 +17633,47 @@
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D894" s="1" t="s">
         <v>139</v>
@@ -17684,13 +17684,13 @@
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B895" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D895" s="1" t="s">
         <v>37</v>
@@ -17701,13 +17701,13 @@
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B896" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D896" s="1" t="s">
         <v>37</v>
@@ -17718,13 +17718,13 @@
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A897" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B897" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D897" s="1" t="s">
         <v>37</v>
@@ -17735,13 +17735,13 @@
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B898" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D898" s="1" t="s">
         <v>37</v>
@@ -17752,13 +17752,13 @@
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B899" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>37</v>
@@ -17769,13 +17769,13 @@
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B900" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D900" s="1" t="s">
         <v>37</v>
@@ -17786,13 +17786,13 @@
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A901" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B901" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D901" s="1" t="s">
         <v>37</v>
@@ -17803,13 +17803,13 @@
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D902" s="1" t="s">
         <v>37</v>
@@ -17820,13 +17820,13 @@
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A903" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B903" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D903" s="1" t="s">
         <v>37</v>
@@ -17837,13 +17837,13 @@
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A904" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B904" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
@@ -17854,10 +17854,10 @@
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>56</v>
@@ -17871,10 +17871,10 @@
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>57</v>
@@ -17888,13 +17888,13 @@
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A907" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>160</v>
@@ -17905,10 +17905,10 @@
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A908" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>56</v>
@@ -17922,10 +17922,10 @@
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A909" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>57</v>
@@ -17939,13 +17939,13 @@
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D910" s="1" t="s">
         <v>162</v>
@@ -17956,10 +17956,10 @@
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A911" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C911" s="1" t="s">
         <v>56</v>
@@ -17973,10 +17973,10 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C912" s="1" t="s">
         <v>57</v>
@@ -17990,13 +17990,13 @@
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>164</v>
@@ -18007,10 +18007,10 @@
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>56</v>
@@ -18024,10 +18024,10 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>57</v>
@@ -18041,13 +18041,13 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D916" s="1" t="s">
         <v>166</v>
@@ -18058,10 +18058,10 @@
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
@@ -18075,10 +18075,10 @@
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>57</v>
@@ -18092,13 +18092,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D919" s="1" t="s">
         <v>168</v>
@@ -18109,10 +18109,10 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>4</v>
@@ -18126,13 +18126,13 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B921" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C921" s="1" t="s">
         <v>518</v>
-      </c>
-      <c r="C921" s="1" t="s">
-        <v>519</v>
       </c>
       <c r="D921" s="1" t="s">
         <v>236</v>
@@ -18143,13 +18143,13 @@
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D922" s="1" t="s">
         <v>236</v>
@@ -18160,27 +18160,27 @@
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D923" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E923" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>4</v>
@@ -18194,10 +18194,10 @@
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>4</v>
@@ -18211,13 +18211,13 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D926" s="1" t="s">
         <v>60</v>
@@ -18228,13 +18228,13 @@
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B927" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D927" s="1" t="s">
         <v>60</v>
@@ -18245,13 +18245,13 @@
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D928" s="1" t="s">
         <v>60</v>
@@ -18262,13 +18262,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A929" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D929" s="1" t="s">
         <v>60</v>
@@ -18279,13 +18279,13 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D930" s="1" t="s">
         <v>60</v>
@@ -18296,13 +18296,13 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A931" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D931" s="1" t="s">
         <v>60</v>
@@ -18313,13 +18313,13 @@
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A932" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B932" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D932" s="1" t="s">
         <v>60</v>
@@ -18330,10 +18330,10 @@
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A933" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B933" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>4</v>
@@ -18347,10 +18347,10 @@
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B934" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C934" s="1" t="s">
         <v>4</v>
@@ -18364,13 +18364,13 @@
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A935" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B935" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="C935" s="1" t="s">
         <v>529</v>
-      </c>
-      <c r="C935" s="1" t="s">
-        <v>530</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
@@ -18381,13 +18381,13 @@
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A936" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C936" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
@@ -18398,13 +18398,13 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A937" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
@@ -18415,13 +18415,13 @@
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A938" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
@@ -18432,13 +18432,13 @@
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
@@ -18449,13 +18449,13 @@
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
@@ -18466,13 +18466,13 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
@@ -18483,13 +18483,13 @@
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
@@ -18500,13 +18500,13 @@
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A943" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
@@ -18517,13 +18517,13 @@
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A944" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
@@ -18534,13 +18534,13 @@
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A945" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
@@ -18551,13 +18551,13 @@
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A946" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
@@ -18568,13 +18568,13 @@
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
@@ -18585,13 +18585,13 @@
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A948" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
@@ -18602,13 +18602,13 @@
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>251</v>
@@ -18619,13 +18619,13 @@
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A950" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>251</v>
@@ -18636,13 +18636,13 @@
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>251</v>
@@ -18653,13 +18653,13 @@
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>251</v>
@@ -18670,13 +18670,13 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A953" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
@@ -18687,13 +18687,13 @@
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B954" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
@@ -18704,13 +18704,13 @@
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A955" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B955" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
@@ -18721,13 +18721,13 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A956" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B956" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
@@ -18738,13 +18738,13 @@
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A957" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B957" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
@@ -18755,13 +18755,13 @@
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A958" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B958" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
@@ -18772,13 +18772,13 @@
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A959" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B959" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
@@ -18789,13 +18789,13 @@
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A960" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B960" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
@@ -18806,13 +18806,13 @@
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A961" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B961" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
@@ -18823,13 +18823,13 @@
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A962" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
@@ -18840,13 +18840,13 @@
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A963" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B963" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
@@ -18857,13 +18857,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B964" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
@@ -18874,13 +18874,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B965" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
@@ -18891,13 +18891,13 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A966" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B966" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
@@ -18908,13 +18908,13 @@
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A967" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B967" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
@@ -18925,13 +18925,13 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B968" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
@@ -18942,13 +18942,13 @@
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>253</v>
@@ -18959,13 +18959,13 @@
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A970" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>253</v>
@@ -18976,13 +18976,13 @@
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A971" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B971" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>253</v>
@@ -18993,13 +18993,13 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A972" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B972" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>253</v>
@@ -19010,10 +19010,10 @@
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A973" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C973" s="1" t="s">
         <v>4</v>
@@ -19027,10 +19027,10 @@
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
@@ -19044,10 +19044,10 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C975" s="1" t="s">
         <v>4</v>
@@ -19061,10 +19061,10 @@
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C976" s="1" t="s">
         <v>4</v>
@@ -19078,10 +19078,10 @@
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A977" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C977" s="1" t="s">
         <v>4</v>
@@ -19095,10 +19095,10 @@
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C978" s="1" t="s">
         <v>4</v>
@@ -19112,13 +19112,13 @@
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B979" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="C979" s="1" t="s">
         <v>556</v>
-      </c>
-      <c r="C979" s="1" t="s">
-        <v>557</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
@@ -19129,13 +19129,13 @@
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B980" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D980" s="1" t="s">
         <v>9</v>
@@ -19146,13 +19146,13 @@
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A981" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B981" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D981" s="1" t="s">
         <v>9</v>
@@ -19163,13 +19163,13 @@
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B982" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D982" s="1" t="s">
         <v>9</v>
@@ -19180,13 +19180,13 @@
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B983" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D983" s="1" t="s">
         <v>9</v>
@@ -19197,13 +19197,13 @@
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B984" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D984" s="1" t="s">
         <v>9</v>
@@ -19214,13 +19214,13 @@
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A985" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B985" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D985" s="1" t="s">
         <v>9</v>
@@ -19231,13 +19231,13 @@
     </row>
     <row r="986" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B986" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D986" s="1" t="s">
         <v>9</v>
@@ -19248,13 +19248,13 @@
     </row>
     <row r="987" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B987" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D987" s="1" t="s">
         <v>9</v>
@@ -19265,13 +19265,13 @@
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B988" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D988" s="1" t="s">
         <v>9</v>
@@ -19282,13 +19282,13 @@
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D989" s="1" t="s">
         <v>9</v>
@@ -19299,10 +19299,10 @@
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B990" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C990" s="1" t="s">
         <v>57</v>
@@ -19316,10 +19316,10 @@
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B991" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C991" s="1" t="s">
         <v>56</v>
@@ -19333,10 +19333,10 @@
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A992" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C992" s="1" t="s">
         <v>4</v>
@@ -19350,10 +19350,10 @@
     </row>
     <row r="993" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C993" s="1" t="s">
         <v>4</v>
@@ -19367,10 +19367,10 @@
     </row>
     <row r="994" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B994" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C994" s="1" t="s">
         <v>4</v>
@@ -19384,13 +19384,13 @@
     </row>
     <row r="995" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B995" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D995" s="1" t="s">
         <v>284</v>
@@ -19401,13 +19401,13 @@
     </row>
     <row r="996" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B996" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D996" s="1" t="s">
         <v>284</v>
@@ -19418,13 +19418,13 @@
     </row>
     <row r="997" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B997" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D997" s="1" t="s">
         <v>284</v>
@@ -19435,10 +19435,10 @@
     </row>
     <row r="998" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A998" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B998" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D998" s="1" t="s">
         <v>291</v>
@@ -19449,13 +19449,13 @@
     </row>
     <row r="999" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D999" s="1" t="s">
         <v>291</v>
@@ -19466,10 +19466,10 @@
     </row>
     <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1000" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>187</v>
@@ -19483,13 +19483,13 @@
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1001" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D1001" s="1" t="s">
         <v>291</v>
@@ -19500,13 +19500,13 @@
     </row>
     <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1002" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D1002" s="1" t="s">
         <v>291</v>
@@ -19517,10 +19517,10 @@
     </row>
     <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C1003" s="1" t="s">
         <v>4</v>
@@ -19534,10 +19534,10 @@
     </row>
     <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1004" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C1004" s="1" t="s">
         <v>4</v>
@@ -19551,10 +19551,10 @@
     </row>
     <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1005" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C1005" s="1" t="s">
         <v>4</v>
@@ -19568,10 +19568,10 @@
     </row>
     <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1006" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C1006" s="1" t="s">
         <v>4</v>
@@ -19585,10 +19585,10 @@
     </row>
     <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1007" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C1007" s="1" t="s">
         <v>4</v>
@@ -19602,10 +19602,10 @@
     </row>
     <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C1008" s="1" t="s">
         <v>4</v>
@@ -19619,10 +19619,10 @@
     </row>
     <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C1009" s="1" t="s">
         <v>4</v>
@@ -19636,10 +19636,10 @@
     </row>
     <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1010" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C1010" s="1" t="s">
         <v>4</v>
@@ -19653,10 +19653,10 @@
     </row>
     <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1011" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1011" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C1011" s="1" t="s">
         <v>4</v>
@@ -19670,16 +19670,16 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1012" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1012" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1012" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="C1012" s="1" t="s">
-        <v>495</v>
-      </c>
       <c r="D1012" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E1012" s="1" t="s">
         <v>144</v>
@@ -19687,61 +19687,61 @@
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1013" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1013" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C1013" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D1013" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1013" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="E1013" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1014" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C1014" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D1014" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="D1014" s="1" t="s">
+      <c r="E1014" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="E1014" s="1" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
-        <v>418</v>
+        <v>583</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1015" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E1015" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="1016" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1016" s="5" t="s">
-        <v>418</v>
+      <c r="A1016" s="1" t="s">
+        <v>583</v>
       </c>
       <c r="B1016" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C1016" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update Dictionary for BART Entry and Exit Stations
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dory\Documents\GitHub\onboard-surveys\make-uniform\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrae.MTC\Documents\GitHub\onboard-surveys\make-uniform\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1374,12 +1374,6 @@
     <t>EMPLOYED_IN_HH_CODE</t>
   </si>
   <si>
-    <t>ENTERSTATION</t>
-  </si>
-  <si>
-    <t>EXITSTATION</t>
-  </si>
-  <si>
     <t>HOME_ADDRESS_LAT</t>
   </si>
   <si>
@@ -2002,6 +1996,12 @@
   </si>
   <si>
     <t>SF Muni Pilot</t>
+  </si>
+  <si>
+    <t>FIRST_ENTERED_BART</t>
+  </si>
+  <si>
+    <t>BART_EXIT_STATION</t>
   </si>
 </sst>
 </file>
@@ -2471,8 +2471,8 @@
   <dimension ref="A1:E1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A620" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B636" sqref="B636"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13267,7 +13267,7 @@
         <v>362</v>
       </c>
       <c r="B635" s="7" t="s">
-        <v>374</v>
+        <v>582</v>
       </c>
       <c r="C635" s="7" t="s">
         <v>4</v>
@@ -13284,7 +13284,7 @@
         <v>362</v>
       </c>
       <c r="B636" s="7" t="s">
-        <v>375</v>
+        <v>583</v>
       </c>
       <c r="C636" s="7" t="s">
         <v>4</v>
@@ -13301,7 +13301,7 @@
         <v>362</v>
       </c>
       <c r="B637" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C637" s="7">
         <v>1</v>
@@ -13318,7 +13318,7 @@
         <v>362</v>
       </c>
       <c r="B638" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C638" s="7">
         <v>2</v>
@@ -13335,7 +13335,7 @@
         <v>362</v>
       </c>
       <c r="B639" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C639" s="7">
         <v>3</v>
@@ -13352,7 +13352,7 @@
         <v>362</v>
       </c>
       <c r="B640" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C640" s="7">
         <v>4</v>
@@ -13369,7 +13369,7 @@
         <v>362</v>
       </c>
       <c r="B641" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C641" s="7">
         <v>1</v>
@@ -13386,7 +13386,7 @@
         <v>362</v>
       </c>
       <c r="B642" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C642" s="7">
         <v>2</v>
@@ -13403,7 +13403,7 @@
         <v>362</v>
       </c>
       <c r="B643" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C643" s="7">
         <v>3</v>
@@ -13420,7 +13420,7 @@
         <v>362</v>
       </c>
       <c r="B644" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C644" s="7">
         <v>4</v>
@@ -13437,7 +13437,7 @@
         <v>362</v>
       </c>
       <c r="B645" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C645" s="7">
         <v>5</v>
@@ -13454,7 +13454,7 @@
         <v>362</v>
       </c>
       <c r="B646" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C646" s="7">
         <v>6</v>
@@ -13471,7 +13471,7 @@
         <v>362</v>
       </c>
       <c r="B647" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C647" s="7">
         <v>7</v>
@@ -13695,7 +13695,7 @@
         <v>153</v>
       </c>
       <c r="C660" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D660" s="7" t="s">
         <v>156</v>
@@ -13712,7 +13712,7 @@
         <v>153</v>
       </c>
       <c r="C661" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D661" s="7" t="s">
         <v>156</v>
@@ -13726,7 +13726,7 @@
         <v>362</v>
       </c>
       <c r="B662" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C662" s="7" t="s">
         <v>4</v>
@@ -13743,7 +13743,7 @@
         <v>362</v>
       </c>
       <c r="B663" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C663" s="7" t="s">
         <v>4</v>
@@ -13811,7 +13811,7 @@
         <v>362</v>
       </c>
       <c r="B667" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C667" s="7" t="s">
         <v>4</v>
@@ -13828,7 +13828,7 @@
         <v>362</v>
       </c>
       <c r="B668" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C668" s="7" t="s">
         <v>4</v>
@@ -13845,7 +13845,7 @@
         <v>362</v>
       </c>
       <c r="B669" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C669" s="7">
         <v>1</v>
@@ -13862,7 +13862,7 @@
         <v>362</v>
       </c>
       <c r="B670" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C670" s="7">
         <v>2</v>
@@ -13879,7 +13879,7 @@
         <v>362</v>
       </c>
       <c r="B671" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C671" s="7">
         <v>3</v>
@@ -13896,7 +13896,7 @@
         <v>362</v>
       </c>
       <c r="B672" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C672" s="7">
         <v>4</v>
@@ -13913,7 +13913,7 @@
         <v>362</v>
       </c>
       <c r="B673" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C673" s="7">
         <v>5</v>
@@ -13930,7 +13930,7 @@
         <v>362</v>
       </c>
       <c r="B674" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C674" s="7">
         <v>6</v>
@@ -13947,7 +13947,7 @@
         <v>362</v>
       </c>
       <c r="B675" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C675" s="7">
         <v>7</v>
@@ -13964,7 +13964,7 @@
         <v>362</v>
       </c>
       <c r="B676" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C676" s="7">
         <v>8</v>
@@ -13981,7 +13981,7 @@
         <v>362</v>
       </c>
       <c r="B677" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C677" s="7">
         <v>9</v>
@@ -13998,7 +13998,7 @@
         <v>362</v>
       </c>
       <c r="B678" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C678" s="7">
         <v>10</v>
@@ -14015,7 +14015,7 @@
         <v>362</v>
       </c>
       <c r="B679" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C679" s="7">
         <v>11</v>
@@ -14032,7 +14032,7 @@
         <v>362</v>
       </c>
       <c r="B680" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C680" s="7">
         <v>12</v>
@@ -14049,7 +14049,7 @@
         <v>362</v>
       </c>
       <c r="B681" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C681" s="7">
         <v>13</v>
@@ -14066,7 +14066,7 @@
         <v>362</v>
       </c>
       <c r="B682" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C682" s="7">
         <v>14</v>
@@ -14083,7 +14083,7 @@
         <v>362</v>
       </c>
       <c r="B683" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C683" s="7">
         <v>15</v>
@@ -14100,7 +14100,7 @@
         <v>362</v>
       </c>
       <c r="B684" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C684" s="7">
         <v>16</v>
@@ -14117,7 +14117,7 @@
         <v>362</v>
       </c>
       <c r="B685" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C685" s="7">
         <v>17</v>
@@ -14134,7 +14134,7 @@
         <v>362</v>
       </c>
       <c r="B686" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C686" s="7" t="s">
         <v>4</v>
@@ -14151,7 +14151,7 @@
         <v>362</v>
       </c>
       <c r="B687" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C687" s="7">
         <v>1</v>
@@ -14168,7 +14168,7 @@
         <v>362</v>
       </c>
       <c r="B688" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C688" s="7">
         <v>2</v>
@@ -14177,7 +14177,7 @@
         <v>139</v>
       </c>
       <c r="E688" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.25">
@@ -14185,7 +14185,7 @@
         <v>362</v>
       </c>
       <c r="B689" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C689" s="7">
         <v>3</v>
@@ -14202,7 +14202,7 @@
         <v>362</v>
       </c>
       <c r="B690" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C690" s="7">
         <v>4</v>
@@ -14219,7 +14219,7 @@
         <v>362</v>
       </c>
       <c r="B691" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C691" s="7">
         <v>5</v>
@@ -14542,7 +14542,7 @@
         <v>362</v>
       </c>
       <c r="B710" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C710" s="7" t="s">
         <v>4</v>
@@ -14627,7 +14627,7 @@
         <v>362</v>
       </c>
       <c r="B715" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C715" s="7" t="s">
         <v>4</v>
@@ -14644,7 +14644,7 @@
         <v>362</v>
       </c>
       <c r="B716" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C716" s="7" t="s">
         <v>4</v>
@@ -14695,7 +14695,7 @@
         <v>362</v>
       </c>
       <c r="B719" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C719" s="7" t="s">
         <v>4</v>
@@ -14712,7 +14712,7 @@
         <v>362</v>
       </c>
       <c r="B720" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C720" s="7" t="s">
         <v>4</v>
@@ -14729,7 +14729,7 @@
         <v>362</v>
       </c>
       <c r="B721" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C721" s="7">
         <v>1</v>
@@ -14746,7 +14746,7 @@
         <v>362</v>
       </c>
       <c r="B722" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C722" s="7">
         <v>2</v>
@@ -14763,7 +14763,7 @@
         <v>362</v>
       </c>
       <c r="B723" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C723" s="7">
         <v>3</v>
@@ -14780,7 +14780,7 @@
         <v>362</v>
       </c>
       <c r="B724" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C724" s="7">
         <v>4</v>
@@ -14797,7 +14797,7 @@
         <v>362</v>
       </c>
       <c r="B725" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C725" s="7">
         <v>5</v>
@@ -14814,7 +14814,7 @@
         <v>362</v>
       </c>
       <c r="B726" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C726" s="7">
         <v>6</v>
@@ -14831,7 +14831,7 @@
         <v>362</v>
       </c>
       <c r="B727" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C727" s="7">
         <v>7</v>
@@ -14848,7 +14848,7 @@
         <v>362</v>
       </c>
       <c r="B728" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C728" s="7">
         <v>8</v>
@@ -14865,7 +14865,7 @@
         <v>362</v>
       </c>
       <c r="B729" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C729" s="7">
         <v>9</v>
@@ -14882,7 +14882,7 @@
         <v>362</v>
       </c>
       <c r="B730" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C730" s="7">
         <v>10</v>
@@ -14899,7 +14899,7 @@
         <v>362</v>
       </c>
       <c r="B731" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C731" s="7">
         <v>11</v>
@@ -14916,7 +14916,7 @@
         <v>362</v>
       </c>
       <c r="B732" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C732" s="7">
         <v>12</v>
@@ -14933,7 +14933,7 @@
         <v>362</v>
       </c>
       <c r="B733" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C733" s="7">
         <v>13</v>
@@ -14950,7 +14950,7 @@
         <v>362</v>
       </c>
       <c r="B734" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C734" s="7">
         <v>14</v>
@@ -14967,7 +14967,7 @@
         <v>362</v>
       </c>
       <c r="B735" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C735" s="7">
         <v>15</v>
@@ -14984,7 +14984,7 @@
         <v>362</v>
       </c>
       <c r="B736" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C736" s="7">
         <v>16</v>
@@ -15001,7 +15001,7 @@
         <v>362</v>
       </c>
       <c r="B737" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C737" s="7">
         <v>17</v>
@@ -15018,7 +15018,7 @@
         <v>362</v>
       </c>
       <c r="B738" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C738" s="7">
         <v>18</v>
@@ -15035,7 +15035,7 @@
         <v>362</v>
       </c>
       <c r="B739" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C739" s="7">
         <v>19</v>
@@ -15052,7 +15052,7 @@
         <v>362</v>
       </c>
       <c r="B740" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C740" s="7">
         <v>20</v>
@@ -15069,7 +15069,7 @@
         <v>362</v>
       </c>
       <c r="B741" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C741" s="7">
         <v>1</v>
@@ -15086,7 +15086,7 @@
         <v>362</v>
       </c>
       <c r="B742" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C742" s="7">
         <v>2</v>
@@ -15103,7 +15103,7 @@
         <v>362</v>
       </c>
       <c r="B743" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C743" s="7">
         <v>3</v>
@@ -15120,7 +15120,7 @@
         <v>362</v>
       </c>
       <c r="B744" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C744" s="7">
         <v>4</v>
@@ -15137,7 +15137,7 @@
         <v>362</v>
       </c>
       <c r="B745" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C745" s="7">
         <v>5</v>
@@ -15154,7 +15154,7 @@
         <v>362</v>
       </c>
       <c r="B746" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C746" s="7">
         <v>6</v>
@@ -15171,7 +15171,7 @@
         <v>362</v>
       </c>
       <c r="B747" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C747" s="7">
         <v>7</v>
@@ -15188,7 +15188,7 @@
         <v>362</v>
       </c>
       <c r="B748" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C748" s="7">
         <v>8</v>
@@ -15205,7 +15205,7 @@
         <v>362</v>
       </c>
       <c r="B749" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C749" s="7">
         <v>9</v>
@@ -15222,7 +15222,7 @@
         <v>362</v>
       </c>
       <c r="B750" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C750" s="7">
         <v>10</v>
@@ -15239,7 +15239,7 @@
         <v>362</v>
       </c>
       <c r="B751" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C751" s="7">
         <v>11</v>
@@ -15256,7 +15256,7 @@
         <v>362</v>
       </c>
       <c r="B752" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C752" s="7">
         <v>12</v>
@@ -15273,7 +15273,7 @@
         <v>362</v>
       </c>
       <c r="B753" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C753" s="7">
         <v>13</v>
@@ -15290,7 +15290,7 @@
         <v>362</v>
       </c>
       <c r="B754" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C754" s="7">
         <v>14</v>
@@ -15307,7 +15307,7 @@
         <v>362</v>
       </c>
       <c r="B755" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C755" s="7">
         <v>15</v>
@@ -15324,7 +15324,7 @@
         <v>362</v>
       </c>
       <c r="B756" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C756" s="7">
         <v>16</v>
@@ -15341,7 +15341,7 @@
         <v>362</v>
       </c>
       <c r="B757" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C757" s="7">
         <v>17</v>
@@ -15358,7 +15358,7 @@
         <v>362</v>
       </c>
       <c r="B758" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C758" s="7">
         <v>18</v>
@@ -15375,7 +15375,7 @@
         <v>362</v>
       </c>
       <c r="B759" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C759" s="7">
         <v>19</v>
@@ -15392,7 +15392,7 @@
         <v>362</v>
       </c>
       <c r="B760" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C760" s="7">
         <v>20</v>
@@ -15409,7 +15409,7 @@
         <v>362</v>
       </c>
       <c r="B761" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C761" s="7" t="s">
         <v>4</v>
@@ -15426,7 +15426,7 @@
         <v>362</v>
       </c>
       <c r="B762" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C762" s="7" t="s">
         <v>4</v>
@@ -15443,7 +15443,7 @@
         <v>362</v>
       </c>
       <c r="B763" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C763" s="7" t="s">
         <v>4</v>
@@ -15460,7 +15460,7 @@
         <v>362</v>
       </c>
       <c r="B764" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C764" s="7" t="s">
         <v>4</v>
@@ -15477,7 +15477,7 @@
         <v>362</v>
       </c>
       <c r="B765" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C765" s="7" t="s">
         <v>4</v>
@@ -15494,7 +15494,7 @@
         <v>362</v>
       </c>
       <c r="B766" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C766" s="7" t="s">
         <v>4</v>
@@ -15630,7 +15630,7 @@
         <v>362</v>
       </c>
       <c r="B774" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C774" s="7" t="s">
         <v>4</v>
@@ -15647,7 +15647,7 @@
         <v>362</v>
       </c>
       <c r="B775" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C775" s="7" t="s">
         <v>4</v>
@@ -15681,10 +15681,10 @@
         <v>362</v>
       </c>
       <c r="B777" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C777" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D777" s="7" t="s">
         <v>284</v>
@@ -15698,10 +15698,10 @@
         <v>362</v>
       </c>
       <c r="B778" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C778" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="C778" s="7" t="s">
-        <v>396</v>
       </c>
       <c r="D778" s="7" t="s">
         <v>284</v>
@@ -15715,10 +15715,10 @@
         <v>362</v>
       </c>
       <c r="B779" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C779" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D779" s="7" t="s">
         <v>284</v>
@@ -15732,10 +15732,10 @@
         <v>362</v>
       </c>
       <c r="B780" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C780" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D780" s="7" t="s">
         <v>284</v>
@@ -15749,7 +15749,7 @@
         <v>362</v>
       </c>
       <c r="B781" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C781" s="7" t="s">
         <v>292</v>
@@ -15766,7 +15766,7 @@
         <v>362</v>
       </c>
       <c r="B782" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C782" s="7" t="s">
         <v>357</v>
@@ -15783,7 +15783,7 @@
         <v>362</v>
       </c>
       <c r="B783" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C783" s="7" t="s">
         <v>293</v>
@@ -15800,7 +15800,7 @@
         <v>362</v>
       </c>
       <c r="B784" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C784" s="7" t="s">
         <v>358</v>
@@ -15817,7 +15817,7 @@
         <v>362</v>
       </c>
       <c r="B785" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C785" s="7" t="s">
         <v>359</v>
@@ -15834,7 +15834,7 @@
         <v>362</v>
       </c>
       <c r="B786" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C786" s="7" t="s">
         <v>4</v>
@@ -15851,7 +15851,7 @@
         <v>362</v>
       </c>
       <c r="B787" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C787" s="7" t="s">
         <v>4</v>
@@ -15868,7 +15868,7 @@
         <v>362</v>
       </c>
       <c r="B788" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C788" s="7" t="s">
         <v>4</v>
@@ -15885,7 +15885,7 @@
         <v>362</v>
       </c>
       <c r="B789" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C789" s="7" t="s">
         <v>4</v>
@@ -15902,7 +15902,7 @@
         <v>362</v>
       </c>
       <c r="B790" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C790" s="7" t="s">
         <v>4</v>
@@ -15919,7 +15919,7 @@
         <v>362</v>
       </c>
       <c r="B791" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C791" s="7" t="s">
         <v>4</v>
@@ -15936,7 +15936,7 @@
         <v>362</v>
       </c>
       <c r="B792" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C792" s="7" t="s">
         <v>4</v>
@@ -15953,7 +15953,7 @@
         <v>362</v>
       </c>
       <c r="B793" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C793" s="7" t="s">
         <v>4</v>
@@ -15970,7 +15970,7 @@
         <v>362</v>
       </c>
       <c r="B794" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C794" s="7" t="s">
         <v>4</v>
@@ -15984,13 +15984,13 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D795" s="1" t="s">
         <v>129</v>
@@ -16001,13 +16001,13 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D796" s="1" t="s">
         <v>129</v>
@@ -16018,13 +16018,13 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D797" s="1" t="s">
         <v>129</v>
@@ -16035,13 +16035,13 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D798" s="1" t="s">
         <v>129</v>
@@ -16052,13 +16052,13 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D799" s="1" t="s">
         <v>129</v>
@@ -16069,13 +16069,13 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D800" s="1" t="s">
         <v>129</v>
@@ -16086,13 +16086,13 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D801" s="1" t="s">
         <v>129</v>
@@ -16103,10 +16103,10 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C802" s="1" t="s">
         <v>57</v>
@@ -16120,10 +16120,10 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>56</v>
@@ -16137,10 +16137,10 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>57</v>
@@ -16154,10 +16154,10 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>56</v>
@@ -16171,10 +16171,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -16188,10 +16188,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -16205,13 +16205,13 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>52</v>
@@ -16222,13 +16222,13 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>52</v>
@@ -16239,13 +16239,13 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>52</v>
@@ -16256,13 +16256,13 @@
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>52</v>
@@ -16273,13 +16273,13 @@
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>52</v>
@@ -16290,13 +16290,13 @@
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>52</v>
@@ -16307,13 +16307,13 @@
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>52</v>
@@ -16324,13 +16324,13 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>52</v>
@@ -16341,13 +16341,13 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>52</v>
@@ -16358,13 +16358,13 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>52</v>
@@ -16375,13 +16375,13 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>52</v>
@@ -16392,13 +16392,13 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>52</v>
@@ -16409,13 +16409,13 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>52</v>
@@ -16426,13 +16426,13 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>52</v>
@@ -16443,13 +16443,13 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>135</v>
@@ -16460,10 +16460,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>50</v>
@@ -16477,10 +16477,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>50</v>
@@ -16494,13 +16494,13 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>135</v>
@@ -16511,10 +16511,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>50</v>
@@ -16528,13 +16528,13 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>135</v>
@@ -16545,13 +16545,13 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>135</v>
@@ -16562,13 +16562,13 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>135</v>
@@ -16579,13 +16579,13 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>135</v>
@@ -16596,13 +16596,13 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16613,13 +16613,13 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>
@@ -16630,13 +16630,13 @@
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>16</v>
@@ -16647,13 +16647,13 @@
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>16</v>
@@ -16664,13 +16664,13 @@
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>16</v>
@@ -16681,13 +16681,13 @@
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -16698,13 +16698,13 @@
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -16715,13 +16715,13 @@
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>16</v>
@@ -16732,13 +16732,13 @@
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>16</v>
@@ -16749,13 +16749,13 @@
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C840" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>16</v>
@@ -16766,13 +16766,13 @@
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>16</v>
@@ -16783,13 +16783,13 @@
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
@@ -16800,13 +16800,13 @@
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -16817,13 +16817,13 @@
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>244</v>
@@ -16834,13 +16834,13 @@
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>244</v>
@@ -16851,13 +16851,13 @@
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>244</v>
@@ -16868,13 +16868,13 @@
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>244</v>
@@ -16885,13 +16885,13 @@
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D848" s="1" t="s">
         <v>148</v>
@@ -16902,13 +16902,13 @@
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C849" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>148</v>
@@ -16919,13 +16919,13 @@
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D850" s="1" t="s">
         <v>148</v>
@@ -16936,13 +16936,13 @@
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>148</v>
@@ -16953,13 +16953,13 @@
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>148</v>
@@ -16970,13 +16970,13 @@
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>148</v>
@@ -16987,13 +16987,13 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>148</v>
@@ -17004,13 +17004,13 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D855" s="1" t="s">
         <v>148</v>
@@ -17021,7 +17021,7 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>274</v>
@@ -17038,7 +17038,7 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>274</v>
@@ -17055,13 +17055,13 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>225</v>
@@ -17072,13 +17072,13 @@
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A859" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>225</v>
@@ -17089,13 +17089,13 @@
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A860" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D860" s="1" t="s">
         <v>225</v>
@@ -17106,13 +17106,13 @@
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A861" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>225</v>
@@ -17123,13 +17123,13 @@
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
@@ -17140,13 +17140,13 @@
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A863" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
@@ -17157,13 +17157,13 @@
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A864" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
@@ -17174,13 +17174,13 @@
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
@@ -17191,13 +17191,13 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
@@ -17208,13 +17208,13 @@
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>225</v>
@@ -17225,13 +17225,13 @@
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D868" s="1" t="s">
         <v>225</v>
@@ -17242,10 +17242,10 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>57</v>
@@ -17259,10 +17259,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>56</v>
@@ -17276,10 +17276,10 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B871" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C871" s="1" t="s">
         <v>4</v>
@@ -17293,10 +17293,10 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B872" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C872" s="1" t="s">
         <v>4</v>
@@ -17310,7 +17310,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>5</v>
@@ -17327,10 +17327,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>57</v>
@@ -17344,10 +17344,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>56</v>
@@ -17361,10 +17361,10 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
@@ -17378,10 +17378,10 @@
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C877" s="1" t="s">
         <v>4</v>
@@ -17395,13 +17395,13 @@
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A878" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D878" s="1" t="s">
         <v>40</v>
@@ -17412,13 +17412,13 @@
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B879" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C879" s="1" t="s">
         <v>464</v>
-      </c>
-      <c r="C879" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>40</v>
@@ -17429,13 +17429,13 @@
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
@@ -17446,13 +17446,13 @@
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
@@ -17463,13 +17463,13 @@
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
@@ -17480,13 +17480,13 @@
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
@@ -17497,13 +17497,13 @@
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
@@ -17514,13 +17514,13 @@
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
@@ -17531,13 +17531,13 @@
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
@@ -17548,13 +17548,13 @@
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
@@ -17565,13 +17565,13 @@
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
@@ -17582,13 +17582,13 @@
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
@@ -17599,13 +17599,13 @@
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
@@ -17616,10 +17616,10 @@
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C891" s="1" t="s">
         <v>4</v>
@@ -17633,47 +17633,47 @@
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D894" s="1" t="s">
         <v>139</v>
@@ -17684,13 +17684,13 @@
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B895" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D895" s="1" t="s">
         <v>37</v>
@@ -17701,13 +17701,13 @@
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B896" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D896" s="1" t="s">
         <v>37</v>
@@ -17718,13 +17718,13 @@
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A897" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B897" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D897" s="1" t="s">
         <v>37</v>
@@ -17735,13 +17735,13 @@
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B898" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D898" s="1" t="s">
         <v>37</v>
@@ -17752,13 +17752,13 @@
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B899" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>37</v>
@@ -17769,13 +17769,13 @@
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B900" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D900" s="1" t="s">
         <v>37</v>
@@ -17786,13 +17786,13 @@
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A901" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B901" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D901" s="1" t="s">
         <v>37</v>
@@ -17803,13 +17803,13 @@
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D902" s="1" t="s">
         <v>37</v>
@@ -17820,13 +17820,13 @@
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A903" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B903" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D903" s="1" t="s">
         <v>37</v>
@@ -17837,13 +17837,13 @@
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A904" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B904" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
@@ -17854,10 +17854,10 @@
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>56</v>
@@ -17871,10 +17871,10 @@
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>57</v>
@@ -17888,13 +17888,13 @@
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A907" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>160</v>
@@ -17905,10 +17905,10 @@
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A908" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>56</v>
@@ -17922,10 +17922,10 @@
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A909" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>57</v>
@@ -17939,13 +17939,13 @@
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D910" s="1" t="s">
         <v>162</v>
@@ -17956,10 +17956,10 @@
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A911" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C911" s="1" t="s">
         <v>56</v>
@@ -17973,10 +17973,10 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C912" s="1" t="s">
         <v>57</v>
@@ -17990,13 +17990,13 @@
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>164</v>
@@ -18007,10 +18007,10 @@
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>56</v>
@@ -18024,10 +18024,10 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>57</v>
@@ -18041,13 +18041,13 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D916" s="1" t="s">
         <v>166</v>
@@ -18058,10 +18058,10 @@
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
@@ -18075,10 +18075,10 @@
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>57</v>
@@ -18092,13 +18092,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D919" s="1" t="s">
         <v>168</v>
@@ -18109,10 +18109,10 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>4</v>
@@ -18126,13 +18126,13 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D921" s="1" t="s">
         <v>236</v>
@@ -18143,13 +18143,13 @@
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B922" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C922" s="1" t="s">
         <v>517</v>
-      </c>
-      <c r="C922" s="1" t="s">
-        <v>519</v>
       </c>
       <c r="D922" s="1" t="s">
         <v>236</v>
@@ -18160,27 +18160,27 @@
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D923" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E923" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>4</v>
@@ -18194,10 +18194,10 @@
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>4</v>
@@ -18211,13 +18211,13 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D926" s="1" t="s">
         <v>60</v>
@@ -18228,13 +18228,13 @@
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B927" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D927" s="1" t="s">
         <v>60</v>
@@ -18245,13 +18245,13 @@
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D928" s="1" t="s">
         <v>60</v>
@@ -18262,13 +18262,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A929" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D929" s="1" t="s">
         <v>60</v>
@@ -18279,13 +18279,13 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D930" s="1" t="s">
         <v>60</v>
@@ -18296,13 +18296,13 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A931" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D931" s="1" t="s">
         <v>60</v>
@@ -18313,13 +18313,13 @@
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A932" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B932" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D932" s="1" t="s">
         <v>60</v>
@@ -18330,10 +18330,10 @@
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A933" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B933" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>4</v>
@@ -18347,10 +18347,10 @@
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B934" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C934" s="1" t="s">
         <v>4</v>
@@ -18364,13 +18364,13 @@
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A935" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
@@ -18381,13 +18381,13 @@
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A936" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B936" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C936" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="C936" s="1" t="s">
-        <v>530</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
@@ -18398,13 +18398,13 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A937" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
@@ -18415,13 +18415,13 @@
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A938" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
@@ -18432,13 +18432,13 @@
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
@@ -18449,13 +18449,13 @@
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
@@ -18466,13 +18466,13 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
@@ -18483,13 +18483,13 @@
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
@@ -18500,13 +18500,13 @@
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A943" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
@@ -18517,13 +18517,13 @@
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A944" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
@@ -18534,13 +18534,13 @@
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A945" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
@@ -18551,13 +18551,13 @@
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A946" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
@@ -18568,13 +18568,13 @@
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
@@ -18585,13 +18585,13 @@
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A948" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
@@ -18602,13 +18602,13 @@
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>251</v>
@@ -18619,13 +18619,13 @@
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A950" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>251</v>
@@ -18636,13 +18636,13 @@
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>251</v>
@@ -18653,13 +18653,13 @@
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>251</v>
@@ -18670,13 +18670,13 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A953" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
@@ -18687,13 +18687,13 @@
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B954" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
@@ -18704,13 +18704,13 @@
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A955" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B955" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
@@ -18721,13 +18721,13 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A956" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B956" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
@@ -18738,13 +18738,13 @@
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A957" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B957" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
@@ -18755,13 +18755,13 @@
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A958" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B958" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
@@ -18772,13 +18772,13 @@
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A959" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B959" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
@@ -18789,13 +18789,13 @@
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A960" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B960" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
@@ -18806,13 +18806,13 @@
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A961" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B961" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
@@ -18823,13 +18823,13 @@
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A962" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
@@ -18840,13 +18840,13 @@
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A963" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B963" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
@@ -18857,13 +18857,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B964" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
@@ -18874,13 +18874,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B965" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
@@ -18891,13 +18891,13 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A966" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B966" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
@@ -18908,13 +18908,13 @@
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A967" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B967" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
@@ -18925,13 +18925,13 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B968" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
@@ -18942,13 +18942,13 @@
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>253</v>
@@ -18959,13 +18959,13 @@
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A970" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>253</v>
@@ -18976,13 +18976,13 @@
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A971" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B971" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>253</v>
@@ -18993,13 +18993,13 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A972" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B972" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>253</v>
@@ -19010,10 +19010,10 @@
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A973" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C973" s="1" t="s">
         <v>4</v>
@@ -19027,10 +19027,10 @@
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
@@ -19044,10 +19044,10 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C975" s="1" t="s">
         <v>4</v>
@@ -19061,10 +19061,10 @@
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C976" s="1" t="s">
         <v>4</v>
@@ -19078,10 +19078,10 @@
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A977" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C977" s="1" t="s">
         <v>4</v>
@@ -19095,10 +19095,10 @@
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C978" s="1" t="s">
         <v>4</v>
@@ -19112,13 +19112,13 @@
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B979" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
@@ -19129,13 +19129,13 @@
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B980" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D980" s="1" t="s">
         <v>9</v>
@@ -19146,13 +19146,13 @@
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A981" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B981" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D981" s="1" t="s">
         <v>9</v>
@@ -19163,13 +19163,13 @@
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B982" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D982" s="1" t="s">
         <v>9</v>
@@ -19180,13 +19180,13 @@
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B983" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D983" s="1" t="s">
         <v>9</v>
@@ -19197,13 +19197,13 @@
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B984" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D984" s="1" t="s">
         <v>9</v>
@@ -19214,13 +19214,13 @@
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A985" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B985" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D985" s="1" t="s">
         <v>9</v>
@@ -19231,13 +19231,13 @@
     </row>
     <row r="986" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B986" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D986" s="1" t="s">
         <v>9</v>
@@ -19248,13 +19248,13 @@
     </row>
     <row r="987" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B987" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D987" s="1" t="s">
         <v>9</v>
@@ -19265,13 +19265,13 @@
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B988" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D988" s="1" t="s">
         <v>9</v>
@@ -19282,13 +19282,13 @@
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D989" s="1" t="s">
         <v>9</v>
@@ -19299,10 +19299,10 @@
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B990" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C990" s="1" t="s">
         <v>57</v>
@@ -19316,10 +19316,10 @@
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B991" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C991" s="1" t="s">
         <v>56</v>
@@ -19333,10 +19333,10 @@
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A992" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C992" s="1" t="s">
         <v>4</v>
@@ -19350,10 +19350,10 @@
     </row>
     <row r="993" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C993" s="1" t="s">
         <v>4</v>
@@ -19367,10 +19367,10 @@
     </row>
     <row r="994" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B994" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C994" s="1" t="s">
         <v>4</v>
@@ -19384,13 +19384,13 @@
     </row>
     <row r="995" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B995" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D995" s="1" t="s">
         <v>284</v>
@@ -19401,13 +19401,13 @@
     </row>
     <row r="996" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B996" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D996" s="1" t="s">
         <v>284</v>
@@ -19418,13 +19418,13 @@
     </row>
     <row r="997" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B997" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D997" s="1" t="s">
         <v>284</v>
@@ -19435,10 +19435,10 @@
     </row>
     <row r="998" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A998" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B998" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D998" s="1" t="s">
         <v>291</v>
@@ -19449,13 +19449,13 @@
     </row>
     <row r="999" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D999" s="1" t="s">
         <v>291</v>
@@ -19466,10 +19466,10 @@
     </row>
     <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1000" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>187</v>
@@ -19483,13 +19483,13 @@
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1001" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D1001" s="1" t="s">
         <v>291</v>
@@ -19500,13 +19500,13 @@
     </row>
     <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1002" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D1002" s="1" t="s">
         <v>291</v>
@@ -19517,10 +19517,10 @@
     </row>
     <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C1003" s="1" t="s">
         <v>4</v>
@@ -19534,10 +19534,10 @@
     </row>
     <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1004" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C1004" s="1" t="s">
         <v>4</v>
@@ -19551,10 +19551,10 @@
     </row>
     <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1005" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C1005" s="1" t="s">
         <v>4</v>
@@ -19568,10 +19568,10 @@
     </row>
     <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1006" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C1006" s="1" t="s">
         <v>4</v>
@@ -19585,10 +19585,10 @@
     </row>
     <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1007" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C1007" s="1" t="s">
         <v>4</v>
@@ -19602,10 +19602,10 @@
     </row>
     <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C1008" s="1" t="s">
         <v>4</v>
@@ -19619,10 +19619,10 @@
     </row>
     <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C1009" s="1" t="s">
         <v>4</v>
@@ -19636,10 +19636,10 @@
     </row>
     <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1010" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C1010" s="1" t="s">
         <v>4</v>
@@ -19653,10 +19653,10 @@
     </row>
     <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1011" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1011" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C1011" s="1" t="s">
         <v>4</v>
@@ -19670,16 +19670,16 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1012" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1012" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C1012" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D1012" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E1012" s="1" t="s">
         <v>144</v>
@@ -19687,61 +19687,61 @@
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1013" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1013" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="C1013" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="C1013" s="1" t="s">
+      <c r="D1013" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="D1013" s="1" t="s">
-        <v>497</v>
-      </c>
       <c r="E1013" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1014" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C1014" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D1014" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="E1014" s="1" t="s">
         <v>496</v>
-      </c>
-      <c r="D1014" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="E1014" s="1" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D1015" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E1015" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="1016" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B1016" s="5" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C1016" s="5" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
made one fix to BART (data and dictionary), updated
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="578">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1452,12 +1452,6 @@
     <t>SRVY_IN_ENGL_SPANISH</t>
   </si>
   <si>
-    <t>FROM_TRANS_LIST1_LOC_LAT</t>
-  </si>
-  <si>
-    <t>FROM_TRANS_LIST1_LOC_LONG</t>
-  </si>
-  <si>
     <t>PAIRED_WGHT_FCTR</t>
   </si>
   <si>
@@ -1468,12 +1462,6 @@
   </si>
   <si>
     <t>EGRESSTRNSFR_LIST3</t>
-  </si>
-  <si>
-    <t>TO_TRNS_LIST1_LOC_LAT</t>
-  </si>
-  <si>
-    <t>TO_TRNS_LIST1_LOC_LONG</t>
   </si>
   <si>
     <t>WORKP_ADDRESS_LAT</t>
@@ -2465,8 +2453,8 @@
   <dimension ref="A1:E1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A992" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1022" sqref="C1022"/>
+      <pane ySplit="1" topLeftCell="A776" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B790" sqref="B790"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13295,7 +13283,7 @@
         <v>362</v>
       </c>
       <c r="B637" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C637" s="7">
         <v>1</v>
@@ -13312,7 +13300,7 @@
         <v>362</v>
       </c>
       <c r="B638" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C638" s="7">
         <v>2</v>
@@ -13329,7 +13317,7 @@
         <v>362</v>
       </c>
       <c r="B639" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C639" s="7">
         <v>3</v>
@@ -13346,7 +13334,7 @@
         <v>362</v>
       </c>
       <c r="B640" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C640" s="7">
         <v>4</v>
@@ -13363,7 +13351,7 @@
         <v>362</v>
       </c>
       <c r="B641" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C641" s="7">
         <v>1</v>
@@ -13380,7 +13368,7 @@
         <v>362</v>
       </c>
       <c r="B642" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C642" s="7">
         <v>2</v>
@@ -13397,7 +13385,7 @@
         <v>362</v>
       </c>
       <c r="B643" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C643" s="7">
         <v>3</v>
@@ -13414,7 +13402,7 @@
         <v>362</v>
       </c>
       <c r="B644" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C644" s="7">
         <v>4</v>
@@ -13431,7 +13419,7 @@
         <v>362</v>
       </c>
       <c r="B645" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C645" s="7">
         <v>5</v>
@@ -13448,7 +13436,7 @@
         <v>362</v>
       </c>
       <c r="B646" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C646" s="7">
         <v>6</v>
@@ -13465,7 +13453,7 @@
         <v>362</v>
       </c>
       <c r="B647" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C647" s="7">
         <v>7</v>
@@ -13689,7 +13677,7 @@
         <v>153</v>
       </c>
       <c r="C660" s="7" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D660" s="7" t="s">
         <v>156</v>
@@ -13706,7 +13694,7 @@
         <v>153</v>
       </c>
       <c r="C661" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D661" s="7" t="s">
         <v>156</v>
@@ -14536,7 +14524,7 @@
         <v>362</v>
       </c>
       <c r="B710" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C710" s="7" t="s">
         <v>4</v>
@@ -15437,7 +15425,7 @@
         <v>362</v>
       </c>
       <c r="B763" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C763" s="7" t="s">
         <v>4</v>
@@ -15488,7 +15476,7 @@
         <v>362</v>
       </c>
       <c r="B766" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C766" s="7" t="s">
         <v>4</v>
@@ -15624,7 +15612,7 @@
         <v>362</v>
       </c>
       <c r="B774" s="7" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C774" s="7" t="s">
         <v>4</v>
@@ -15641,7 +15629,7 @@
         <v>362</v>
       </c>
       <c r="B775" s="7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C775" s="7" t="s">
         <v>4</v>
@@ -15828,7 +15816,7 @@
         <v>362</v>
       </c>
       <c r="B786" s="7" t="s">
-        <v>406</v>
+        <v>543</v>
       </c>
       <c r="C786" s="7" t="s">
         <v>4</v>
@@ -15845,7 +15833,7 @@
         <v>362</v>
       </c>
       <c r="B787" s="7" t="s">
-        <v>407</v>
+        <v>573</v>
       </c>
       <c r="C787" s="7" t="s">
         <v>4</v>
@@ -15862,7 +15850,7 @@
         <v>362</v>
       </c>
       <c r="B788" s="7" t="s">
-        <v>400</v>
+        <v>574</v>
       </c>
       <c r="C788" s="7" t="s">
         <v>4</v>
@@ -15879,7 +15867,7 @@
         <v>362</v>
       </c>
       <c r="B789" s="7" t="s">
-        <v>401</v>
+        <v>575</v>
       </c>
       <c r="C789" s="7" t="s">
         <v>4</v>
@@ -15896,7 +15884,7 @@
         <v>362</v>
       </c>
       <c r="B790" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C790" s="7" t="s">
         <v>4</v>
@@ -15913,7 +15901,7 @@
         <v>362</v>
       </c>
       <c r="B791" s="7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C791" s="7" t="s">
         <v>4</v>
@@ -15930,7 +15918,7 @@
         <v>362</v>
       </c>
       <c r="B792" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C792" s="7" t="s">
         <v>4</v>
@@ -15947,7 +15935,7 @@
         <v>362</v>
       </c>
       <c r="B793" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C793" s="7" t="s">
         <v>4</v>
@@ -15964,7 +15952,7 @@
         <v>362</v>
       </c>
       <c r="B794" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C794" s="7" t="s">
         <v>4</v>
@@ -15978,13 +15966,13 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D795" s="1" t="s">
         <v>129</v>
@@ -15995,13 +15983,13 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D796" s="1" t="s">
         <v>129</v>
@@ -16012,13 +16000,13 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="D797" s="1" t="s">
         <v>129</v>
@@ -16029,13 +16017,13 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D798" s="1" t="s">
         <v>129</v>
@@ -16046,13 +16034,13 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D799" s="1" t="s">
         <v>129</v>
@@ -16063,13 +16051,13 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D800" s="1" t="s">
         <v>129</v>
@@ -16080,13 +16068,13 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="D801" s="1" t="s">
         <v>129</v>
@@ -16097,10 +16085,10 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C802" s="1" t="s">
         <v>57</v>
@@ -16114,10 +16102,10 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>56</v>
@@ -16131,10 +16119,10 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>57</v>
@@ -16148,10 +16136,10 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>56</v>
@@ -16165,10 +16153,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -16182,10 +16170,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -16199,13 +16187,13 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>52</v>
@@ -16216,13 +16204,13 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>52</v>
@@ -16233,13 +16221,13 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>52</v>
@@ -16250,13 +16238,13 @@
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>52</v>
@@ -16267,13 +16255,13 @@
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>52</v>
@@ -16284,13 +16272,13 @@
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>52</v>
@@ -16301,13 +16289,13 @@
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>52</v>
@@ -16318,13 +16306,13 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>52</v>
@@ -16335,13 +16323,13 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>52</v>
@@ -16352,13 +16340,13 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>52</v>
@@ -16369,13 +16357,13 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>52</v>
@@ -16386,13 +16374,13 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>52</v>
@@ -16403,13 +16391,13 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>52</v>
@@ -16420,13 +16408,13 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>52</v>
@@ -16437,13 +16425,13 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>135</v>
@@ -16454,10 +16442,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>50</v>
@@ -16471,10 +16459,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>50</v>
@@ -16488,13 +16476,13 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>135</v>
@@ -16505,10 +16493,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>50</v>
@@ -16522,13 +16510,13 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>135</v>
@@ -16539,13 +16527,13 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>135</v>
@@ -16556,13 +16544,13 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>135</v>
@@ -16573,13 +16561,13 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>135</v>
@@ -16590,13 +16578,13 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16607,13 +16595,13 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>
@@ -16624,13 +16612,13 @@
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>16</v>
@@ -16641,13 +16629,13 @@
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>16</v>
@@ -16658,13 +16646,13 @@
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>16</v>
@@ -16675,13 +16663,13 @@
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -16692,13 +16680,13 @@
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -16709,13 +16697,13 @@
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>16</v>
@@ -16726,13 +16714,13 @@
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>16</v>
@@ -16743,13 +16731,13 @@
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C840" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>16</v>
@@ -16760,13 +16748,13 @@
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>16</v>
@@ -16777,13 +16765,13 @@
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
@@ -16794,13 +16782,13 @@
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -16811,13 +16799,13 @@
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>244</v>
@@ -16828,13 +16816,13 @@
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>244</v>
@@ -16845,13 +16833,13 @@
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>244</v>
@@ -16862,13 +16850,13 @@
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>244</v>
@@ -16879,13 +16867,13 @@
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D848" s="1" t="s">
         <v>148</v>
@@ -16896,13 +16884,13 @@
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C849" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>148</v>
@@ -16913,13 +16901,13 @@
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D850" s="1" t="s">
         <v>148</v>
@@ -16930,13 +16918,13 @@
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>148</v>
@@ -16947,13 +16935,13 @@
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>148</v>
@@ -16964,13 +16952,13 @@
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>148</v>
@@ -16981,13 +16969,13 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>148</v>
@@ -16998,13 +16986,13 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D855" s="1" t="s">
         <v>148</v>
@@ -17015,7 +17003,7 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>274</v>
@@ -17032,7 +17020,7 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>274</v>
@@ -17049,13 +17037,13 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>225</v>
@@ -17066,13 +17054,13 @@
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A859" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>225</v>
@@ -17083,13 +17071,13 @@
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A860" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D860" s="1" t="s">
         <v>225</v>
@@ -17100,13 +17088,13 @@
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A861" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>225</v>
@@ -17117,13 +17105,13 @@
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
@@ -17134,13 +17122,13 @@
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A863" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
@@ -17151,13 +17139,13 @@
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A864" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
@@ -17168,13 +17156,13 @@
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
@@ -17185,13 +17173,13 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
@@ -17202,13 +17190,13 @@
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>225</v>
@@ -17219,13 +17207,13 @@
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D868" s="1" t="s">
         <v>225</v>
@@ -17236,10 +17224,10 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>57</v>
@@ -17253,10 +17241,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>56</v>
@@ -17270,7 +17258,7 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B871" s="1" t="s">
         <v>78</v>
@@ -17287,7 +17275,7 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B872" s="1" t="s">
         <v>79</v>
@@ -17304,7 +17292,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>5</v>
@@ -17321,10 +17309,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>57</v>
@@ -17338,10 +17326,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>56</v>
@@ -17355,7 +17343,7 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B876" s="1" t="s">
         <v>94</v>
@@ -17372,7 +17360,7 @@
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B877" s="1" t="s">
         <v>96</v>
@@ -17389,13 +17377,13 @@
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A878" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="D878" s="1" t="s">
         <v>40</v>
@@ -17406,13 +17394,13 @@
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>40</v>
@@ -17423,13 +17411,13 @@
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
@@ -17440,13 +17428,13 @@
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B881" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C881" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="C881" s="1" t="s">
-        <v>461</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
@@ -17457,13 +17445,13 @@
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
@@ -17474,13 +17462,13 @@
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
@@ -17491,13 +17479,13 @@
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
@@ -17508,13 +17496,13 @@
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
@@ -17525,13 +17513,13 @@
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
@@ -17542,13 +17530,13 @@
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
@@ -17559,13 +17547,13 @@
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
@@ -17576,13 +17564,13 @@
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
@@ -17593,13 +17581,13 @@
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
@@ -17610,10 +17598,10 @@
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C891" s="1" t="s">
         <v>4</v>
@@ -17627,47 +17615,47 @@
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D894" s="1" t="s">
         <v>139</v>
@@ -17678,13 +17666,13 @@
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B895" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D895" s="1" t="s">
         <v>37</v>
@@ -17695,13 +17683,13 @@
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B896" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D896" s="1" t="s">
         <v>37</v>
@@ -17712,13 +17700,13 @@
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A897" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B897" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D897" s="1" t="s">
         <v>37</v>
@@ -17729,13 +17717,13 @@
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B898" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D898" s="1" t="s">
         <v>37</v>
@@ -17746,13 +17734,13 @@
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B899" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>37</v>
@@ -17763,13 +17751,13 @@
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B900" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D900" s="1" t="s">
         <v>37</v>
@@ -17780,13 +17768,13 @@
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A901" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B901" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D901" s="1" t="s">
         <v>37</v>
@@ -17797,13 +17785,13 @@
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D902" s="1" t="s">
         <v>37</v>
@@ -17814,13 +17802,13 @@
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A903" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B903" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D903" s="1" t="s">
         <v>37</v>
@@ -17831,13 +17819,13 @@
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A904" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B904" s="10" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
@@ -17848,10 +17836,10 @@
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>56</v>
@@ -17865,10 +17853,10 @@
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>57</v>
@@ -17882,13 +17870,13 @@
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A907" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>160</v>
@@ -17899,10 +17887,10 @@
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A908" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B908" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="B908" s="1" t="s">
-        <v>555</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>56</v>
@@ -17916,10 +17904,10 @@
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A909" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B909" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="B909" s="1" t="s">
-        <v>555</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>57</v>
@@ -17933,13 +17921,13 @@
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B910" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="B910" s="1" t="s">
-        <v>555</v>
-      </c>
       <c r="C910" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D910" s="1" t="s">
         <v>162</v>
@@ -17950,10 +17938,10 @@
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A911" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C911" s="1" t="s">
         <v>56</v>
@@ -17967,10 +17955,10 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C912" s="1" t="s">
         <v>57</v>
@@ -17984,13 +17972,13 @@
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>164</v>
@@ -18001,10 +17989,10 @@
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>56</v>
@@ -18018,10 +18006,10 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>57</v>
@@ -18035,13 +18023,13 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D916" s="1" t="s">
         <v>166</v>
@@ -18052,10 +18040,10 @@
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
@@ -18069,10 +18057,10 @@
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>57</v>
@@ -18086,13 +18074,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D919" s="1" t="s">
         <v>168</v>
@@ -18103,10 +18091,10 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>4</v>
@@ -18120,13 +18108,13 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D921" s="1" t="s">
         <v>236</v>
@@ -18137,13 +18125,13 @@
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D922" s="1" t="s">
         <v>236</v>
@@ -18154,27 +18142,27 @@
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D923" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E923" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>4</v>
@@ -18188,10 +18176,10 @@
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>4</v>
@@ -18205,13 +18193,13 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D926" s="1" t="s">
         <v>60</v>
@@ -18222,13 +18210,13 @@
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B927" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D927" s="1" t="s">
         <v>60</v>
@@ -18239,13 +18227,13 @@
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D928" s="1" t="s">
         <v>60</v>
@@ -18256,13 +18244,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A929" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D929" s="1" t="s">
         <v>60</v>
@@ -18273,13 +18261,13 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="D930" s="1" t="s">
         <v>60</v>
@@ -18290,13 +18278,13 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A931" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D931" s="1" t="s">
         <v>60</v>
@@ -18307,13 +18295,13 @@
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A932" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B932" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="D932" s="1" t="s">
         <v>60</v>
@@ -18324,10 +18312,10 @@
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A933" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B933" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>4</v>
@@ -18341,10 +18329,10 @@
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B934" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C934" s="1" t="s">
         <v>4</v>
@@ -18358,13 +18346,13 @@
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A935" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
@@ -18375,13 +18363,13 @@
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A936" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C936" s="1" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
@@ -18392,13 +18380,13 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A937" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
@@ -18409,13 +18397,13 @@
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A938" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B938" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C938" s="1" t="s">
         <v>512</v>
-      </c>
-      <c r="C938" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
@@ -18426,13 +18414,13 @@
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
@@ -18443,13 +18431,13 @@
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
@@ -18460,13 +18448,13 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
@@ -18477,13 +18465,13 @@
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
@@ -18494,13 +18482,13 @@
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A943" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
@@ -18511,13 +18499,13 @@
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A944" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
@@ -18528,13 +18516,13 @@
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A945" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
@@ -18545,13 +18533,13 @@
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A946" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
@@ -18562,13 +18550,13 @@
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
@@ -18579,13 +18567,13 @@
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A948" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
@@ -18596,13 +18584,13 @@
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>251</v>
@@ -18613,13 +18601,13 @@
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A950" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>251</v>
@@ -18630,13 +18618,13 @@
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>251</v>
@@ -18647,13 +18635,13 @@
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>251</v>
@@ -18664,13 +18652,13 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A953" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
@@ -18681,13 +18669,13 @@
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B954" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
@@ -18698,13 +18686,13 @@
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A955" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B955" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
@@ -18715,13 +18703,13 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A956" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B956" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
@@ -18732,13 +18720,13 @@
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A957" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B957" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
@@ -18749,13 +18737,13 @@
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A958" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B958" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
@@ -18766,13 +18754,13 @@
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A959" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B959" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
@@ -18783,13 +18771,13 @@
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A960" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B960" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
@@ -18800,13 +18788,13 @@
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A961" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B961" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
@@ -18817,13 +18805,13 @@
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A962" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
@@ -18834,13 +18822,13 @@
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A963" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B963" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
@@ -18851,13 +18839,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B964" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
@@ -18868,13 +18856,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B965" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
@@ -18885,13 +18873,13 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A966" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B966" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
@@ -18902,13 +18890,13 @@
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A967" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B967" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
@@ -18919,13 +18907,13 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B968" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
@@ -18936,13 +18924,13 @@
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>253</v>
@@ -18953,13 +18941,13 @@
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A970" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>253</v>
@@ -18970,13 +18958,13 @@
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A971" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B971" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>253</v>
@@ -18987,13 +18975,13 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A972" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B972" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>253</v>
@@ -19004,10 +18992,10 @@
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A973" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B973" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C973" s="1" t="s">
         <v>4</v>
@@ -19021,10 +19009,10 @@
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
@@ -19038,10 +19026,10 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C975" s="1" t="s">
         <v>4</v>
@@ -19055,10 +19043,10 @@
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="C976" s="1" t="s">
         <v>4</v>
@@ -19072,10 +19060,10 @@
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A977" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="C977" s="1" t="s">
         <v>4</v>
@@ -19089,10 +19077,10 @@
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="C978" s="1" t="s">
         <v>4</v>
@@ -19106,13 +19094,13 @@
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B979" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
@@ -19123,13 +19111,13 @@
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B980" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D980" s="1" t="s">
         <v>9</v>
@@ -19140,13 +19128,13 @@
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A981" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B981" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D981" s="1" t="s">
         <v>9</v>
@@ -19157,13 +19145,13 @@
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B982" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D982" s="1" t="s">
         <v>9</v>
@@ -19174,13 +19162,13 @@
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B983" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D983" s="1" t="s">
         <v>9</v>
@@ -19191,13 +19179,13 @@
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B984" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D984" s="1" t="s">
         <v>9</v>
@@ -19208,13 +19196,13 @@
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A985" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B985" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D985" s="1" t="s">
         <v>9</v>
@@ -19225,13 +19213,13 @@
     </row>
     <row r="986" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B986" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D986" s="1" t="s">
         <v>9</v>
@@ -19242,13 +19230,13 @@
     </row>
     <row r="987" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B987" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D987" s="1" t="s">
         <v>9</v>
@@ -19259,13 +19247,13 @@
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B988" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D988" s="1" t="s">
         <v>9</v>
@@ -19276,13 +19264,13 @@
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D989" s="1" t="s">
         <v>9</v>
@@ -19293,10 +19281,10 @@
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B990" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C990" s="1" t="s">
         <v>57</v>
@@ -19310,10 +19298,10 @@
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B991" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C991" s="1" t="s">
         <v>56</v>
@@ -19327,10 +19315,10 @@
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A992" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C992" s="1" t="s">
         <v>4</v>
@@ -19344,10 +19332,10 @@
     </row>
     <row r="993" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C993" s="1" t="s">
         <v>4</v>
@@ -19361,7 +19349,7 @@
     </row>
     <row r="994" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B994" s="1" t="s">
         <v>6</v>
@@ -19378,13 +19366,13 @@
     </row>
     <row r="995" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B995" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D995" s="1" t="s">
         <v>284</v>
@@ -19395,13 +19383,13 @@
     </row>
     <row r="996" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B996" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D996" s="1" t="s">
         <v>284</v>
@@ -19412,13 +19400,13 @@
     </row>
     <row r="997" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B997" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D997" s="1" t="s">
         <v>284</v>
@@ -19429,10 +19417,10 @@
     </row>
     <row r="998" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A998" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B998" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D998" s="1" t="s">
         <v>291</v>
@@ -19443,13 +19431,13 @@
     </row>
     <row r="999" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D999" s="1" t="s">
         <v>291</v>
@@ -19460,10 +19448,10 @@
     </row>
     <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1000" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>187</v>
@@ -19477,13 +19465,13 @@
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1001" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D1001" s="1" t="s">
         <v>291</v>
@@ -19494,13 +19482,13 @@
     </row>
     <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1002" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="D1002" s="1" t="s">
         <v>291</v>
@@ -19511,10 +19499,10 @@
     </row>
     <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C1003" s="1" t="s">
         <v>4</v>
@@ -19528,10 +19516,10 @@
     </row>
     <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1004" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C1004" s="1" t="s">
         <v>4</v>
@@ -19545,10 +19533,10 @@
     </row>
     <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1005" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="C1005" s="1" t="s">
         <v>4</v>
@@ -19562,10 +19550,10 @@
     </row>
     <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1006" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="C1006" s="1" t="s">
         <v>4</v>
@@ -19579,10 +19567,10 @@
     </row>
     <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1007" s="1" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C1007" s="1" t="s">
         <v>4</v>
@@ -19596,10 +19584,10 @@
     </row>
     <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C1008" s="1" t="s">
         <v>4</v>
@@ -19613,10 +19601,10 @@
     </row>
     <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C1009" s="1" t="s">
         <v>4</v>
@@ -19630,10 +19618,10 @@
     </row>
     <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1010" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C1010" s="1" t="s">
         <v>4</v>
@@ -19647,10 +19635,10 @@
     </row>
     <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1011" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1011" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C1011" s="1" t="s">
         <v>4</v>
@@ -19664,16 +19652,16 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1012" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1012" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1012" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1012" s="1" t="s">
         <v>486</v>
-      </c>
-      <c r="C1012" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="D1012" s="1" t="s">
-        <v>490</v>
       </c>
       <c r="E1012" s="1" t="s">
         <v>144</v>
@@ -19681,61 +19669,61 @@
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1013" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1013" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1013" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1013" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C1013" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="D1013" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="E1013" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1014" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1014" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D1014" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C1014" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="D1014" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="E1014" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1015" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C1015" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1015" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="C1015" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="D1015" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="E1015" s="1" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="1016" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1016" s="5" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C1016" s="5" t="s">
         <v>4</v>
@@ -19749,10 +19737,10 @@
     </row>
     <row r="1017" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1017" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1017" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C1017" s="1">
         <v>0</v>
@@ -19766,10 +19754,10 @@
     </row>
     <row r="1018" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1018" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C1018" s="1">
         <v>1</v>
@@ -19783,10 +19771,10 @@
     </row>
     <row r="1019" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1019" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1019" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C1019" s="1">
         <v>2</v>
@@ -19800,10 +19788,10 @@
     </row>
     <row r="1020" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1020" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C1020" s="1">
         <v>3</v>
@@ -19817,10 +19805,10 @@
     </row>
     <row r="1021" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1021" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1021" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="C1021" s="1">
         <v>4</v>
@@ -19834,10 +19822,10 @@
     </row>
     <row r="1022" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1022" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1022" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C1022" s="1">
         <v>0</v>
@@ -19851,10 +19839,10 @@
     </row>
     <row r="1023" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1023" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1023" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C1023" s="1">
         <v>1</v>
@@ -19868,10 +19856,10 @@
     </row>
     <row r="1024" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1024" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1024" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C1024" s="1">
         <v>2</v>
@@ -19885,10 +19873,10 @@
     </row>
     <row r="1025" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1025" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1025" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C1025" s="1">
         <v>3</v>
@@ -19902,10 +19890,10 @@
     </row>
     <row r="1026" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1026" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="C1026" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
started on tranche 1 update
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -245,6 +245,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="A973" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>David Ory:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+START HERE. Above variables in yellow need to be added to the data.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1515,9 +1539,6 @@
     <t>Used Uber or similar service</t>
   </si>
   <si>
-    <t>ACCESS_MODE</t>
-  </si>
-  <si>
     <t>WENT2SCHL_B4_TRIP</t>
   </si>
   <si>
@@ -1611,9 +1632,6 @@
     <t>HOME_LANG_OTHER</t>
   </si>
   <si>
-    <t>ORIGIN_PLACE_TYPE</t>
-  </si>
-  <si>
     <t>Your usual WORKPLACE</t>
   </si>
   <si>
@@ -1659,9 +1677,6 @@
     <t>Airport (airline passengers only)</t>
   </si>
   <si>
-    <t>DESTIN_PLACE_TYPE</t>
-  </si>
-  <si>
     <t>Very well</t>
   </si>
   <si>
@@ -1848,9 +1863,6 @@
     <t>None (0)</t>
   </si>
   <si>
-    <t>COUNT_EMPLOYED_HH</t>
-  </si>
-  <si>
     <t>GO2SCHL_AFTR_TRIP</t>
   </si>
   <si>
@@ -1893,9 +1905,6 @@
     <t>Not employed</t>
   </si>
   <si>
-    <t>SF Muni Pilot</t>
-  </si>
-  <si>
     <t>AM_INDIAN_ALASKA_NAT</t>
   </si>
   <si>
@@ -1941,9 +1950,6 @@
     <t>ALIGHTING_LON</t>
   </si>
   <si>
-    <t>EGRESS_MODE</t>
-  </si>
-  <si>
     <t>GENDER</t>
   </si>
   <si>
@@ -1984,13 +1990,31 @@
   </si>
   <si>
     <t>PREV_TRANSFERS_CODE</t>
+  </si>
+  <si>
+    <t>SF Muni Early Tranche</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_ACCESS_MODE</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_DESTIN_TYPE_PLACE</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_EGRESS_MODE</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_COUNT_EMPLOYED_HH</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_ORIGIN_TYPE_PLACE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2041,8 +2065,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2058,6 +2095,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2078,7 +2127,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2107,6 +2156,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2453,14 +2509,14 @@
   <dimension ref="A1:E1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A776" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B790" sqref="B790"/>
+      <pane ySplit="1" topLeftCell="A964" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B977" sqref="B977"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.375" style="1" customWidth="1"/>
@@ -15816,7 +15872,7 @@
         <v>362</v>
       </c>
       <c r="B786" s="7" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C786" s="7" t="s">
         <v>4</v>
@@ -15833,7 +15889,7 @@
         <v>362</v>
       </c>
       <c r="B787" s="7" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="C787" s="7" t="s">
         <v>4</v>
@@ -15850,7 +15906,7 @@
         <v>362</v>
       </c>
       <c r="B788" s="7" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="C788" s="7" t="s">
         <v>4</v>
@@ -15867,7 +15923,7 @@
         <v>362</v>
       </c>
       <c r="B789" s="7" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C789" s="7" t="s">
         <v>4</v>
@@ -15966,10 +16022,10 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>414</v>
@@ -15983,10 +16039,10 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>415</v>
@@ -16000,10 +16056,10 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C797" s="1" t="s">
         <v>416</v>
@@ -16017,10 +16073,10 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C798" s="1" t="s">
         <v>417</v>
@@ -16034,10 +16090,10 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C799" s="1" t="s">
         <v>418</v>
@@ -16051,10 +16107,10 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C800" s="1" t="s">
         <v>419</v>
@@ -16068,10 +16124,10 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>421</v>
+        <v>573</v>
       </c>
       <c r="C801" s="1" t="s">
         <v>420</v>
@@ -16085,10 +16141,10 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C802" s="1" t="s">
         <v>57</v>
@@ -16102,10 +16158,10 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>56</v>
@@ -16119,10 +16175,10 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>57</v>
@@ -16136,10 +16192,10 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>56</v>
@@ -16153,10 +16209,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -16170,10 +16226,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -16187,13 +16243,13 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>52</v>
@@ -16204,13 +16260,13 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>52</v>
@@ -16221,13 +16277,13 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>52</v>
@@ -16238,13 +16294,13 @@
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>52</v>
@@ -16255,13 +16311,13 @@
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>52</v>
@@ -16272,13 +16328,13 @@
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>52</v>
@@ -16289,13 +16345,13 @@
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>52</v>
@@ -16306,13 +16362,13 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>52</v>
@@ -16323,13 +16379,13 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>52</v>
@@ -16340,13 +16396,13 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>52</v>
@@ -16357,13 +16413,13 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>52</v>
@@ -16374,13 +16430,13 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>52</v>
@@ -16391,13 +16447,13 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>52</v>
@@ -16408,13 +16464,13 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>469</v>
+        <v>574</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>52</v>
@@ -16425,13 +16481,13 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>135</v>
@@ -16442,10 +16498,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>50</v>
@@ -16459,10 +16515,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>50</v>
@@ -16476,10 +16532,10 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C825" s="1" t="s">
         <v>417</v>
@@ -16493,10 +16549,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>50</v>
@@ -16510,13 +16566,13 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>135</v>
@@ -16527,13 +16583,13 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>135</v>
@@ -16544,13 +16600,13 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>135</v>
@@ -16561,13 +16617,13 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>563</v>
+        <v>575</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>135</v>
@@ -16578,13 +16634,13 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16595,13 +16651,13 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>
@@ -16612,13 +16668,13 @@
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>16</v>
@@ -16629,13 +16685,13 @@
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>16</v>
@@ -16646,13 +16702,13 @@
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>16</v>
@@ -16663,13 +16719,13 @@
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -16680,13 +16736,13 @@
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -16697,13 +16753,13 @@
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>16</v>
@@ -16714,13 +16770,13 @@
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>16</v>
@@ -16731,13 +16787,13 @@
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C840" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>16</v>
@@ -16748,13 +16804,13 @@
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>16</v>
@@ -16765,13 +16821,13 @@
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
@@ -16782,13 +16838,13 @@
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>532</v>
+        <v>576</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -16799,13 +16855,13 @@
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>244</v>
@@ -16816,13 +16872,13 @@
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>244</v>
@@ -16833,13 +16889,13 @@
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>244</v>
@@ -16850,13 +16906,13 @@
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>244</v>
@@ -16867,13 +16923,13 @@
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D848" s="1" t="s">
         <v>148</v>
@@ -16884,13 +16940,13 @@
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C849" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>148</v>
@@ -16901,13 +16957,13 @@
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D850" s="1" t="s">
         <v>148</v>
@@ -16918,13 +16974,13 @@
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>148</v>
@@ -16935,13 +16991,13 @@
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>148</v>
@@ -16952,13 +17008,13 @@
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>148</v>
@@ -16969,13 +17025,13 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>148</v>
@@ -16986,13 +17042,13 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D855" s="1" t="s">
         <v>148</v>
@@ -17003,7 +17059,7 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>274</v>
@@ -17020,7 +17076,7 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>274</v>
@@ -17037,13 +17093,13 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>225</v>
@@ -17054,13 +17110,13 @@
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A859" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>225</v>
@@ -17071,13 +17127,13 @@
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A860" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D860" s="1" t="s">
         <v>225</v>
@@ -17088,13 +17144,13 @@
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A861" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>225</v>
@@ -17105,13 +17161,13 @@
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
@@ -17122,13 +17178,13 @@
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A863" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
@@ -17139,13 +17195,13 @@
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A864" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
@@ -17156,13 +17212,13 @@
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
@@ -17173,13 +17229,13 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
@@ -17190,13 +17246,13 @@
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>225</v>
@@ -17207,13 +17263,13 @@
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D868" s="1" t="s">
         <v>225</v>
@@ -17224,10 +17280,10 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>57</v>
@@ -17241,10 +17297,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>56</v>
@@ -17258,7 +17314,7 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B871" s="1" t="s">
         <v>78</v>
@@ -17275,7 +17331,7 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B872" s="1" t="s">
         <v>79</v>
@@ -17292,7 +17348,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>5</v>
@@ -17309,10 +17365,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>57</v>
@@ -17326,10 +17382,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>56</v>
@@ -17343,16 +17399,16 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>94</v>
+        <v>472</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D876" s="1" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="E876" s="1" t="s">
         <v>4</v>
@@ -17360,16 +17416,16 @@
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C877" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D877" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E877" s="1" t="s">
         <v>4</v>
@@ -17377,217 +17433,217 @@
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A878" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B878" s="1" t="s">
-        <v>453</v>
+        <v>96</v>
       </c>
       <c r="C878" s="1" t="s">
-        <v>454</v>
+        <v>4</v>
       </c>
       <c r="D878" s="1" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="E878" s="1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E879" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B880" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C880" s="1" t="s">
         <v>453</v>
-      </c>
-      <c r="C880" s="1" t="s">
-        <v>456</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E880" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E881" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E882" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E883" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E884" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E885" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E886" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E887" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E888" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
       </c>
       <c r="E889" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>453</v>
+        <v>577</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
@@ -17598,64 +17654,64 @@
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>475</v>
+        <v>577</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
       <c r="D891" s="1" t="s">
-        <v>176</v>
+        <v>40</v>
       </c>
       <c r="E891" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D894" s="1" t="s">
         <v>139</v>
@@ -17666,13 +17722,13 @@
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B895" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D895" s="1" t="s">
         <v>37</v>
@@ -17683,13 +17739,13 @@
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B896" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D896" s="1" t="s">
         <v>37</v>
@@ -17700,13 +17756,13 @@
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A897" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B897" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D897" s="1" t="s">
         <v>37</v>
@@ -17717,13 +17773,13 @@
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B898" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D898" s="1" t="s">
         <v>37</v>
@@ -17734,13 +17790,13 @@
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B899" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>37</v>
@@ -17751,13 +17807,13 @@
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B900" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D900" s="1" t="s">
         <v>37</v>
@@ -17768,13 +17824,13 @@
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A901" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B901" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D901" s="1" t="s">
         <v>37</v>
@@ -17785,13 +17841,13 @@
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D902" s="1" t="s">
         <v>37</v>
@@ -17802,13 +17858,13 @@
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A903" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B903" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D903" s="1" t="s">
         <v>37</v>
@@ -17819,13 +17875,13 @@
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A904" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B904" s="10" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
@@ -17836,10 +17892,10 @@
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>56</v>
@@ -17853,10 +17909,10 @@
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>57</v>
@@ -17870,13 +17926,13 @@
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A907" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>160</v>
@@ -17887,10 +17943,10 @@
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A908" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>56</v>
@@ -17904,10 +17960,10 @@
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A909" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>57</v>
@@ -17921,13 +17977,13 @@
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D910" s="1" t="s">
         <v>162</v>
@@ -17938,10 +17994,10 @@
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A911" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C911" s="1" t="s">
         <v>56</v>
@@ -17955,10 +18011,10 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C912" s="1" t="s">
         <v>57</v>
@@ -17972,13 +18028,13 @@
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>164</v>
@@ -17989,10 +18045,10 @@
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>56</v>
@@ -18006,10 +18062,10 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>57</v>
@@ -18023,13 +18079,13 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D916" s="1" t="s">
         <v>166</v>
@@ -18040,10 +18096,10 @@
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B917" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="B917" s="1" t="s">
-        <v>552</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
@@ -18057,10 +18113,10 @@
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B918" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="B918" s="1" t="s">
-        <v>552</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>57</v>
@@ -18074,13 +18130,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B919" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="B919" s="1" t="s">
-        <v>552</v>
-      </c>
       <c r="C919" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D919" s="1" t="s">
         <v>168</v>
@@ -18091,10 +18147,10 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>4</v>
@@ -18108,13 +18164,13 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D921" s="1" t="s">
         <v>236</v>
@@ -18125,13 +18181,13 @@
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D922" s="1" t="s">
         <v>236</v>
@@ -18142,27 +18198,27 @@
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D923" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E923" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>4</v>
@@ -18176,10 +18232,10 @@
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>4</v>
@@ -18193,13 +18249,13 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D926" s="1" t="s">
         <v>60</v>
@@ -18210,13 +18266,13 @@
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B927" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D927" s="1" t="s">
         <v>60</v>
@@ -18227,13 +18283,13 @@
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D928" s="1" t="s">
         <v>60</v>
@@ -18244,13 +18300,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A929" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D929" s="1" t="s">
         <v>60</v>
@@ -18261,13 +18317,13 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D930" s="1" t="s">
         <v>60</v>
@@ -18278,13 +18334,13 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A931" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D931" s="1" t="s">
         <v>60</v>
@@ -18295,13 +18351,13 @@
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A932" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B932" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D932" s="1" t="s">
         <v>60</v>
@@ -18312,10 +18368,10 @@
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A933" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B933" s="1" t="s">
-        <v>540</v>
+        <v>572</v>
+      </c>
+      <c r="B933" s="12" t="s">
+        <v>536</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>4</v>
@@ -18329,10 +18385,10 @@
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B934" s="1" t="s">
-        <v>541</v>
+        <v>572</v>
+      </c>
+      <c r="B934" s="12" t="s">
+        <v>537</v>
       </c>
       <c r="C934" s="1" t="s">
         <v>4</v>
@@ -18346,13 +18402,13 @@
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A935" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
@@ -18363,13 +18419,13 @@
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A936" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C936" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
@@ -18380,13 +18436,13 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A937" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B937" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C937" s="1" t="s">
         <v>508</v>
-      </c>
-      <c r="C937" s="1" t="s">
-        <v>511</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
@@ -18397,13 +18453,13 @@
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A938" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
@@ -18414,13 +18470,13 @@
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
@@ -18431,13 +18487,13 @@
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
@@ -18448,13 +18504,13 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
@@ -18465,13 +18521,13 @@
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
@@ -18482,13 +18538,13 @@
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A943" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
@@ -18499,13 +18555,13 @@
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A944" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
@@ -18516,13 +18572,13 @@
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A945" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
@@ -18533,13 +18589,13 @@
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A946" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
@@ -18550,13 +18606,13 @@
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
@@ -18567,13 +18623,13 @@
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A948" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
@@ -18584,13 +18640,13 @@
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>251</v>
@@ -18601,13 +18657,13 @@
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A950" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>251</v>
@@ -18618,13 +18674,13 @@
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>251</v>
@@ -18635,13 +18691,13 @@
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>251</v>
@@ -18652,13 +18708,13 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A953" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
@@ -18669,13 +18725,13 @@
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B954" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
@@ -18686,13 +18742,13 @@
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A955" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B955" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
@@ -18703,13 +18759,13 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A956" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B956" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
@@ -18720,13 +18776,13 @@
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A957" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B957" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
@@ -18737,13 +18793,13 @@
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A958" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B958" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
@@ -18754,13 +18810,13 @@
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A959" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B959" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
@@ -18771,13 +18827,13 @@
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A960" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B960" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
@@ -18788,13 +18844,13 @@
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A961" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B961" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
@@ -18805,13 +18861,13 @@
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A962" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
@@ -18822,13 +18878,13 @@
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A963" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B963" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
@@ -18839,13 +18895,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B964" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
@@ -18856,13 +18912,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B965" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
@@ -18873,13 +18929,13 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A966" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B966" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
@@ -18890,13 +18946,13 @@
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A967" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B967" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
@@ -18907,13 +18963,13 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B968" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
@@ -18924,13 +18980,13 @@
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>253</v>
@@ -18941,13 +18997,13 @@
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A970" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>253</v>
@@ -18958,13 +19014,13 @@
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A971" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B971" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>253</v>
@@ -18975,13 +19031,13 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A972" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B972" s="10" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>253</v>
@@ -18990,29 +19046,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="973" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A973" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B973" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="C973" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D973" s="1" t="s">
+    <row r="973" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A973" s="13" t="s">
+        <v>572</v>
+      </c>
+      <c r="B973" s="13" t="s">
+        <v>560</v>
+      </c>
+      <c r="C973" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D973" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E973" s="1" t="s">
+      <c r="E973" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
@@ -19026,10 +19082,10 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="C975" s="1" t="s">
         <v>4</v>
@@ -19043,10 +19099,10 @@
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="C976" s="1" t="s">
         <v>4</v>
@@ -19060,10 +19116,10 @@
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A977" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="C977" s="1" t="s">
         <v>4</v>
@@ -19077,10 +19133,10 @@
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="C978" s="1" t="s">
         <v>4</v>
@@ -19094,13 +19150,13 @@
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B979" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
@@ -19111,13 +19167,13 @@
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B980" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D980" s="1" t="s">
         <v>9</v>
@@ -19128,13 +19184,13 @@
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A981" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B981" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D981" s="1" t="s">
         <v>9</v>
@@ -19145,13 +19201,13 @@
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B982" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D982" s="1" t="s">
         <v>9</v>
@@ -19162,13 +19218,13 @@
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B983" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D983" s="1" t="s">
         <v>9</v>
@@ -19179,13 +19235,13 @@
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B984" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D984" s="1" t="s">
         <v>9</v>
@@ -19196,13 +19252,13 @@
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A985" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B985" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D985" s="1" t="s">
         <v>9</v>
@@ -19213,13 +19269,13 @@
     </row>
     <row r="986" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B986" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D986" s="1" t="s">
         <v>9</v>
@@ -19230,13 +19286,13 @@
     </row>
     <row r="987" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B987" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D987" s="1" t="s">
         <v>9</v>
@@ -19247,13 +19303,13 @@
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B988" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D988" s="1" t="s">
         <v>9</v>
@@ -19264,13 +19320,13 @@
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D989" s="1" t="s">
         <v>9</v>
@@ -19281,10 +19337,10 @@
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B990" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C990" s="1" t="s">
         <v>57</v>
@@ -19298,10 +19354,10 @@
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B991" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C991" s="1" t="s">
         <v>56</v>
@@ -19315,10 +19371,10 @@
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A992" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="C992" s="1" t="s">
         <v>4</v>
@@ -19332,10 +19388,10 @@
     </row>
     <row r="993" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="C993" s="1" t="s">
         <v>4</v>
@@ -19349,7 +19405,7 @@
     </row>
     <row r="994" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B994" s="1" t="s">
         <v>6</v>
@@ -19366,13 +19422,13 @@
     </row>
     <row r="995" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B995" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D995" s="1" t="s">
         <v>284</v>
@@ -19383,13 +19439,13 @@
     </row>
     <row r="996" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B996" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="D996" s="1" t="s">
         <v>284</v>
@@ -19400,13 +19456,13 @@
     </row>
     <row r="997" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B997" s="1" t="s">
         <v>394</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="D997" s="1" t="s">
         <v>284</v>
@@ -19417,10 +19473,10 @@
     </row>
     <row r="998" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A998" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B998" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="D998" s="1" t="s">
         <v>291</v>
@@ -19431,13 +19487,13 @@
     </row>
     <row r="999" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D999" s="1" t="s">
         <v>291</v>
@@ -19448,10 +19504,10 @@
     </row>
     <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1000" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>187</v>
@@ -19465,13 +19521,13 @@
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1001" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D1001" s="1" t="s">
         <v>291</v>
@@ -19482,13 +19538,13 @@
     </row>
     <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1002" s="1" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D1002" s="1" t="s">
         <v>291</v>
@@ -19499,10 +19555,10 @@
     </row>
     <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C1003" s="1" t="s">
         <v>4</v>
@@ -19516,10 +19572,10 @@
     </row>
     <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1004" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="C1004" s="1" t="s">
         <v>4</v>
@@ -19533,10 +19589,10 @@
     </row>
     <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1005" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="C1005" s="1" t="s">
         <v>4</v>
@@ -19550,10 +19606,10 @@
     </row>
     <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1006" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C1006" s="1" t="s">
         <v>4</v>
@@ -19567,10 +19623,10 @@
     </row>
     <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1007" s="1" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C1007" s="1" t="s">
         <v>4</v>
@@ -19584,10 +19640,10 @@
     </row>
     <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="C1008" s="1" t="s">
         <v>4</v>
@@ -19601,10 +19657,10 @@
     </row>
     <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="C1009" s="1" t="s">
         <v>4</v>
@@ -19618,10 +19674,10 @@
     </row>
     <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1010" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="C1010" s="1" t="s">
         <v>4</v>
@@ -19635,10 +19691,10 @@
     </row>
     <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1011" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1011" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C1011" s="1" t="s">
         <v>4</v>
@@ -19652,16 +19708,16 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1012" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1012" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C1012" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1012" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="D1012" s="1" t="s">
-        <v>486</v>
       </c>
       <c r="E1012" s="1" t="s">
         <v>144</v>
@@ -19669,61 +19725,61 @@
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1013" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1013" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C1013" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D1013" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E1013" s="1" t="s">
         <v>484</v>
-      </c>
-      <c r="D1013" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="E1013" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1014" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C1014" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="C1014" s="1" t="s">
-        <v>485</v>
-      </c>
       <c r="D1014" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E1014" s="1" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D1015" s="1" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E1015" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="1016" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1016" s="5" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C1016" s="5" t="s">
         <v>4</v>
@@ -19737,10 +19793,10 @@
     </row>
     <row r="1017" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1017" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1017" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C1017" s="1">
         <v>0</v>
@@ -19754,10 +19810,10 @@
     </row>
     <row r="1018" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1018" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C1018" s="1">
         <v>1</v>
@@ -19771,10 +19827,10 @@
     </row>
     <row r="1019" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1019" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1019" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C1019" s="1">
         <v>2</v>
@@ -19788,10 +19844,10 @@
     </row>
     <row r="1020" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1020" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C1020" s="1">
         <v>3</v>
@@ -19805,10 +19861,10 @@
     </row>
     <row r="1021" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1021" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1021" s="1" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C1021" s="1">
         <v>4</v>
@@ -19822,10 +19878,10 @@
     </row>
     <row r="1022" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1022" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1022" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C1022" s="1">
         <v>0</v>
@@ -19839,10 +19895,10 @@
     </row>
     <row r="1023" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1023" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1023" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C1023" s="1">
         <v>1</v>
@@ -19856,10 +19912,10 @@
     </row>
     <row r="1024" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1024" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1024" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C1024" s="1">
         <v>2</v>
@@ -19873,10 +19929,10 @@
     </row>
     <row r="1025" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1025" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1025" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C1025" s="1">
         <v>3</v>
@@ -19890,10 +19946,10 @@
     </row>
     <row r="1026" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1026" s="1" t="s">
-        <v>547</v>
+        <v>572</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C1026" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
through dictionary and non-geo summaries
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -245,36 +245,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="A973" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>David Ory:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-START HERE. Above variables in yellow need to be added to the data.</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="580">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -1590,39 +1566,6 @@
     <t>FARE_CATEGORY</t>
   </si>
   <si>
-    <t>Under $10,000</t>
-  </si>
-  <si>
-    <t>$10,000 to $24,999</t>
-  </si>
-  <si>
-    <t>$25,000 to $34,999</t>
-  </si>
-  <si>
-    <t>$35,000 - $49,999</t>
-  </si>
-  <si>
-    <t>$50,000 - $64,999</t>
-  </si>
-  <si>
-    <t>$65,000 - $74,999</t>
-  </si>
-  <si>
-    <t>$75,000 - $84,999</t>
-  </si>
-  <si>
-    <t>$85,000 - $99,999</t>
-  </si>
-  <si>
-    <t>$100,000 - $124,999</t>
-  </si>
-  <si>
-    <t>$125,000 - $149,999</t>
-  </si>
-  <si>
-    <t>$150,000 OR OVER</t>
-  </si>
-  <si>
     <t>INCOME</t>
   </si>
   <si>
@@ -1866,15 +1809,6 @@
     <t>GO2SCHL_AFTR_TRIP</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Callback</t>
-  </si>
-  <si>
-    <t>Paper</t>
-  </si>
-  <si>
     <t>SPANI</t>
   </si>
   <si>
@@ -1986,12 +1920,6 @@
     <t>LAST_ALIGHT_LON</t>
   </si>
   <si>
-    <t>NEXT_TRANSFERS_CODE</t>
-  </si>
-  <si>
-    <t>PREV_TRANSFERS_CODE</t>
-  </si>
-  <si>
     <t>SF Muni Early Tranche</t>
   </si>
   <si>
@@ -2008,13 +1936,67 @@
   </si>
   <si>
     <t>FINAL_SUGGESTED_ORIGIN_TYPE_PLACE</t>
+  </si>
+  <si>
+    <t>SURVEY_METHOD</t>
+  </si>
+  <si>
+    <t>FIRST_TRANSIT_BOARDING_LAT</t>
+  </si>
+  <si>
+    <t>FIRST_TRANSIT_BOARDING_LON</t>
+  </si>
+  <si>
+    <t>FINAL_TRANSIT_ALIGHTING_LAT</t>
+  </si>
+  <si>
+    <t>FINAL_TRANSIT_ALIGHTING_LON</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_NEXT_TRANSFERS_CODE</t>
+  </si>
+  <si>
+    <t>FINAL_SUGGESTED_PREV_TRANSFERS_CODE</t>
+  </si>
+  <si>
+    <t>$40,000-$49,999</t>
+  </si>
+  <si>
+    <t>Less than $10,000</t>
+  </si>
+  <si>
+    <t>$10,000-$24,999</t>
+  </si>
+  <si>
+    <t>$25,000-$34,999</t>
+  </si>
+  <si>
+    <t>$35,000-$39,999</t>
+  </si>
+  <si>
+    <t>$50,000-$59,999</t>
+  </si>
+  <si>
+    <t>$60,000-$74,999</t>
+  </si>
+  <si>
+    <t>$75,000-$99,999</t>
+  </si>
+  <si>
+    <t>$100,000-$149,999</t>
+  </si>
+  <si>
+    <t>$150,000-$199,999</t>
+  </si>
+  <si>
+    <t>$200,000 or more</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2065,21 +2047,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2095,18 +2064,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2127,7 +2084,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2156,13 +2113,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2509,8 +2459,8 @@
   <dimension ref="A1:E1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A964" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B977" sqref="B977"/>
+      <pane ySplit="1" topLeftCell="A841" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E858" sqref="E858"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15872,7 +15822,7 @@
         <v>362</v>
       </c>
       <c r="B786" s="7" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="C786" s="7" t="s">
         <v>4</v>
@@ -15889,7 +15839,7 @@
         <v>362</v>
       </c>
       <c r="B787" s="7" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="C787" s="7" t="s">
         <v>4</v>
@@ -15906,7 +15856,7 @@
         <v>362</v>
       </c>
       <c r="B788" s="7" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="C788" s="7" t="s">
         <v>4</v>
@@ -15923,7 +15873,7 @@
         <v>362</v>
       </c>
       <c r="B789" s="7" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="C789" s="7" t="s">
         <v>4</v>
@@ -16022,10 +15972,10 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C795" s="1" t="s">
         <v>414</v>
@@ -16039,10 +15989,10 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C796" s="1" t="s">
         <v>415</v>
@@ -16056,10 +16006,10 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C797" s="1" t="s">
         <v>416</v>
@@ -16073,10 +16023,10 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C798" s="1" t="s">
         <v>417</v>
@@ -16090,10 +16040,10 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C799" s="1" t="s">
         <v>418</v>
@@ -16107,10 +16057,10 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C800" s="1" t="s">
         <v>419</v>
@@ -16124,10 +16074,10 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C801" s="1" t="s">
         <v>420</v>
@@ -16141,7 +16091,7 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B802" s="1" t="s">
         <v>421</v>
@@ -16158,7 +16108,7 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B803" s="1" t="s">
         <v>421</v>
@@ -16175,7 +16125,7 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B804" s="1" t="s">
         <v>422</v>
@@ -16192,7 +16142,7 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B805" s="1" t="s">
         <v>422</v>
@@ -16209,10 +16159,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -16226,10 +16176,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -16243,13 +16193,13 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B808" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C808" s="1" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>52</v>
@@ -16260,13 +16210,13 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B809" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C809" s="1" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>52</v>
@@ -16277,13 +16227,13 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B810" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C810" s="1" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>52</v>
@@ -16294,13 +16244,13 @@
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B811" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C811" s="1" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>52</v>
@@ -16311,13 +16261,13 @@
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B812" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C812" s="1" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>52</v>
@@ -16328,13 +16278,13 @@
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B813" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C813" s="1" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>52</v>
@@ -16345,13 +16295,13 @@
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B814" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C814" s="1" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>52</v>
@@ -16362,13 +16312,13 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B815" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C815" s="1" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>52</v>
@@ -16379,13 +16329,13 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B816" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C816" s="1" t="s">
-        <v>466</v>
+        <v>455</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>52</v>
@@ -16396,13 +16346,13 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B817" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C817" s="1" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>52</v>
@@ -16413,13 +16363,13 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C818" s="1" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>52</v>
@@ -16430,13 +16380,13 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B819" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C819" s="1" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>52</v>
@@ -16447,13 +16397,13 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B820" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C820" s="1" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>52</v>
@@ -16464,13 +16414,13 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B821" s="1" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C821" s="1" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>52</v>
@@ -16481,10 +16431,10 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C822" s="1" t="s">
         <v>423</v>
@@ -16498,10 +16448,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>50</v>
@@ -16515,10 +16465,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>50</v>
@@ -16532,10 +16482,10 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C825" s="1" t="s">
         <v>417</v>
@@ -16549,10 +16499,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>50</v>
@@ -16566,10 +16516,10 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C827" s="1" t="s">
         <v>424</v>
@@ -16583,10 +16533,10 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C828" s="1" t="s">
         <v>425</v>
@@ -16600,10 +16550,10 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C829" s="1" t="s">
         <v>426</v>
@@ -16617,10 +16567,10 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C830" s="1" t="s">
         <v>427</v>
@@ -16634,13 +16584,13 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B831" s="1" t="s">
         <v>428</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16651,13 +16601,13 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B832" s="1" t="s">
         <v>428</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>
@@ -16668,13 +16618,13 @@
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>16</v>
@@ -16685,13 +16635,13 @@
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>16</v>
@@ -16702,13 +16652,13 @@
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>16</v>
@@ -16719,13 +16669,13 @@
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -16736,13 +16686,13 @@
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -16753,13 +16703,13 @@
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>16</v>
@@ -16770,13 +16720,13 @@
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>16</v>
@@ -16787,13 +16737,13 @@
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C840" s="1" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>16</v>
@@ -16804,13 +16754,13 @@
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>16</v>
@@ -16821,13 +16771,13 @@
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
@@ -16838,13 +16788,13 @@
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -16855,13 +16805,13 @@
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>467</v>
+        <v>456</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>244</v>
@@ -16872,13 +16822,13 @@
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>468</v>
+        <v>457</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>244</v>
@@ -16889,13 +16839,13 @@
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>469</v>
+        <v>458</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>244</v>
@@ -16906,13 +16856,13 @@
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>470</v>
+        <v>459</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>244</v>
@@ -16923,7 +16873,7 @@
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B848" s="1" t="s">
         <v>437</v>
@@ -16940,7 +16890,7 @@
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B849" s="1" t="s">
         <v>437</v>
@@ -16957,7 +16907,7 @@
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B850" s="1" t="s">
         <v>437</v>
@@ -16974,7 +16924,7 @@
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B851" s="1" t="s">
         <v>437</v>
@@ -16991,7 +16941,7 @@
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B852" s="1" t="s">
         <v>437</v>
@@ -17008,7 +16958,7 @@
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B853" s="1" t="s">
         <v>437</v>
@@ -17025,7 +16975,7 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B854" s="1" t="s">
         <v>437</v>
@@ -17042,7 +16992,7 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B855" s="1" t="s">
         <v>437</v>
@@ -17059,7 +17009,7 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>274</v>
@@ -17076,7 +17026,7 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>274</v>
@@ -17093,13 +17043,13 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>438</v>
+        <v>570</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>225</v>
@@ -17110,13 +17060,13 @@
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A859" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>439</v>
+        <v>571</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>225</v>
@@ -17127,13 +17077,13 @@
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A860" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B860" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C860" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="B860" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C860" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="D860" s="1" t="s">
         <v>225</v>
@@ -17144,13 +17094,13 @@
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A861" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>441</v>
+        <v>573</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>225</v>
@@ -17161,30 +17111,30 @@
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>442</v>
+        <v>569</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E862" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A863" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>443</v>
+        <v>574</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
@@ -17195,30 +17145,30 @@
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A864" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>444</v>
+        <v>575</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E864" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>445</v>
+        <v>576</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
@@ -17229,13 +17179,13 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>446</v>
+        <v>577</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
@@ -17246,30 +17196,30 @@
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>447</v>
+        <v>578</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>225</v>
       </c>
       <c r="E867" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>449</v>
+        <v>438</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>448</v>
+        <v>579</v>
       </c>
       <c r="D868" s="1" t="s">
         <v>225</v>
@@ -17280,10 +17230,10 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>57</v>
@@ -17297,10 +17247,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>56</v>
@@ -17314,7 +17264,7 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B871" s="1" t="s">
         <v>78</v>
@@ -17331,7 +17281,7 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B872" s="1" t="s">
         <v>79</v>
@@ -17348,7 +17298,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>5</v>
@@ -17365,10 +17315,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>57</v>
@@ -17382,10 +17332,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>451</v>
+        <v>440</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>56</v>
@@ -17399,10 +17349,10 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
@@ -17416,7 +17366,7 @@
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B877" s="1" t="s">
         <v>94</v>
@@ -17433,7 +17383,7 @@
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A878" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B878" s="1" t="s">
         <v>96</v>
@@ -17450,13 +17400,13 @@
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>40</v>
@@ -17467,13 +17417,13 @@
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>453</v>
+        <v>442</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
@@ -17484,13 +17434,13 @@
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>454</v>
+        <v>443</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
@@ -17501,13 +17451,13 @@
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
@@ -17518,13 +17468,13 @@
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
@@ -17535,13 +17485,13 @@
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
@@ -17552,13 +17502,13 @@
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
@@ -17569,13 +17519,13 @@
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
@@ -17586,13 +17536,13 @@
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
@@ -17603,13 +17553,13 @@
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
@@ -17620,13 +17570,13 @@
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
@@ -17637,13 +17587,13 @@
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
@@ -17654,13 +17604,13 @@
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="D891" s="1" t="s">
         <v>40</v>
@@ -17671,47 +17621,47 @@
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>475</v>
+        <v>464</v>
       </c>
       <c r="D894" s="1" t="s">
         <v>139</v>
@@ -17722,13 +17672,13 @@
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B895" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="D895" s="1" t="s">
         <v>37</v>
@@ -17739,13 +17689,13 @@
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B896" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="D896" s="1" t="s">
         <v>37</v>
@@ -17756,13 +17706,13 @@
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A897" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B897" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="D897" s="1" t="s">
         <v>37</v>
@@ -17773,13 +17723,13 @@
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B898" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="D898" s="1" t="s">
         <v>37</v>
@@ -17790,13 +17740,13 @@
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B899" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>37</v>
@@ -17807,13 +17757,13 @@
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B900" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="D900" s="1" t="s">
         <v>37</v>
@@ -17824,13 +17774,13 @@
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A901" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B901" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="D901" s="1" t="s">
         <v>37</v>
@@ -17841,13 +17791,13 @@
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="D902" s="1" t="s">
         <v>37</v>
@@ -17858,13 +17808,13 @@
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A903" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B903" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="D903" s="1" t="s">
         <v>37</v>
@@ -17875,13 +17825,13 @@
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A904" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B904" s="10" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
@@ -17892,10 +17842,10 @@
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>56</v>
@@ -17909,10 +17859,10 @@
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>57</v>
@@ -17926,13 +17876,13 @@
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A907" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>160</v>
@@ -17943,10 +17893,10 @@
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A908" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>56</v>
@@ -17960,10 +17910,10 @@
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A909" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>57</v>
@@ -17977,13 +17927,13 @@
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D910" s="1" t="s">
         <v>162</v>
@@ -17994,10 +17944,10 @@
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A911" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="C911" s="1" t="s">
         <v>56</v>
@@ -18011,10 +17961,10 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="C912" s="1" t="s">
         <v>57</v>
@@ -18028,13 +17978,13 @@
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>164</v>
@@ -18045,10 +17995,10 @@
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>56</v>
@@ -18062,10 +18012,10 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>57</v>
@@ -18079,13 +18029,13 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D916" s="1" t="s">
         <v>166</v>
@@ -18096,10 +18046,10 @@
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
@@ -18113,10 +18063,10 @@
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>57</v>
@@ -18130,13 +18080,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="D919" s="1" t="s">
         <v>168</v>
@@ -18147,10 +18097,10 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>4</v>
@@ -18164,13 +18114,13 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
       <c r="D921" s="1" t="s">
         <v>236</v>
@@ -18181,13 +18131,13 @@
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="D922" s="1" t="s">
         <v>236</v>
@@ -18198,27 +18148,27 @@
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="D923" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E923" s="1" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>4</v>
@@ -18232,10 +18182,10 @@
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>4</v>
@@ -18249,13 +18199,13 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
       <c r="D926" s="1" t="s">
         <v>60</v>
@@ -18266,13 +18216,13 @@
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B927" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="D927" s="1" t="s">
         <v>60</v>
@@ -18283,13 +18233,13 @@
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="D928" s="1" t="s">
         <v>60</v>
@@ -18300,13 +18250,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A929" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="D929" s="1" t="s">
         <v>60</v>
@@ -18317,13 +18267,13 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="D930" s="1" t="s">
         <v>60</v>
@@ -18334,13 +18284,13 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A931" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="D931" s="1" t="s">
         <v>60</v>
@@ -18351,13 +18301,13 @@
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A932" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B932" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="D932" s="1" t="s">
         <v>60</v>
@@ -18368,10 +18318,10 @@
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A933" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B933" s="12" t="s">
-        <v>536</v>
+        <v>556</v>
+      </c>
+      <c r="B933" s="5" t="s">
+        <v>522</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>4</v>
@@ -18385,10 +18335,10 @@
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B934" s="12" t="s">
-        <v>537</v>
+        <v>556</v>
+      </c>
+      <c r="B934" s="5" t="s">
+        <v>523</v>
       </c>
       <c r="C934" s="1" t="s">
         <v>4</v>
@@ -18402,13 +18352,13 @@
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A935" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
@@ -18419,13 +18369,13 @@
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A936" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B936" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C936" s="1" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
@@ -18436,13 +18386,13 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A937" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
@@ -18453,13 +18403,13 @@
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A938" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
@@ -18470,13 +18420,13 @@
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
@@ -18487,13 +18437,13 @@
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
@@ -18504,13 +18454,13 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
@@ -18521,13 +18471,13 @@
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
@@ -18538,13 +18488,13 @@
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A943" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
@@ -18555,13 +18505,13 @@
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A944" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
@@ -18572,13 +18522,13 @@
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A945" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B945" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C945" s="1" t="s">
         <v>505</v>
-      </c>
-      <c r="C945" s="1" t="s">
-        <v>516</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
@@ -18589,13 +18539,13 @@
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A946" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
@@ -18606,13 +18556,13 @@
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
@@ -18623,13 +18573,13 @@
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A948" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
@@ -18640,13 +18590,13 @@
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>251</v>
@@ -18657,13 +18607,13 @@
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A950" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>251</v>
@@ -18674,13 +18624,13 @@
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>251</v>
@@ -18691,13 +18641,13 @@
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>251</v>
@@ -18708,13 +18658,13 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A953" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
@@ -18725,13 +18675,13 @@
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B954" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
@@ -18742,13 +18692,13 @@
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A955" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B955" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
@@ -18759,13 +18709,13 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A956" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B956" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
@@ -18776,13 +18726,13 @@
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A957" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B957" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
@@ -18793,13 +18743,13 @@
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A958" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B958" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
@@ -18810,13 +18760,13 @@
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A959" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B959" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
@@ -18827,13 +18777,13 @@
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A960" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B960" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
@@ -18844,13 +18794,13 @@
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A961" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B961" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
@@ -18861,13 +18811,13 @@
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A962" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
@@ -18878,13 +18828,13 @@
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A963" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B963" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
@@ -18895,13 +18845,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B964" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
@@ -18912,13 +18862,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B965" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
@@ -18929,13 +18879,13 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A966" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B966" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>519</v>
+        <v>508</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
@@ -18946,13 +18896,13 @@
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A967" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B967" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
@@ -18963,13 +18913,13 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B968" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
@@ -18980,13 +18930,13 @@
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>253</v>
@@ -18997,13 +18947,13 @@
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A970" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>253</v>
@@ -19014,13 +18964,13 @@
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A971" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B971" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>253</v>
@@ -19031,13 +18981,13 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A972" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B972" s="10" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>253</v>
@@ -19046,29 +18996,29 @@
         <v>23</v>
       </c>
     </row>
-    <row r="973" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A973" s="13" t="s">
-        <v>572</v>
-      </c>
-      <c r="B973" s="13" t="s">
-        <v>560</v>
-      </c>
-      <c r="C973" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D973" s="13" t="s">
+    <row r="973" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A973" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="B973" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="C973" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D973" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E973" s="13" t="s">
+      <c r="E973" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
@@ -19082,10 +19032,10 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="C975" s="1" t="s">
         <v>4</v>
@@ -19099,10 +19049,10 @@
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="C976" s="1" t="s">
         <v>4</v>
@@ -19116,10 +19066,10 @@
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A977" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="C977" s="1" t="s">
         <v>4</v>
@@ -19133,10 +19083,10 @@
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="C978" s="1" t="s">
         <v>4</v>
@@ -19150,13 +19100,13 @@
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B979" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
@@ -19167,13 +19117,13 @@
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B980" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="D980" s="1" t="s">
         <v>9</v>
@@ -19184,13 +19134,13 @@
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A981" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B981" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>486</v>
+        <v>475</v>
       </c>
       <c r="D981" s="1" t="s">
         <v>9</v>
@@ -19201,13 +19151,13 @@
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B982" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="D982" s="1" t="s">
         <v>9</v>
@@ -19218,13 +19168,13 @@
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B983" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="D983" s="1" t="s">
         <v>9</v>
@@ -19235,13 +19185,13 @@
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B984" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="D984" s="1" t="s">
         <v>9</v>
@@ -19252,13 +19202,13 @@
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A985" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B985" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="D985" s="1" t="s">
         <v>9</v>
@@ -19269,13 +19219,13 @@
     </row>
     <row r="986" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B986" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="D986" s="1" t="s">
         <v>9</v>
@@ -19286,13 +19236,13 @@
     </row>
     <row r="987" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B987" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="D987" s="1" t="s">
         <v>9</v>
@@ -19303,13 +19253,13 @@
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B988" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="D988" s="1" t="s">
         <v>9</v>
@@ -19320,13 +19270,13 @@
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="D989" s="1" t="s">
         <v>9</v>
@@ -19337,10 +19287,10 @@
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B990" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="C990" s="1" t="s">
         <v>57</v>
@@ -19354,10 +19304,10 @@
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B991" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="C991" s="1" t="s">
         <v>56</v>
@@ -19371,10 +19321,10 @@
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A992" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="C992" s="1" t="s">
         <v>4</v>
@@ -19388,10 +19338,10 @@
     </row>
     <row r="993" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="C993" s="1" t="s">
         <v>4</v>
@@ -19405,7 +19355,7 @@
     </row>
     <row r="994" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B994" s="1" t="s">
         <v>6</v>
@@ -19422,13 +19372,13 @@
     </row>
     <row r="995" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B995" s="1" t="s">
-        <v>394</v>
+        <v>562</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>531</v>
+        <v>395</v>
       </c>
       <c r="D995" s="1" t="s">
         <v>284</v>
@@ -19439,13 +19389,13 @@
     </row>
     <row r="996" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B996" s="1" t="s">
-        <v>394</v>
+        <v>562</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>530</v>
+        <v>396</v>
       </c>
       <c r="D996" s="1" t="s">
         <v>284</v>
@@ -19456,13 +19406,13 @@
     </row>
     <row r="997" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B997" s="1" t="s">
-        <v>394</v>
+        <v>562</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>532</v>
+        <v>397</v>
       </c>
       <c r="D997" s="1" t="s">
         <v>284</v>
@@ -19473,10 +19423,10 @@
     </row>
     <row r="998" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A998" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B998" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
+      </c>
+      <c r="B998" s="5" t="s">
+        <v>539</v>
       </c>
       <c r="D998" s="1" t="s">
         <v>291</v>
@@ -19487,13 +19437,13 @@
     </row>
     <row r="999" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B999" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
+      </c>
+      <c r="B999" s="5" t="s">
+        <v>539</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="D999" s="1" t="s">
         <v>291</v>
@@ -19504,10 +19454,10 @@
     </row>
     <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B1000" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
+      </c>
+      <c r="B1000" s="5" t="s">
+        <v>539</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>187</v>
@@ -19521,13 +19471,13 @@
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B1001" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
+      </c>
+      <c r="B1001" s="5" t="s">
+        <v>539</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="D1001" s="1" t="s">
         <v>291</v>
@@ -19538,13 +19488,13 @@
     </row>
     <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B1002" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
+      </c>
+      <c r="B1002" s="5" t="s">
+        <v>539</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="D1002" s="1" t="s">
         <v>291</v>
@@ -19555,10 +19505,10 @@
     </row>
     <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>539</v>
+        <v>563</v>
       </c>
       <c r="C1003" s="1" t="s">
         <v>4</v>
@@ -19572,10 +19522,10 @@
     </row>
     <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1004" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C1004" s="1" t="s">
         <v>4</v>
@@ -19589,10 +19539,10 @@
     </row>
     <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1005" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C1005" s="1" t="s">
         <v>4</v>
@@ -19606,10 +19556,10 @@
     </row>
     <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1006" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C1006" s="1" t="s">
         <v>4</v>
@@ -19623,10 +19573,10 @@
     </row>
     <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="B1007" s="1" t="s">
-        <v>538</v>
+        <v>556</v>
+      </c>
+      <c r="B1007" s="5" t="s">
+        <v>524</v>
       </c>
       <c r="C1007" s="1" t="s">
         <v>4</v>
@@ -19640,10 +19590,10 @@
     </row>
     <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="C1008" s="1" t="s">
         <v>4</v>
@@ -19657,10 +19607,10 @@
     </row>
     <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="C1009" s="1" t="s">
         <v>4</v>
@@ -19674,10 +19624,10 @@
     </row>
     <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1010" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="C1010" s="1" t="s">
         <v>4</v>
@@ -19691,10 +19641,10 @@
     </row>
     <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1011" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1011" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="C1011" s="1" t="s">
         <v>4</v>
@@ -19708,16 +19658,16 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1012" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1012" s="1" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C1012" s="1" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="D1012" s="1" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="E1012" s="1" t="s">
         <v>144</v>
@@ -19725,61 +19675,61 @@
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1013" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1013" s="1" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C1013" s="1" t="s">
-        <v>481</v>
+        <v>470</v>
       </c>
       <c r="D1013" s="1" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="E1013" s="1" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
     </row>
     <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1014" s="1" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C1014" s="1" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
       <c r="D1014" s="1" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="E1014" s="1" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
     </row>
     <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="D1015" s="1" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="E1015" s="1" t="s">
-        <v>477</v>
+        <v>466</v>
       </c>
     </row>
     <row r="1016" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1016" s="5" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="C1016" s="5" t="s">
         <v>4</v>
@@ -19793,10 +19743,10 @@
     </row>
     <row r="1017" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1017" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1017" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C1017" s="1">
         <v>0</v>
@@ -19810,10 +19760,10 @@
     </row>
     <row r="1018" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1018" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C1018" s="1">
         <v>1</v>
@@ -19827,10 +19777,10 @@
     </row>
     <row r="1019" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1019" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1019" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C1019" s="1">
         <v>2</v>
@@ -19844,10 +19794,10 @@
     </row>
     <row r="1020" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1020" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C1020" s="1">
         <v>3</v>
@@ -19861,10 +19811,10 @@
     </row>
     <row r="1021" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1021" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1021" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C1021" s="1">
         <v>4</v>
@@ -19878,10 +19828,10 @@
     </row>
     <row r="1022" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1022" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1022" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C1022" s="1">
         <v>0</v>
@@ -19895,10 +19845,10 @@
     </row>
     <row r="1023" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1023" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1023" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C1023" s="1">
         <v>1</v>
@@ -19912,10 +19862,10 @@
     </row>
     <row r="1024" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1024" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1024" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C1024" s="1">
         <v>2</v>
@@ -19929,10 +19879,10 @@
     </row>
     <row r="1025" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1025" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1025" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C1025" s="1">
         <v>3</v>
@@ -19946,10 +19896,10 @@
     </row>
     <row r="1026" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1026" s="1" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C1026" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Updated BART enter and exit station variable names
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dory\Documents\GitHub\onboard-surveys\make-uniform\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrae.MTC\Documents\GitHub\onboard-surveys\make-uniform\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1374,12 +1374,6 @@
     <t>EMPLOYED_IN_HH_CODE</t>
   </si>
   <si>
-    <t>ENTERSTATION</t>
-  </si>
-  <si>
-    <t>EXITSTATION</t>
-  </si>
-  <si>
     <t>HOME_ADDRESS_LAT</t>
   </si>
   <si>
@@ -1990,6 +1984,12 @@
   </si>
   <si>
     <t>$200,000 or more</t>
+  </si>
+  <si>
+    <t>FIRST_ENTERED_BART</t>
+  </si>
+  <si>
+    <t>BART_EXIT_STATION</t>
   </si>
 </sst>
 </file>
@@ -2459,8 +2459,8 @@
   <dimension ref="A1:E1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A841" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E858" sqref="E858"/>
+      <pane ySplit="1" topLeftCell="A615" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B640" sqref="B640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13255,7 +13255,7 @@
         <v>362</v>
       </c>
       <c r="B635" s="7" t="s">
-        <v>374</v>
+        <v>578</v>
       </c>
       <c r="C635" s="7" t="s">
         <v>4</v>
@@ -13272,7 +13272,7 @@
         <v>362</v>
       </c>
       <c r="B636" s="7" t="s">
-        <v>375</v>
+        <v>579</v>
       </c>
       <c r="C636" s="7" t="s">
         <v>4</v>
@@ -13289,7 +13289,7 @@
         <v>362</v>
       </c>
       <c r="B637" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C637" s="7">
         <v>1</v>
@@ -13306,7 +13306,7 @@
         <v>362</v>
       </c>
       <c r="B638" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C638" s="7">
         <v>2</v>
@@ -13323,7 +13323,7 @@
         <v>362</v>
       </c>
       <c r="B639" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C639" s="7">
         <v>3</v>
@@ -13340,7 +13340,7 @@
         <v>362</v>
       </c>
       <c r="B640" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C640" s="7">
         <v>4</v>
@@ -13357,7 +13357,7 @@
         <v>362</v>
       </c>
       <c r="B641" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C641" s="7">
         <v>1</v>
@@ -13374,7 +13374,7 @@
         <v>362</v>
       </c>
       <c r="B642" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C642" s="7">
         <v>2</v>
@@ -13391,7 +13391,7 @@
         <v>362</v>
       </c>
       <c r="B643" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C643" s="7">
         <v>3</v>
@@ -13408,7 +13408,7 @@
         <v>362</v>
       </c>
       <c r="B644" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C644" s="7">
         <v>4</v>
@@ -13425,7 +13425,7 @@
         <v>362</v>
       </c>
       <c r="B645" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C645" s="7">
         <v>5</v>
@@ -13442,7 +13442,7 @@
         <v>362</v>
       </c>
       <c r="B646" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C646" s="7">
         <v>6</v>
@@ -13459,7 +13459,7 @@
         <v>362</v>
       </c>
       <c r="B647" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C647" s="7">
         <v>7</v>
@@ -13683,7 +13683,7 @@
         <v>153</v>
       </c>
       <c r="C660" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D660" s="7" t="s">
         <v>156</v>
@@ -13700,7 +13700,7 @@
         <v>153</v>
       </c>
       <c r="C661" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D661" s="7" t="s">
         <v>156</v>
@@ -13714,7 +13714,7 @@
         <v>362</v>
       </c>
       <c r="B662" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C662" s="7" t="s">
         <v>4</v>
@@ -13731,7 +13731,7 @@
         <v>362</v>
       </c>
       <c r="B663" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C663" s="7" t="s">
         <v>4</v>
@@ -13799,7 +13799,7 @@
         <v>362</v>
       </c>
       <c r="B667" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C667" s="7" t="s">
         <v>4</v>
@@ -13816,7 +13816,7 @@
         <v>362</v>
       </c>
       <c r="B668" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C668" s="7" t="s">
         <v>4</v>
@@ -13833,7 +13833,7 @@
         <v>362</v>
       </c>
       <c r="B669" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C669" s="7">
         <v>1</v>
@@ -13850,7 +13850,7 @@
         <v>362</v>
       </c>
       <c r="B670" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C670" s="7">
         <v>2</v>
@@ -13867,7 +13867,7 @@
         <v>362</v>
       </c>
       <c r="B671" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C671" s="7">
         <v>3</v>
@@ -13884,7 +13884,7 @@
         <v>362</v>
       </c>
       <c r="B672" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C672" s="7">
         <v>4</v>
@@ -13901,7 +13901,7 @@
         <v>362</v>
       </c>
       <c r="B673" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C673" s="7">
         <v>5</v>
@@ -13918,7 +13918,7 @@
         <v>362</v>
       </c>
       <c r="B674" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C674" s="7">
         <v>6</v>
@@ -13935,7 +13935,7 @@
         <v>362</v>
       </c>
       <c r="B675" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C675" s="7">
         <v>7</v>
@@ -13952,7 +13952,7 @@
         <v>362</v>
       </c>
       <c r="B676" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C676" s="7">
         <v>8</v>
@@ -13969,7 +13969,7 @@
         <v>362</v>
       </c>
       <c r="B677" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C677" s="7">
         <v>9</v>
@@ -13986,7 +13986,7 @@
         <v>362</v>
       </c>
       <c r="B678" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C678" s="7">
         <v>10</v>
@@ -14003,7 +14003,7 @@
         <v>362</v>
       </c>
       <c r="B679" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C679" s="7">
         <v>11</v>
@@ -14020,7 +14020,7 @@
         <v>362</v>
       </c>
       <c r="B680" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C680" s="7">
         <v>12</v>
@@ -14037,7 +14037,7 @@
         <v>362</v>
       </c>
       <c r="B681" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C681" s="7">
         <v>13</v>
@@ -14054,7 +14054,7 @@
         <v>362</v>
       </c>
       <c r="B682" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C682" s="7">
         <v>14</v>
@@ -14071,7 +14071,7 @@
         <v>362</v>
       </c>
       <c r="B683" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C683" s="7">
         <v>15</v>
@@ -14088,7 +14088,7 @@
         <v>362</v>
       </c>
       <c r="B684" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C684" s="7">
         <v>16</v>
@@ -14105,7 +14105,7 @@
         <v>362</v>
       </c>
       <c r="B685" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C685" s="7">
         <v>17</v>
@@ -14122,7 +14122,7 @@
         <v>362</v>
       </c>
       <c r="B686" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C686" s="7" t="s">
         <v>4</v>
@@ -14139,7 +14139,7 @@
         <v>362</v>
       </c>
       <c r="B687" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C687" s="7">
         <v>1</v>
@@ -14156,7 +14156,7 @@
         <v>362</v>
       </c>
       <c r="B688" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C688" s="7">
         <v>2</v>
@@ -14165,7 +14165,7 @@
         <v>139</v>
       </c>
       <c r="E688" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="689" spans="1:5" x14ac:dyDescent="0.25">
@@ -14173,7 +14173,7 @@
         <v>362</v>
       </c>
       <c r="B689" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C689" s="7">
         <v>3</v>
@@ -14190,7 +14190,7 @@
         <v>362</v>
       </c>
       <c r="B690" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C690" s="7">
         <v>4</v>
@@ -14207,7 +14207,7 @@
         <v>362</v>
       </c>
       <c r="B691" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C691" s="7">
         <v>5</v>
@@ -14530,7 +14530,7 @@
         <v>362</v>
       </c>
       <c r="B710" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C710" s="7" t="s">
         <v>4</v>
@@ -14615,7 +14615,7 @@
         <v>362</v>
       </c>
       <c r="B715" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C715" s="7" t="s">
         <v>4</v>
@@ -14632,7 +14632,7 @@
         <v>362</v>
       </c>
       <c r="B716" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C716" s="7" t="s">
         <v>4</v>
@@ -14683,7 +14683,7 @@
         <v>362</v>
       </c>
       <c r="B719" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C719" s="7" t="s">
         <v>4</v>
@@ -14700,7 +14700,7 @@
         <v>362</v>
       </c>
       <c r="B720" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C720" s="7" t="s">
         <v>4</v>
@@ -14717,7 +14717,7 @@
         <v>362</v>
       </c>
       <c r="B721" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C721" s="7">
         <v>1</v>
@@ -14734,7 +14734,7 @@
         <v>362</v>
       </c>
       <c r="B722" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C722" s="7">
         <v>2</v>
@@ -14751,7 +14751,7 @@
         <v>362</v>
       </c>
       <c r="B723" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C723" s="7">
         <v>3</v>
@@ -14768,7 +14768,7 @@
         <v>362</v>
       </c>
       <c r="B724" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C724" s="7">
         <v>4</v>
@@ -14785,7 +14785,7 @@
         <v>362</v>
       </c>
       <c r="B725" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C725" s="7">
         <v>5</v>
@@ -14802,7 +14802,7 @@
         <v>362</v>
       </c>
       <c r="B726" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C726" s="7">
         <v>6</v>
@@ -14819,7 +14819,7 @@
         <v>362</v>
       </c>
       <c r="B727" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C727" s="7">
         <v>7</v>
@@ -14836,7 +14836,7 @@
         <v>362</v>
       </c>
       <c r="B728" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C728" s="7">
         <v>8</v>
@@ -14853,7 +14853,7 @@
         <v>362</v>
       </c>
       <c r="B729" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C729" s="7">
         <v>9</v>
@@ -14870,7 +14870,7 @@
         <v>362</v>
       </c>
       <c r="B730" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C730" s="7">
         <v>10</v>
@@ -14887,7 +14887,7 @@
         <v>362</v>
       </c>
       <c r="B731" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C731" s="7">
         <v>11</v>
@@ -14904,7 +14904,7 @@
         <v>362</v>
       </c>
       <c r="B732" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C732" s="7">
         <v>12</v>
@@ -14921,7 +14921,7 @@
         <v>362</v>
       </c>
       <c r="B733" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C733" s="7">
         <v>13</v>
@@ -14938,7 +14938,7 @@
         <v>362</v>
       </c>
       <c r="B734" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C734" s="7">
         <v>14</v>
@@ -14955,7 +14955,7 @@
         <v>362</v>
       </c>
       <c r="B735" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C735" s="7">
         <v>15</v>
@@ -14972,7 +14972,7 @@
         <v>362</v>
       </c>
       <c r="B736" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C736" s="7">
         <v>16</v>
@@ -14989,7 +14989,7 @@
         <v>362</v>
       </c>
       <c r="B737" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C737" s="7">
         <v>17</v>
@@ -15006,7 +15006,7 @@
         <v>362</v>
       </c>
       <c r="B738" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C738" s="7">
         <v>18</v>
@@ -15023,7 +15023,7 @@
         <v>362</v>
       </c>
       <c r="B739" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C739" s="7">
         <v>19</v>
@@ -15040,7 +15040,7 @@
         <v>362</v>
       </c>
       <c r="B740" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C740" s="7">
         <v>20</v>
@@ -15057,7 +15057,7 @@
         <v>362</v>
       </c>
       <c r="B741" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C741" s="7">
         <v>1</v>
@@ -15074,7 +15074,7 @@
         <v>362</v>
       </c>
       <c r="B742" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C742" s="7">
         <v>2</v>
@@ -15091,7 +15091,7 @@
         <v>362</v>
       </c>
       <c r="B743" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C743" s="7">
         <v>3</v>
@@ -15108,7 +15108,7 @@
         <v>362</v>
       </c>
       <c r="B744" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C744" s="7">
         <v>4</v>
@@ -15125,7 +15125,7 @@
         <v>362</v>
       </c>
       <c r="B745" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C745" s="7">
         <v>5</v>
@@ -15142,7 +15142,7 @@
         <v>362</v>
       </c>
       <c r="B746" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C746" s="7">
         <v>6</v>
@@ -15159,7 +15159,7 @@
         <v>362</v>
       </c>
       <c r="B747" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C747" s="7">
         <v>7</v>
@@ -15176,7 +15176,7 @@
         <v>362</v>
       </c>
       <c r="B748" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C748" s="7">
         <v>8</v>
@@ -15193,7 +15193,7 @@
         <v>362</v>
       </c>
       <c r="B749" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C749" s="7">
         <v>9</v>
@@ -15210,7 +15210,7 @@
         <v>362</v>
       </c>
       <c r="B750" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C750" s="7">
         <v>10</v>
@@ -15227,7 +15227,7 @@
         <v>362</v>
       </c>
       <c r="B751" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C751" s="7">
         <v>11</v>
@@ -15244,7 +15244,7 @@
         <v>362</v>
       </c>
       <c r="B752" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C752" s="7">
         <v>12</v>
@@ -15261,7 +15261,7 @@
         <v>362</v>
       </c>
       <c r="B753" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C753" s="7">
         <v>13</v>
@@ -15278,7 +15278,7 @@
         <v>362</v>
       </c>
       <c r="B754" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C754" s="7">
         <v>14</v>
@@ -15295,7 +15295,7 @@
         <v>362</v>
       </c>
       <c r="B755" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C755" s="7">
         <v>15</v>
@@ -15312,7 +15312,7 @@
         <v>362</v>
       </c>
       <c r="B756" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C756" s="7">
         <v>16</v>
@@ -15329,7 +15329,7 @@
         <v>362</v>
       </c>
       <c r="B757" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C757" s="7">
         <v>17</v>
@@ -15346,7 +15346,7 @@
         <v>362</v>
       </c>
       <c r="B758" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C758" s="7">
         <v>18</v>
@@ -15363,7 +15363,7 @@
         <v>362</v>
       </c>
       <c r="B759" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C759" s="7">
         <v>19</v>
@@ -15380,7 +15380,7 @@
         <v>362</v>
       </c>
       <c r="B760" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C760" s="7">
         <v>20</v>
@@ -15397,7 +15397,7 @@
         <v>362</v>
       </c>
       <c r="B761" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C761" s="7" t="s">
         <v>4</v>
@@ -15414,7 +15414,7 @@
         <v>362</v>
       </c>
       <c r="B762" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C762" s="7" t="s">
         <v>4</v>
@@ -15431,7 +15431,7 @@
         <v>362</v>
       </c>
       <c r="B763" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C763" s="7" t="s">
         <v>4</v>
@@ -15448,7 +15448,7 @@
         <v>362</v>
       </c>
       <c r="B764" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C764" s="7" t="s">
         <v>4</v>
@@ -15465,7 +15465,7 @@
         <v>362</v>
       </c>
       <c r="B765" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C765" s="7" t="s">
         <v>4</v>
@@ -15482,7 +15482,7 @@
         <v>362</v>
       </c>
       <c r="B766" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C766" s="7" t="s">
         <v>4</v>
@@ -15618,7 +15618,7 @@
         <v>362</v>
       </c>
       <c r="B774" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C774" s="7" t="s">
         <v>4</v>
@@ -15635,7 +15635,7 @@
         <v>362</v>
       </c>
       <c r="B775" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C775" s="7" t="s">
         <v>4</v>
@@ -15669,10 +15669,10 @@
         <v>362</v>
       </c>
       <c r="B777" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C777" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D777" s="7" t="s">
         <v>284</v>
@@ -15686,10 +15686,10 @@
         <v>362</v>
       </c>
       <c r="B778" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C778" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="C778" s="7" t="s">
-        <v>396</v>
       </c>
       <c r="D778" s="7" t="s">
         <v>284</v>
@@ -15703,10 +15703,10 @@
         <v>362</v>
       </c>
       <c r="B779" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C779" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D779" s="7" t="s">
         <v>284</v>
@@ -15720,10 +15720,10 @@
         <v>362</v>
       </c>
       <c r="B780" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C780" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D780" s="7" t="s">
         <v>284</v>
@@ -15737,7 +15737,7 @@
         <v>362</v>
       </c>
       <c r="B781" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C781" s="7" t="s">
         <v>292</v>
@@ -15754,7 +15754,7 @@
         <v>362</v>
       </c>
       <c r="B782" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C782" s="7" t="s">
         <v>357</v>
@@ -15771,7 +15771,7 @@
         <v>362</v>
       </c>
       <c r="B783" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C783" s="7" t="s">
         <v>293</v>
@@ -15788,7 +15788,7 @@
         <v>362</v>
       </c>
       <c r="B784" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C784" s="7" t="s">
         <v>358</v>
@@ -15805,7 +15805,7 @@
         <v>362</v>
       </c>
       <c r="B785" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C785" s="7" t="s">
         <v>359</v>
@@ -15822,7 +15822,7 @@
         <v>362</v>
       </c>
       <c r="B786" s="7" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C786" s="7" t="s">
         <v>4</v>
@@ -15839,7 +15839,7 @@
         <v>362</v>
       </c>
       <c r="B787" s="7" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C787" s="7" t="s">
         <v>4</v>
@@ -15856,7 +15856,7 @@
         <v>362</v>
       </c>
       <c r="B788" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C788" s="7" t="s">
         <v>4</v>
@@ -15873,7 +15873,7 @@
         <v>362</v>
       </c>
       <c r="B789" s="7" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C789" s="7" t="s">
         <v>4</v>
@@ -15890,7 +15890,7 @@
         <v>362</v>
       </c>
       <c r="B790" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C790" s="7" t="s">
         <v>4</v>
@@ -15907,7 +15907,7 @@
         <v>362</v>
       </c>
       <c r="B791" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C791" s="7" t="s">
         <v>4</v>
@@ -15924,7 +15924,7 @@
         <v>362</v>
       </c>
       <c r="B792" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C792" s="7" t="s">
         <v>4</v>
@@ -15941,7 +15941,7 @@
         <v>362</v>
       </c>
       <c r="B793" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C793" s="7" t="s">
         <v>4</v>
@@ -15958,7 +15958,7 @@
         <v>362</v>
       </c>
       <c r="B794" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C794" s="7" t="s">
         <v>4</v>
@@ -15972,13 +15972,13 @@
     </row>
     <row r="795" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A795" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B795" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C795" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D795" s="1" t="s">
         <v>129</v>
@@ -15989,13 +15989,13 @@
     </row>
     <row r="796" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A796" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B796" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C796" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D796" s="1" t="s">
         <v>129</v>
@@ -16006,13 +16006,13 @@
     </row>
     <row r="797" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B797" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C797" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D797" s="1" t="s">
         <v>129</v>
@@ -16023,13 +16023,13 @@
     </row>
     <row r="798" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B798" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C798" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D798" s="1" t="s">
         <v>129</v>
@@ -16040,13 +16040,13 @@
     </row>
     <row r="799" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B799" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C799" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D799" s="1" t="s">
         <v>129</v>
@@ -16057,13 +16057,13 @@
     </row>
     <row r="800" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B800" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C800" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D800" s="1" t="s">
         <v>129</v>
@@ -16074,13 +16074,13 @@
     </row>
     <row r="801" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B801" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C801" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D801" s="1" t="s">
         <v>129</v>
@@ -16091,10 +16091,10 @@
     </row>
     <row r="802" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B802" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C802" s="1" t="s">
         <v>57</v>
@@ -16108,10 +16108,10 @@
     </row>
     <row r="803" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B803" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C803" s="1" t="s">
         <v>56</v>
@@ -16125,10 +16125,10 @@
     </row>
     <row r="804" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B804" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C804" s="1" t="s">
         <v>57</v>
@@ -16142,10 +16142,10 @@
     </row>
     <row r="805" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A805" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B805" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C805" s="1" t="s">
         <v>56</v>
@@ -16159,10 +16159,10 @@
     </row>
     <row r="806" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A806" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B806" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C806" s="1" t="s">
         <v>4</v>
@@ -16176,10 +16176,10 @@
     </row>
     <row r="807" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A807" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B807" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C807" s="1" t="s">
         <v>4</v>
@@ -16193,13 +16193,13 @@
     </row>
     <row r="808" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A808" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B808" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B808" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C808" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D808" s="1" t="s">
         <v>52</v>
@@ -16210,13 +16210,13 @@
     </row>
     <row r="809" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A809" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B809" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B809" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C809" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D809" s="1" t="s">
         <v>52</v>
@@ -16227,13 +16227,13 @@
     </row>
     <row r="810" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A810" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B810" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B810" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C810" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D810" s="1" t="s">
         <v>52</v>
@@ -16244,13 +16244,13 @@
     </row>
     <row r="811" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A811" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B811" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B811" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C811" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D811" s="1" t="s">
         <v>52</v>
@@ -16261,13 +16261,13 @@
     </row>
     <row r="812" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A812" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B812" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B812" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C812" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D812" s="1" t="s">
         <v>52</v>
@@ -16278,13 +16278,13 @@
     </row>
     <row r="813" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A813" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B813" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B813" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C813" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D813" s="1" t="s">
         <v>52</v>
@@ -16295,13 +16295,13 @@
     </row>
     <row r="814" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A814" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B814" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B814" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C814" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D814" s="1" t="s">
         <v>52</v>
@@ -16312,13 +16312,13 @@
     </row>
     <row r="815" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A815" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B815" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B815" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C815" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D815" s="1" t="s">
         <v>52</v>
@@ -16329,13 +16329,13 @@
     </row>
     <row r="816" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A816" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B816" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B816" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C816" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D816" s="1" t="s">
         <v>52</v>
@@ -16346,13 +16346,13 @@
     </row>
     <row r="817" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A817" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B817" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B817" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C817" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D817" s="1" t="s">
         <v>52</v>
@@ -16363,13 +16363,13 @@
     </row>
     <row r="818" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B818" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B818" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C818" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D818" s="1" t="s">
         <v>52</v>
@@ -16380,13 +16380,13 @@
     </row>
     <row r="819" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A819" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B819" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B819" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C819" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D819" s="1" t="s">
         <v>52</v>
@@ -16397,13 +16397,13 @@
     </row>
     <row r="820" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B820" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B820" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C820" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D820" s="1" t="s">
         <v>52</v>
@@ -16414,13 +16414,13 @@
     </row>
     <row r="821" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A821" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B821" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="B821" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="C821" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D821" s="1" t="s">
         <v>52</v>
@@ -16431,13 +16431,13 @@
     </row>
     <row r="822" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B822" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C822" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D822" s="1" t="s">
         <v>135</v>
@@ -16448,10 +16448,10 @@
     </row>
     <row r="823" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A823" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B823" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C823" s="1" t="s">
         <v>50</v>
@@ -16465,10 +16465,10 @@
     </row>
     <row r="824" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B824" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C824" s="1" t="s">
         <v>50</v>
@@ -16482,13 +16482,13 @@
     </row>
     <row r="825" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A825" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B825" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C825" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D825" s="1" t="s">
         <v>135</v>
@@ -16499,10 +16499,10 @@
     </row>
     <row r="826" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B826" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C826" s="1" t="s">
         <v>50</v>
@@ -16516,13 +16516,13 @@
     </row>
     <row r="827" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A827" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B827" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C827" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D827" s="1" t="s">
         <v>135</v>
@@ -16533,13 +16533,13 @@
     </row>
     <row r="828" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B828" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C828" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D828" s="1" t="s">
         <v>135</v>
@@ -16550,13 +16550,13 @@
     </row>
     <row r="829" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A829" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B829" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C829" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D829" s="1" t="s">
         <v>135</v>
@@ -16567,13 +16567,13 @@
     </row>
     <row r="830" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B830" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C830" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D830" s="1" t="s">
         <v>135</v>
@@ -16584,13 +16584,13 @@
     </row>
     <row r="831" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A831" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B831" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C831" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D831" s="1" t="s">
         <v>249</v>
@@ -16601,13 +16601,13 @@
     </row>
     <row r="832" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A832" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B832" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C832" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D832" s="1" t="s">
         <v>249</v>
@@ -16618,13 +16618,13 @@
     </row>
     <row r="833" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A833" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B833" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C833" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D833" s="1" t="s">
         <v>16</v>
@@ -16635,13 +16635,13 @@
     </row>
     <row r="834" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B834" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C834" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D834" s="1" t="s">
         <v>16</v>
@@ -16652,13 +16652,13 @@
     </row>
     <row r="835" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B835" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C835" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D835" s="1" t="s">
         <v>16</v>
@@ -16669,13 +16669,13 @@
     </row>
     <row r="836" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A836" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B836" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C836" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D836" s="1" t="s">
         <v>16</v>
@@ -16686,13 +16686,13 @@
     </row>
     <row r="837" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A837" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B837" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C837" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>16</v>
@@ -16703,13 +16703,13 @@
     </row>
     <row r="838" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B838" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C838" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>16</v>
@@ -16720,13 +16720,13 @@
     </row>
     <row r="839" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C839" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D839" s="1" t="s">
         <v>16</v>
@@ -16737,13 +16737,13 @@
     </row>
     <row r="840" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C840" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D840" s="1" t="s">
         <v>16</v>
@@ -16754,13 +16754,13 @@
     </row>
     <row r="841" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C841" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D841" s="1" t="s">
         <v>16</v>
@@ -16771,13 +16771,13 @@
     </row>
     <row r="842" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C842" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D842" s="1" t="s">
         <v>16</v>
@@ -16788,13 +16788,13 @@
     </row>
     <row r="843" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C843" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D843" s="1" t="s">
         <v>16</v>
@@ -16805,13 +16805,13 @@
     </row>
     <row r="844" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C844" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D844" s="1" t="s">
         <v>244</v>
@@ -16822,13 +16822,13 @@
     </row>
     <row r="845" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C845" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D845" s="1" t="s">
         <v>244</v>
@@ -16839,13 +16839,13 @@
     </row>
     <row r="846" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C846" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D846" s="1" t="s">
         <v>244</v>
@@ -16856,13 +16856,13 @@
     </row>
     <row r="847" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C847" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D847" s="1" t="s">
         <v>244</v>
@@ -16873,13 +16873,13 @@
     </row>
     <row r="848" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C848" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D848" s="1" t="s">
         <v>148</v>
@@ -16890,13 +16890,13 @@
     </row>
     <row r="849" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C849" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D849" s="1" t="s">
         <v>148</v>
@@ -16907,13 +16907,13 @@
     </row>
     <row r="850" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C850" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D850" s="1" t="s">
         <v>148</v>
@@ -16924,13 +16924,13 @@
     </row>
     <row r="851" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C851" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D851" s="1" t="s">
         <v>148</v>
@@ -16941,13 +16941,13 @@
     </row>
     <row r="852" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C852" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D852" s="1" t="s">
         <v>148</v>
@@ -16958,13 +16958,13 @@
     </row>
     <row r="853" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C853" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D853" s="1" t="s">
         <v>148</v>
@@ -16975,13 +16975,13 @@
     </row>
     <row r="854" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C854" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D854" s="1" t="s">
         <v>148</v>
@@ -16992,13 +16992,13 @@
     </row>
     <row r="855" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C855" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D855" s="1" t="s">
         <v>148</v>
@@ -17009,7 +17009,7 @@
     </row>
     <row r="856" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B856" s="1" t="s">
         <v>274</v>
@@ -17026,7 +17026,7 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A857" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B857" s="1" t="s">
         <v>274</v>
@@ -17043,13 +17043,13 @@
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A858" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B858" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C858" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D858" s="1" t="s">
         <v>225</v>
@@ -17060,13 +17060,13 @@
     </row>
     <row r="859" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A859" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B859" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C859" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D859" s="1" t="s">
         <v>225</v>
@@ -17077,13 +17077,13 @@
     </row>
     <row r="860" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A860" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B860" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C860" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D860" s="1" t="s">
         <v>225</v>
@@ -17094,13 +17094,13 @@
     </row>
     <row r="861" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A861" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B861" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C861" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="D861" s="1" t="s">
         <v>225</v>
@@ -17111,13 +17111,13 @@
     </row>
     <row r="862" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B862" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C862" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D862" s="1" t="s">
         <v>225</v>
@@ -17128,13 +17128,13 @@
     </row>
     <row r="863" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A863" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B863" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C863" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D863" s="1" t="s">
         <v>225</v>
@@ -17145,13 +17145,13 @@
     </row>
     <row r="864" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A864" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B864" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C864" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D864" s="1" t="s">
         <v>225</v>
@@ -17162,13 +17162,13 @@
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B865" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C865" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D865" s="1" t="s">
         <v>225</v>
@@ -17179,13 +17179,13 @@
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B866" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C866" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D866" s="1" t="s">
         <v>225</v>
@@ -17196,13 +17196,13 @@
     </row>
     <row r="867" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A867" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B867" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C867" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D867" s="1" t="s">
         <v>225</v>
@@ -17213,13 +17213,13 @@
     </row>
     <row r="868" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A868" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B868" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C868" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D868" s="1" t="s">
         <v>225</v>
@@ -17230,10 +17230,10 @@
     </row>
     <row r="869" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B869" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C869" s="1" t="s">
         <v>57</v>
@@ -17247,10 +17247,10 @@
     </row>
     <row r="870" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B870" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C870" s="1" t="s">
         <v>56</v>
@@ -17264,7 +17264,7 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B871" s="1" t="s">
         <v>78</v>
@@ -17281,7 +17281,7 @@
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A872" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B872" s="1" t="s">
         <v>79</v>
@@ -17298,7 +17298,7 @@
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A873" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B873" s="1" t="s">
         <v>5</v>
@@ -17315,10 +17315,10 @@
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B874" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C874" s="1" t="s">
         <v>57</v>
@@ -17332,10 +17332,10 @@
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B875" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C875" s="1" t="s">
         <v>56</v>
@@ -17349,10 +17349,10 @@
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B876" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C876" s="1" t="s">
         <v>4</v>
@@ -17366,7 +17366,7 @@
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A877" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B877" s="1" t="s">
         <v>94</v>
@@ -17383,7 +17383,7 @@
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A878" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B878" s="1" t="s">
         <v>96</v>
@@ -17400,13 +17400,13 @@
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B879" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C879" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D879" s="1" t="s">
         <v>40</v>
@@ -17417,13 +17417,13 @@
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B880" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C880" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D880" s="1" t="s">
         <v>40</v>
@@ -17434,13 +17434,13 @@
     </row>
     <row r="881" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B881" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C881" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D881" s="1" t="s">
         <v>40</v>
@@ -17451,13 +17451,13 @@
     </row>
     <row r="882" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B882" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C882" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D882" s="1" t="s">
         <v>40</v>
@@ -17468,13 +17468,13 @@
     </row>
     <row r="883" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A883" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B883" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C883" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D883" s="1" t="s">
         <v>40</v>
@@ -17485,13 +17485,13 @@
     </row>
     <row r="884" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A884" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B884" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C884" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D884" s="1" t="s">
         <v>40</v>
@@ -17502,13 +17502,13 @@
     </row>
     <row r="885" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A885" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B885" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C885" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D885" s="1" t="s">
         <v>40</v>
@@ -17519,13 +17519,13 @@
     </row>
     <row r="886" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A886" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B886" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C886" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D886" s="1" t="s">
         <v>40</v>
@@ -17536,13 +17536,13 @@
     </row>
     <row r="887" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B887" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C887" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D887" s="1" t="s">
         <v>40</v>
@@ -17553,13 +17553,13 @@
     </row>
     <row r="888" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B888" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C888" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D888" s="1" t="s">
         <v>40</v>
@@ -17570,13 +17570,13 @@
     </row>
     <row r="889" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A889" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B889" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C889" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D889" s="1" t="s">
         <v>40</v>
@@ -17587,13 +17587,13 @@
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A890" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B890" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C890" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D890" s="1" t="s">
         <v>40</v>
@@ -17604,13 +17604,13 @@
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A891" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B891" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C891" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D891" s="1" t="s">
         <v>40</v>
@@ -17621,47 +17621,47 @@
     </row>
     <row r="892" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A892" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B892" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C892" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D892" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E892" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="893" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D893" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E893" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B894" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C894" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D894" s="1" t="s">
         <v>139</v>
@@ -17672,13 +17672,13 @@
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A895" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B895" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C895" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D895" s="1" t="s">
         <v>37</v>
@@ -17689,13 +17689,13 @@
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A896" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B896" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C896" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D896" s="1" t="s">
         <v>37</v>
@@ -17706,13 +17706,13 @@
     </row>
     <row r="897" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A897" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B897" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C897" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D897" s="1" t="s">
         <v>37</v>
@@ -17723,13 +17723,13 @@
     </row>
     <row r="898" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A898" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B898" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C898" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D898" s="1" t="s">
         <v>37</v>
@@ -17740,13 +17740,13 @@
     </row>
     <row r="899" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B899" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C899" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D899" s="1" t="s">
         <v>37</v>
@@ -17757,13 +17757,13 @@
     </row>
     <row r="900" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B900" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C900" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D900" s="1" t="s">
         <v>37</v>
@@ -17774,13 +17774,13 @@
     </row>
     <row r="901" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A901" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B901" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C901" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D901" s="1" t="s">
         <v>37</v>
@@ -17791,13 +17791,13 @@
     </row>
     <row r="902" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A902" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B902" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C902" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D902" s="1" t="s">
         <v>37</v>
@@ -17808,13 +17808,13 @@
     </row>
     <row r="903" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A903" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B903" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C903" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D903" s="1" t="s">
         <v>37</v>
@@ -17825,13 +17825,13 @@
     </row>
     <row r="904" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A904" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B904" s="10" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C904" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D904" s="1" t="s">
         <v>37</v>
@@ -17842,10 +17842,10 @@
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B905" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C905" s="1" t="s">
         <v>56</v>
@@ -17859,10 +17859,10 @@
     </row>
     <row r="906" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A906" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B906" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C906" s="1" t="s">
         <v>57</v>
@@ -17876,13 +17876,13 @@
     </row>
     <row r="907" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A907" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B907" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C907" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D907" s="1" t="s">
         <v>160</v>
@@ -17893,10 +17893,10 @@
     </row>
     <row r="908" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A908" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B908" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C908" s="1" t="s">
         <v>56</v>
@@ -17910,10 +17910,10 @@
     </row>
     <row r="909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A909" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B909" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C909" s="1" t="s">
         <v>57</v>
@@ -17927,13 +17927,13 @@
     </row>
     <row r="910" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B910" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C910" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D910" s="1" t="s">
         <v>162</v>
@@ -17944,10 +17944,10 @@
     </row>
     <row r="911" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A911" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B911" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C911" s="1" t="s">
         <v>56</v>
@@ -17961,10 +17961,10 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B912" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C912" s="1" t="s">
         <v>57</v>
@@ -17978,13 +17978,13 @@
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A913" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B913" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C913" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D913" s="1" t="s">
         <v>164</v>
@@ -17995,10 +17995,10 @@
     </row>
     <row r="914" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A914" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B914" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C914" s="1" t="s">
         <v>56</v>
@@ -18012,10 +18012,10 @@
     </row>
     <row r="915" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B915" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C915" s="1" t="s">
         <v>57</v>
@@ -18029,13 +18029,13 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A916" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B916" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C916" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D916" s="1" t="s">
         <v>166</v>
@@ -18046,10 +18046,10 @@
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A917" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B917" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C917" s="1" t="s">
         <v>56</v>
@@ -18063,10 +18063,10 @@
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B918" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C918" s="1" t="s">
         <v>57</v>
@@ -18080,13 +18080,13 @@
     </row>
     <row r="919" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A919" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B919" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C919" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D919" s="1" t="s">
         <v>168</v>
@@ -18097,10 +18097,10 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A920" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B920" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C920" s="1" t="s">
         <v>4</v>
@@ -18114,13 +18114,13 @@
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B921" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C921" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D921" s="1" t="s">
         <v>236</v>
@@ -18131,13 +18131,13 @@
     </row>
     <row r="922" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A922" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B922" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C922" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D922" s="1" t="s">
         <v>236</v>
@@ -18148,27 +18148,27 @@
     </row>
     <row r="923" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A923" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B923" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C923" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D923" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E923" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="924" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A924" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B924" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C924" s="1" t="s">
         <v>4</v>
@@ -18182,10 +18182,10 @@
     </row>
     <row r="925" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A925" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B925" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C925" s="1" t="s">
         <v>4</v>
@@ -18199,13 +18199,13 @@
     </row>
     <row r="926" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A926" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B926" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C926" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D926" s="1" t="s">
         <v>60</v>
@@ -18216,13 +18216,13 @@
     </row>
     <row r="927" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B927" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C927" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D927" s="1" t="s">
         <v>60</v>
@@ -18233,13 +18233,13 @@
     </row>
     <row r="928" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A928" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B928" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C928" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D928" s="1" t="s">
         <v>60</v>
@@ -18250,13 +18250,13 @@
     </row>
     <row r="929" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A929" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B929" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C929" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D929" s="1" t="s">
         <v>60</v>
@@ -18267,13 +18267,13 @@
     </row>
     <row r="930" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B930" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C930" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D930" s="1" t="s">
         <v>60</v>
@@ -18284,13 +18284,13 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A931" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B931" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C931" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D931" s="1" t="s">
         <v>60</v>
@@ -18301,13 +18301,13 @@
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A932" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B932" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C932" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D932" s="1" t="s">
         <v>60</v>
@@ -18318,10 +18318,10 @@
     </row>
     <row r="933" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A933" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B933" s="5" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C933" s="1" t="s">
         <v>4</v>
@@ -18335,10 +18335,10 @@
     </row>
     <row r="934" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B934" s="5" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C934" s="1" t="s">
         <v>4</v>
@@ -18352,13 +18352,13 @@
     </row>
     <row r="935" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A935" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B935" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C935" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D935" s="1" t="s">
         <v>251</v>
@@ -18369,13 +18369,13 @@
     </row>
     <row r="936" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A936" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B936" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C936" s="1" t="s">
         <v>494</v>
-      </c>
-      <c r="C936" s="1" t="s">
-        <v>496</v>
       </c>
       <c r="D936" s="1" t="s">
         <v>251</v>
@@ -18386,13 +18386,13 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A937" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B937" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C937" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D937" s="1" t="s">
         <v>251</v>
@@ -18403,13 +18403,13 @@
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A938" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B938" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C938" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D938" s="1" t="s">
         <v>251</v>
@@ -18420,13 +18420,13 @@
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A939" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B939" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C939" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D939" s="1" t="s">
         <v>251</v>
@@ -18437,13 +18437,13 @@
     </row>
     <row r="940" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B940" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C940" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D940" s="1" t="s">
         <v>251</v>
@@ -18454,13 +18454,13 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B941" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C941" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D941" s="1" t="s">
         <v>251</v>
@@ -18471,13 +18471,13 @@
     </row>
     <row r="942" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A942" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B942" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C942" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D942" s="1" t="s">
         <v>251</v>
@@ -18488,13 +18488,13 @@
     </row>
     <row r="943" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A943" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B943" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C943" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D943" s="1" t="s">
         <v>251</v>
@@ -18505,13 +18505,13 @@
     </row>
     <row r="944" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A944" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B944" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C944" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D944" s="1" t="s">
         <v>251</v>
@@ -18522,13 +18522,13 @@
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A945" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B945" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C945" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D945" s="1" t="s">
         <v>251</v>
@@ -18539,13 +18539,13 @@
     </row>
     <row r="946" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A946" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B946" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C946" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D946" s="1" t="s">
         <v>251</v>
@@ -18556,13 +18556,13 @@
     </row>
     <row r="947" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A947" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B947" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C947" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D947" s="1" t="s">
         <v>251</v>
@@ -18573,13 +18573,13 @@
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A948" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B948" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C948" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D948" s="1" t="s">
         <v>251</v>
@@ -18590,13 +18590,13 @@
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B949" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C949" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D949" s="1" t="s">
         <v>251</v>
@@ -18607,13 +18607,13 @@
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A950" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B950" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C950" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D950" s="1" t="s">
         <v>251</v>
@@ -18624,13 +18624,13 @@
     </row>
     <row r="951" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B951" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C951" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D951" s="1" t="s">
         <v>251</v>
@@ -18641,13 +18641,13 @@
     </row>
     <row r="952" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B952" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C952" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D952" s="1" t="s">
         <v>251</v>
@@ -18658,13 +18658,13 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A953" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B953" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C953" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D953" s="1" t="s">
         <v>253</v>
@@ -18675,13 +18675,13 @@
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B954" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C954" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D954" s="1" t="s">
         <v>253</v>
@@ -18692,13 +18692,13 @@
     </row>
     <row r="955" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A955" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B955" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C955" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D955" s="1" t="s">
         <v>253</v>
@@ -18709,13 +18709,13 @@
     </row>
     <row r="956" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A956" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B956" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C956" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D956" s="1" t="s">
         <v>253</v>
@@ -18726,13 +18726,13 @@
     </row>
     <row r="957" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A957" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B957" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C957" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D957" s="1" t="s">
         <v>253</v>
@@ -18743,13 +18743,13 @@
     </row>
     <row r="958" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A958" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B958" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C958" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D958" s="1" t="s">
         <v>253</v>
@@ -18760,13 +18760,13 @@
     </row>
     <row r="959" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A959" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B959" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C959" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D959" s="1" t="s">
         <v>253</v>
@@ -18777,13 +18777,13 @@
     </row>
     <row r="960" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A960" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B960" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C960" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D960" s="1" t="s">
         <v>253</v>
@@ -18794,13 +18794,13 @@
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A961" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B961" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C961" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D961" s="1" t="s">
         <v>253</v>
@@ -18811,13 +18811,13 @@
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A962" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B962" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C962" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D962" s="1" t="s">
         <v>253</v>
@@ -18828,13 +18828,13 @@
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A963" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B963" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C963" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D963" s="1" t="s">
         <v>253</v>
@@ -18845,13 +18845,13 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B964" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C964" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D964" s="1" t="s">
         <v>253</v>
@@ -18862,13 +18862,13 @@
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B965" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C965" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D965" s="1" t="s">
         <v>253</v>
@@ -18879,13 +18879,13 @@
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A966" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B966" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C966" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D966" s="1" t="s">
         <v>253</v>
@@ -18896,13 +18896,13 @@
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A967" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B967" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C967" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D967" s="1" t="s">
         <v>253</v>
@@ -18913,13 +18913,13 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B968" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C968" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D968" s="1" t="s">
         <v>253</v>
@@ -18930,13 +18930,13 @@
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B969" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C969" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D969" s="1" t="s">
         <v>253</v>
@@ -18947,13 +18947,13 @@
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A970" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B970" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C970" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D970" s="1" t="s">
         <v>253</v>
@@ -18964,13 +18964,13 @@
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A971" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B971" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C971" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D971" s="1" t="s">
         <v>253</v>
@@ -18981,13 +18981,13 @@
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A972" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B972" s="10" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C972" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D972" s="1" t="s">
         <v>253</v>
@@ -18998,10 +18998,10 @@
     </row>
     <row r="973" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A973" s="5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B973" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C973" s="5" t="s">
         <v>4</v>
@@ -19015,10 +19015,10 @@
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B974" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C974" s="1" t="s">
         <v>4</v>
@@ -19032,10 +19032,10 @@
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B975" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C975" s="1" t="s">
         <v>4</v>
@@ -19049,10 +19049,10 @@
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B976" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C976" s="1" t="s">
         <v>4</v>
@@ -19066,10 +19066,10 @@
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A977" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B977" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C977" s="1" t="s">
         <v>4</v>
@@ -19083,10 +19083,10 @@
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B978" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C978" s="1" t="s">
         <v>4</v>
@@ -19100,13 +19100,13 @@
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B979" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C979" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D979" s="1" t="s">
         <v>9</v>
@@ -19117,13 +19117,13 @@
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B980" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C980" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D980" s="1" t="s">
         <v>9</v>
@@ -19134,13 +19134,13 @@
     </row>
     <row r="981" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A981" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B981" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C981" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D981" s="1" t="s">
         <v>9</v>
@@ -19151,13 +19151,13 @@
     </row>
     <row r="982" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B982" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C982" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D982" s="1" t="s">
         <v>9</v>
@@ -19168,13 +19168,13 @@
     </row>
     <row r="983" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B983" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C983" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D983" s="1" t="s">
         <v>9</v>
@@ -19185,13 +19185,13 @@
     </row>
     <row r="984" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B984" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C984" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D984" s="1" t="s">
         <v>9</v>
@@ -19202,13 +19202,13 @@
     </row>
     <row r="985" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A985" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B985" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C985" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D985" s="1" t="s">
         <v>9</v>
@@ -19219,13 +19219,13 @@
     </row>
     <row r="986" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B986" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C986" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D986" s="1" t="s">
         <v>9</v>
@@ -19236,13 +19236,13 @@
     </row>
     <row r="987" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B987" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C987" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D987" s="1" t="s">
         <v>9</v>
@@ -19253,13 +19253,13 @@
     </row>
     <row r="988" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B988" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C988" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D988" s="1" t="s">
         <v>9</v>
@@ -19270,13 +19270,13 @@
     </row>
     <row r="989" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A989" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B989" s="10" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C989" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D989" s="1" t="s">
         <v>9</v>
@@ -19287,10 +19287,10 @@
     </row>
     <row r="990" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B990" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C990" s="1" t="s">
         <v>57</v>
@@ -19304,10 +19304,10 @@
     </row>
     <row r="991" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B991" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C991" s="1" t="s">
         <v>56</v>
@@ -19321,10 +19321,10 @@
     </row>
     <row r="992" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A992" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B992" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C992" s="1" t="s">
         <v>4</v>
@@ -19338,10 +19338,10 @@
     </row>
     <row r="993" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B993" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C993" s="1" t="s">
         <v>4</v>
@@ -19355,7 +19355,7 @@
     </row>
     <row r="994" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B994" s="1" t="s">
         <v>6</v>
@@ -19372,13 +19372,13 @@
     </row>
     <row r="995" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A995" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B995" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C995" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D995" s="1" t="s">
         <v>284</v>
@@ -19389,13 +19389,13 @@
     </row>
     <row r="996" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B996" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C996" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D996" s="1" t="s">
         <v>284</v>
@@ -19406,13 +19406,13 @@
     </row>
     <row r="997" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B997" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C997" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D997" s="1" t="s">
         <v>284</v>
@@ -19423,10 +19423,10 @@
     </row>
     <row r="998" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A998" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B998" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D998" s="1" t="s">
         <v>291</v>
@@ -19437,13 +19437,13 @@
     </row>
     <row r="999" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B999" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C999" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D999" s="1" t="s">
         <v>291</v>
@@ -19454,10 +19454,10 @@
     </row>
     <row r="1000" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1000" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C1000" s="1" t="s">
         <v>187</v>
@@ -19471,13 +19471,13 @@
     </row>
     <row r="1001" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1001" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1001" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C1001" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D1001" s="1" t="s">
         <v>291</v>
@@ -19488,13 +19488,13 @@
     </row>
     <row r="1002" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1002" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C1002" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D1002" s="1" t="s">
         <v>291</v>
@@ -19505,10 +19505,10 @@
     </row>
     <row r="1003" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1003" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C1003" s="1" t="s">
         <v>4</v>
@@ -19522,10 +19522,10 @@
     </row>
     <row r="1004" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1004" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1004" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C1004" s="1" t="s">
         <v>4</v>
@@ -19539,10 +19539,10 @@
     </row>
     <row r="1005" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1005" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1005" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C1005" s="1" t="s">
         <v>4</v>
@@ -19556,10 +19556,10 @@
     </row>
     <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1006" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C1006" s="1" t="s">
         <v>4</v>
@@ -19573,10 +19573,10 @@
     </row>
     <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1007" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1007" s="5" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C1007" s="1" t="s">
         <v>4</v>
@@ -19590,10 +19590,10 @@
     </row>
     <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1008" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1008" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C1008" s="1" t="s">
         <v>4</v>
@@ -19607,10 +19607,10 @@
     </row>
     <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1009" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1009" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C1009" s="1" t="s">
         <v>4</v>
@@ -19624,10 +19624,10 @@
     </row>
     <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1010" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1010" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C1010" s="1" t="s">
         <v>4</v>
@@ -19641,10 +19641,10 @@
     </row>
     <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1011" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1011" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C1011" s="1" t="s">
         <v>4</v>
@@ -19658,16 +19658,16 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1012" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1012" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C1012" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D1012" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E1012" s="1" t="s">
         <v>144</v>
@@ -19675,61 +19675,61 @@
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1013" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1013" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C1013" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="C1013" s="1" t="s">
+      <c r="D1013" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D1013" s="1" t="s">
-        <v>472</v>
-      </c>
       <c r="E1013" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1014" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C1014" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D1014" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1014" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="D1014" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="E1014" s="1" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1015" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C1015" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D1015" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E1015" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="1016" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1016" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1016" s="5" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C1016" s="5" t="s">
         <v>4</v>
@@ -19743,10 +19743,10 @@
     </row>
     <row r="1017" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1017" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1017" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C1017" s="1">
         <v>0</v>
@@ -19760,10 +19760,10 @@
     </row>
     <row r="1018" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1018" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1018" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C1018" s="1">
         <v>1</v>
@@ -19777,10 +19777,10 @@
     </row>
     <row r="1019" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1019" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1019" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C1019" s="1">
         <v>2</v>
@@ -19794,10 +19794,10 @@
     </row>
     <row r="1020" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1020" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1020" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C1020" s="1">
         <v>3</v>
@@ -19811,10 +19811,10 @@
     </row>
     <row r="1021" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1021" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1021" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C1021" s="1">
         <v>4</v>
@@ -19828,10 +19828,10 @@
     </row>
     <row r="1022" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1022" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1022" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C1022" s="1">
         <v>0</v>
@@ -19845,10 +19845,10 @@
     </row>
     <row r="1023" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1023" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1023" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C1023" s="1">
         <v>1</v>
@@ -19862,10 +19862,10 @@
     </row>
     <row r="1024" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1024" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1024" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C1024" s="1">
         <v>2</v>
@@ -19879,10 +19879,10 @@
     </row>
     <row r="1025" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1025" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1025" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C1025" s="1">
         <v>3</v>
@@ -19896,10 +19896,10 @@
     </row>
     <row r="1026" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1026" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C1026" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
Updated data dictionary for Muni (date fields) and VTA
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sisrae\Documents\GitHub\onboard-surveys\make-uniform\production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzorn\Documents\onboard-surveys\make-uniform\production\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6663" uniqueCount="644">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -2176,6 +2176,12 @@
   </si>
   <si>
     <t>AC Transit Monthly Pass on Clipper</t>
+  </si>
+  <si>
+    <t>completed_date</t>
+  </si>
+  <si>
+    <t>completed_time</t>
   </si>
 </sst>
 </file>
@@ -2696,8 +2702,8 @@
   <dimension ref="A1:F1521"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1513" sqref="B1513"/>
+      <pane ySplit="1" topLeftCell="A1493" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1323" sqref="B1323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -22734,7 +22740,7 @@
         <v>610</v>
       </c>
       <c r="B1178" s="12" t="s">
-        <v>520</v>
+        <v>642</v>
       </c>
       <c r="C1178" s="12" t="s">
         <v>4</v>
@@ -22754,7 +22760,7 @@
         <v>610</v>
       </c>
       <c r="B1179" s="12" t="s">
-        <v>521</v>
+        <v>643</v>
       </c>
       <c r="C1179" s="12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Remove depart hour and return hour variables for VTA
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Dictionary" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dictionary!$A$1:$E$1963</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dictionary!$A$1:$E$1887</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6629" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6485" uniqueCount="647">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -2182,114 +2182,6 @@
   </si>
   <si>
     <t>completed_time</t>
-  </si>
-  <si>
-    <t>1 - 5 am</t>
-  </si>
-  <si>
-    <t>5 - 6 am</t>
-  </si>
-  <si>
-    <t>6 - 7 am</t>
-  </si>
-  <si>
-    <t>7 - 8 am</t>
-  </si>
-  <si>
-    <t>8 - 9 am</t>
-  </si>
-  <si>
-    <t>9 - 10 am</t>
-  </si>
-  <si>
-    <t>10 - 11 am</t>
-  </si>
-  <si>
-    <t>11 am  - 12 pm</t>
-  </si>
-  <si>
-    <t>12 - 1 pm</t>
-  </si>
-  <si>
-    <t>1 - 2 pm</t>
-  </si>
-  <si>
-    <t>2 - 3 pm</t>
-  </si>
-  <si>
-    <t>3 - 4 pm</t>
-  </si>
-  <si>
-    <t>4 - 5 pm</t>
-  </si>
-  <si>
-    <t>5 - 6 pm</t>
-  </si>
-  <si>
-    <t>6 - 7 pm</t>
-  </si>
-  <si>
-    <t>7 - 8 pm</t>
-  </si>
-  <si>
-    <t>8 - 9 pm</t>
-  </si>
-  <si>
-    <t>9 - 10 pm</t>
-  </si>
-  <si>
-    <t>10 - 11 pm</t>
-  </si>
-  <si>
-    <t>11 pm - 12 am</t>
-  </si>
-  <si>
-    <t>Before 6:30 am</t>
-  </si>
-  <si>
-    <t>6:30 - 7:30 am</t>
-  </si>
-  <si>
-    <t>7:30 - 8:30 am</t>
-  </si>
-  <si>
-    <t>8:30 - 9:30 am</t>
-  </si>
-  <si>
-    <t>9:30 - 10:30 am</t>
-  </si>
-  <si>
-    <t>10:30 - 11:30 am</t>
-  </si>
-  <si>
-    <t>11:30 am - 12:30 pm</t>
-  </si>
-  <si>
-    <t>12:30 - 1:30 pm</t>
-  </si>
-  <si>
-    <t>1:30 - 2:30 pm</t>
-  </si>
-  <si>
-    <t>2:30 - 3:30 pm</t>
-  </si>
-  <si>
-    <t>3:30 - 4:30 pm</t>
-  </si>
-  <si>
-    <t>4:30 - 5:30 pm</t>
-  </si>
-  <si>
-    <t>5:30 - 6:30 pm</t>
-  </si>
-  <si>
-    <t>6:30 - 7:30 pm</t>
-  </si>
-  <si>
-    <t>7:30 - 9:00 pm</t>
-  </si>
-  <si>
-    <t>After 9:00 pm</t>
   </si>
   <si>
     <t>bie</t>
@@ -2862,11 +2754,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1963"/>
+  <dimension ref="A1:F1887"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1474" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1496" sqref="B1496"/>
+      <pane ySplit="1" topLeftCell="A1152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1269" sqref="B1269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20366,7 +20258,7 @@
         <v>129</v>
       </c>
       <c r="E1029" s="13" t="s">
-        <v>679</v>
+        <v>643</v>
       </c>
     </row>
     <row r="1030" spans="1:5" x14ac:dyDescent="0.2">
@@ -23927,7 +23819,7 @@
         <v>610</v>
       </c>
       <c r="B1239" s="13" t="s">
-        <v>680</v>
+        <v>644</v>
       </c>
       <c r="C1239" s="13" t="s">
         <v>616</v>
@@ -23944,7 +23836,7 @@
         <v>610</v>
       </c>
       <c r="B1240" s="13" t="s">
-        <v>680</v>
+        <v>644</v>
       </c>
       <c r="C1240" s="13" t="s">
         <v>617</v>
@@ -23961,7 +23853,7 @@
         <v>610</v>
       </c>
       <c r="B1241" s="13" t="s">
-        <v>680</v>
+        <v>644</v>
       </c>
       <c r="C1241" s="13" t="s">
         <v>393</v>
@@ -24214,7 +24106,7 @@
         <v>610</v>
       </c>
       <c r="B1256" s="14" t="s">
-        <v>682</v>
+        <v>646</v>
       </c>
       <c r="C1256" s="13" t="s">
         <v>4</v>
@@ -27019,15 +26911,15 @@
         <v>619</v>
       </c>
       <c r="B1421" s="17" t="s">
-        <v>251</v>
+        <v>592</v>
       </c>
       <c r="C1421" s="17" t="s">
-        <v>643</v>
+        <v>4</v>
       </c>
       <c r="D1421" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1421" s="17">
+        <v>117</v>
+      </c>
+      <c r="E1421" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -27036,16 +26928,16 @@
         <v>619</v>
       </c>
       <c r="B1422" s="17" t="s">
-        <v>251</v>
+        <v>593</v>
       </c>
       <c r="C1422" s="17" t="s">
-        <v>644</v>
+        <v>4</v>
       </c>
       <c r="D1422" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1422" s="17">
-        <v>5</v>
+        <v>119</v>
+      </c>
+      <c r="E1422" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1423" spans="1:5" x14ac:dyDescent="0.2">
@@ -27053,16 +26945,16 @@
         <v>619</v>
       </c>
       <c r="B1423" s="17" t="s">
-        <v>251</v>
+        <v>594</v>
       </c>
       <c r="C1423" s="17" t="s">
-        <v>645</v>
+        <v>4</v>
       </c>
       <c r="D1423" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1423" s="17">
-        <v>6</v>
+        <v>121</v>
+      </c>
+      <c r="E1423" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1424" spans="1:5" x14ac:dyDescent="0.2">
@@ -27070,16 +26962,16 @@
         <v>619</v>
       </c>
       <c r="B1424" s="17" t="s">
-        <v>251</v>
+        <v>595</v>
       </c>
       <c r="C1424" s="17" t="s">
-        <v>646</v>
+        <v>4</v>
       </c>
       <c r="D1424" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1424" s="17">
-        <v>7</v>
+        <v>123</v>
+      </c>
+      <c r="E1424" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1425" spans="1:5" x14ac:dyDescent="0.2">
@@ -27087,16 +26979,16 @@
         <v>619</v>
       </c>
       <c r="B1425" s="17" t="s">
-        <v>251</v>
+        <v>596</v>
       </c>
       <c r="C1425" s="17" t="s">
-        <v>647</v>
+        <v>4</v>
       </c>
       <c r="D1425" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1425" s="17">
-        <v>8</v>
+        <v>126</v>
+      </c>
+      <c r="E1425" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1426" spans="1:5" x14ac:dyDescent="0.2">
@@ -27104,16 +26996,16 @@
         <v>619</v>
       </c>
       <c r="B1426" s="17" t="s">
-        <v>251</v>
+        <v>597</v>
       </c>
       <c r="C1426" s="17" t="s">
-        <v>648</v>
+        <v>4</v>
       </c>
       <c r="D1426" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1426" s="17">
-        <v>9</v>
+        <v>127</v>
+      </c>
+      <c r="E1426" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1427" spans="1:5" x14ac:dyDescent="0.2">
@@ -27121,15 +27013,15 @@
         <v>619</v>
       </c>
       <c r="B1427" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1427" s="17" t="s">
-        <v>649</v>
+        <v>515</v>
       </c>
       <c r="D1427" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1427" s="17">
+        <v>9</v>
+      </c>
+      <c r="E1427" s="17" t="s">
         <v>10</v>
       </c>
     </row>
@@ -27138,16 +27030,16 @@
         <v>619</v>
       </c>
       <c r="B1428" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1428" s="17" t="s">
-        <v>650</v>
+        <v>472</v>
       </c>
       <c r="D1428" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1428" s="17">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E1428" s="17" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="1429" spans="1:5" x14ac:dyDescent="0.2">
@@ -27155,16 +27047,16 @@
         <v>619</v>
       </c>
       <c r="B1429" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1429" s="17" t="s">
-        <v>651</v>
+        <v>473</v>
       </c>
       <c r="D1429" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1429" s="17">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="E1429" s="17" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="1430" spans="1:5" x14ac:dyDescent="0.2">
@@ -27172,16 +27064,16 @@
         <v>619</v>
       </c>
       <c r="B1430" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1430" s="17" t="s">
-        <v>652</v>
+        <v>474</v>
       </c>
       <c r="D1430" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1430" s="17">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E1430" s="17" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="1431" spans="1:5" x14ac:dyDescent="0.2">
@@ -27189,16 +27081,16 @@
         <v>619</v>
       </c>
       <c r="B1431" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1431" s="17" t="s">
-        <v>653</v>
+        <v>475</v>
       </c>
       <c r="D1431" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1431" s="17">
-        <v>14</v>
+        <v>9</v>
+      </c>
+      <c r="E1431" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1432" spans="1:5" x14ac:dyDescent="0.2">
@@ -27206,15 +27098,15 @@
         <v>619</v>
       </c>
       <c r="B1432" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1432" s="17" t="s">
-        <v>654</v>
+        <v>476</v>
       </c>
       <c r="D1432" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1432" s="17">
+        <v>9</v>
+      </c>
+      <c r="E1432" s="17" t="s">
         <v>15</v>
       </c>
     </row>
@@ -27223,16 +27115,16 @@
         <v>619</v>
       </c>
       <c r="B1433" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1433" s="17" t="s">
-        <v>655</v>
+        <v>477</v>
       </c>
       <c r="D1433" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1433" s="17">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="E1433" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1434" spans="1:5" x14ac:dyDescent="0.2">
@@ -27240,16 +27132,16 @@
         <v>619</v>
       </c>
       <c r="B1434" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1434" s="17" t="s">
-        <v>656</v>
+        <v>478</v>
       </c>
       <c r="D1434" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1434" s="17">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="E1434" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1435" spans="1:5" x14ac:dyDescent="0.2">
@@ -27257,16 +27149,16 @@
         <v>619</v>
       </c>
       <c r="B1435" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1435" s="17" t="s">
-        <v>657</v>
+        <v>479</v>
       </c>
       <c r="D1435" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1435" s="17">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="E1435" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1436" spans="1:5" x14ac:dyDescent="0.2">
@@ -27274,16 +27166,16 @@
         <v>619</v>
       </c>
       <c r="B1436" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1436" s="17" t="s">
-        <v>658</v>
+        <v>480</v>
       </c>
       <c r="D1436" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1436" s="17">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="E1436" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1437" spans="1:5" x14ac:dyDescent="0.2">
@@ -27291,16 +27183,16 @@
         <v>619</v>
       </c>
       <c r="B1437" s="17" t="s">
-        <v>251</v>
+        <v>9</v>
       </c>
       <c r="C1437" s="17" t="s">
-        <v>659</v>
+        <v>615</v>
       </c>
       <c r="D1437" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1437" s="17">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="E1437" s="17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="1438" spans="1:5" x14ac:dyDescent="0.2">
@@ -27308,16 +27200,16 @@
         <v>619</v>
       </c>
       <c r="B1438" s="17" t="s">
-        <v>251</v>
+        <v>72</v>
       </c>
       <c r="C1438" s="17" t="s">
-        <v>660</v>
+        <v>57</v>
       </c>
       <c r="D1438" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1438" s="17">
-        <v>21</v>
+        <v>72</v>
+      </c>
+      <c r="E1438" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="1439" spans="1:5" x14ac:dyDescent="0.2">
@@ -27325,16 +27217,16 @@
         <v>619</v>
       </c>
       <c r="B1439" s="17" t="s">
-        <v>251</v>
+        <v>72</v>
       </c>
       <c r="C1439" s="17" t="s">
-        <v>661</v>
+        <v>56</v>
       </c>
       <c r="D1439" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1439" s="17">
-        <v>22</v>
+        <v>72</v>
+      </c>
+      <c r="E1439" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="1440" spans="1:5" x14ac:dyDescent="0.2">
@@ -27342,16 +27234,16 @@
         <v>619</v>
       </c>
       <c r="B1440" s="17" t="s">
-        <v>251</v>
+        <v>81</v>
       </c>
       <c r="C1440" s="17" t="s">
-        <v>662</v>
+        <v>4</v>
       </c>
       <c r="D1440" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1440" s="17">
-        <v>23</v>
+        <v>81</v>
+      </c>
+      <c r="E1440" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1441" spans="1:5" x14ac:dyDescent="0.2">
@@ -27359,16 +27251,16 @@
         <v>619</v>
       </c>
       <c r="B1441" s="17" t="s">
-        <v>253</v>
+        <v>85</v>
       </c>
       <c r="C1441" s="17" t="s">
-        <v>663</v>
+        <v>4</v>
       </c>
       <c r="D1441" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1441" s="17">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="E1441" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1442" spans="1:5" x14ac:dyDescent="0.2">
@@ -27376,16 +27268,16 @@
         <v>619</v>
       </c>
       <c r="B1442" s="17" t="s">
-        <v>253</v>
+        <v>7</v>
       </c>
       <c r="C1442" s="17" t="s">
-        <v>664</v>
+        <v>4</v>
       </c>
       <c r="D1442" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1442" s="17">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E1442" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1443" spans="1:5" x14ac:dyDescent="0.2">
@@ -27393,16 +27285,16 @@
         <v>619</v>
       </c>
       <c r="B1443" s="17" t="s">
-        <v>253</v>
+        <v>644</v>
       </c>
       <c r="C1443" s="17" t="s">
-        <v>665</v>
+        <v>616</v>
       </c>
       <c r="D1443" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1443" s="17">
-        <v>7</v>
+        <v>284</v>
+      </c>
+      <c r="E1443" s="17" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="1444" spans="1:5" x14ac:dyDescent="0.2">
@@ -27410,16 +27302,16 @@
         <v>619</v>
       </c>
       <c r="B1444" s="17" t="s">
-        <v>253</v>
+        <v>644</v>
       </c>
       <c r="C1444" s="17" t="s">
-        <v>666</v>
+        <v>645</v>
       </c>
       <c r="D1444" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1444" s="17">
-        <v>8</v>
+        <v>284</v>
+      </c>
+      <c r="E1444" s="17" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="1445" spans="1:5" x14ac:dyDescent="0.2">
@@ -27427,16 +27319,16 @@
         <v>619</v>
       </c>
       <c r="B1445" s="17" t="s">
-        <v>253</v>
+        <v>644</v>
       </c>
       <c r="C1445" s="17" t="s">
-        <v>667</v>
+        <v>393</v>
       </c>
       <c r="D1445" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1445" s="17">
-        <v>9</v>
+        <v>284</v>
+      </c>
+      <c r="E1445" s="17" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="1446" spans="1:5" x14ac:dyDescent="0.2">
@@ -27444,16 +27336,14 @@
         <v>619</v>
       </c>
       <c r="B1446" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1446" s="17" t="s">
-        <v>668</v>
-      </c>
+        <v>598</v>
+      </c>
+      <c r="C1446" s="17"/>
       <c r="D1446" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1446" s="17">
-        <v>10</v>
+        <v>291</v>
+      </c>
+      <c r="E1446" s="17" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="1447" spans="1:5" x14ac:dyDescent="0.2">
@@ -27461,16 +27351,16 @@
         <v>619</v>
       </c>
       <c r="B1447" s="17" t="s">
-        <v>253</v>
+        <v>598</v>
       </c>
       <c r="C1447" s="17" t="s">
-        <v>669</v>
+        <v>292</v>
       </c>
       <c r="D1447" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1447" s="17">
-        <v>11</v>
+        <v>291</v>
+      </c>
+      <c r="E1447" s="17" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="1448" spans="1:5" x14ac:dyDescent="0.2">
@@ -27478,16 +27368,16 @@
         <v>619</v>
       </c>
       <c r="B1448" s="17" t="s">
-        <v>253</v>
+        <v>598</v>
       </c>
       <c r="C1448" s="17" t="s">
-        <v>670</v>
+        <v>293</v>
       </c>
       <c r="D1448" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1448" s="17">
-        <v>12</v>
+        <v>291</v>
+      </c>
+      <c r="E1448" s="17" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="1449" spans="1:5" x14ac:dyDescent="0.2">
@@ -27495,16 +27385,16 @@
         <v>619</v>
       </c>
       <c r="B1449" s="17" t="s">
-        <v>253</v>
+        <v>598</v>
       </c>
       <c r="C1449" s="17" t="s">
-        <v>671</v>
+        <v>599</v>
       </c>
       <c r="D1449" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1449" s="17">
-        <v>13</v>
+        <v>291</v>
+      </c>
+      <c r="E1449" s="17" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="1450" spans="1:5" x14ac:dyDescent="0.2">
@@ -27512,16 +27402,16 @@
         <v>619</v>
       </c>
       <c r="B1450" s="17" t="s">
-        <v>253</v>
+        <v>598</v>
       </c>
       <c r="C1450" s="17" t="s">
-        <v>672</v>
+        <v>600</v>
       </c>
       <c r="D1450" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1450" s="17">
-        <v>14</v>
+        <v>291</v>
+      </c>
+      <c r="E1450" s="17" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="1451" spans="1:5" x14ac:dyDescent="0.2">
@@ -27529,16 +27419,16 @@
         <v>619</v>
       </c>
       <c r="B1451" s="17" t="s">
-        <v>253</v>
+        <v>598</v>
       </c>
       <c r="C1451" s="17" t="s">
-        <v>673</v>
+        <v>451</v>
       </c>
       <c r="D1451" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1451" s="17">
-        <v>15</v>
+        <v>291</v>
+      </c>
+      <c r="E1451" s="17" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="1452" spans="1:5" x14ac:dyDescent="0.2">
@@ -27546,16 +27436,16 @@
         <v>619</v>
       </c>
       <c r="B1452" s="17" t="s">
-        <v>253</v>
+        <v>598</v>
       </c>
       <c r="C1452" s="17" t="s">
-        <v>674</v>
+        <v>359</v>
       </c>
       <c r="D1452" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1452" s="17">
-        <v>16</v>
+        <v>291</v>
+      </c>
+      <c r="E1452" s="17" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="1453" spans="1:5" x14ac:dyDescent="0.2">
@@ -27563,16 +27453,16 @@
         <v>619</v>
       </c>
       <c r="B1453" s="17" t="s">
-        <v>253</v>
+        <v>110</v>
       </c>
       <c r="C1453" s="17" t="s">
-        <v>675</v>
+        <v>4</v>
       </c>
       <c r="D1453" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1453" s="17">
-        <v>17</v>
+        <v>110</v>
+      </c>
+      <c r="E1453" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1454" spans="1:5" x14ac:dyDescent="0.2">
@@ -27580,16 +27470,16 @@
         <v>619</v>
       </c>
       <c r="B1454" s="17" t="s">
-        <v>253</v>
+        <v>111</v>
       </c>
       <c r="C1454" s="17" t="s">
-        <v>676</v>
+        <v>4</v>
       </c>
       <c r="D1454" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1454" s="17">
-        <v>18</v>
+        <v>111</v>
+      </c>
+      <c r="E1454" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1455" spans="1:5" x14ac:dyDescent="0.2">
@@ -27597,16 +27487,16 @@
         <v>619</v>
       </c>
       <c r="B1455" s="17" t="s">
-        <v>253</v>
+        <v>108</v>
       </c>
       <c r="C1455" s="17" t="s">
-        <v>677</v>
+        <v>4</v>
       </c>
       <c r="D1455" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1455" s="17">
-        <v>20</v>
+        <v>108</v>
+      </c>
+      <c r="E1455" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1456" spans="1:5" x14ac:dyDescent="0.2">
@@ -27614,16 +27504,16 @@
         <v>619</v>
       </c>
       <c r="B1456" s="17" t="s">
-        <v>253</v>
+        <v>109</v>
       </c>
       <c r="C1456" s="17" t="s">
-        <v>678</v>
+        <v>4</v>
       </c>
       <c r="D1456" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E1456" s="17">
-        <v>21</v>
+        <v>109</v>
+      </c>
+      <c r="E1456" s="17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="1457" spans="1:5" x14ac:dyDescent="0.2">
@@ -27631,13 +27521,13 @@
         <v>619</v>
       </c>
       <c r="B1457" s="17" t="s">
-        <v>592</v>
+        <v>634</v>
       </c>
       <c r="C1457" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D1457" s="17" t="s">
-        <v>117</v>
+        <v>342</v>
       </c>
       <c r="E1457" s="17" t="s">
         <v>4</v>
@@ -27648,13 +27538,13 @@
         <v>619</v>
       </c>
       <c r="B1458" s="17" t="s">
-        <v>593</v>
+        <v>602</v>
       </c>
       <c r="C1458" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D1458" s="17" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="E1458" s="17" t="s">
         <v>4</v>
@@ -27665,13 +27555,13 @@
         <v>619</v>
       </c>
       <c r="B1459" s="17" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="C1459" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D1459" s="17" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="E1459" s="17" t="s">
         <v>4</v>
@@ -27681,14 +27571,14 @@
       <c r="A1460" s="17" t="s">
         <v>619</v>
       </c>
-      <c r="B1460" s="17" t="s">
-        <v>595</v>
+      <c r="B1460" s="18" t="s">
+        <v>601</v>
       </c>
       <c r="C1460" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D1460" s="17" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="E1460" s="17" t="s">
         <v>4</v>
@@ -27698,14 +27588,14 @@
       <c r="A1461" s="17" t="s">
         <v>619</v>
       </c>
-      <c r="B1461" s="17" t="s">
-        <v>596</v>
+      <c r="B1461" s="18" t="s">
+        <v>646</v>
       </c>
       <c r="C1461" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D1461" s="17" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E1461" s="17" t="s">
         <v>4</v>
@@ -27716,16 +27606,16 @@
         <v>619</v>
       </c>
       <c r="B1462" s="17" t="s">
-        <v>597</v>
+        <v>470</v>
       </c>
       <c r="C1462" s="17" t="s">
-        <v>4</v>
+        <v>638</v>
       </c>
       <c r="D1462" s="17" t="s">
-        <v>127</v>
+        <v>470</v>
       </c>
       <c r="E1462" s="17" t="s">
-        <v>4</v>
+        <v>144</v>
       </c>
     </row>
     <row r="1463" spans="1:5" x14ac:dyDescent="0.2">
@@ -27733,16 +27623,16 @@
         <v>619</v>
       </c>
       <c r="B1463" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="C1463" s="17" t="s">
-        <v>515</v>
+        <v>635</v>
       </c>
       <c r="D1463" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="E1463" s="17" t="s">
-        <v>10</v>
+        <v>471</v>
       </c>
     </row>
     <row r="1464" spans="1:5" x14ac:dyDescent="0.2">
@@ -27750,16 +27640,16 @@
         <v>619</v>
       </c>
       <c r="B1464" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="C1464" s="17" t="s">
-        <v>472</v>
+        <v>636</v>
       </c>
       <c r="D1464" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="E1464" s="17" t="s">
-        <v>14</v>
+        <v>471</v>
       </c>
     </row>
     <row r="1465" spans="1:5" x14ac:dyDescent="0.2">
@@ -27767,16 +27657,16 @@
         <v>619</v>
       </c>
       <c r="B1465" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="C1465" s="17" t="s">
-        <v>473</v>
+        <v>637</v>
       </c>
       <c r="D1465" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="E1465" s="17" t="s">
-        <v>11</v>
+        <v>471</v>
       </c>
     </row>
     <row r="1466" spans="1:5" x14ac:dyDescent="0.2">
@@ -27784,16 +27674,16 @@
         <v>619</v>
       </c>
       <c r="B1466" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="C1466" s="17" t="s">
-        <v>474</v>
+        <v>639</v>
       </c>
       <c r="D1466" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="E1466" s="17" t="s">
-        <v>12</v>
+        <v>471</v>
       </c>
     </row>
     <row r="1467" spans="1:5" x14ac:dyDescent="0.2">
@@ -27801,16 +27691,16 @@
         <v>619</v>
       </c>
       <c r="B1467" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="C1467" s="17" t="s">
-        <v>475</v>
+        <v>640</v>
       </c>
       <c r="D1467" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="E1467" s="17" t="s">
-        <v>15</v>
+        <v>471</v>
       </c>
     </row>
     <row r="1468" spans="1:5" x14ac:dyDescent="0.2">
@@ -27818,16 +27708,16 @@
         <v>619</v>
       </c>
       <c r="B1468" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="C1468" s="17" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="D1468" s="17" t="s">
-        <v>9</v>
+        <v>470</v>
       </c>
       <c r="E1468" s="17" t="s">
-        <v>15</v>
+        <v>464</v>
       </c>
     </row>
     <row r="1469" spans="1:5" x14ac:dyDescent="0.2">
@@ -27835,16 +27725,16 @@
         <v>619</v>
       </c>
       <c r="B1469" s="17" t="s">
-        <v>9</v>
+        <v>604</v>
       </c>
       <c r="C1469" s="17" t="s">
-        <v>477</v>
+        <v>4</v>
       </c>
       <c r="D1469" s="17" t="s">
-        <v>9</v>
+        <v>345</v>
       </c>
       <c r="E1469" s="17" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1470" spans="1:5" x14ac:dyDescent="0.2">
@@ -27852,16 +27742,16 @@
         <v>619</v>
       </c>
       <c r="B1470" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1470" s="17" t="s">
-        <v>478</v>
+        <v>136</v>
+      </c>
+      <c r="C1470" s="17">
+        <v>0</v>
       </c>
       <c r="D1470" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1470" s="17" t="s">
-        <v>15</v>
+        <v>136</v>
+      </c>
+      <c r="E1470" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="1471" spans="1:5" x14ac:dyDescent="0.2">
@@ -27869,16 +27759,16 @@
         <v>619</v>
       </c>
       <c r="B1471" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1471" s="17" t="s">
-        <v>479</v>
+        <v>136</v>
+      </c>
+      <c r="C1471" s="17">
+        <v>1</v>
       </c>
       <c r="D1471" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1471" s="17" t="s">
-        <v>15</v>
+        <v>136</v>
+      </c>
+      <c r="E1471" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="1472" spans="1:5" x14ac:dyDescent="0.2">
@@ -27886,16 +27776,16 @@
         <v>619</v>
       </c>
       <c r="B1472" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1472" s="17" t="s">
-        <v>480</v>
+        <v>136</v>
+      </c>
+      <c r="C1472" s="17">
+        <v>2</v>
       </c>
       <c r="D1472" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1472" s="17" t="s">
-        <v>15</v>
+        <v>136</v>
+      </c>
+      <c r="E1472" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="1473" spans="1:5" x14ac:dyDescent="0.2">
@@ -27903,16 +27793,16 @@
         <v>619</v>
       </c>
       <c r="B1473" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1473" s="17" t="s">
-        <v>615</v>
+        <v>136</v>
+      </c>
+      <c r="C1473" s="17">
+        <v>3</v>
       </c>
       <c r="D1473" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1473" s="17" t="s">
-        <v>15</v>
+        <v>136</v>
+      </c>
+      <c r="E1473" s="17">
+        <v>3</v>
       </c>
     </row>
     <row r="1474" spans="1:5" x14ac:dyDescent="0.2">
@@ -27920,16 +27810,16 @@
         <v>619</v>
       </c>
       <c r="B1474" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1474" s="17" t="s">
-        <v>57</v>
+        <v>136</v>
+      </c>
+      <c r="C1474" s="17">
+        <v>4</v>
       </c>
       <c r="D1474" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1474" s="17" t="s">
-        <v>76</v>
+        <v>136</v>
+      </c>
+      <c r="E1474" s="17">
+        <v>4</v>
       </c>
     </row>
     <row r="1475" spans="1:5" x14ac:dyDescent="0.2">
@@ -27937,16 +27827,16 @@
         <v>619</v>
       </c>
       <c r="B1475" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1475" s="17" t="s">
-        <v>56</v>
+        <v>137</v>
+      </c>
+      <c r="C1475" s="17">
+        <v>0</v>
       </c>
       <c r="D1475" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1475" s="17" t="s">
-        <v>75</v>
+        <v>137</v>
+      </c>
+      <c r="E1475" s="17">
+        <v>0</v>
       </c>
     </row>
     <row r="1476" spans="1:5" x14ac:dyDescent="0.2">
@@ -27954,16 +27844,16 @@
         <v>619</v>
       </c>
       <c r="B1476" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1476" s="17" t="s">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="C1476" s="17">
+        <v>1</v>
       </c>
       <c r="D1476" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1476" s="17" t="s">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="E1476" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="1477" spans="1:5" x14ac:dyDescent="0.2">
@@ -27971,16 +27861,16 @@
         <v>619</v>
       </c>
       <c r="B1477" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C1477" s="17" t="s">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="C1477" s="17">
+        <v>2</v>
       </c>
       <c r="D1477" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1477" s="17" t="s">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="E1477" s="17">
+        <v>2</v>
       </c>
     </row>
     <row r="1478" spans="1:5" x14ac:dyDescent="0.2">
@@ -27988,16 +27878,16 @@
         <v>619</v>
       </c>
       <c r="B1478" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1478" s="17" t="s">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="C1478" s="17">
+        <v>3</v>
       </c>
       <c r="D1478" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1478" s="17" t="s">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="E1478" s="17">
+        <v>3</v>
       </c>
     </row>
     <row r="1479" spans="1:5" x14ac:dyDescent="0.2">
@@ -28005,627 +27895,269 @@
         <v>619</v>
       </c>
       <c r="B1479" s="17" t="s">
-        <v>680</v>
-      </c>
-      <c r="C1479" s="17" t="s">
-        <v>616</v>
+        <v>137</v>
+      </c>
+      <c r="C1479" s="17">
+        <v>4</v>
       </c>
       <c r="D1479" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="E1479" s="17" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="1480" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1480" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1480" s="17" t="s">
-        <v>680</v>
-      </c>
-      <c r="C1480" s="17" t="s">
-        <v>681</v>
-      </c>
-      <c r="D1480" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="E1480" s="17" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="1481" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1481" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1481" s="17" t="s">
-        <v>680</v>
-      </c>
-      <c r="C1481" s="17" t="s">
-        <v>393</v>
-      </c>
-      <c r="D1481" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="E1481" s="17" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="1482" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1482" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1482" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1482" s="17"/>
-      <c r="D1482" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1482" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="1483" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1483" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1483" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1483" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="D1483" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1483" s="17" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="1484" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1484" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1484" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1484" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1484" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1484" s="17" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="1485" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1485" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1485" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1485" s="17" t="s">
-        <v>599</v>
-      </c>
-      <c r="D1485" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1485" s="17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="1486" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1486" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1486" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1486" s="17" t="s">
-        <v>600</v>
-      </c>
-      <c r="D1486" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1486" s="17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="1487" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1487" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1487" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1487" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="D1487" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1487" s="17" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="1488" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1488" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1488" s="17" t="s">
-        <v>598</v>
-      </c>
-      <c r="C1488" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="D1488" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="E1488" s="17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="1489" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1489" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1489" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1489" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1489" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1489" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1490" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1490" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1490" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1490" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1490" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1490" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1491" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1491" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1491" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1491" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1491" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="E1491" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1492" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1492" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1492" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1492" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1492" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1492" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1493" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1493" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1493" s="17" t="s">
-        <v>634</v>
-      </c>
-      <c r="C1493" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1493" s="17" t="s">
-        <v>342</v>
-      </c>
-      <c r="E1493" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1494" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1494" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1494" s="17" t="s">
-        <v>602</v>
-      </c>
-      <c r="C1494" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1494" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1494" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1495" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1495" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1495" s="17" t="s">
-        <v>603</v>
-      </c>
-      <c r="C1495" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1495" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1495" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1496" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1496" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1496" s="18" t="s">
-        <v>601</v>
-      </c>
-      <c r="C1496" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1496" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1496" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1497" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1497" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1497" s="18" t="s">
-        <v>682</v>
-      </c>
-      <c r="C1497" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1497" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1497" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1498" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1498" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1498" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1498" s="17" t="s">
-        <v>638</v>
-      </c>
-      <c r="D1498" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1498" s="17" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="1499" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1499" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1499" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1499" s="17" t="s">
-        <v>635</v>
-      </c>
-      <c r="D1499" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1499" s="17" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="1500" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1500" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1500" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1500" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="D1500" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1500" s="17" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="1501" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1501" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1501" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1501" s="17" t="s">
-        <v>637</v>
-      </c>
-      <c r="D1501" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1501" s="17" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="1502" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1502" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1502" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1502" s="17" t="s">
-        <v>639</v>
-      </c>
-      <c r="D1502" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1502" s="17" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="1503" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1503" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1503" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1503" s="17" t="s">
-        <v>640</v>
-      </c>
-      <c r="D1503" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1503" s="17" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="1504" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1504" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1504" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1504" s="17" t="s">
-        <v>451</v>
-      </c>
-      <c r="D1504" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1504" s="17" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="1505" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1505" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1505" s="17" t="s">
-        <v>604</v>
-      </c>
-      <c r="C1505" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1505" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="E1505" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1506" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1506" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1506" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1506" s="17">
-        <v>0</v>
-      </c>
-      <c r="D1506" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1506" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1507" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1507" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1507" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1507" s="17">
-        <v>1</v>
-      </c>
-      <c r="D1507" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1507" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1508" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1508" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1508" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1508" s="17">
-        <v>2</v>
-      </c>
-      <c r="D1508" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1508" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1509" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1509" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1509" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1509" s="17">
-        <v>3</v>
-      </c>
-      <c r="D1509" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1509" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1510" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1510" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1510" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1510" s="17">
-        <v>4</v>
-      </c>
-      <c r="D1510" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1510" s="17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="1511" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1511" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1511" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="C1511" s="17">
-        <v>0</v>
-      </c>
-      <c r="D1511" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1511" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1512" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1512" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1512" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1512" s="17">
-        <v>1</v>
-      </c>
-      <c r="D1512" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1512" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1513" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1513" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1513" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1513" s="17">
-        <v>2</v>
-      </c>
-      <c r="D1513" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1513" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="1514" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1514" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1514" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1514" s="17">
-        <v>3</v>
-      </c>
-      <c r="D1514" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1514" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="1515" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1515" s="17" t="s">
-        <v>619</v>
-      </c>
-      <c r="B1515" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1515" s="17">
-        <v>4</v>
-      </c>
-      <c r="D1515" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1515" s="17">
-        <v>4</v>
-      </c>
+      <c r="E1479" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1480" s="21"/>
+      <c r="B1480" s="21"/>
+      <c r="C1480" s="21"/>
+      <c r="D1480" s="21"/>
+      <c r="E1480" s="21"/>
+    </row>
+    <row r="1481" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1481" s="21"/>
+      <c r="B1481" s="21"/>
+      <c r="C1481" s="21"/>
+      <c r="D1481" s="21"/>
+      <c r="E1481" s="21"/>
+    </row>
+    <row r="1482" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1482" s="21"/>
+      <c r="B1482" s="21"/>
+      <c r="C1482" s="21"/>
+      <c r="D1482" s="21"/>
+      <c r="E1482" s="21"/>
+    </row>
+    <row r="1483" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1483" s="21"/>
+      <c r="B1483" s="21"/>
+      <c r="C1483" s="21"/>
+      <c r="D1483" s="21"/>
+      <c r="E1483" s="21"/>
+    </row>
+    <row r="1484" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1484" s="21"/>
+      <c r="B1484" s="21"/>
+      <c r="C1484" s="21"/>
+      <c r="D1484" s="21"/>
+      <c r="E1484" s="21"/>
+    </row>
+    <row r="1485" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1485" s="21"/>
+      <c r="B1485" s="21"/>
+      <c r="C1485" s="21"/>
+      <c r="D1485" s="21"/>
+      <c r="E1485" s="21"/>
+    </row>
+    <row r="1486" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1486" s="21"/>
+      <c r="B1486" s="21"/>
+      <c r="C1486" s="21"/>
+      <c r="D1486" s="21"/>
+      <c r="E1486" s="21"/>
+    </row>
+    <row r="1487" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1487" s="21"/>
+      <c r="B1487" s="21"/>
+      <c r="C1487" s="21"/>
+      <c r="D1487" s="21"/>
+      <c r="E1487" s="21"/>
+    </row>
+    <row r="1488" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1488" s="21"/>
+      <c r="B1488" s="21"/>
+      <c r="C1488" s="21"/>
+      <c r="D1488" s="21"/>
+      <c r="E1488" s="21"/>
+    </row>
+    <row r="1489" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1489" s="21"/>
+      <c r="B1489" s="21"/>
+      <c r="C1489" s="21"/>
+      <c r="D1489" s="21"/>
+      <c r="E1489" s="21"/>
+    </row>
+    <row r="1490" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1490" s="21"/>
+      <c r="B1490" s="21"/>
+      <c r="C1490" s="21"/>
+      <c r="D1490" s="21"/>
+      <c r="E1490" s="21"/>
+    </row>
+    <row r="1491" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1491" s="21"/>
+      <c r="B1491" s="21"/>
+      <c r="C1491" s="21"/>
+      <c r="D1491" s="21"/>
+      <c r="E1491" s="21"/>
+    </row>
+    <row r="1492" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1492" s="21"/>
+      <c r="B1492" s="21"/>
+      <c r="C1492" s="21"/>
+      <c r="D1492" s="21"/>
+      <c r="E1492" s="21"/>
+    </row>
+    <row r="1493" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1493" s="21"/>
+      <c r="B1493" s="21"/>
+      <c r="C1493" s="21"/>
+      <c r="D1493" s="21"/>
+      <c r="E1493" s="21"/>
+    </row>
+    <row r="1494" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1494" s="21"/>
+      <c r="B1494" s="21"/>
+      <c r="C1494" s="21"/>
+      <c r="D1494" s="21"/>
+      <c r="E1494" s="21"/>
+    </row>
+    <row r="1495" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1495" s="21"/>
+      <c r="B1495" s="21"/>
+      <c r="C1495" s="21"/>
+      <c r="D1495" s="21"/>
+      <c r="E1495" s="21"/>
+    </row>
+    <row r="1496" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1496" s="21"/>
+      <c r="B1496" s="21"/>
+      <c r="C1496" s="21"/>
+      <c r="D1496" s="21"/>
+      <c r="E1496" s="21"/>
+    </row>
+    <row r="1497" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1497" s="21"/>
+      <c r="B1497" s="21"/>
+      <c r="C1497" s="21"/>
+      <c r="D1497" s="21"/>
+      <c r="E1497" s="21"/>
+    </row>
+    <row r="1498" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1498" s="21"/>
+      <c r="B1498" s="21"/>
+      <c r="C1498" s="21"/>
+      <c r="D1498" s="21"/>
+      <c r="E1498" s="21"/>
+    </row>
+    <row r="1499" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1499" s="21"/>
+      <c r="B1499" s="21"/>
+      <c r="C1499" s="21"/>
+      <c r="D1499" s="21"/>
+      <c r="E1499" s="21"/>
+    </row>
+    <row r="1500" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1500" s="21"/>
+      <c r="B1500" s="21"/>
+      <c r="C1500" s="21"/>
+      <c r="D1500" s="21"/>
+      <c r="E1500" s="21"/>
+    </row>
+    <row r="1501" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1501" s="21"/>
+      <c r="B1501" s="21"/>
+      <c r="C1501" s="21"/>
+      <c r="D1501" s="21"/>
+      <c r="E1501" s="21"/>
+    </row>
+    <row r="1502" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1502" s="21"/>
+      <c r="B1502" s="21"/>
+      <c r="C1502" s="21"/>
+      <c r="D1502" s="21"/>
+      <c r="E1502" s="21"/>
+    </row>
+    <row r="1503" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1503" s="21"/>
+      <c r="B1503" s="21"/>
+      <c r="C1503" s="21"/>
+      <c r="D1503" s="21"/>
+      <c r="E1503" s="21"/>
+    </row>
+    <row r="1504" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1504" s="21"/>
+      <c r="B1504" s="21"/>
+      <c r="C1504" s="21"/>
+      <c r="D1504" s="21"/>
+      <c r="E1504" s="21"/>
+    </row>
+    <row r="1505" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1505" s="21"/>
+      <c r="B1505" s="21"/>
+      <c r="C1505" s="21"/>
+      <c r="D1505" s="21"/>
+      <c r="E1505" s="21"/>
+    </row>
+    <row r="1506" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1506" s="21"/>
+      <c r="B1506" s="21"/>
+      <c r="C1506" s="21"/>
+      <c r="D1506" s="21"/>
+      <c r="E1506" s="21"/>
+    </row>
+    <row r="1507" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1507" s="21"/>
+      <c r="B1507" s="21"/>
+      <c r="C1507" s="21"/>
+      <c r="D1507" s="21"/>
+      <c r="E1507" s="21"/>
+    </row>
+    <row r="1508" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1508" s="21"/>
+      <c r="B1508" s="21"/>
+      <c r="C1508" s="21"/>
+      <c r="D1508" s="21"/>
+      <c r="E1508" s="21"/>
+    </row>
+    <row r="1509" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1509" s="21"/>
+      <c r="B1509" s="21"/>
+      <c r="C1509" s="21"/>
+      <c r="D1509" s="21"/>
+      <c r="E1509" s="21"/>
+    </row>
+    <row r="1510" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1510" s="21"/>
+      <c r="B1510" s="21"/>
+      <c r="C1510" s="21"/>
+      <c r="D1510" s="21"/>
+      <c r="E1510" s="21"/>
+    </row>
+    <row r="1511" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1511" s="21"/>
+      <c r="B1511" s="21"/>
+      <c r="C1511" s="21"/>
+      <c r="D1511" s="21"/>
+      <c r="E1511" s="21"/>
+    </row>
+    <row r="1512" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1512" s="21"/>
+      <c r="B1512" s="21"/>
+      <c r="C1512" s="21"/>
+      <c r="D1512" s="21"/>
+      <c r="E1512" s="21"/>
+    </row>
+    <row r="1513" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1513" s="21"/>
+      <c r="B1513" s="21"/>
+      <c r="C1513" s="21"/>
+      <c r="D1513" s="21"/>
+      <c r="E1513" s="21"/>
+    </row>
+    <row r="1514" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1514" s="21"/>
+      <c r="B1514" s="21"/>
+      <c r="C1514" s="21"/>
+      <c r="D1514" s="21"/>
+      <c r="E1514" s="21"/>
+    </row>
+    <row r="1515" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1515" s="21"/>
+      <c r="B1515" s="21"/>
+      <c r="C1515" s="21"/>
+      <c r="D1515" s="21"/>
+      <c r="E1515" s="21"/>
     </row>
     <row r="1516" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1516" s="21"/>
@@ -28720,98 +28252,98 @@
     </row>
     <row r="1529" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1529" s="21"/>
-      <c r="B1529" s="21"/>
+      <c r="B1529" s="22"/>
       <c r="C1529" s="21"/>
       <c r="D1529" s="21"/>
       <c r="E1529" s="21"/>
     </row>
     <row r="1530" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1530" s="21"/>
-      <c r="B1530" s="21"/>
+      <c r="B1530" s="22"/>
       <c r="C1530" s="21"/>
       <c r="D1530" s="21"/>
       <c r="E1530" s="21"/>
     </row>
     <row r="1531" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1531" s="21"/>
-      <c r="B1531" s="21"/>
+      <c r="B1531" s="22"/>
       <c r="C1531" s="21"/>
       <c r="D1531" s="21"/>
       <c r="E1531" s="21"/>
     </row>
     <row r="1532" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1532" s="21"/>
-      <c r="B1532" s="21"/>
+      <c r="B1532" s="22"/>
       <c r="C1532" s="21"/>
       <c r="D1532" s="21"/>
       <c r="E1532" s="21"/>
     </row>
     <row r="1533" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1533" s="21"/>
-      <c r="B1533" s="21"/>
+      <c r="B1533" s="22"/>
       <c r="C1533" s="21"/>
       <c r="D1533" s="21"/>
       <c r="E1533" s="21"/>
     </row>
     <row r="1534" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1534" s="21"/>
-      <c r="B1534" s="21"/>
+      <c r="B1534" s="22"/>
       <c r="C1534" s="21"/>
       <c r="D1534" s="21"/>
       <c r="E1534" s="21"/>
     </row>
     <row r="1535" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1535" s="21"/>
-      <c r="B1535" s="21"/>
+      <c r="B1535" s="22"/>
       <c r="C1535" s="21"/>
       <c r="D1535" s="21"/>
       <c r="E1535" s="21"/>
     </row>
     <row r="1536" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1536" s="21"/>
-      <c r="B1536" s="21"/>
+      <c r="B1536" s="22"/>
       <c r="C1536" s="21"/>
       <c r="D1536" s="21"/>
       <c r="E1536" s="21"/>
     </row>
     <row r="1537" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1537" s="21"/>
-      <c r="B1537" s="21"/>
+      <c r="B1537" s="22"/>
       <c r="C1537" s="21"/>
       <c r="D1537" s="21"/>
       <c r="E1537" s="21"/>
     </row>
     <row r="1538" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1538" s="21"/>
-      <c r="B1538" s="21"/>
+      <c r="B1538" s="22"/>
       <c r="C1538" s="21"/>
       <c r="D1538" s="21"/>
       <c r="E1538" s="21"/>
     </row>
     <row r="1539" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1539" s="21"/>
-      <c r="B1539" s="21"/>
+      <c r="B1539" s="22"/>
       <c r="C1539" s="21"/>
       <c r="D1539" s="21"/>
       <c r="E1539" s="21"/>
     </row>
     <row r="1540" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1540" s="21"/>
-      <c r="B1540" s="21"/>
+      <c r="B1540" s="22"/>
       <c r="C1540" s="21"/>
       <c r="D1540" s="21"/>
       <c r="E1540" s="21"/>
     </row>
     <row r="1541" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1541" s="21"/>
-      <c r="B1541" s="21"/>
+      <c r="B1541" s="22"/>
       <c r="C1541" s="21"/>
       <c r="D1541" s="21"/>
       <c r="E1541" s="21"/>
     </row>
     <row r="1542" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1542" s="21"/>
-      <c r="B1542" s="21"/>
+      <c r="B1542" s="22"/>
       <c r="C1542" s="21"/>
       <c r="D1542" s="21"/>
       <c r="E1542" s="21"/>
@@ -28938,14 +28470,14 @@
     <row r="1560" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1560" s="21"/>
       <c r="B1560" s="21"/>
-      <c r="C1560" s="21"/>
+      <c r="C1560" s="23"/>
       <c r="D1560" s="21"/>
       <c r="E1560" s="21"/>
     </row>
     <row r="1561" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1561" s="21"/>
       <c r="B1561" s="21"/>
-      <c r="C1561" s="21"/>
+      <c r="C1561" s="23"/>
       <c r="D1561" s="21"/>
       <c r="E1561" s="21"/>
     </row>
@@ -29105,140 +28637,140 @@
     </row>
     <row r="1584" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1584" s="21"/>
-      <c r="B1584" s="21"/>
+      <c r="B1584" s="22"/>
       <c r="C1584" s="21"/>
       <c r="D1584" s="21"/>
       <c r="E1584" s="21"/>
     </row>
     <row r="1585" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1585" s="21"/>
-      <c r="B1585" s="21"/>
+      <c r="B1585" s="22"/>
       <c r="C1585" s="21"/>
       <c r="D1585" s="21"/>
       <c r="E1585" s="21"/>
     </row>
     <row r="1586" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1586" s="21"/>
-      <c r="B1586" s="21"/>
+      <c r="B1586" s="22"/>
       <c r="C1586" s="21"/>
       <c r="D1586" s="21"/>
       <c r="E1586" s="21"/>
     </row>
     <row r="1587" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1587" s="21"/>
-      <c r="B1587" s="21"/>
+      <c r="B1587" s="22"/>
       <c r="C1587" s="21"/>
       <c r="D1587" s="21"/>
       <c r="E1587" s="21"/>
     </row>
     <row r="1588" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1588" s="21"/>
-      <c r="B1588" s="21"/>
+      <c r="B1588" s="22"/>
       <c r="C1588" s="21"/>
       <c r="D1588" s="21"/>
       <c r="E1588" s="21"/>
     </row>
     <row r="1589" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1589" s="21"/>
-      <c r="B1589" s="21"/>
+      <c r="B1589" s="22"/>
       <c r="C1589" s="21"/>
       <c r="D1589" s="21"/>
       <c r="E1589" s="21"/>
     </row>
     <row r="1590" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1590" s="21"/>
-      <c r="B1590" s="21"/>
+      <c r="B1590" s="22"/>
       <c r="C1590" s="21"/>
       <c r="D1590" s="21"/>
       <c r="E1590" s="21"/>
     </row>
     <row r="1591" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1591" s="21"/>
-      <c r="B1591" s="21"/>
+      <c r="B1591" s="22"/>
       <c r="C1591" s="21"/>
       <c r="D1591" s="21"/>
       <c r="E1591" s="21"/>
     </row>
     <row r="1592" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1592" s="21"/>
-      <c r="B1592" s="21"/>
+      <c r="B1592" s="22"/>
       <c r="C1592" s="21"/>
       <c r="D1592" s="21"/>
       <c r="E1592" s="21"/>
     </row>
     <row r="1593" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1593" s="21"/>
-      <c r="B1593" s="21"/>
+      <c r="B1593" s="22"/>
       <c r="C1593" s="21"/>
       <c r="D1593" s="21"/>
       <c r="E1593" s="21"/>
     </row>
     <row r="1594" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1594" s="21"/>
-      <c r="B1594" s="21"/>
+      <c r="B1594" s="22"/>
       <c r="C1594" s="21"/>
       <c r="D1594" s="21"/>
       <c r="E1594" s="21"/>
     </row>
     <row r="1595" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1595" s="21"/>
-      <c r="B1595" s="21"/>
+      <c r="B1595" s="22"/>
       <c r="C1595" s="21"/>
       <c r="D1595" s="21"/>
       <c r="E1595" s="21"/>
     </row>
     <row r="1596" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1596" s="21"/>
-      <c r="B1596" s="21"/>
+      <c r="B1596" s="22"/>
       <c r="C1596" s="21"/>
       <c r="D1596" s="21"/>
       <c r="E1596" s="21"/>
     </row>
     <row r="1597" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1597" s="21"/>
-      <c r="B1597" s="21"/>
+      <c r="B1597" s="22"/>
       <c r="C1597" s="21"/>
       <c r="D1597" s="21"/>
       <c r="E1597" s="21"/>
     </row>
     <row r="1598" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1598" s="21"/>
-      <c r="B1598" s="21"/>
+      <c r="B1598" s="22"/>
       <c r="C1598" s="21"/>
       <c r="D1598" s="21"/>
       <c r="E1598" s="21"/>
     </row>
     <row r="1599" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1599" s="21"/>
-      <c r="B1599" s="21"/>
+      <c r="B1599" s="22"/>
       <c r="C1599" s="21"/>
       <c r="D1599" s="21"/>
       <c r="E1599" s="21"/>
     </row>
     <row r="1600" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1600" s="21"/>
-      <c r="B1600" s="21"/>
+      <c r="B1600" s="22"/>
       <c r="C1600" s="21"/>
       <c r="D1600" s="21"/>
       <c r="E1600" s="21"/>
     </row>
     <row r="1601" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1601" s="21"/>
-      <c r="B1601" s="21"/>
+      <c r="B1601" s="22"/>
       <c r="C1601" s="21"/>
       <c r="D1601" s="21"/>
       <c r="E1601" s="21"/>
     </row>
     <row r="1602" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1602" s="21"/>
-      <c r="B1602" s="21"/>
+      <c r="B1602" s="22"/>
       <c r="C1602" s="21"/>
       <c r="D1602" s="21"/>
       <c r="E1602" s="21"/>
     </row>
     <row r="1603" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1603" s="21"/>
-      <c r="B1603" s="21"/>
+      <c r="B1603" s="22"/>
       <c r="C1603" s="21"/>
       <c r="D1603" s="21"/>
       <c r="E1603" s="21"/>
@@ -29252,194 +28784,197 @@
     </row>
     <row r="1605" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1605" s="21"/>
-      <c r="B1605" s="22"/>
+      <c r="B1605" s="21"/>
       <c r="C1605" s="21"/>
       <c r="D1605" s="21"/>
       <c r="E1605" s="21"/>
     </row>
     <row r="1606" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1606" s="21"/>
-      <c r="B1606" s="22"/>
+      <c r="B1606" s="21"/>
       <c r="C1606" s="21"/>
       <c r="D1606" s="21"/>
       <c r="E1606" s="21"/>
     </row>
     <row r="1607" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1607" s="21"/>
-      <c r="B1607" s="22"/>
+      <c r="B1607" s="21"/>
       <c r="C1607" s="21"/>
       <c r="D1607" s="21"/>
       <c r="E1607" s="21"/>
     </row>
     <row r="1608" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1608" s="21"/>
-      <c r="B1608" s="22"/>
+      <c r="B1608" s="21"/>
       <c r="C1608" s="21"/>
       <c r="D1608" s="21"/>
       <c r="E1608" s="21"/>
     </row>
     <row r="1609" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1609" s="21"/>
-      <c r="B1609" s="22"/>
+      <c r="B1609" s="21"/>
       <c r="C1609" s="21"/>
       <c r="D1609" s="21"/>
       <c r="E1609" s="21"/>
     </row>
     <row r="1610" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1610" s="21"/>
-      <c r="B1610" s="22"/>
+      <c r="B1610" s="21"/>
       <c r="C1610" s="21"/>
       <c r="D1610" s="21"/>
       <c r="E1610" s="21"/>
     </row>
     <row r="1611" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1611" s="21"/>
-      <c r="B1611" s="22"/>
+      <c r="B1611" s="21"/>
       <c r="C1611" s="21"/>
       <c r="D1611" s="21"/>
       <c r="E1611" s="21"/>
     </row>
     <row r="1612" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1612" s="21"/>
-      <c r="B1612" s="22"/>
+      <c r="B1612" s="21"/>
       <c r="C1612" s="21"/>
       <c r="D1612" s="21"/>
       <c r="E1612" s="21"/>
     </row>
     <row r="1613" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1613" s="21"/>
-      <c r="B1613" s="22"/>
+      <c r="B1613" s="21"/>
       <c r="C1613" s="21"/>
       <c r="D1613" s="21"/>
       <c r="E1613" s="21"/>
     </row>
     <row r="1614" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1614" s="21"/>
-      <c r="B1614" s="22"/>
+      <c r="B1614" s="21"/>
       <c r="C1614" s="21"/>
       <c r="D1614" s="21"/>
       <c r="E1614" s="21"/>
     </row>
     <row r="1615" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1615" s="21"/>
-      <c r="B1615" s="22"/>
+      <c r="B1615" s="21"/>
       <c r="C1615" s="21"/>
       <c r="D1615" s="21"/>
       <c r="E1615" s="21"/>
     </row>
     <row r="1616" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1616" s="21"/>
-      <c r="B1616" s="22"/>
+      <c r="B1616" s="21"/>
       <c r="C1616" s="21"/>
       <c r="D1616" s="21"/>
       <c r="E1616" s="21"/>
     </row>
-    <row r="1617" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1617" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1617" s="21"/>
-      <c r="B1617" s="22"/>
+      <c r="B1617" s="21"/>
       <c r="C1617" s="21"/>
       <c r="D1617" s="21"/>
       <c r="E1617" s="21"/>
     </row>
-    <row r="1618" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1618" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1618" s="21"/>
-      <c r="B1618" s="22"/>
+      <c r="B1618" s="21"/>
       <c r="C1618" s="21"/>
       <c r="D1618" s="21"/>
       <c r="E1618" s="21"/>
     </row>
-    <row r="1619" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1619" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1619" s="21"/>
       <c r="B1619" s="21"/>
       <c r="C1619" s="21"/>
       <c r="D1619" s="21"/>
       <c r="E1619" s="21"/>
     </row>
-    <row r="1620" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1620" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1620" s="21"/>
       <c r="B1620" s="21"/>
       <c r="C1620" s="21"/>
       <c r="D1620" s="21"/>
       <c r="E1620" s="21"/>
     </row>
-    <row r="1621" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1621" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1621" s="21"/>
       <c r="B1621" s="21"/>
       <c r="C1621" s="21"/>
       <c r="D1621" s="21"/>
       <c r="E1621" s="21"/>
     </row>
-    <row r="1622" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1622" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1622" s="21"/>
       <c r="B1622" s="21"/>
       <c r="C1622" s="21"/>
       <c r="D1622" s="21"/>
       <c r="E1622" s="21"/>
     </row>
-    <row r="1623" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1623" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1623" s="21"/>
       <c r="B1623" s="21"/>
       <c r="C1623" s="21"/>
       <c r="D1623" s="21"/>
       <c r="E1623" s="21"/>
     </row>
-    <row r="1624" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1624" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1624" s="21"/>
       <c r="B1624" s="21"/>
       <c r="C1624" s="21"/>
       <c r="D1624" s="21"/>
       <c r="E1624" s="21"/>
-    </row>
-    <row r="1625" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1624" s="5"/>
+    </row>
+    <row r="1625" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1625" s="21"/>
       <c r="B1625" s="21"/>
       <c r="C1625" s="21"/>
       <c r="D1625" s="21"/>
       <c r="E1625" s="21"/>
-    </row>
-    <row r="1626" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1625" s="5"/>
+    </row>
+    <row r="1626" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1626" s="21"/>
       <c r="B1626" s="21"/>
       <c r="C1626" s="21"/>
       <c r="D1626" s="21"/>
       <c r="E1626" s="21"/>
-    </row>
-    <row r="1627" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F1626" s="5"/>
+    </row>
+    <row r="1627" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1627" s="21"/>
       <c r="B1627" s="21"/>
       <c r="C1627" s="21"/>
       <c r="D1627" s="21"/>
       <c r="E1627" s="21"/>
     </row>
-    <row r="1628" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1628" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1628" s="21"/>
       <c r="B1628" s="21"/>
       <c r="C1628" s="21"/>
       <c r="D1628" s="21"/>
       <c r="E1628" s="21"/>
     </row>
-    <row r="1629" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1629" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1629" s="21"/>
       <c r="B1629" s="21"/>
       <c r="C1629" s="21"/>
       <c r="D1629" s="21"/>
       <c r="E1629" s="21"/>
     </row>
-    <row r="1630" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1630" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1630" s="21"/>
       <c r="B1630" s="21"/>
       <c r="C1630" s="21"/>
       <c r="D1630" s="21"/>
       <c r="E1630" s="21"/>
     </row>
-    <row r="1631" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1631" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1631" s="21"/>
       <c r="B1631" s="21"/>
       <c r="C1631" s="21"/>
       <c r="D1631" s="21"/>
       <c r="E1631" s="21"/>
     </row>
-    <row r="1632" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1632" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1632" s="21"/>
       <c r="B1632" s="21"/>
       <c r="C1632" s="21"/>
@@ -29469,15 +29004,15 @@
     </row>
     <row r="1636" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1636" s="21"/>
-      <c r="B1636" s="21"/>
-      <c r="C1636" s="23"/>
+      <c r="B1636" s="24"/>
+      <c r="C1636" s="21"/>
       <c r="D1636" s="21"/>
       <c r="E1636" s="21"/>
     </row>
     <row r="1637" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1637" s="21"/>
-      <c r="B1637" s="21"/>
-      <c r="C1637" s="23"/>
+      <c r="B1637" s="24"/>
+      <c r="C1637" s="21"/>
       <c r="D1637" s="21"/>
       <c r="E1637" s="21"/>
     </row>
@@ -29573,600 +29108,597 @@
       <c r="E1650" s="21"/>
     </row>
     <row r="1651" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1651" s="21"/>
-      <c r="B1651" s="21"/>
-      <c r="C1651" s="21"/>
-      <c r="D1651" s="21"/>
-      <c r="E1651" s="21"/>
+      <c r="A1651" s="25"/>
+      <c r="B1651" s="26"/>
+      <c r="C1651" s="27"/>
+      <c r="D1651" s="25"/>
+      <c r="E1651" s="25"/>
     </row>
     <row r="1652" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1652" s="21"/>
-      <c r="B1652" s="21"/>
-      <c r="C1652" s="21"/>
-      <c r="D1652" s="21"/>
-      <c r="E1652" s="21"/>
+      <c r="A1652" s="25"/>
+      <c r="B1652" s="26"/>
+      <c r="C1652" s="27"/>
+      <c r="D1652" s="25"/>
+      <c r="E1652" s="25"/>
     </row>
     <row r="1653" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1653" s="21"/>
-      <c r="B1653" s="21"/>
-      <c r="C1653" s="21"/>
-      <c r="D1653" s="21"/>
-      <c r="E1653" s="21"/>
+      <c r="A1653" s="25"/>
+      <c r="B1653" s="26"/>
+      <c r="C1653" s="27"/>
+      <c r="D1653" s="25"/>
+      <c r="E1653" s="25"/>
     </row>
     <row r="1654" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1654" s="21"/>
-      <c r="B1654" s="21"/>
-      <c r="C1654" s="21"/>
-      <c r="D1654" s="21"/>
-      <c r="E1654" s="21"/>
+      <c r="A1654" s="25"/>
+      <c r="B1654" s="26"/>
+      <c r="C1654" s="27"/>
+      <c r="D1654" s="25"/>
+      <c r="E1654" s="25"/>
     </row>
     <row r="1655" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1655" s="21"/>
-      <c r="B1655" s="21"/>
-      <c r="C1655" s="21"/>
-      <c r="D1655" s="21"/>
-      <c r="E1655" s="21"/>
+      <c r="A1655" s="25"/>
+      <c r="B1655" s="26"/>
+      <c r="C1655" s="27"/>
+      <c r="D1655" s="25"/>
+      <c r="E1655" s="25"/>
     </row>
     <row r="1656" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1656" s="21"/>
-      <c r="B1656" s="21"/>
-      <c r="C1656" s="21"/>
-      <c r="D1656" s="21"/>
-      <c r="E1656" s="21"/>
+      <c r="A1656" s="25"/>
+      <c r="B1656" s="26"/>
+      <c r="C1656" s="27"/>
+      <c r="D1656" s="25"/>
+      <c r="E1656" s="25"/>
     </row>
     <row r="1657" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1657" s="21"/>
-      <c r="B1657" s="21"/>
-      <c r="C1657" s="21"/>
-      <c r="D1657" s="21"/>
-      <c r="E1657" s="21"/>
+      <c r="A1657" s="25"/>
+      <c r="B1657" s="26"/>
+      <c r="C1657" s="27"/>
+      <c r="D1657" s="25"/>
+      <c r="E1657" s="25"/>
     </row>
     <row r="1658" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1658" s="21"/>
-      <c r="B1658" s="21"/>
-      <c r="C1658" s="21"/>
-      <c r="D1658" s="21"/>
-      <c r="E1658" s="21"/>
+      <c r="A1658" s="25"/>
+      <c r="B1658" s="26"/>
+      <c r="C1658" s="27"/>
+      <c r="D1658" s="25"/>
+      <c r="E1658" s="25"/>
     </row>
     <row r="1659" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1659" s="21"/>
-      <c r="B1659" s="21"/>
-      <c r="C1659" s="21"/>
-      <c r="D1659" s="21"/>
-      <c r="E1659" s="21"/>
+      <c r="A1659" s="25"/>
+      <c r="B1659" s="26"/>
+      <c r="C1659" s="27"/>
+      <c r="D1659" s="25"/>
+      <c r="E1659" s="25"/>
     </row>
     <row r="1660" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1660" s="21"/>
-      <c r="B1660" s="22"/>
-      <c r="C1660" s="21"/>
-      <c r="D1660" s="21"/>
-      <c r="E1660" s="21"/>
+      <c r="A1660" s="25"/>
+      <c r="B1660" s="25"/>
+      <c r="C1660" s="25"/>
+      <c r="D1660" s="25"/>
+      <c r="E1660" s="25"/>
     </row>
     <row r="1661" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1661" s="21"/>
-      <c r="B1661" s="22"/>
-      <c r="C1661" s="21"/>
-      <c r="D1661" s="21"/>
-      <c r="E1661" s="21"/>
+      <c r="A1661" s="25"/>
+      <c r="B1661" s="25"/>
+      <c r="C1661" s="25"/>
+      <c r="D1661" s="25"/>
+      <c r="E1661" s="25"/>
     </row>
     <row r="1662" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1662" s="21"/>
-      <c r="B1662" s="22"/>
-      <c r="C1662" s="21"/>
-      <c r="D1662" s="21"/>
-      <c r="E1662" s="21"/>
+      <c r="A1662" s="25"/>
+      <c r="B1662" s="25"/>
+      <c r="C1662" s="25"/>
+      <c r="D1662" s="25"/>
+      <c r="E1662" s="25"/>
     </row>
     <row r="1663" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1663" s="21"/>
-      <c r="B1663" s="22"/>
-      <c r="C1663" s="21"/>
-      <c r="D1663" s="21"/>
-      <c r="E1663" s="21"/>
+      <c r="A1663" s="25"/>
+      <c r="B1663" s="25"/>
+      <c r="C1663" s="25"/>
+      <c r="D1663" s="25"/>
+      <c r="E1663" s="25"/>
     </row>
     <row r="1664" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1664" s="21"/>
-      <c r="B1664" s="22"/>
-      <c r="C1664" s="21"/>
-      <c r="D1664" s="21"/>
-      <c r="E1664" s="21"/>
+      <c r="A1664" s="25"/>
+      <c r="B1664" s="25"/>
+      <c r="C1664" s="25"/>
+      <c r="D1664" s="25"/>
+      <c r="E1664" s="25"/>
     </row>
     <row r="1665" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1665" s="21"/>
-      <c r="B1665" s="22"/>
-      <c r="C1665" s="21"/>
-      <c r="D1665" s="21"/>
-      <c r="E1665" s="21"/>
+      <c r="A1665" s="25"/>
+      <c r="B1665" s="25"/>
+      <c r="C1665" s="25"/>
+      <c r="D1665" s="25"/>
+      <c r="E1665" s="25"/>
     </row>
     <row r="1666" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1666" s="21"/>
-      <c r="B1666" s="22"/>
-      <c r="C1666" s="21"/>
-      <c r="D1666" s="21"/>
-      <c r="E1666" s="21"/>
+      <c r="A1666" s="25"/>
+      <c r="B1666" s="25"/>
+      <c r="C1666" s="25"/>
+      <c r="D1666" s="25"/>
+      <c r="E1666" s="25"/>
     </row>
     <row r="1667" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1667" s="21"/>
-      <c r="B1667" s="22"/>
-      <c r="C1667" s="21"/>
-      <c r="D1667" s="21"/>
-      <c r="E1667" s="21"/>
+      <c r="A1667" s="25"/>
+      <c r="B1667" s="25"/>
+      <c r="C1667" s="25"/>
+      <c r="D1667" s="25"/>
+      <c r="E1667" s="25"/>
     </row>
     <row r="1668" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1668" s="21"/>
-      <c r="B1668" s="22"/>
-      <c r="C1668" s="21"/>
-      <c r="D1668" s="21"/>
-      <c r="E1668" s="21"/>
+      <c r="A1668" s="25"/>
+      <c r="B1668" s="25"/>
+      <c r="C1668" s="25"/>
+      <c r="D1668" s="25"/>
+      <c r="E1668" s="25"/>
     </row>
     <row r="1669" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1669" s="21"/>
-      <c r="B1669" s="22"/>
-      <c r="C1669" s="21"/>
-      <c r="D1669" s="21"/>
-      <c r="E1669" s="21"/>
+      <c r="A1669" s="25"/>
+      <c r="B1669" s="25"/>
+      <c r="C1669" s="25"/>
+      <c r="D1669" s="25"/>
+      <c r="E1669" s="25"/>
     </row>
     <row r="1670" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1670" s="21"/>
-      <c r="B1670" s="22"/>
-      <c r="C1670" s="21"/>
-      <c r="D1670" s="21"/>
-      <c r="E1670" s="21"/>
+      <c r="A1670" s="25"/>
+      <c r="B1670" s="25"/>
+      <c r="C1670" s="25"/>
+      <c r="D1670" s="25"/>
+      <c r="E1670" s="25"/>
     </row>
     <row r="1671" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1671" s="21"/>
-      <c r="B1671" s="22"/>
-      <c r="C1671" s="21"/>
-      <c r="D1671" s="21"/>
-      <c r="E1671" s="21"/>
+      <c r="A1671" s="25"/>
+      <c r="B1671" s="25"/>
+      <c r="C1671" s="25"/>
+      <c r="D1671" s="25"/>
+      <c r="E1671" s="25"/>
     </row>
     <row r="1672" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1672" s="21"/>
-      <c r="B1672" s="22"/>
-      <c r="C1672" s="21"/>
-      <c r="D1672" s="21"/>
-      <c r="E1672" s="21"/>
+      <c r="A1672" s="25"/>
+      <c r="B1672" s="25"/>
+      <c r="C1672" s="25"/>
+      <c r="D1672" s="25"/>
+      <c r="E1672" s="25"/>
     </row>
     <row r="1673" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1673" s="21"/>
-      <c r="B1673" s="22"/>
-      <c r="C1673" s="21"/>
-      <c r="D1673" s="21"/>
-      <c r="E1673" s="21"/>
+      <c r="A1673" s="25"/>
+      <c r="B1673" s="25"/>
+      <c r="C1673" s="25"/>
+      <c r="D1673" s="25"/>
+      <c r="E1673" s="25"/>
     </row>
     <row r="1674" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1674" s="21"/>
-      <c r="B1674" s="22"/>
-      <c r="C1674" s="21"/>
-      <c r="D1674" s="21"/>
-      <c r="E1674" s="21"/>
+      <c r="A1674" s="25"/>
+      <c r="B1674" s="25"/>
+      <c r="C1674" s="25"/>
+      <c r="D1674" s="25"/>
+      <c r="E1674" s="25"/>
     </row>
     <row r="1675" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1675" s="21"/>
-      <c r="B1675" s="22"/>
-      <c r="C1675" s="21"/>
-      <c r="D1675" s="21"/>
-      <c r="E1675" s="21"/>
+      <c r="A1675" s="25"/>
+      <c r="B1675" s="25"/>
+      <c r="C1675" s="25"/>
+      <c r="D1675" s="25"/>
+      <c r="E1675" s="25"/>
     </row>
     <row r="1676" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1676" s="21"/>
-      <c r="B1676" s="22"/>
-      <c r="C1676" s="21"/>
-      <c r="D1676" s="21"/>
-      <c r="E1676" s="21"/>
+      <c r="A1676" s="25"/>
+      <c r="B1676" s="25"/>
+      <c r="C1676" s="25"/>
+      <c r="D1676" s="25"/>
+      <c r="E1676" s="25"/>
     </row>
     <row r="1677" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1677" s="21"/>
-      <c r="B1677" s="22"/>
-      <c r="C1677" s="21"/>
-      <c r="D1677" s="21"/>
-      <c r="E1677" s="21"/>
+      <c r="A1677" s="25"/>
+      <c r="B1677" s="25"/>
+      <c r="C1677" s="25"/>
+      <c r="D1677" s="25"/>
+      <c r="E1677" s="25"/>
     </row>
     <row r="1678" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1678" s="21"/>
-      <c r="B1678" s="22"/>
-      <c r="C1678" s="21"/>
-      <c r="D1678" s="21"/>
-      <c r="E1678" s="21"/>
+      <c r="A1678" s="25"/>
+      <c r="B1678" s="25"/>
+      <c r="C1678" s="25"/>
+      <c r="D1678" s="25"/>
+      <c r="E1678" s="25"/>
     </row>
     <row r="1679" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1679" s="21"/>
-      <c r="B1679" s="22"/>
-      <c r="C1679" s="21"/>
-      <c r="D1679" s="21"/>
-      <c r="E1679" s="21"/>
+      <c r="A1679" s="25"/>
+      <c r="B1679" s="25"/>
+      <c r="C1679" s="25"/>
+      <c r="D1679" s="25"/>
+      <c r="E1679" s="25"/>
     </row>
     <row r="1680" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1680" s="21"/>
-      <c r="B1680" s="21"/>
-      <c r="C1680" s="21"/>
-      <c r="D1680" s="21"/>
-      <c r="E1680" s="21"/>
+      <c r="A1680" s="25"/>
+      <c r="B1680" s="25"/>
+      <c r="C1680" s="25"/>
+      <c r="D1680" s="25"/>
+      <c r="E1680" s="25"/>
     </row>
     <row r="1681" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1681" s="21"/>
-      <c r="B1681" s="21"/>
-      <c r="C1681" s="21"/>
-      <c r="D1681" s="21"/>
-      <c r="E1681" s="21"/>
+      <c r="A1681" s="25"/>
+      <c r="B1681" s="25"/>
+      <c r="C1681" s="25"/>
+      <c r="D1681" s="25"/>
+      <c r="E1681" s="25"/>
     </row>
     <row r="1682" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1682" s="21"/>
-      <c r="B1682" s="21"/>
-      <c r="C1682" s="21"/>
-      <c r="D1682" s="21"/>
-      <c r="E1682" s="21"/>
+      <c r="A1682" s="25"/>
+      <c r="B1682" s="25"/>
+      <c r="C1682" s="25"/>
+      <c r="D1682" s="25"/>
+      <c r="E1682" s="25"/>
     </row>
     <row r="1683" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1683" s="21"/>
-      <c r="B1683" s="21"/>
-      <c r="C1683" s="21"/>
-      <c r="D1683" s="21"/>
-      <c r="E1683" s="21"/>
+      <c r="A1683" s="25"/>
+      <c r="B1683" s="25"/>
+      <c r="C1683" s="25"/>
+      <c r="D1683" s="25"/>
+      <c r="E1683" s="25"/>
     </row>
     <row r="1684" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1684" s="21"/>
-      <c r="B1684" s="21"/>
-      <c r="C1684" s="21"/>
-      <c r="D1684" s="21"/>
-      <c r="E1684" s="21"/>
+      <c r="A1684" s="25"/>
+      <c r="B1684" s="25"/>
+      <c r="C1684" s="25"/>
+      <c r="D1684" s="25"/>
+      <c r="E1684" s="25"/>
     </row>
     <row r="1685" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1685" s="21"/>
-      <c r="B1685" s="21"/>
-      <c r="C1685" s="21"/>
-      <c r="D1685" s="21"/>
-      <c r="E1685" s="21"/>
+      <c r="A1685" s="25"/>
+      <c r="B1685" s="25"/>
+      <c r="C1685" s="25"/>
+      <c r="D1685" s="25"/>
+      <c r="E1685" s="25"/>
     </row>
     <row r="1686" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1686" s="21"/>
-      <c r="B1686" s="21"/>
-      <c r="C1686" s="21"/>
-      <c r="D1686" s="21"/>
-      <c r="E1686" s="21"/>
+      <c r="A1686" s="25"/>
+      <c r="B1686" s="25"/>
+      <c r="C1686" s="25"/>
+      <c r="D1686" s="25"/>
+      <c r="E1686" s="25"/>
     </row>
     <row r="1687" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1687" s="21"/>
-      <c r="B1687" s="21"/>
-      <c r="C1687" s="21"/>
-      <c r="D1687" s="21"/>
-      <c r="E1687" s="21"/>
+      <c r="A1687" s="25"/>
+      <c r="B1687" s="25"/>
+      <c r="C1687" s="25"/>
+      <c r="D1687" s="25"/>
+      <c r="E1687" s="25"/>
     </row>
     <row r="1688" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1688" s="21"/>
-      <c r="B1688" s="21"/>
-      <c r="C1688" s="21"/>
-      <c r="D1688" s="21"/>
-      <c r="E1688" s="21"/>
+      <c r="A1688" s="25"/>
+      <c r="B1688" s="25"/>
+      <c r="C1688" s="25"/>
+      <c r="D1688" s="25"/>
+      <c r="E1688" s="25"/>
     </row>
     <row r="1689" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1689" s="21"/>
-      <c r="B1689" s="21"/>
-      <c r="C1689" s="21"/>
-      <c r="D1689" s="21"/>
-      <c r="E1689" s="21"/>
+      <c r="A1689" s="25"/>
+      <c r="B1689" s="25"/>
+      <c r="C1689" s="25"/>
+      <c r="D1689" s="25"/>
+      <c r="E1689" s="25"/>
     </row>
     <row r="1690" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1690" s="21"/>
-      <c r="B1690" s="21"/>
-      <c r="C1690" s="21"/>
-      <c r="D1690" s="21"/>
-      <c r="E1690" s="21"/>
+      <c r="A1690" s="25"/>
+      <c r="B1690" s="25"/>
+      <c r="C1690" s="25"/>
+      <c r="D1690" s="25"/>
+      <c r="E1690" s="25"/>
     </row>
     <row r="1691" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1691" s="21"/>
-      <c r="B1691" s="21"/>
-      <c r="C1691" s="21"/>
-      <c r="D1691" s="21"/>
-      <c r="E1691" s="21"/>
+      <c r="A1691" s="25"/>
+      <c r="B1691" s="25"/>
+      <c r="C1691" s="25"/>
+      <c r="D1691" s="25"/>
+      <c r="E1691" s="25"/>
     </row>
     <row r="1692" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1692" s="21"/>
-      <c r="B1692" s="21"/>
-      <c r="C1692" s="21"/>
-      <c r="D1692" s="21"/>
-      <c r="E1692" s="21"/>
+      <c r="A1692" s="25"/>
+      <c r="B1692" s="25"/>
+      <c r="C1692" s="25"/>
+      <c r="D1692" s="25"/>
+      <c r="E1692" s="25"/>
     </row>
     <row r="1693" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1693" s="21"/>
-      <c r="B1693" s="21"/>
-      <c r="C1693" s="21"/>
-      <c r="D1693" s="21"/>
-      <c r="E1693" s="21"/>
+      <c r="A1693" s="25"/>
+      <c r="B1693" s="25"/>
+      <c r="C1693" s="25"/>
+      <c r="D1693" s="25"/>
+      <c r="E1693" s="25"/>
     </row>
     <row r="1694" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1694" s="21"/>
-      <c r="B1694" s="21"/>
-      <c r="C1694" s="21"/>
-      <c r="D1694" s="21"/>
-      <c r="E1694" s="21"/>
+      <c r="A1694" s="25"/>
+      <c r="B1694" s="25"/>
+      <c r="C1694" s="25"/>
+      <c r="D1694" s="25"/>
+      <c r="E1694" s="25"/>
     </row>
     <row r="1695" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1695" s="21"/>
-      <c r="B1695" s="21"/>
-      <c r="C1695" s="21"/>
-      <c r="D1695" s="21"/>
-      <c r="E1695" s="21"/>
+      <c r="A1695" s="25"/>
+      <c r="B1695" s="25"/>
+      <c r="C1695" s="25"/>
+      <c r="D1695" s="25"/>
+      <c r="E1695" s="25"/>
     </row>
     <row r="1696" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1696" s="21"/>
-      <c r="B1696" s="21"/>
-      <c r="C1696" s="21"/>
-      <c r="D1696" s="21"/>
-      <c r="E1696" s="21"/>
-    </row>
-    <row r="1697" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1697" s="21"/>
-      <c r="B1697" s="21"/>
-      <c r="C1697" s="21"/>
-      <c r="D1697" s="21"/>
-      <c r="E1697" s="21"/>
-    </row>
-    <row r="1698" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1698" s="21"/>
-      <c r="B1698" s="21"/>
-      <c r="C1698" s="21"/>
-      <c r="D1698" s="21"/>
-      <c r="E1698" s="21"/>
-    </row>
-    <row r="1699" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1699" s="21"/>
-      <c r="B1699" s="21"/>
-      <c r="C1699" s="21"/>
-      <c r="D1699" s="21"/>
-      <c r="E1699" s="21"/>
-    </row>
-    <row r="1700" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1700" s="21"/>
-      <c r="B1700" s="21"/>
-      <c r="C1700" s="21"/>
-      <c r="D1700" s="21"/>
-      <c r="E1700" s="21"/>
-      <c r="F1700" s="5"/>
-    </row>
-    <row r="1701" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1701" s="21"/>
-      <c r="B1701" s="21"/>
-      <c r="C1701" s="21"/>
-      <c r="D1701" s="21"/>
-      <c r="E1701" s="21"/>
-      <c r="F1701" s="5"/>
-    </row>
-    <row r="1702" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1702" s="21"/>
-      <c r="B1702" s="21"/>
-      <c r="C1702" s="21"/>
-      <c r="D1702" s="21"/>
-      <c r="E1702" s="21"/>
-      <c r="F1702" s="5"/>
-    </row>
-    <row r="1703" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1703" s="21"/>
-      <c r="B1703" s="21"/>
-      <c r="C1703" s="21"/>
-      <c r="D1703" s="21"/>
-      <c r="E1703" s="21"/>
-    </row>
-    <row r="1704" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1704" s="21"/>
-      <c r="B1704" s="21"/>
-      <c r="C1704" s="21"/>
-      <c r="D1704" s="21"/>
-      <c r="E1704" s="21"/>
-    </row>
-    <row r="1705" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1705" s="21"/>
-      <c r="B1705" s="21"/>
-      <c r="C1705" s="21"/>
-      <c r="D1705" s="21"/>
-      <c r="E1705" s="21"/>
-    </row>
-    <row r="1706" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1706" s="21"/>
-      <c r="B1706" s="21"/>
-      <c r="C1706" s="21"/>
-      <c r="D1706" s="21"/>
-      <c r="E1706" s="21"/>
-    </row>
-    <row r="1707" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1707" s="21"/>
-      <c r="B1707" s="21"/>
-      <c r="C1707" s="21"/>
-      <c r="D1707" s="21"/>
-      <c r="E1707" s="21"/>
-    </row>
-    <row r="1708" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1708" s="21"/>
-      <c r="B1708" s="21"/>
-      <c r="C1708" s="21"/>
-      <c r="D1708" s="21"/>
-      <c r="E1708" s="21"/>
-    </row>
-    <row r="1709" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1709" s="21"/>
-      <c r="B1709" s="21"/>
-      <c r="C1709" s="21"/>
-      <c r="D1709" s="21"/>
-      <c r="E1709" s="21"/>
-    </row>
-    <row r="1710" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1710" s="21"/>
-      <c r="B1710" s="21"/>
-      <c r="C1710" s="21"/>
-      <c r="D1710" s="21"/>
-      <c r="E1710" s="21"/>
-    </row>
-    <row r="1711" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1711" s="21"/>
-      <c r="B1711" s="21"/>
-      <c r="C1711" s="21"/>
-      <c r="D1711" s="21"/>
-      <c r="E1711" s="21"/>
-    </row>
-    <row r="1712" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1712" s="21"/>
-      <c r="B1712" s="24"/>
-      <c r="C1712" s="21"/>
-      <c r="D1712" s="21"/>
-      <c r="E1712" s="21"/>
+      <c r="A1696" s="25"/>
+      <c r="B1696" s="25"/>
+      <c r="C1696" s="25"/>
+      <c r="D1696" s="25"/>
+      <c r="E1696" s="25"/>
+    </row>
+    <row r="1697" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1697" s="25"/>
+      <c r="B1697" s="25"/>
+      <c r="C1697" s="25"/>
+      <c r="D1697" s="25"/>
+      <c r="E1697" s="25"/>
+    </row>
+    <row r="1698" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1698" s="25"/>
+      <c r="B1698" s="25"/>
+      <c r="C1698" s="25"/>
+      <c r="D1698" s="25"/>
+      <c r="E1698" s="25"/>
+    </row>
+    <row r="1699" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1699" s="25"/>
+      <c r="B1699" s="25"/>
+      <c r="C1699" s="25"/>
+      <c r="D1699" s="25"/>
+      <c r="E1699" s="25"/>
+    </row>
+    <row r="1700" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1700" s="25"/>
+      <c r="B1700" s="25"/>
+      <c r="C1700" s="25"/>
+      <c r="D1700" s="25"/>
+      <c r="E1700" s="25"/>
+    </row>
+    <row r="1701" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1701" s="25"/>
+      <c r="B1701" s="25"/>
+      <c r="C1701" s="25"/>
+      <c r="D1701" s="25"/>
+      <c r="E1701" s="25"/>
+    </row>
+    <row r="1702" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1702" s="25"/>
+      <c r="B1702" s="25"/>
+      <c r="C1702" s="25"/>
+      <c r="D1702" s="25"/>
+      <c r="E1702" s="25"/>
+    </row>
+    <row r="1703" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1703" s="25"/>
+      <c r="B1703" s="25"/>
+      <c r="C1703" s="25"/>
+      <c r="D1703" s="25"/>
+      <c r="E1703" s="25"/>
+    </row>
+    <row r="1704" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1704" s="25"/>
+      <c r="B1704" s="25"/>
+      <c r="C1704" s="25"/>
+      <c r="D1704" s="25"/>
+      <c r="E1704" s="25"/>
+    </row>
+    <row r="1705" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1705" s="25"/>
+      <c r="B1705" s="25"/>
+      <c r="C1705" s="25"/>
+      <c r="D1705" s="25"/>
+      <c r="E1705" s="25"/>
+    </row>
+    <row r="1706" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1706" s="25"/>
+      <c r="B1706" s="25"/>
+      <c r="C1706" s="25"/>
+      <c r="D1706" s="25"/>
+      <c r="E1706" s="25"/>
+    </row>
+    <row r="1707" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1707" s="25"/>
+      <c r="B1707" s="25"/>
+      <c r="C1707" s="25"/>
+      <c r="D1707" s="25"/>
+      <c r="E1707" s="25"/>
+    </row>
+    <row r="1708" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1708" s="25"/>
+      <c r="B1708" s="25"/>
+      <c r="C1708" s="25"/>
+      <c r="D1708" s="25"/>
+      <c r="E1708" s="25"/>
+    </row>
+    <row r="1709" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1709" s="25"/>
+      <c r="B1709" s="25"/>
+      <c r="C1709" s="25"/>
+      <c r="D1709" s="25"/>
+      <c r="E1709" s="25"/>
+    </row>
+    <row r="1710" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1710" s="25"/>
+      <c r="B1710" s="25"/>
+      <c r="C1710" s="25"/>
+      <c r="D1710" s="25"/>
+      <c r="E1710" s="25"/>
+    </row>
+    <row r="1711" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1711" s="25"/>
+      <c r="B1711" s="25"/>
+      <c r="C1711" s="25"/>
+      <c r="D1711" s="25"/>
+      <c r="E1711" s="25"/>
+    </row>
+    <row r="1712" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1712" s="25"/>
+      <c r="B1712" s="25"/>
+      <c r="C1712" s="25"/>
+      <c r="D1712" s="25"/>
+      <c r="E1712" s="25"/>
     </row>
     <row r="1713" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1713" s="21"/>
-      <c r="B1713" s="24"/>
-      <c r="C1713" s="21"/>
-      <c r="D1713" s="21"/>
-      <c r="E1713" s="21"/>
+      <c r="A1713" s="25"/>
+      <c r="B1713" s="25"/>
+      <c r="C1713" s="25"/>
+      <c r="D1713" s="25"/>
+      <c r="E1713" s="25"/>
     </row>
     <row r="1714" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1714" s="21"/>
-      <c r="B1714" s="21"/>
-      <c r="C1714" s="21"/>
-      <c r="D1714" s="21"/>
-      <c r="E1714" s="21"/>
+      <c r="A1714" s="25"/>
+      <c r="B1714" s="25"/>
+      <c r="C1714" s="25"/>
+      <c r="D1714" s="25"/>
+      <c r="E1714" s="25"/>
     </row>
     <row r="1715" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1715" s="21"/>
-      <c r="B1715" s="21"/>
-      <c r="C1715" s="21"/>
-      <c r="D1715" s="21"/>
-      <c r="E1715" s="21"/>
+      <c r="A1715" s="25"/>
+      <c r="B1715" s="25"/>
+      <c r="C1715" s="25"/>
+      <c r="D1715" s="25"/>
+      <c r="E1715" s="25"/>
     </row>
     <row r="1716" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1716" s="21"/>
-      <c r="B1716" s="21"/>
-      <c r="C1716" s="21"/>
-      <c r="D1716" s="21"/>
-      <c r="E1716" s="21"/>
+      <c r="A1716" s="25"/>
+      <c r="B1716" s="25"/>
+      <c r="C1716" s="25"/>
+      <c r="D1716" s="25"/>
+      <c r="E1716" s="25"/>
     </row>
     <row r="1717" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1717" s="21"/>
-      <c r="B1717" s="21"/>
-      <c r="C1717" s="21"/>
-      <c r="D1717" s="21"/>
-      <c r="E1717" s="21"/>
+      <c r="A1717" s="25"/>
+      <c r="B1717" s="25"/>
+      <c r="C1717" s="25"/>
+      <c r="D1717" s="25"/>
+      <c r="E1717" s="25"/>
     </row>
     <row r="1718" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1718" s="21"/>
-      <c r="B1718" s="21"/>
-      <c r="C1718" s="21"/>
-      <c r="D1718" s="21"/>
-      <c r="E1718" s="21"/>
+      <c r="A1718" s="25"/>
+      <c r="B1718" s="25"/>
+      <c r="C1718" s="25"/>
+      <c r="D1718" s="25"/>
+      <c r="E1718" s="25"/>
     </row>
     <row r="1719" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1719" s="21"/>
-      <c r="B1719" s="21"/>
-      <c r="C1719" s="21"/>
-      <c r="D1719" s="21"/>
-      <c r="E1719" s="21"/>
+      <c r="A1719" s="25"/>
+      <c r="B1719" s="25"/>
+      <c r="C1719" s="25"/>
+      <c r="D1719" s="25"/>
+      <c r="E1719" s="25"/>
     </row>
     <row r="1720" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1720" s="21"/>
-      <c r="B1720" s="21"/>
-      <c r="C1720" s="21"/>
-      <c r="D1720" s="21"/>
-      <c r="E1720" s="21"/>
+      <c r="A1720" s="25"/>
+      <c r="B1720" s="25"/>
+      <c r="C1720" s="25"/>
+      <c r="D1720" s="25"/>
+      <c r="E1720" s="25"/>
     </row>
     <row r="1721" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1721" s="21"/>
-      <c r="B1721" s="21"/>
-      <c r="C1721" s="21"/>
-      <c r="D1721" s="21"/>
-      <c r="E1721" s="21"/>
+      <c r="A1721" s="25"/>
+      <c r="B1721" s="25"/>
+      <c r="C1721" s="25"/>
+      <c r="D1721" s="25"/>
+      <c r="E1721" s="25"/>
     </row>
     <row r="1722" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1722" s="21"/>
-      <c r="B1722" s="21"/>
-      <c r="C1722" s="21"/>
-      <c r="D1722" s="21"/>
-      <c r="E1722" s="21"/>
+      <c r="A1722" s="25"/>
+      <c r="B1722" s="25"/>
+      <c r="C1722" s="25"/>
+      <c r="D1722" s="25"/>
+      <c r="E1722" s="25"/>
     </row>
     <row r="1723" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1723" s="21"/>
-      <c r="B1723" s="21"/>
-      <c r="C1723" s="21"/>
-      <c r="D1723" s="21"/>
-      <c r="E1723" s="21"/>
+      <c r="A1723" s="25"/>
+      <c r="B1723" s="25"/>
+      <c r="C1723" s="25"/>
+      <c r="D1723" s="25"/>
+      <c r="E1723" s="25"/>
     </row>
     <row r="1724" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1724" s="21"/>
-      <c r="B1724" s="21"/>
-      <c r="C1724" s="21"/>
-      <c r="D1724" s="21"/>
-      <c r="E1724" s="21"/>
+      <c r="A1724" s="25"/>
+      <c r="B1724" s="25"/>
+      <c r="C1724" s="25"/>
+      <c r="D1724" s="25"/>
+      <c r="E1724" s="25"/>
     </row>
     <row r="1725" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1725" s="21"/>
-      <c r="B1725" s="21"/>
-      <c r="C1725" s="21"/>
-      <c r="D1725" s="21"/>
-      <c r="E1725" s="21"/>
+      <c r="A1725" s="25"/>
+      <c r="B1725" s="25"/>
+      <c r="C1725" s="25"/>
+      <c r="D1725" s="25"/>
+      <c r="E1725" s="25"/>
     </row>
     <row r="1726" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1726" s="21"/>
-      <c r="B1726" s="21"/>
-      <c r="C1726" s="21"/>
-      <c r="D1726" s="21"/>
-      <c r="E1726" s="21"/>
+      <c r="A1726" s="25"/>
+      <c r="B1726" s="25"/>
+      <c r="C1726" s="25"/>
+      <c r="D1726" s="25"/>
+      <c r="E1726" s="25"/>
     </row>
     <row r="1727" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1727" s="25"/>
-      <c r="B1727" s="26"/>
-      <c r="C1727" s="27"/>
+      <c r="B1727" s="25"/>
+      <c r="C1727" s="25"/>
       <c r="D1727" s="25"/>
       <c r="E1727" s="25"/>
     </row>
     <row r="1728" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1728" s="25"/>
-      <c r="B1728" s="26"/>
-      <c r="C1728" s="27"/>
+      <c r="B1728" s="25"/>
+      <c r="C1728" s="25"/>
       <c r="D1728" s="25"/>
       <c r="E1728" s="25"/>
     </row>
     <row r="1729" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1729" s="25"/>
-      <c r="B1729" s="26"/>
-      <c r="C1729" s="27"/>
+      <c r="B1729" s="25"/>
+      <c r="C1729" s="25"/>
       <c r="D1729" s="25"/>
       <c r="E1729" s="25"/>
     </row>
     <row r="1730" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1730" s="25"/>
-      <c r="B1730" s="26"/>
-      <c r="C1730" s="27"/>
+      <c r="B1730" s="25"/>
+      <c r="C1730" s="25"/>
       <c r="D1730" s="25"/>
       <c r="E1730" s="25"/>
     </row>
     <row r="1731" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1731" s="25"/>
-      <c r="B1731" s="26"/>
-      <c r="C1731" s="27"/>
+      <c r="B1731" s="25"/>
+      <c r="C1731" s="25"/>
       <c r="D1731" s="25"/>
       <c r="E1731" s="25"/>
     </row>
     <row r="1732" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1732" s="25"/>
-      <c r="B1732" s="26"/>
-      <c r="C1732" s="27"/>
+      <c r="B1732" s="25"/>
+      <c r="C1732" s="25"/>
       <c r="D1732" s="25"/>
       <c r="E1732" s="25"/>
     </row>
     <row r="1733" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1733" s="25"/>
-      <c r="B1733" s="26"/>
-      <c r="C1733" s="27"/>
+      <c r="B1733" s="25"/>
+      <c r="C1733" s="25"/>
       <c r="D1733" s="25"/>
       <c r="E1733" s="25"/>
     </row>
     <row r="1734" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1734" s="25"/>
-      <c r="B1734" s="26"/>
-      <c r="C1734" s="27"/>
+      <c r="B1734" s="25"/>
+      <c r="C1734" s="25"/>
       <c r="D1734" s="25"/>
       <c r="E1734" s="25"/>
     </row>
     <row r="1735" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1735" s="25"/>
-      <c r="B1735" s="26"/>
-      <c r="C1735" s="27"/>
+      <c r="B1735" s="25"/>
+      <c r="C1735" s="25"/>
       <c r="D1735" s="25"/>
       <c r="E1735" s="25"/>
     </row>
@@ -30215,7 +29747,7 @@
     <row r="1742" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1742" s="25"/>
       <c r="B1742" s="25"/>
-      <c r="C1742" s="25"/>
+      <c r="C1742" s="28"/>
       <c r="D1742" s="25"/>
       <c r="E1742" s="25"/>
     </row>
@@ -30250,7 +29782,7 @@
     <row r="1747" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1747" s="25"/>
       <c r="B1747" s="25"/>
-      <c r="C1747" s="25"/>
+      <c r="C1747" s="28"/>
       <c r="D1747" s="25"/>
       <c r="E1747" s="25"/>
     </row>
@@ -30312,112 +29844,112 @@
     </row>
     <row r="1756" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1756" s="25"/>
-      <c r="B1756" s="25"/>
+      <c r="B1756" s="29"/>
       <c r="C1756" s="25"/>
       <c r="D1756" s="25"/>
       <c r="E1756" s="25"/>
     </row>
     <row r="1757" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1757" s="25"/>
-      <c r="B1757" s="25"/>
+      <c r="B1757" s="29"/>
       <c r="C1757" s="25"/>
       <c r="D1757" s="25"/>
       <c r="E1757" s="25"/>
     </row>
     <row r="1758" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1758" s="25"/>
-      <c r="B1758" s="25"/>
+      <c r="B1758" s="29"/>
       <c r="C1758" s="25"/>
       <c r="D1758" s="25"/>
       <c r="E1758" s="25"/>
     </row>
     <row r="1759" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1759" s="25"/>
-      <c r="B1759" s="25"/>
+      <c r="B1759" s="29"/>
       <c r="C1759" s="25"/>
       <c r="D1759" s="25"/>
       <c r="E1759" s="25"/>
     </row>
     <row r="1760" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1760" s="25"/>
-      <c r="B1760" s="25"/>
+      <c r="B1760" s="29"/>
       <c r="C1760" s="25"/>
       <c r="D1760" s="25"/>
       <c r="E1760" s="25"/>
     </row>
     <row r="1761" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1761" s="25"/>
-      <c r="B1761" s="25"/>
+      <c r="B1761" s="29"/>
       <c r="C1761" s="25"/>
       <c r="D1761" s="25"/>
       <c r="E1761" s="25"/>
     </row>
     <row r="1762" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1762" s="25"/>
-      <c r="B1762" s="25"/>
+      <c r="B1762" s="29"/>
       <c r="C1762" s="25"/>
       <c r="D1762" s="25"/>
       <c r="E1762" s="25"/>
     </row>
     <row r="1763" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1763" s="25"/>
-      <c r="B1763" s="25"/>
+      <c r="B1763" s="29"/>
       <c r="C1763" s="25"/>
       <c r="D1763" s="25"/>
       <c r="E1763" s="25"/>
     </row>
     <row r="1764" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1764" s="25"/>
-      <c r="B1764" s="25"/>
+      <c r="B1764" s="29"/>
       <c r="C1764" s="25"/>
       <c r="D1764" s="25"/>
       <c r="E1764" s="25"/>
     </row>
     <row r="1765" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1765" s="25"/>
-      <c r="B1765" s="25"/>
+      <c r="B1765" s="29"/>
       <c r="C1765" s="25"/>
       <c r="D1765" s="25"/>
       <c r="E1765" s="25"/>
     </row>
     <row r="1766" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1766" s="25"/>
-      <c r="B1766" s="25"/>
+      <c r="B1766" s="29"/>
       <c r="C1766" s="25"/>
       <c r="D1766" s="25"/>
       <c r="E1766" s="25"/>
     </row>
     <row r="1767" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1767" s="25"/>
-      <c r="B1767" s="25"/>
+      <c r="B1767" s="29"/>
       <c r="C1767" s="25"/>
       <c r="D1767" s="25"/>
       <c r="E1767" s="25"/>
     </row>
     <row r="1768" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1768" s="25"/>
-      <c r="B1768" s="25"/>
+      <c r="B1768" s="29"/>
       <c r="C1768" s="25"/>
       <c r="D1768" s="25"/>
       <c r="E1768" s="25"/>
     </row>
     <row r="1769" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1769" s="25"/>
-      <c r="B1769" s="25"/>
+      <c r="B1769" s="29"/>
       <c r="C1769" s="25"/>
       <c r="D1769" s="25"/>
       <c r="E1769" s="25"/>
     </row>
     <row r="1770" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1770" s="25"/>
-      <c r="B1770" s="25"/>
+      <c r="B1770" s="29"/>
       <c r="C1770" s="25"/>
       <c r="D1770" s="25"/>
       <c r="E1770" s="25"/>
     </row>
     <row r="1771" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1771" s="25"/>
-      <c r="B1771" s="25"/>
+      <c r="B1771" s="29"/>
       <c r="C1771" s="25"/>
       <c r="D1771" s="25"/>
       <c r="E1771" s="25"/>
@@ -30460,7 +29992,7 @@
     <row r="1777" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1777" s="25"/>
       <c r="B1777" s="25"/>
-      <c r="C1777" s="25"/>
+      <c r="C1777" s="28"/>
       <c r="D1777" s="25"/>
       <c r="E1777" s="25"/>
     </row>
@@ -30747,7 +30279,7 @@
     <row r="1818" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1818" s="25"/>
       <c r="B1818" s="25"/>
-      <c r="C1818" s="28"/>
+      <c r="C1818" s="25"/>
       <c r="D1818" s="25"/>
       <c r="E1818" s="25"/>
     </row>
@@ -30782,7 +30314,7 @@
     <row r="1823" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1823" s="25"/>
       <c r="B1823" s="25"/>
-      <c r="C1823" s="28"/>
+      <c r="C1823" s="25"/>
       <c r="D1823" s="25"/>
       <c r="E1823" s="25"/>
     </row>
@@ -30844,112 +30376,112 @@
     </row>
     <row r="1832" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1832" s="25"/>
-      <c r="B1832" s="29"/>
+      <c r="B1832" s="25"/>
       <c r="C1832" s="25"/>
       <c r="D1832" s="25"/>
       <c r="E1832" s="25"/>
     </row>
     <row r="1833" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1833" s="25"/>
-      <c r="B1833" s="29"/>
+      <c r="B1833" s="25"/>
       <c r="C1833" s="25"/>
       <c r="D1833" s="25"/>
       <c r="E1833" s="25"/>
     </row>
     <row r="1834" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1834" s="25"/>
-      <c r="B1834" s="29"/>
+      <c r="B1834" s="25"/>
       <c r="C1834" s="25"/>
       <c r="D1834" s="25"/>
       <c r="E1834" s="25"/>
     </row>
     <row r="1835" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1835" s="25"/>
-      <c r="B1835" s="29"/>
+      <c r="B1835" s="25"/>
       <c r="C1835" s="25"/>
       <c r="D1835" s="25"/>
       <c r="E1835" s="25"/>
     </row>
     <row r="1836" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1836" s="25"/>
-      <c r="B1836" s="29"/>
+      <c r="B1836" s="25"/>
       <c r="C1836" s="25"/>
       <c r="D1836" s="25"/>
       <c r="E1836" s="25"/>
     </row>
     <row r="1837" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1837" s="25"/>
-      <c r="B1837" s="29"/>
+      <c r="B1837" s="25"/>
       <c r="C1837" s="25"/>
       <c r="D1837" s="25"/>
       <c r="E1837" s="25"/>
     </row>
     <row r="1838" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1838" s="25"/>
-      <c r="B1838" s="29"/>
+      <c r="B1838" s="25"/>
       <c r="C1838" s="25"/>
       <c r="D1838" s="25"/>
       <c r="E1838" s="25"/>
     </row>
     <row r="1839" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1839" s="25"/>
-      <c r="B1839" s="29"/>
+      <c r="B1839" s="25"/>
       <c r="C1839" s="25"/>
       <c r="D1839" s="25"/>
       <c r="E1839" s="25"/>
     </row>
     <row r="1840" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1840" s="25"/>
-      <c r="B1840" s="29"/>
+      <c r="B1840" s="25"/>
       <c r="C1840" s="25"/>
       <c r="D1840" s="25"/>
       <c r="E1840" s="25"/>
     </row>
     <row r="1841" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1841" s="25"/>
-      <c r="B1841" s="29"/>
+      <c r="B1841" s="25"/>
       <c r="C1841" s="25"/>
       <c r="D1841" s="25"/>
       <c r="E1841" s="25"/>
     </row>
     <row r="1842" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1842" s="25"/>
-      <c r="B1842" s="29"/>
+      <c r="B1842" s="25"/>
       <c r="C1842" s="25"/>
       <c r="D1842" s="25"/>
       <c r="E1842" s="25"/>
     </row>
     <row r="1843" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1843" s="25"/>
-      <c r="B1843" s="29"/>
+      <c r="B1843" s="25"/>
       <c r="C1843" s="25"/>
       <c r="D1843" s="25"/>
       <c r="E1843" s="25"/>
     </row>
     <row r="1844" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1844" s="25"/>
-      <c r="B1844" s="29"/>
+      <c r="B1844" s="25"/>
       <c r="C1844" s="25"/>
       <c r="D1844" s="25"/>
       <c r="E1844" s="25"/>
     </row>
     <row r="1845" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1845" s="25"/>
-      <c r="B1845" s="29"/>
+      <c r="B1845" s="25"/>
       <c r="C1845" s="25"/>
       <c r="D1845" s="25"/>
       <c r="E1845" s="25"/>
     </row>
     <row r="1846" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1846" s="25"/>
-      <c r="B1846" s="29"/>
+      <c r="B1846" s="25"/>
       <c r="C1846" s="25"/>
       <c r="D1846" s="25"/>
       <c r="E1846" s="25"/>
     </row>
     <row r="1847" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1847" s="25"/>
-      <c r="B1847" s="29"/>
+      <c r="B1847" s="25"/>
       <c r="C1847" s="25"/>
       <c r="D1847" s="25"/>
       <c r="E1847" s="25"/>
@@ -30992,7 +30524,7 @@
     <row r="1853" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1853" s="25"/>
       <c r="B1853" s="25"/>
-      <c r="C1853" s="28"/>
+      <c r="C1853" s="25"/>
       <c r="D1853" s="25"/>
       <c r="E1853" s="25"/>
     </row>
@@ -31012,14 +30544,14 @@
     </row>
     <row r="1856" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1856" s="25"/>
-      <c r="B1856" s="25"/>
+      <c r="B1856" s="26"/>
       <c r="C1856" s="25"/>
       <c r="D1856" s="25"/>
       <c r="E1856" s="25"/>
     </row>
     <row r="1857" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1857" s="25"/>
-      <c r="B1857" s="25"/>
+      <c r="B1857" s="26"/>
       <c r="C1857" s="25"/>
       <c r="D1857" s="25"/>
       <c r="E1857" s="25"/>
@@ -31234,540 +30766,8 @@
       <c r="D1887" s="25"/>
       <c r="E1887" s="25"/>
     </row>
-    <row r="1888" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1888" s="25"/>
-      <c r="B1888" s="25"/>
-      <c r="C1888" s="25"/>
-      <c r="D1888" s="25"/>
-      <c r="E1888" s="25"/>
-    </row>
-    <row r="1889" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1889" s="25"/>
-      <c r="B1889" s="25"/>
-      <c r="C1889" s="25"/>
-      <c r="D1889" s="25"/>
-      <c r="E1889" s="25"/>
-    </row>
-    <row r="1890" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1890" s="25"/>
-      <c r="B1890" s="25"/>
-      <c r="C1890" s="25"/>
-      <c r="D1890" s="25"/>
-      <c r="E1890" s="25"/>
-    </row>
-    <row r="1891" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1891" s="25"/>
-      <c r="B1891" s="25"/>
-      <c r="C1891" s="25"/>
-      <c r="D1891" s="25"/>
-      <c r="E1891" s="25"/>
-    </row>
-    <row r="1892" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1892" s="25"/>
-      <c r="B1892" s="25"/>
-      <c r="C1892" s="25"/>
-      <c r="D1892" s="25"/>
-      <c r="E1892" s="25"/>
-    </row>
-    <row r="1893" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1893" s="25"/>
-      <c r="B1893" s="25"/>
-      <c r="C1893" s="25"/>
-      <c r="D1893" s="25"/>
-      <c r="E1893" s="25"/>
-    </row>
-    <row r="1894" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1894" s="25"/>
-      <c r="B1894" s="25"/>
-      <c r="C1894" s="25"/>
-      <c r="D1894" s="25"/>
-      <c r="E1894" s="25"/>
-    </row>
-    <row r="1895" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1895" s="25"/>
-      <c r="B1895" s="25"/>
-      <c r="C1895" s="25"/>
-      <c r="D1895" s="25"/>
-      <c r="E1895" s="25"/>
-    </row>
-    <row r="1896" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1896" s="25"/>
-      <c r="B1896" s="25"/>
-      <c r="C1896" s="25"/>
-      <c r="D1896" s="25"/>
-      <c r="E1896" s="25"/>
-    </row>
-    <row r="1897" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1897" s="25"/>
-      <c r="B1897" s="25"/>
-      <c r="C1897" s="25"/>
-      <c r="D1897" s="25"/>
-      <c r="E1897" s="25"/>
-    </row>
-    <row r="1898" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1898" s="25"/>
-      <c r="B1898" s="25"/>
-      <c r="C1898" s="25"/>
-      <c r="D1898" s="25"/>
-      <c r="E1898" s="25"/>
-    </row>
-    <row r="1899" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1899" s="25"/>
-      <c r="B1899" s="25"/>
-      <c r="C1899" s="25"/>
-      <c r="D1899" s="25"/>
-      <c r="E1899" s="25"/>
-    </row>
-    <row r="1900" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1900" s="25"/>
-      <c r="B1900" s="25"/>
-      <c r="C1900" s="25"/>
-      <c r="D1900" s="25"/>
-      <c r="E1900" s="25"/>
-    </row>
-    <row r="1901" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1901" s="25"/>
-      <c r="B1901" s="25"/>
-      <c r="C1901" s="25"/>
-      <c r="D1901" s="25"/>
-      <c r="E1901" s="25"/>
-    </row>
-    <row r="1902" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1902" s="25"/>
-      <c r="B1902" s="25"/>
-      <c r="C1902" s="25"/>
-      <c r="D1902" s="25"/>
-      <c r="E1902" s="25"/>
-    </row>
-    <row r="1903" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1903" s="25"/>
-      <c r="B1903" s="25"/>
-      <c r="C1903" s="25"/>
-      <c r="D1903" s="25"/>
-      <c r="E1903" s="25"/>
-    </row>
-    <row r="1904" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1904" s="25"/>
-      <c r="B1904" s="25"/>
-      <c r="C1904" s="25"/>
-      <c r="D1904" s="25"/>
-      <c r="E1904" s="25"/>
-    </row>
-    <row r="1905" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1905" s="25"/>
-      <c r="B1905" s="25"/>
-      <c r="C1905" s="25"/>
-      <c r="D1905" s="25"/>
-      <c r="E1905" s="25"/>
-    </row>
-    <row r="1906" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1906" s="25"/>
-      <c r="B1906" s="25"/>
-      <c r="C1906" s="25"/>
-      <c r="D1906" s="25"/>
-      <c r="E1906" s="25"/>
-    </row>
-    <row r="1907" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1907" s="25"/>
-      <c r="B1907" s="25"/>
-      <c r="C1907" s="25"/>
-      <c r="D1907" s="25"/>
-      <c r="E1907" s="25"/>
-    </row>
-    <row r="1908" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1908" s="25"/>
-      <c r="B1908" s="25"/>
-      <c r="C1908" s="25"/>
-      <c r="D1908" s="25"/>
-      <c r="E1908" s="25"/>
-    </row>
-    <row r="1909" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1909" s="25"/>
-      <c r="B1909" s="25"/>
-      <c r="C1909" s="25"/>
-      <c r="D1909" s="25"/>
-      <c r="E1909" s="25"/>
-    </row>
-    <row r="1910" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1910" s="25"/>
-      <c r="B1910" s="25"/>
-      <c r="C1910" s="25"/>
-      <c r="D1910" s="25"/>
-      <c r="E1910" s="25"/>
-    </row>
-    <row r="1911" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1911" s="25"/>
-      <c r="B1911" s="25"/>
-      <c r="C1911" s="25"/>
-      <c r="D1911" s="25"/>
-      <c r="E1911" s="25"/>
-    </row>
-    <row r="1912" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1912" s="25"/>
-      <c r="B1912" s="25"/>
-      <c r="C1912" s="25"/>
-      <c r="D1912" s="25"/>
-      <c r="E1912" s="25"/>
-    </row>
-    <row r="1913" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1913" s="25"/>
-      <c r="B1913" s="25"/>
-      <c r="C1913" s="25"/>
-      <c r="D1913" s="25"/>
-      <c r="E1913" s="25"/>
-    </row>
-    <row r="1914" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1914" s="25"/>
-      <c r="B1914" s="25"/>
-      <c r="C1914" s="25"/>
-      <c r="D1914" s="25"/>
-      <c r="E1914" s="25"/>
-    </row>
-    <row r="1915" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1915" s="25"/>
-      <c r="B1915" s="25"/>
-      <c r="C1915" s="25"/>
-      <c r="D1915" s="25"/>
-      <c r="E1915" s="25"/>
-    </row>
-    <row r="1916" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1916" s="25"/>
-      <c r="B1916" s="25"/>
-      <c r="C1916" s="25"/>
-      <c r="D1916" s="25"/>
-      <c r="E1916" s="25"/>
-    </row>
-    <row r="1917" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1917" s="25"/>
-      <c r="B1917" s="25"/>
-      <c r="C1917" s="25"/>
-      <c r="D1917" s="25"/>
-      <c r="E1917" s="25"/>
-    </row>
-    <row r="1918" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1918" s="25"/>
-      <c r="B1918" s="25"/>
-      <c r="C1918" s="25"/>
-      <c r="D1918" s="25"/>
-      <c r="E1918" s="25"/>
-    </row>
-    <row r="1919" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1919" s="25"/>
-      <c r="B1919" s="25"/>
-      <c r="C1919" s="25"/>
-      <c r="D1919" s="25"/>
-      <c r="E1919" s="25"/>
-    </row>
-    <row r="1920" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1920" s="25"/>
-      <c r="B1920" s="25"/>
-      <c r="C1920" s="25"/>
-      <c r="D1920" s="25"/>
-      <c r="E1920" s="25"/>
-    </row>
-    <row r="1921" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1921" s="25"/>
-      <c r="B1921" s="25"/>
-      <c r="C1921" s="25"/>
-      <c r="D1921" s="25"/>
-      <c r="E1921" s="25"/>
-    </row>
-    <row r="1922" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1922" s="25"/>
-      <c r="B1922" s="25"/>
-      <c r="C1922" s="25"/>
-      <c r="D1922" s="25"/>
-      <c r="E1922" s="25"/>
-    </row>
-    <row r="1923" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1923" s="25"/>
-      <c r="B1923" s="25"/>
-      <c r="C1923" s="25"/>
-      <c r="D1923" s="25"/>
-      <c r="E1923" s="25"/>
-    </row>
-    <row r="1924" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1924" s="25"/>
-      <c r="B1924" s="25"/>
-      <c r="C1924" s="25"/>
-      <c r="D1924" s="25"/>
-      <c r="E1924" s="25"/>
-    </row>
-    <row r="1925" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1925" s="25"/>
-      <c r="B1925" s="25"/>
-      <c r="C1925" s="25"/>
-      <c r="D1925" s="25"/>
-      <c r="E1925" s="25"/>
-    </row>
-    <row r="1926" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1926" s="25"/>
-      <c r="B1926" s="25"/>
-      <c r="C1926" s="25"/>
-      <c r="D1926" s="25"/>
-      <c r="E1926" s="25"/>
-    </row>
-    <row r="1927" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1927" s="25"/>
-      <c r="B1927" s="25"/>
-      <c r="C1927" s="25"/>
-      <c r="D1927" s="25"/>
-      <c r="E1927" s="25"/>
-    </row>
-    <row r="1928" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1928" s="25"/>
-      <c r="B1928" s="25"/>
-      <c r="C1928" s="25"/>
-      <c r="D1928" s="25"/>
-      <c r="E1928" s="25"/>
-    </row>
-    <row r="1929" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1929" s="25"/>
-      <c r="B1929" s="25"/>
-      <c r="C1929" s="25"/>
-      <c r="D1929" s="25"/>
-      <c r="E1929" s="25"/>
-    </row>
-    <row r="1930" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1930" s="25"/>
-      <c r="B1930" s="25"/>
-      <c r="C1930" s="25"/>
-      <c r="D1930" s="25"/>
-      <c r="E1930" s="25"/>
-    </row>
-    <row r="1931" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1931" s="25"/>
-      <c r="B1931" s="25"/>
-      <c r="C1931" s="25"/>
-      <c r="D1931" s="25"/>
-      <c r="E1931" s="25"/>
-    </row>
-    <row r="1932" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1932" s="25"/>
-      <c r="B1932" s="26"/>
-      <c r="C1932" s="25"/>
-      <c r="D1932" s="25"/>
-      <c r="E1932" s="25"/>
-    </row>
-    <row r="1933" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1933" s="25"/>
-      <c r="B1933" s="26"/>
-      <c r="C1933" s="25"/>
-      <c r="D1933" s="25"/>
-      <c r="E1933" s="25"/>
-    </row>
-    <row r="1934" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1934" s="25"/>
-      <c r="B1934" s="25"/>
-      <c r="C1934" s="25"/>
-      <c r="D1934" s="25"/>
-      <c r="E1934" s="25"/>
-    </row>
-    <row r="1935" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1935" s="25"/>
-      <c r="B1935" s="25"/>
-      <c r="C1935" s="25"/>
-      <c r="D1935" s="25"/>
-      <c r="E1935" s="25"/>
-    </row>
-    <row r="1936" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1936" s="25"/>
-      <c r="B1936" s="25"/>
-      <c r="C1936" s="25"/>
-      <c r="D1936" s="25"/>
-      <c r="E1936" s="25"/>
-    </row>
-    <row r="1937" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1937" s="25"/>
-      <c r="B1937" s="25"/>
-      <c r="C1937" s="25"/>
-      <c r="D1937" s="25"/>
-      <c r="E1937" s="25"/>
-    </row>
-    <row r="1938" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1938" s="25"/>
-      <c r="B1938" s="25"/>
-      <c r="C1938" s="25"/>
-      <c r="D1938" s="25"/>
-      <c r="E1938" s="25"/>
-    </row>
-    <row r="1939" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1939" s="25"/>
-      <c r="B1939" s="25"/>
-      <c r="C1939" s="25"/>
-      <c r="D1939" s="25"/>
-      <c r="E1939" s="25"/>
-    </row>
-    <row r="1940" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1940" s="25"/>
-      <c r="B1940" s="25"/>
-      <c r="C1940" s="25"/>
-      <c r="D1940" s="25"/>
-      <c r="E1940" s="25"/>
-    </row>
-    <row r="1941" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1941" s="25"/>
-      <c r="B1941" s="25"/>
-      <c r="C1941" s="25"/>
-      <c r="D1941" s="25"/>
-      <c r="E1941" s="25"/>
-    </row>
-    <row r="1942" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1942" s="25"/>
-      <c r="B1942" s="25"/>
-      <c r="C1942" s="25"/>
-      <c r="D1942" s="25"/>
-      <c r="E1942" s="25"/>
-    </row>
-    <row r="1943" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1943" s="25"/>
-      <c r="B1943" s="25"/>
-      <c r="C1943" s="25"/>
-      <c r="D1943" s="25"/>
-      <c r="E1943" s="25"/>
-    </row>
-    <row r="1944" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1944" s="25"/>
-      <c r="B1944" s="25"/>
-      <c r="C1944" s="25"/>
-      <c r="D1944" s="25"/>
-      <c r="E1944" s="25"/>
-    </row>
-    <row r="1945" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1945" s="25"/>
-      <c r="B1945" s="25"/>
-      <c r="C1945" s="25"/>
-      <c r="D1945" s="25"/>
-      <c r="E1945" s="25"/>
-    </row>
-    <row r="1946" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1946" s="25"/>
-      <c r="B1946" s="25"/>
-      <c r="C1946" s="25"/>
-      <c r="D1946" s="25"/>
-      <c r="E1946" s="25"/>
-    </row>
-    <row r="1947" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1947" s="25"/>
-      <c r="B1947" s="25"/>
-      <c r="C1947" s="25"/>
-      <c r="D1947" s="25"/>
-      <c r="E1947" s="25"/>
-    </row>
-    <row r="1948" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1948" s="25"/>
-      <c r="B1948" s="25"/>
-      <c r="C1948" s="25"/>
-      <c r="D1948" s="25"/>
-      <c r="E1948" s="25"/>
-    </row>
-    <row r="1949" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1949" s="25"/>
-      <c r="B1949" s="25"/>
-      <c r="C1949" s="25"/>
-      <c r="D1949" s="25"/>
-      <c r="E1949" s="25"/>
-    </row>
-    <row r="1950" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1950" s="25"/>
-      <c r="B1950" s="25"/>
-      <c r="C1950" s="25"/>
-      <c r="D1950" s="25"/>
-      <c r="E1950" s="25"/>
-    </row>
-    <row r="1951" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1951" s="25"/>
-      <c r="B1951" s="25"/>
-      <c r="C1951" s="25"/>
-      <c r="D1951" s="25"/>
-      <c r="E1951" s="25"/>
-    </row>
-    <row r="1952" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1952" s="25"/>
-      <c r="B1952" s="25"/>
-      <c r="C1952" s="25"/>
-      <c r="D1952" s="25"/>
-      <c r="E1952" s="25"/>
-    </row>
-    <row r="1953" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1953" s="25"/>
-      <c r="B1953" s="25"/>
-      <c r="C1953" s="25"/>
-      <c r="D1953" s="25"/>
-      <c r="E1953" s="25"/>
-    </row>
-    <row r="1954" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1954" s="25"/>
-      <c r="B1954" s="25"/>
-      <c r="C1954" s="25"/>
-      <c r="D1954" s="25"/>
-      <c r="E1954" s="25"/>
-    </row>
-    <row r="1955" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1955" s="25"/>
-      <c r="B1955" s="25"/>
-      <c r="C1955" s="25"/>
-      <c r="D1955" s="25"/>
-      <c r="E1955" s="25"/>
-    </row>
-    <row r="1956" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1956" s="25"/>
-      <c r="B1956" s="25"/>
-      <c r="C1956" s="25"/>
-      <c r="D1956" s="25"/>
-      <c r="E1956" s="25"/>
-    </row>
-    <row r="1957" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1957" s="25"/>
-      <c r="B1957" s="25"/>
-      <c r="C1957" s="25"/>
-      <c r="D1957" s="25"/>
-      <c r="E1957" s="25"/>
-    </row>
-    <row r="1958" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1958" s="25"/>
-      <c r="B1958" s="25"/>
-      <c r="C1958" s="25"/>
-      <c r="D1958" s="25"/>
-      <c r="E1958" s="25"/>
-    </row>
-    <row r="1959" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1959" s="25"/>
-      <c r="B1959" s="25"/>
-      <c r="C1959" s="25"/>
-      <c r="D1959" s="25"/>
-      <c r="E1959" s="25"/>
-    </row>
-    <row r="1960" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1960" s="25"/>
-      <c r="B1960" s="25"/>
-      <c r="C1960" s="25"/>
-      <c r="D1960" s="25"/>
-      <c r="E1960" s="25"/>
-    </row>
-    <row r="1961" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1961" s="25"/>
-      <c r="B1961" s="25"/>
-      <c r="C1961" s="25"/>
-      <c r="D1961" s="25"/>
-      <c r="E1961" s="25"/>
-    </row>
-    <row r="1962" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1962" s="25"/>
-      <c r="B1962" s="25"/>
-      <c r="C1962" s="25"/>
-      <c r="D1962" s="25"/>
-      <c r="E1962" s="25"/>
-    </row>
-    <row r="1963" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1963" s="25"/>
-      <c r="B1963" s="25"/>
-      <c r="C1963" s="25"/>
-      <c r="D1963" s="25"/>
-      <c r="E1963" s="25"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E1963"/>
+  <autoFilter ref="A1:E1887"/>
   <sortState ref="A2:E257">
     <sortCondition ref="A2:A257"/>
     <sortCondition ref="B2:B257"/>

</xml_diff>

<commit_message>
Fixed bie to bike in Muni
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6505" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6505" uniqueCount="646">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -2182,9 +2182,6 @@
   </si>
   <si>
     <t>completed_time</t>
-  </si>
-  <si>
-    <t>bie</t>
   </si>
   <si>
     <t>survey_production_type</t>
@@ -2757,8 +2754,8 @@
   <dimension ref="A1:F1891"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1314" sqref="C1314"/>
+      <pane ySplit="1" topLeftCell="A1006" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1032" sqref="E1032"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20275,7 +20272,7 @@
         <v>129</v>
       </c>
       <c r="E1030" s="13" t="s">
-        <v>643</v>
+        <v>131</v>
       </c>
     </row>
     <row r="1031" spans="1:5" x14ac:dyDescent="0.2">
@@ -23870,7 +23867,7 @@
         <v>610</v>
       </c>
       <c r="B1242" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C1242" s="13" t="s">
         <v>616</v>
@@ -23887,7 +23884,7 @@
         <v>610</v>
       </c>
       <c r="B1243" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C1243" s="13" t="s">
         <v>617</v>
@@ -23904,7 +23901,7 @@
         <v>610</v>
       </c>
       <c r="B1244" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C1244" s="13" t="s">
         <v>393</v>
@@ -24157,7 +24154,7 @@
         <v>610</v>
       </c>
       <c r="B1259" s="14" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C1259" s="13" t="s">
         <v>4</v>
@@ -27353,7 +27350,7 @@
         <v>619</v>
       </c>
       <c r="B1447" s="17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C1447" s="17" t="s">
         <v>616</v>
@@ -27370,10 +27367,10 @@
         <v>619</v>
       </c>
       <c r="B1448" s="17" t="s">
+        <v>643</v>
+      </c>
+      <c r="C1448" s="17" t="s">
         <v>644</v>
-      </c>
-      <c r="C1448" s="17" t="s">
-        <v>645</v>
       </c>
       <c r="D1448" s="17" t="s">
         <v>284</v>
@@ -27387,7 +27384,7 @@
         <v>619</v>
       </c>
       <c r="B1449" s="17" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C1449" s="17" t="s">
         <v>393</v>
@@ -27657,7 +27654,7 @@
         <v>619</v>
       </c>
       <c r="B1465" s="18" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C1465" s="17" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
initial pass through dictionary
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Dictionary!$A$1:$E$1485</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7462" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7658" uniqueCount="720">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -2299,6 +2299,120 @@
   </si>
   <si>
     <t>race_dmy_amcn_ind</t>
+  </si>
+  <si>
+    <t>Yes - K-12th grade</t>
+  </si>
+  <si>
+    <t>Yes – vocational/technical/trade school</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>MANDARIN</t>
+  </si>
+  <si>
+    <t>CANTONESE</t>
+  </si>
+  <si>
+    <t>TAGALOG/FILIPINO</t>
+  </si>
+  <si>
+    <t>Cash value on Clipper</t>
+  </si>
+  <si>
+    <t>Monthly pass on Clipper</t>
+  </si>
+  <si>
+    <t>EasyPass</t>
+  </si>
+  <si>
+    <t>(0) None</t>
+  </si>
+  <si>
+    <t>(1) One</t>
+  </si>
+  <si>
+    <t>(2) Two</t>
+  </si>
+  <si>
+    <t>(3) Three</t>
+  </si>
+  <si>
+    <t>(4+) Four or more</t>
+  </si>
+  <si>
+    <t>day_type</t>
+  </si>
+  <si>
+    <t>Before 5:00 am</t>
+  </si>
+  <si>
+    <t>5:00 - 5:59 am</t>
+  </si>
+  <si>
+    <t>6:00 - 6:59 am</t>
+  </si>
+  <si>
+    <t>7:00 - 7:59 am</t>
+  </si>
+  <si>
+    <t>8:00 - 8:59 am</t>
+  </si>
+  <si>
+    <t>9:00 - 9:59 am</t>
+  </si>
+  <si>
+    <t>10:00 - 10:59 am</t>
+  </si>
+  <si>
+    <t>11:00 - 11:59 am</t>
+  </si>
+  <si>
+    <t>12:00 - 12:59 pm</t>
+  </si>
+  <si>
+    <t>1:00 - 1:59 pm</t>
+  </si>
+  <si>
+    <t>2:00 - 2:59 pm</t>
+  </si>
+  <si>
+    <t>3:00 - 3:59 pm</t>
+  </si>
+  <si>
+    <t>4:00 - 4:59 pm</t>
+  </si>
+  <si>
+    <t>5:00 - 5:59 pm</t>
+  </si>
+  <si>
+    <t>6:00 - 6:59 pm</t>
+  </si>
+  <si>
+    <t>7:00 - 7:59 pm</t>
+  </si>
+  <si>
+    <t>8:00 - 8:59 pm</t>
+  </si>
+  <si>
+    <t>9:00 - 9:59 pm</t>
+  </si>
+  <si>
+    <t>10:00 - 10:59 pm</t>
+  </si>
+  <si>
+    <t>11:00 pm or later</t>
+  </si>
+  <si>
+    <t>I don't know / I am not certain</t>
+  </si>
+  <si>
+    <t>Did not leave home today / not applicable (visitor)</t>
+  </si>
+  <si>
+    <t>race_dmy_whi_mdl</t>
   </si>
 </sst>
 </file>
@@ -2454,7 +2568,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2510,6 +2624,12 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2862,11 +2982,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1681"/>
+  <dimension ref="A1:E1726"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1581" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1594" sqref="B1594:B1596"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -30157,12 +30277,12 @@
         <v>654</v>
       </c>
     </row>
-    <row r="1606" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1606" s="21" t="s">
+    <row r="1606" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1606" s="27" t="s">
         <v>646</v>
       </c>
       <c r="B1606" s="21" t="s">
-        <v>168</v>
+        <v>719</v>
       </c>
       <c r="C1606" s="21" t="s">
         <v>56</v>
@@ -30174,12 +30294,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1607" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1607" s="21" t="s">
+    <row r="1607" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1607" s="27" t="s">
         <v>646</v>
       </c>
       <c r="B1607" s="21" t="s">
-        <v>168</v>
+        <v>719</v>
       </c>
       <c r="C1607" s="21" t="s">
         <v>57</v>
@@ -30191,12 +30311,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1608" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1608" s="21" t="s">
+    <row r="1608" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1608" s="27" t="s">
         <v>646</v>
       </c>
       <c r="B1608" s="21" t="s">
-        <v>168</v>
+        <v>719</v>
       </c>
       <c r="C1608" s="21" t="s">
         <v>483</v>
@@ -30335,7 +30455,7 @@
         <v>60</v>
       </c>
       <c r="C1616" s="23" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D1616" s="21" t="s">
         <v>60</v>
@@ -30352,7 +30472,7 @@
         <v>60</v>
       </c>
       <c r="C1617" s="23" t="s">
-        <v>630</v>
+        <v>682</v>
       </c>
       <c r="D1617" s="21" t="s">
         <v>60</v>
@@ -30369,7 +30489,7 @@
         <v>60</v>
       </c>
       <c r="C1618" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D1618" s="21" t="s">
         <v>60</v>
@@ -30385,8 +30505,8 @@
       <c r="B1619" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C1619" s="21" t="s">
-        <v>451</v>
+      <c r="C1619" s="23" t="s">
+        <v>683</v>
       </c>
       <c r="D1619" s="21" t="s">
         <v>60</v>
@@ -30400,30 +30520,30 @@
         <v>646</v>
       </c>
       <c r="B1620" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1620" s="23" t="s">
-        <v>632</v>
+        <v>641</v>
+      </c>
+      <c r="C1620" s="21" t="s">
+        <v>4</v>
       </c>
       <c r="D1620" s="21" t="s">
-        <v>60</v>
+        <v>255</v>
       </c>
       <c r="E1620" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="1621" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1621" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1621" s="27" t="s">
         <v>646</v>
       </c>
       <c r="B1621" s="21" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C1621" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1621" s="21" t="s">
-        <v>255</v>
+        <v>347</v>
       </c>
       <c r="E1621" s="21" t="s">
         <v>4</v>
@@ -30434,13 +30554,13 @@
         <v>646</v>
       </c>
       <c r="B1622" s="21" t="s">
-        <v>642</v>
+        <v>592</v>
       </c>
       <c r="C1622" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1622" s="21" t="s">
-        <v>347</v>
+        <v>117</v>
       </c>
       <c r="E1622" s="21" t="s">
         <v>4</v>
@@ -30451,13 +30571,13 @@
         <v>646</v>
       </c>
       <c r="B1623" s="21" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C1623" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1623" s="21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E1623" s="21" t="s">
         <v>4</v>
@@ -30468,13 +30588,13 @@
         <v>646</v>
       </c>
       <c r="B1624" s="21" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C1624" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1624" s="21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E1624" s="21" t="s">
         <v>4</v>
@@ -30485,13 +30605,13 @@
         <v>646</v>
       </c>
       <c r="B1625" s="21" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C1625" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1625" s="21" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E1625" s="21" t="s">
         <v>4</v>
@@ -30502,13 +30622,13 @@
         <v>646</v>
       </c>
       <c r="B1626" s="21" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C1626" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1626" s="21" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E1626" s="21" t="s">
         <v>4</v>
@@ -30519,13 +30639,13 @@
         <v>646</v>
       </c>
       <c r="B1627" s="21" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C1627" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1627" s="21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E1627" s="21" t="s">
         <v>4</v>
@@ -30536,16 +30656,16 @@
         <v>646</v>
       </c>
       <c r="B1628" s="21" t="s">
-        <v>597</v>
+        <v>9</v>
       </c>
       <c r="C1628" s="21" t="s">
-        <v>4</v>
+        <v>515</v>
       </c>
       <c r="D1628" s="21" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="E1628" s="21" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1629" spans="1:5" x14ac:dyDescent="0.35">
@@ -30556,13 +30676,13 @@
         <v>9</v>
       </c>
       <c r="C1629" s="21" t="s">
-        <v>515</v>
+        <v>472</v>
       </c>
       <c r="D1629" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E1629" s="21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="1630" spans="1:5" x14ac:dyDescent="0.35">
@@ -30573,13 +30693,13 @@
         <v>9</v>
       </c>
       <c r="C1630" s="21" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D1630" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E1630" s="21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="1631" spans="1:5" x14ac:dyDescent="0.35">
@@ -30590,13 +30710,13 @@
         <v>9</v>
       </c>
       <c r="C1631" s="21" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D1631" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E1631" s="21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="1632" spans="1:5" x14ac:dyDescent="0.35">
@@ -30607,13 +30727,13 @@
         <v>9</v>
       </c>
       <c r="C1632" s="21" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D1632" s="21" t="s">
         <v>9</v>
       </c>
       <c r="E1632" s="21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1633" spans="1:5" x14ac:dyDescent="0.35">
@@ -30624,7 +30744,7 @@
         <v>9</v>
       </c>
       <c r="C1633" s="21" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D1633" s="21" t="s">
         <v>9</v>
@@ -30641,7 +30761,7 @@
         <v>9</v>
       </c>
       <c r="C1634" s="21" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D1634" s="21" t="s">
         <v>9</v>
@@ -30658,7 +30778,7 @@
         <v>9</v>
       </c>
       <c r="C1635" s="21" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D1635" s="21" t="s">
         <v>9</v>
@@ -30675,7 +30795,7 @@
         <v>9</v>
       </c>
       <c r="C1636" s="21" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D1636" s="21" t="s">
         <v>9</v>
@@ -30692,7 +30812,7 @@
         <v>9</v>
       </c>
       <c r="C1637" s="21" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D1637" s="21" t="s">
         <v>9</v>
@@ -30709,7 +30829,7 @@
         <v>9</v>
       </c>
       <c r="C1638" s="21" t="s">
-        <v>480</v>
+        <v>615</v>
       </c>
       <c r="D1638" s="21" t="s">
         <v>9</v>
@@ -30723,16 +30843,16 @@
         <v>646</v>
       </c>
       <c r="B1639" s="21" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C1639" s="21" t="s">
-        <v>615</v>
+        <v>57</v>
       </c>
       <c r="D1639" s="21" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="E1639" s="21" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="1640" spans="1:5" x14ac:dyDescent="0.35">
@@ -30743,13 +30863,13 @@
         <v>72</v>
       </c>
       <c r="C1640" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1640" s="21" t="s">
         <v>72</v>
       </c>
       <c r="E1640" s="21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="1641" spans="1:5" x14ac:dyDescent="0.35">
@@ -30757,16 +30877,16 @@
         <v>646</v>
       </c>
       <c r="B1641" s="21" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C1641" s="21" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="D1641" s="21" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E1641" s="21" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1642" spans="1:5" x14ac:dyDescent="0.35">
@@ -30774,13 +30894,13 @@
         <v>646</v>
       </c>
       <c r="B1642" s="21" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C1642" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1642" s="21" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E1642" s="21" t="s">
         <v>4</v>
@@ -30791,13 +30911,13 @@
         <v>646</v>
       </c>
       <c r="B1643" s="21" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="C1643" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1643" s="21" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="E1643" s="21" t="s">
         <v>4</v>
@@ -30808,16 +30928,16 @@
         <v>646</v>
       </c>
       <c r="B1644" s="21" t="s">
-        <v>7</v>
+        <v>284</v>
       </c>
       <c r="C1644" s="21" t="s">
-        <v>4</v>
+        <v>616</v>
       </c>
       <c r="D1644" s="21" t="s">
-        <v>7</v>
+        <v>284</v>
       </c>
       <c r="E1644" s="21" t="s">
-        <v>4</v>
+        <v>285</v>
       </c>
     </row>
     <row r="1645" spans="1:5" x14ac:dyDescent="0.35">
@@ -30825,16 +30945,16 @@
         <v>646</v>
       </c>
       <c r="B1645" s="21" t="s">
-        <v>643</v>
+        <v>284</v>
       </c>
       <c r="C1645" s="21" t="s">
-        <v>616</v>
+        <v>644</v>
       </c>
       <c r="D1645" s="21" t="s">
         <v>284</v>
       </c>
       <c r="E1645" s="21" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="1646" spans="1:5" x14ac:dyDescent="0.35">
@@ -30842,16 +30962,16 @@
         <v>646</v>
       </c>
       <c r="B1646" s="21" t="s">
-        <v>643</v>
+        <v>284</v>
       </c>
       <c r="C1646" s="21" t="s">
-        <v>644</v>
+        <v>684</v>
       </c>
       <c r="D1646" s="21" t="s">
         <v>284</v>
       </c>
       <c r="E1646" s="21" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="1647" spans="1:5" x14ac:dyDescent="0.35">
@@ -30859,16 +30979,16 @@
         <v>646</v>
       </c>
       <c r="B1647" s="21" t="s">
-        <v>643</v>
+        <v>598</v>
       </c>
       <c r="C1647" s="21" t="s">
-        <v>393</v>
+        <v>360</v>
       </c>
       <c r="D1647" s="21" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E1647" s="21" t="s">
-        <v>287</v>
+        <v>360</v>
       </c>
     </row>
     <row r="1648" spans="1:5" x14ac:dyDescent="0.35">
@@ -30878,12 +30998,14 @@
       <c r="B1648" s="21" t="s">
         <v>598</v>
       </c>
-      <c r="C1648" s="21"/>
+      <c r="C1648" s="21" t="s">
+        <v>179</v>
+      </c>
       <c r="D1648" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1648" s="21" t="s">
-        <v>360</v>
+        <v>179</v>
       </c>
     </row>
     <row r="1649" spans="1:5" x14ac:dyDescent="0.35">
@@ -30894,13 +31016,13 @@
         <v>598</v>
       </c>
       <c r="C1649" s="21" t="s">
-        <v>292</v>
+        <v>685</v>
       </c>
       <c r="D1649" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1649" s="21" t="s">
-        <v>360</v>
+        <v>187</v>
       </c>
     </row>
     <row r="1650" spans="1:5" x14ac:dyDescent="0.35">
@@ -30911,13 +31033,13 @@
         <v>598</v>
       </c>
       <c r="C1650" s="21" t="s">
-        <v>293</v>
+        <v>686</v>
       </c>
       <c r="D1650" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1650" s="21" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="1651" spans="1:5" x14ac:dyDescent="0.35">
@@ -30928,13 +31050,13 @@
         <v>598</v>
       </c>
       <c r="C1651" s="21" t="s">
-        <v>599</v>
+        <v>687</v>
       </c>
       <c r="D1651" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1651" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="1652" spans="1:5" x14ac:dyDescent="0.35">
@@ -30945,13 +31067,13 @@
         <v>598</v>
       </c>
       <c r="C1652" s="21" t="s">
-        <v>600</v>
+        <v>217</v>
       </c>
       <c r="D1652" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1652" s="21" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
     </row>
     <row r="1653" spans="1:5" x14ac:dyDescent="0.35">
@@ -30962,13 +31084,13 @@
         <v>598</v>
       </c>
       <c r="C1653" s="21" t="s">
-        <v>451</v>
+        <v>183</v>
       </c>
       <c r="D1653" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1653" s="21" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="1654" spans="1:5" x14ac:dyDescent="0.35">
@@ -30979,13 +31101,13 @@
         <v>598</v>
       </c>
       <c r="C1654" s="21" t="s">
-        <v>359</v>
+        <v>180</v>
       </c>
       <c r="D1654" s="21" t="s">
         <v>291</v>
       </c>
       <c r="E1654" s="21" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
     </row>
     <row r="1655" spans="1:5" x14ac:dyDescent="0.35">
@@ -30993,16 +31115,16 @@
         <v>646</v>
       </c>
       <c r="B1655" s="21" t="s">
-        <v>110</v>
+        <v>598</v>
       </c>
       <c r="C1655" s="21" t="s">
-        <v>4</v>
+        <v>451</v>
       </c>
       <c r="D1655" s="21" t="s">
-        <v>110</v>
+        <v>291</v>
       </c>
       <c r="E1655" s="21" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
     </row>
     <row r="1656" spans="1:5" x14ac:dyDescent="0.35">
@@ -31010,13 +31132,13 @@
         <v>646</v>
       </c>
       <c r="B1656" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C1656" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1656" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1656" s="21" t="s">
         <v>4</v>
@@ -31027,13 +31149,13 @@
         <v>646</v>
       </c>
       <c r="B1657" s="21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C1657" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1657" s="21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E1657" s="21" t="s">
         <v>4</v>
@@ -31044,13 +31166,13 @@
         <v>646</v>
       </c>
       <c r="B1658" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1658" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1658" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E1658" s="21" t="s">
         <v>4</v>
@@ -31061,13 +31183,13 @@
         <v>646</v>
       </c>
       <c r="B1659" s="21" t="s">
-        <v>634</v>
+        <v>109</v>
       </c>
       <c r="C1659" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1659" s="21" t="s">
-        <v>342</v>
+        <v>109</v>
       </c>
       <c r="E1659" s="21" t="s">
         <v>4</v>
@@ -31078,13 +31200,13 @@
         <v>646</v>
       </c>
       <c r="B1660" s="21" t="s">
-        <v>602</v>
+        <v>634</v>
       </c>
       <c r="C1660" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1660" s="21" t="s">
-        <v>99</v>
+        <v>342</v>
       </c>
       <c r="E1660" s="21" t="s">
         <v>4</v>
@@ -31095,13 +31217,13 @@
         <v>646</v>
       </c>
       <c r="B1661" s="21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C1661" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1661" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E1661" s="21" t="s">
         <v>4</v>
@@ -31111,14 +31233,14 @@
       <c r="A1662" s="21" t="s">
         <v>646</v>
       </c>
-      <c r="B1662" s="22" t="s">
-        <v>601</v>
+      <c r="B1662" s="21" t="s">
+        <v>603</v>
       </c>
       <c r="C1662" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1662" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E1662" s="21" t="s">
         <v>4</v>
@@ -31129,13 +31251,13 @@
         <v>646</v>
       </c>
       <c r="B1663" s="22" t="s">
-        <v>645</v>
+        <v>601</v>
       </c>
       <c r="C1663" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D1663" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E1663" s="21" t="s">
         <v>4</v>
@@ -31145,17 +31267,17 @@
       <c r="A1664" s="21" t="s">
         <v>646</v>
       </c>
-      <c r="B1664" s="21" t="s">
-        <v>470</v>
+      <c r="B1664" s="22" t="s">
+        <v>645</v>
       </c>
       <c r="C1664" s="21" t="s">
-        <v>638</v>
+        <v>4</v>
       </c>
       <c r="D1664" s="21" t="s">
-        <v>470</v>
+        <v>107</v>
       </c>
       <c r="E1664" s="21" t="s">
-        <v>144</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1665" spans="1:5" x14ac:dyDescent="0.35">
@@ -31166,13 +31288,13 @@
         <v>470</v>
       </c>
       <c r="C1665" s="21" t="s">
-        <v>635</v>
+        <v>688</v>
       </c>
       <c r="D1665" s="21" t="s">
         <v>470</v>
       </c>
       <c r="E1665" s="21" t="s">
-        <v>471</v>
+        <v>144</v>
       </c>
     </row>
     <row r="1666" spans="1:5" x14ac:dyDescent="0.35">
@@ -31183,7 +31305,7 @@
         <v>470</v>
       </c>
       <c r="C1666" s="21" t="s">
-        <v>636</v>
+        <v>689</v>
       </c>
       <c r="D1666" s="21" t="s">
         <v>470</v>
@@ -31200,7 +31322,7 @@
         <v>470</v>
       </c>
       <c r="C1667" s="21" t="s">
-        <v>637</v>
+        <v>690</v>
       </c>
       <c r="D1667" s="21" t="s">
         <v>470</v>
@@ -31214,16 +31336,16 @@
         <v>646</v>
       </c>
       <c r="B1668" s="21" t="s">
-        <v>470</v>
+        <v>604</v>
       </c>
       <c r="C1668" s="21" t="s">
-        <v>639</v>
+        <v>4</v>
       </c>
       <c r="D1668" s="21" t="s">
-        <v>470</v>
+        <v>345</v>
       </c>
       <c r="E1668" s="21" t="s">
-        <v>471</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1669" spans="1:5" x14ac:dyDescent="0.35">
@@ -31231,16 +31353,16 @@
         <v>646</v>
       </c>
       <c r="B1669" s="21" t="s">
-        <v>470</v>
+        <v>136</v>
       </c>
       <c r="C1669" s="21" t="s">
-        <v>640</v>
+        <v>691</v>
       </c>
       <c r="D1669" s="21" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1669" s="21" t="s">
-        <v>471</v>
+        <v>136</v>
+      </c>
+      <c r="E1669" s="21">
+        <v>0</v>
       </c>
     </row>
     <row r="1670" spans="1:5" x14ac:dyDescent="0.35">
@@ -31248,16 +31370,16 @@
         <v>646</v>
       </c>
       <c r="B1670" s="21" t="s">
-        <v>470</v>
+        <v>136</v>
       </c>
       <c r="C1670" s="21" t="s">
-        <v>451</v>
+        <v>692</v>
       </c>
       <c r="D1670" s="21" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1670" s="21" t="s">
-        <v>464</v>
+        <v>136</v>
+      </c>
+      <c r="E1670" s="21">
+        <v>1</v>
       </c>
     </row>
     <row r="1671" spans="1:5" x14ac:dyDescent="0.35">
@@ -31265,16 +31387,16 @@
         <v>646</v>
       </c>
       <c r="B1671" s="21" t="s">
-        <v>604</v>
+        <v>136</v>
       </c>
       <c r="C1671" s="21" t="s">
-        <v>4</v>
+        <v>693</v>
       </c>
       <c r="D1671" s="21" t="s">
-        <v>345</v>
-      </c>
-      <c r="E1671" s="21" t="s">
-        <v>4</v>
+        <v>136</v>
+      </c>
+      <c r="E1671" s="21">
+        <v>2</v>
       </c>
     </row>
     <row r="1672" spans="1:5" x14ac:dyDescent="0.35">
@@ -31284,14 +31406,14 @@
       <c r="B1672" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C1672" s="21">
-        <v>0</v>
+      <c r="C1672" s="21" t="s">
+        <v>694</v>
       </c>
       <c r="D1672" s="21" t="s">
         <v>136</v>
       </c>
       <c r="E1672" s="21">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1673" spans="1:5" x14ac:dyDescent="0.35">
@@ -31301,14 +31423,14 @@
       <c r="B1673" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C1673" s="21">
-        <v>1</v>
+      <c r="C1673" s="21" t="s">
+        <v>695</v>
       </c>
       <c r="D1673" s="21" t="s">
         <v>136</v>
       </c>
       <c r="E1673" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1674" spans="1:5" x14ac:dyDescent="0.35">
@@ -31316,16 +31438,16 @@
         <v>646</v>
       </c>
       <c r="B1674" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1674" s="21">
-        <v>2</v>
+        <v>137</v>
+      </c>
+      <c r="C1674" s="21" t="s">
+        <v>691</v>
       </c>
       <c r="D1674" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1674" s="21">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1675" spans="1:5" x14ac:dyDescent="0.35">
@@ -31333,16 +31455,16 @@
         <v>646</v>
       </c>
       <c r="B1675" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1675" s="21">
-        <v>3</v>
+        <v>137</v>
+      </c>
+      <c r="C1675" s="21" t="s">
+        <v>692</v>
       </c>
       <c r="D1675" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1675" s="21">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1676" spans="1:5" x14ac:dyDescent="0.35">
@@ -31350,16 +31472,16 @@
         <v>646</v>
       </c>
       <c r="B1676" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1676" s="21">
-        <v>4</v>
+        <v>137</v>
+      </c>
+      <c r="C1676" s="21" t="s">
+        <v>693</v>
       </c>
       <c r="D1676" s="21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1676" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1677" spans="1:5" x14ac:dyDescent="0.35">
@@ -31369,14 +31491,14 @@
       <c r="B1677" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C1677" s="21">
-        <v>0</v>
+      <c r="C1677" s="21" t="s">
+        <v>694</v>
       </c>
       <c r="D1677" s="21" t="s">
         <v>137</v>
       </c>
       <c r="E1677" s="21">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1678" spans="1:5" x14ac:dyDescent="0.35">
@@ -31386,65 +31508,830 @@
       <c r="B1678" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C1678" s="21">
-        <v>1</v>
+      <c r="C1678" s="21" t="s">
+        <v>695</v>
       </c>
       <c r="D1678" s="21" t="s">
         <v>137</v>
       </c>
       <c r="E1678" s="21">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1679" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1679" s="21" t="s">
+      <c r="A1679" s="26" t="s">
         <v>646</v>
       </c>
-      <c r="B1679" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1679" s="21">
-        <v>2</v>
-      </c>
-      <c r="D1679" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1679" s="21">
-        <v>2</v>
+      <c r="B1679" s="26" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1679" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1679" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1679" s="26" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="1680" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1680" s="21" t="s">
+      <c r="A1680" s="26" t="s">
         <v>646</v>
       </c>
-      <c r="B1680" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1680" s="21">
-        <v>3</v>
-      </c>
-      <c r="D1680" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1680" s="21">
-        <v>3</v>
+      <c r="B1680" s="26" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1680" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1680" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1680" s="26" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="1681" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1681" s="21" t="s">
+      <c r="A1681" s="26" t="s">
         <v>646</v>
       </c>
-      <c r="B1681" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1681" s="21">
-        <v>4</v>
-      </c>
-      <c r="D1681" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1681" s="21">
-        <v>4</v>
+      <c r="B1681" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1681" s="26" t="s">
+        <v>697</v>
+      </c>
+      <c r="D1681" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1681" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1682" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1682" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1682" s="26" t="s">
+        <v>698</v>
+      </c>
+      <c r="D1682" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1682" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1683" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1683" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1683" s="26" t="s">
+        <v>699</v>
+      </c>
+      <c r="D1683" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1683" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1684" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1684" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1684" s="26" t="s">
+        <v>700</v>
+      </c>
+      <c r="D1684" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1684" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1685" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1685" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1685" s="26" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1685" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1685" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1686" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1686" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1686" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="D1686" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1686" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1687" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1687" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1687" s="26" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1687" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1687" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1688" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1688" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1688" s="26" t="s">
+        <v>704</v>
+      </c>
+      <c r="D1688" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1688" s="26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1689" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1689" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1689" s="26" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1689" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1689" s="26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1690" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1690" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1690" s="26" t="s">
+        <v>706</v>
+      </c>
+      <c r="D1690" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1690" s="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1691" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1691" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1691" s="26" t="s">
+        <v>707</v>
+      </c>
+      <c r="D1691" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1691" s="26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1692" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1692" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1692" s="26" t="s">
+        <v>708</v>
+      </c>
+      <c r="D1692" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1692" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1693" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1693" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1693" s="26" t="s">
+        <v>709</v>
+      </c>
+      <c r="D1693" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1693" s="26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1694" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1694" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1694" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="D1694" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1694" s="26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1695" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1695" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1695" s="26" t="s">
+        <v>711</v>
+      </c>
+      <c r="D1695" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1695" s="26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1696" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1696" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1696" s="26" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1696" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1696" s="26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1697" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1697" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1697" s="26" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1697" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1697" s="26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1698" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1698" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1698" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1698" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1698" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1699" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1699" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1699" s="26" t="s">
+        <v>715</v>
+      </c>
+      <c r="D1699" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1699" s="26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1700" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1700" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1700" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="D1700" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1700" s="26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1701" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1701" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1701" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="D1701" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1701" s="26" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1702" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1702" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1702" s="26" t="s">
+        <v>718</v>
+      </c>
+      <c r="D1702" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1702" s="26" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1703" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1703" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1703" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="D1703" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1703" s="26" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1704" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1704" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1704" s="26" t="s">
+        <v>697</v>
+      </c>
+      <c r="D1704" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1704" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1705" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1705" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1705" s="26" t="s">
+        <v>698</v>
+      </c>
+      <c r="D1705" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1705" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1706" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1706" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1706" s="26" t="s">
+        <v>699</v>
+      </c>
+      <c r="D1706" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1706" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1707" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1707" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1707" s="26" t="s">
+        <v>700</v>
+      </c>
+      <c r="D1707" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1707" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1708" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1708" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1708" s="26" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1708" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1708" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1709" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1709" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1709" s="26" t="s">
+        <v>702</v>
+      </c>
+      <c r="D1709" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1709" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1710" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1710" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1710" s="26" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1710" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1710" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1711" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1711" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1711" s="26" t="s">
+        <v>704</v>
+      </c>
+      <c r="D1711" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1711" s="26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1712" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1712" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1712" s="26" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1712" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1712" s="26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1713" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1713" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1713" s="26" t="s">
+        <v>706</v>
+      </c>
+      <c r="D1713" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1713" s="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1714" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1714" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1714" s="26" t="s">
+        <v>707</v>
+      </c>
+      <c r="D1714" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1714" s="26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1715" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1715" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1715" s="26" t="s">
+        <v>708</v>
+      </c>
+      <c r="D1715" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1715" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1716" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1716" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1716" s="26" t="s">
+        <v>709</v>
+      </c>
+      <c r="D1716" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1716" s="26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1717" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1717" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1717" s="26" t="s">
+        <v>710</v>
+      </c>
+      <c r="D1717" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1717" s="26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1718" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1718" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1718" s="26" t="s">
+        <v>711</v>
+      </c>
+      <c r="D1718" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1718" s="26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1719" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1719" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1719" s="26" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1719" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1719" s="26">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1720" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1720" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1720" s="26" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1720" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1720" s="26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1721" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1721" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1721" s="26" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1721" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1721" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1722" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1722" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1722" s="26" t="s">
+        <v>715</v>
+      </c>
+      <c r="D1722" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1722" s="26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1723" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1723" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1723" s="26" t="s">
+        <v>716</v>
+      </c>
+      <c r="D1723" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1723" s="26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1724" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1724" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1724" s="26" t="s">
+        <v>717</v>
+      </c>
+      <c r="D1724" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1724" s="26" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1725" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1725" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1725" s="26" t="s">
+        <v>718</v>
+      </c>
+      <c r="D1725" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1725" s="26" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1726" s="26" t="s">
+        <v>646</v>
+      </c>
+      <c r="B1726" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1726" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="D1726" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1726" s="26" t="s">
+        <v>654</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started on Marin transit
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7658" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8769" uniqueCount="754">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -2413,6 +2413,108 @@
   </si>
   <si>
     <t>race_dmy_whi_mdl</t>
+  </si>
+  <si>
+    <t>Marin Transit</t>
+  </si>
+  <si>
+    <t>Getto1bus_c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>schbefore</t>
+  </si>
+  <si>
+    <t>Workbefore</t>
+  </si>
+  <si>
+    <t>ENDLAT</t>
+  </si>
+  <si>
+    <t>ENDLON</t>
+  </si>
+  <si>
+    <t>FromTo_c2</t>
+  </si>
+  <si>
+    <t>Gettolotsbus_c1</t>
+  </si>
+  <si>
+    <t>Gettolotsbus_c2</t>
+  </si>
+  <si>
+    <t>Hhwork</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>engspk</t>
+  </si>
+  <si>
+    <t>Farecat</t>
+  </si>
+  <si>
+    <t>Workafter</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Hisp</t>
+  </si>
+  <si>
+    <t>HOMELAT</t>
+  </si>
+  <si>
+    <t>HOMELONG</t>
+  </si>
+  <si>
+    <t>sys_RespNum</t>
+  </si>
+  <si>
+    <t>Langhh</t>
+  </si>
+  <si>
+    <t>TIBETAN</t>
+  </si>
+  <si>
+    <t>NEPALI</t>
+  </si>
+  <si>
+    <t>ASL</t>
+  </si>
+  <si>
+    <t>STARTLAT</t>
+  </si>
+  <si>
+    <t>STARTLONG</t>
+  </si>
+  <si>
+    <t>FromTo_c1</t>
+  </si>
+  <si>
+    <t>pass (Marin local)</t>
+  </si>
+  <si>
+    <t>pass (youth)</t>
+  </si>
+  <si>
+    <t>pass (College of Marin)</t>
+  </si>
+  <si>
+    <t>pass (RTC discount)</t>
+  </si>
+  <si>
+    <t>Fare</t>
+  </si>
+  <si>
+    <t>Hh</t>
+  </si>
+  <si>
+    <t>START HERE, BUILD DUMMIES IN DATA FILE (AND WORKERS)</t>
   </si>
 </sst>
 </file>
@@ -2513,7 +2615,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2548,6 +2650,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2568,7 +2682,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2629,6 +2743,26 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2982,16 +3116,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1726"/>
+  <dimension ref="A1:E2016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A1871" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1885" sqref="A1885"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.92578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="40.92578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="30.640625" style="3" bestFit="1" customWidth="1"/>
@@ -32331,6 +32465,4668 @@
         <v>253</v>
       </c>
       <c r="E1726" s="26" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1727" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1727" s="29" t="s">
+        <v>721</v>
+      </c>
+      <c r="C1727" s="30">
+        <v>1</v>
+      </c>
+      <c r="D1727" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1727" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1728" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1728" s="29" t="s">
+        <v>721</v>
+      </c>
+      <c r="C1728" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1728" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1728" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1729" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1729" s="29" t="s">
+        <v>721</v>
+      </c>
+      <c r="C1729" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1729" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1729" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1730" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1730" s="29" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1730" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1730" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1730" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1731" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1731" s="29" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1731" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1731" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1731" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1732" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1732" s="29" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1732" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1732" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1732" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1733" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1733" s="29" t="s">
+        <v>728</v>
+      </c>
+      <c r="C1733" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1733" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1733" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1734" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1734" s="28" t="s">
+        <v>723</v>
+      </c>
+      <c r="C1734" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1734" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1734" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1735" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1735" s="28" t="s">
+        <v>723</v>
+      </c>
+      <c r="C1735" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1735" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1735" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1736" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1736" s="28" t="s">
+        <v>724</v>
+      </c>
+      <c r="C1736" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1736" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1736" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1737" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1737" s="28" t="s">
+        <v>724</v>
+      </c>
+      <c r="C1737" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1737" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1737" s="28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1738" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1738" s="28" t="s">
+        <v>725</v>
+      </c>
+      <c r="C1738" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1738" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1738" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1739" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1739" s="28" t="s">
+        <v>726</v>
+      </c>
+      <c r="C1739" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1739" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1739" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1740" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1740" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1740" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1740" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1740" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1741" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1741" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1741" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1741" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1741" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1742" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1742" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1742" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1742" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1742" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1743" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1743" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1743" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1743" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1743" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1744" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1744" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1744" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1744" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1744" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1745" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1745" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1745" s="28">
+        <v>11</v>
+      </c>
+      <c r="D1745" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1745" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1746" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1746" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1746" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1746" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1746" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1747" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1747" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1747" s="28">
+        <v>10</v>
+      </c>
+      <c r="D1747" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1747" s="28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1748" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1748" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1748" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1748" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1748" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1749" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1749" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1749" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1749" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1749" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1750" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1750" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1750" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1750" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1750" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1751" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1751" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1751" s="28">
+        <v>12</v>
+      </c>
+      <c r="D1751" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1751" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1752" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1752" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1752" s="28">
+        <v>13</v>
+      </c>
+      <c r="D1752" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1752" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1753" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1753" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1753" s="28">
+        <v>14</v>
+      </c>
+      <c r="D1753" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1753" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1754" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1754" s="28" t="s">
+        <v>727</v>
+      </c>
+      <c r="C1754" s="28">
+        <v>15</v>
+      </c>
+      <c r="D1754" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1754" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1755" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1755" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1755" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1755" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1755" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1756" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1756" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1756" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1756" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1756" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1757" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1757" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1757" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1757" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1757" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1758" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1758" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1758" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1758" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1758" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1759" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1759" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1759" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1759" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1759" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1760" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1760" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1760" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1760" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1760" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1761" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1761" s="28" t="s">
+        <v>729</v>
+      </c>
+      <c r="C1761" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1761" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1761" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1762" s="28"/>
+      <c r="B1762" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1762" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="D1762" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1762" s="35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1763" s="28"/>
+      <c r="B1763" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1763" s="35" t="s">
+        <v>525</v>
+      </c>
+      <c r="D1763" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1763" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1764" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1764" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1764" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1764" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1764" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1765" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1765" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1765" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1765" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1765" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1766" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1766" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1766" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1766" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1766" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1767" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1767" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1767" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1767" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1767" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1768" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1768" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1768" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1768" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1768" s="28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1769" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1769" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1769" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1769" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1769" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1770" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1770" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1770" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1770" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1770" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1771" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1771" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1771" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1771" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1771" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1772" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1772" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1772" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1772" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1772" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1773" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1773" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1773" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1773" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1773" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1774" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1774" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1774" s="28">
+        <v>13</v>
+      </c>
+      <c r="D1774" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1774" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1775" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1775" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1775" s="28">
+        <v>14</v>
+      </c>
+      <c r="D1775" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1775" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1776" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1776" s="28" t="s">
+        <v>730</v>
+      </c>
+      <c r="C1776" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1776" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1776" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1777" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1777" s="28" t="s">
+        <v>732</v>
+      </c>
+      <c r="C1777" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1777" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1777" s="28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1778" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1778" s="28" t="s">
+        <v>732</v>
+      </c>
+      <c r="C1778" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1778" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1778" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1779" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1779" s="28" t="s">
+        <v>732</v>
+      </c>
+      <c r="C1779" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1779" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1779" s="28" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1780" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1780" s="28" t="s">
+        <v>732</v>
+      </c>
+      <c r="C1780" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1780" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1780" s="28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1781" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1781" s="28" t="s">
+        <v>732</v>
+      </c>
+      <c r="C1781" s="34" t="s">
+        <v>722</v>
+      </c>
+      <c r="D1781" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="E1781" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1782" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1782" s="28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C1782" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1782" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1782" s="28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1783" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1783" s="28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C1783" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1783" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1783" s="28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1784" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1784" s="28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C1784" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1784" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1784" s="28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1785" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1785" s="28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C1785" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1785" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1785" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1786" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1786" s="28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C1786" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1786" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1786" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1787" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1787" s="28" t="s">
+        <v>733</v>
+      </c>
+      <c r="C1787" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1787" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1787" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1788" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1788" s="28" t="s">
+        <v>734</v>
+      </c>
+      <c r="C1788" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1788" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1788" s="28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1789" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1789" s="28" t="s">
+        <v>734</v>
+      </c>
+      <c r="C1789" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1789" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1789" s="28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1790" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1790" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1790" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1790" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1790" s="28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1791" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1791" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1791" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1791" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1791" s="28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1792" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1792" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1792" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1792" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1792" s="28" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1793" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1793" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1793" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1793" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1793" s="28" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1794" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1794" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1794" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1794" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1794" s="28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1795" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1795" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1795" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1795" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1795" s="28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1796" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1796" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1796" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1796" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1796" s="28" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1797" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1797" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1797" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1797" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1797" s="28" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1798" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1798" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1798" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1798" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1798" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1799" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1799" s="28" t="s">
+        <v>735</v>
+      </c>
+      <c r="C1799" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1799" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1799" s="28" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1800" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1800" s="28" t="s">
+        <v>736</v>
+      </c>
+      <c r="C1800" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1800" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1800" s="28" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1801" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1801" s="28" t="s">
+        <v>736</v>
+      </c>
+      <c r="C1801" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1801" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1801" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1802" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1802" s="28" t="s">
+        <v>736</v>
+      </c>
+      <c r="C1802" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1802" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1802" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1803" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1803" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="C1803" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1803" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1803" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1804" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1804" s="28" t="s">
+        <v>738</v>
+      </c>
+      <c r="C1804" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1804" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1804" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1805" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1805" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="C1805" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1805" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1805" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1806" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1806" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1806" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1806" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1806" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1807" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1807" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1807" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1807" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1807" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1808" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1808" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1808" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1808" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1808" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1809" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1809" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1809" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1809" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1809" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1810" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1810" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1810" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1810" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1810" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1811" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1811" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1811" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1811" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1811" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1812" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1812" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1812" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1812" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1812" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1813" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1813" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1813" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1813" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1813" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1814" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1814" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1814" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1814" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1814" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1815" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1815" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1815" s="28">
+        <v>10</v>
+      </c>
+      <c r="D1815" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1815" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1816" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1816" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1816" s="28">
+        <v>11</v>
+      </c>
+      <c r="D1816" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1816" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1817" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1817" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1817" s="28">
+        <v>12</v>
+      </c>
+      <c r="D1817" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1817" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1818" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1818" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1818" s="28">
+        <v>13</v>
+      </c>
+      <c r="D1818" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1818" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1819" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1819" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1819" s="28">
+        <v>14</v>
+      </c>
+      <c r="D1819" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1819" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1820" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1820" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1820" s="28">
+        <v>15</v>
+      </c>
+      <c r="D1820" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1820" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1821" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1821" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1821" s="28">
+        <v>16</v>
+      </c>
+      <c r="D1821" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1821" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1822" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1822" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1822" s="28">
+        <v>17</v>
+      </c>
+      <c r="D1822" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1822" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1823" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1823" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1823" s="28">
+        <v>18</v>
+      </c>
+      <c r="D1823" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1823" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1824" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1824" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1824" s="28">
+        <v>19</v>
+      </c>
+      <c r="D1824" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1824" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1825" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1825" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1825" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1825" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1825" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1826" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1826" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1826" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1826" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1826" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1827" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1827" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1827" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1827" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1827" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1828" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1828" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1828" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1828" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1828" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1829" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1829" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1829" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1829" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1829" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1830" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1830" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1830" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1830" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1830" s="28" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1831" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1831" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1831" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1831" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1831" s="28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1832" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1832" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1832" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1832" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1832" s="28" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1833" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1833" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1833" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1833" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1833" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1834" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1834" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1834" s="28">
+        <v>10</v>
+      </c>
+      <c r="D1834" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1834" s="28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1835" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1835" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1835" s="28">
+        <v>11</v>
+      </c>
+      <c r="D1835" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1835" s="28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1836" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1836" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1836" s="28">
+        <v>12</v>
+      </c>
+      <c r="D1836" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1836" s="28" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1837" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1837" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1837" s="28">
+        <v>13</v>
+      </c>
+      <c r="D1837" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1837" s="28" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1838" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1838" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1838" s="28">
+        <v>14</v>
+      </c>
+      <c r="D1838" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1838" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1839" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1839" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1839" s="28">
+        <v>15</v>
+      </c>
+      <c r="D1839" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1839" s="28" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1840" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1840" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1840" s="28">
+        <v>16</v>
+      </c>
+      <c r="D1840" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1840" s="28" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1841" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1841" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1841" s="28">
+        <v>17</v>
+      </c>
+      <c r="D1841" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1841" s="28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1842" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1842" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1842" s="28">
+        <v>18</v>
+      </c>
+      <c r="D1842" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1842" s="28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1843" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1843" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1843" s="28">
+        <v>19</v>
+      </c>
+      <c r="D1843" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1843" s="28" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1844" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1844" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="C1844" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1844" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1844" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1845" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1845" s="28" t="s">
+        <v>744</v>
+      </c>
+      <c r="C1845" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1845" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1845" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1846" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1846" s="28" t="s">
+        <v>745</v>
+      </c>
+      <c r="C1846" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1846" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1846" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1847" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1847" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1847" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1847" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1847" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1848" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1848" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1848" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1848" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1848" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1849" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1849" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1849" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1849" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1849" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1850" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1850" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1850" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1850" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1850" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1851" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1851" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1851" s="31">
+        <v>8</v>
+      </c>
+      <c r="D1851" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1851" s="28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1852" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1852" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1852" s="28">
+        <v>11</v>
+      </c>
+      <c r="D1852" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1852" s="28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1853" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1853" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1853" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1853" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1853" s="28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1854" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1854" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1854" s="28">
+        <v>10</v>
+      </c>
+      <c r="D1854" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1854" s="28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1855" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1855" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1855" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1855" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1855" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1856" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1856" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1856" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1856" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1856" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1857" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1857" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1857" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1857" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1857" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1858" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1858" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1858" s="28">
+        <v>12</v>
+      </c>
+      <c r="D1858" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1858" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1859" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1859" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1859" s="28">
+        <v>13</v>
+      </c>
+      <c r="D1859" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1859" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1860" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1860" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1860" s="28">
+        <v>14</v>
+      </c>
+      <c r="D1860" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1860" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1861" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1861" s="28" t="s">
+        <v>746</v>
+      </c>
+      <c r="C1861" s="28">
+        <v>15</v>
+      </c>
+      <c r="D1861" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1861" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1862" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1862" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1862" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1862" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1862" s="28" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1863" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1863" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1863" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1863" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1863" s="28" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1864" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1864" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1864" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1864" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1864" s="28" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1865" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1865" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1865" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1865" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1865" s="28" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1866" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1866" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1866" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1866" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1866" s="28" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1867" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1867" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1867" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1867" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1867" s="28" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1868" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1868" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1868" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1868" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1868" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1869" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1869" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1869" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1869" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1869" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1870" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1870" s="28" t="s">
+        <v>751</v>
+      </c>
+      <c r="C1870" s="28">
+        <v>0</v>
+      </c>
+      <c r="D1870" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1870" s="28" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1871" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1871" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1871" s="28">
+        <v>1</v>
+      </c>
+      <c r="D1871" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1871" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1872" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1872" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1872" s="28">
+        <v>2</v>
+      </c>
+      <c r="D1872" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1872" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1873" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1873" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1873" s="28">
+        <v>3</v>
+      </c>
+      <c r="D1873" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1873" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1874" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1874" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1874" s="28">
+        <v>4</v>
+      </c>
+      <c r="D1874" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1874" s="28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1875" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1875" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1875" s="28">
+        <v>5</v>
+      </c>
+      <c r="D1875" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1875" s="28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1876" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1876" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1876" s="28">
+        <v>6</v>
+      </c>
+      <c r="D1876" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1876" s="28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1877" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1877" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1877" s="28">
+        <v>7</v>
+      </c>
+      <c r="D1877" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1877" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1878" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1878" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1878" s="28">
+        <v>8</v>
+      </c>
+      <c r="D1878" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1878" s="28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1879" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1879" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1879" s="28">
+        <v>9</v>
+      </c>
+      <c r="D1879" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1879" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1880" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1880" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1880" s="28">
+        <v>12</v>
+      </c>
+      <c r="D1880" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1880" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1881" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1881" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1881" s="28">
+        <v>13</v>
+      </c>
+      <c r="D1881" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1881" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1882" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1882" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1882" s="28">
+        <v>14</v>
+      </c>
+      <c r="D1882" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1882" s="28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1883" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1883" s="32" t="s">
+        <v>752</v>
+      </c>
+      <c r="C1883" s="28" t="s">
+        <v>731</v>
+      </c>
+      <c r="D1883" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1883" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1884" s="35" t="s">
+        <v>753</v>
+      </c>
+      <c r="B1884" s="28" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1884" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1884" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1884" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1885" s="28"/>
+      <c r="B1885" s="28" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1885" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1885" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1885" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1886" s="28"/>
+      <c r="B1886" s="28" t="s">
+        <v>681</v>
+      </c>
+      <c r="C1886" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1886" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1886" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1887" s="28"/>
+      <c r="B1887" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1887" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1887" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1887" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1888" s="28"/>
+      <c r="B1888" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1888" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1888" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1888" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1889" s="28"/>
+      <c r="B1889" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1889" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1889" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1889" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1890" s="28"/>
+      <c r="B1890" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1890" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1890" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1890" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1891" s="28"/>
+      <c r="B1891" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1891" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1891" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1891" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1892" s="28"/>
+      <c r="B1892" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1892" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1892" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1892" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1893" s="28"/>
+      <c r="B1893" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1893" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1893" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1893" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1894" s="28"/>
+      <c r="B1894" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1894" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1894" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1894" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1895" s="28"/>
+      <c r="B1895" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1895" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1895" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1895" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1896" s="28"/>
+      <c r="B1896" s="28" t="s">
+        <v>719</v>
+      </c>
+      <c r="C1896" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1896" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1896" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1897" s="28"/>
+      <c r="B1897" s="28" t="s">
+        <v>719</v>
+      </c>
+      <c r="C1897" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1897" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1897" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1898" s="28"/>
+      <c r="B1898" s="28" t="s">
+        <v>719</v>
+      </c>
+      <c r="C1898" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1898" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1898" s="28" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1899" s="28"/>
+      <c r="B1899" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1899" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1899" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1899" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1900" s="28"/>
+      <c r="B1900" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1900" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1900" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1900" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1901" s="28"/>
+      <c r="B1901" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1901" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="D1901" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1901" s="28" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1902" s="28"/>
+      <c r="B1902" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1902" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="D1902" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1902" s="28" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1903" s="28"/>
+      <c r="B1903" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1903" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1903" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1903" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1904" s="28"/>
+      <c r="B1904" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1904" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1904" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1904" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1905" s="28"/>
+      <c r="B1905" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1905" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="D1905" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1905" s="28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1906" s="28"/>
+      <c r="B1906" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1906" s="31" t="s">
+        <v>630</v>
+      </c>
+      <c r="D1906" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1906" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1907" s="28"/>
+      <c r="B1907" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1907" s="31" t="s">
+        <v>682</v>
+      </c>
+      <c r="D1907" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1907" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1908" s="28"/>
+      <c r="B1908" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1908" s="31" t="s">
+        <v>631</v>
+      </c>
+      <c r="D1908" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1908" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1909" s="28"/>
+      <c r="B1909" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1909" s="31" t="s">
+        <v>683</v>
+      </c>
+      <c r="D1909" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1909" s="28" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1910" s="28"/>
+      <c r="B1910" s="28" t="s">
+        <v>641</v>
+      </c>
+      <c r="C1910" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1910" s="28" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1910" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1911" s="28"/>
+      <c r="B1911" s="28" t="s">
+        <v>642</v>
+      </c>
+      <c r="C1911" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1911" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1911" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1912" s="28"/>
+      <c r="B1912" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="C1912" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1912" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1912" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1913" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1913" s="28"/>
+      <c r="B1913" s="28" t="s">
+        <v>593</v>
+      </c>
+      <c r="C1913" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1913" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1913" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1914" s="28"/>
+      <c r="B1914" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="C1914" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1914" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1914" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1915" s="28"/>
+      <c r="B1915" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="C1915" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1915" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1915" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1916" s="28"/>
+      <c r="B1916" s="28" t="s">
+        <v>596</v>
+      </c>
+      <c r="C1916" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1916" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1916" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1917" s="28"/>
+      <c r="B1917" s="28" t="s">
+        <v>597</v>
+      </c>
+      <c r="C1917" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1917" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1917" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1918" s="28"/>
+      <c r="B1918" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1918" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1918" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1918" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1919" s="28"/>
+      <c r="B1919" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1919" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="D1919" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1919" s="28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1920" s="28"/>
+      <c r="B1920" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1920" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="D1920" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1920" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1921" s="28"/>
+      <c r="B1921" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1921" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1921" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1921" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1922" s="28"/>
+      <c r="B1922" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1922" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1922" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1922" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1923" s="28"/>
+      <c r="B1923" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1923" s="28" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1923" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1923" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1924" s="28"/>
+      <c r="B1924" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1924" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="D1924" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1924" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1925" s="28"/>
+      <c r="B1925" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1925" s="28" t="s">
+        <v>478</v>
+      </c>
+      <c r="D1925" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1925" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1926" s="28"/>
+      <c r="B1926" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1926" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1926" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1926" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1927" s="28"/>
+      <c r="B1927" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1927" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="D1927" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1927" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1928" s="28"/>
+      <c r="B1928" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1928" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="D1928" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1928" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1929" s="28"/>
+      <c r="B1929" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1929" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1929" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1929" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1930" s="28"/>
+      <c r="B1930" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1930" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1930" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1930" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1931" s="28"/>
+      <c r="B1931" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1931" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1931" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1931" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1932" s="28"/>
+      <c r="B1932" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1932" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1932" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1932" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1933" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1933" s="28"/>
+      <c r="B1933" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1933" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1933" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1933" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1934" s="28"/>
+      <c r="B1934" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1934" s="28" t="s">
+        <v>616</v>
+      </c>
+      <c r="D1934" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1934" s="28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1935" s="28"/>
+      <c r="B1935" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1935" s="28" t="s">
+        <v>644</v>
+      </c>
+      <c r="D1935" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1935" s="28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1936" s="28"/>
+      <c r="B1936" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C1936" s="28" t="s">
+        <v>684</v>
+      </c>
+      <c r="D1936" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1936" s="28" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1937" s="28"/>
+      <c r="B1937" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1937" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1937" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1937" s="28" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1938" s="28"/>
+      <c r="B1938" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1938" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1938" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1938" s="28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1939" s="28"/>
+      <c r="B1939" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1939" s="28" t="s">
+        <v>685</v>
+      </c>
+      <c r="D1939" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1939" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1940" s="28"/>
+      <c r="B1940" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1940" s="28" t="s">
+        <v>686</v>
+      </c>
+      <c r="D1940" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1940" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1941" s="28"/>
+      <c r="B1941" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1941" s="28" t="s">
+        <v>687</v>
+      </c>
+      <c r="D1941" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1941" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1942" s="28"/>
+      <c r="B1942" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1942" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1942" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1942" s="28" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1943" s="28"/>
+      <c r="B1943" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1943" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1943" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1943" s="28" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1944" s="28"/>
+      <c r="B1944" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1944" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1944" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1944" s="28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1945" s="28"/>
+      <c r="B1945" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1945" s="28" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1945" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1945" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1946" s="28"/>
+      <c r="B1946" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1946" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1946" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1946" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1947" s="28"/>
+      <c r="B1947" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1947" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1947" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1947" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1948" s="28"/>
+      <c r="B1948" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1948" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1948" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1948" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1949" s="28"/>
+      <c r="B1949" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1949" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1949" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1949" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1950" s="28"/>
+      <c r="B1950" s="28" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1950" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1950" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1950" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1951" s="28"/>
+      <c r="B1951" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="C1951" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1951" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1951" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1952" s="28"/>
+      <c r="B1952" s="28" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1952" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1952" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1952" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1953" s="28"/>
+      <c r="B1953" s="29" t="s">
+        <v>601</v>
+      </c>
+      <c r="C1953" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1953" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1953" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1954" s="28"/>
+      <c r="B1954" s="29" t="s">
+        <v>645</v>
+      </c>
+      <c r="C1954" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1954" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1954" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1955" s="28"/>
+      <c r="B1955" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1955" s="28" t="s">
+        <v>688</v>
+      </c>
+      <c r="D1955" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1955" s="28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="1956" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1956" s="28"/>
+      <c r="B1956" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1956" s="28" t="s">
+        <v>689</v>
+      </c>
+      <c r="D1956" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1956" s="28" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="1957" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1957" s="28"/>
+      <c r="B1957" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="C1957" s="28" t="s">
+        <v>690</v>
+      </c>
+      <c r="D1957" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="E1957" s="28" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="1958" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1958" s="28"/>
+      <c r="B1958" s="28" t="s">
+        <v>604</v>
+      </c>
+      <c r="C1958" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1958" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="E1958" s="28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1959" s="28"/>
+      <c r="B1959" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1959" s="28" t="s">
+        <v>691</v>
+      </c>
+      <c r="D1959" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1959" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1960" s="28"/>
+      <c r="B1960" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1960" s="28" t="s">
+        <v>692</v>
+      </c>
+      <c r="D1960" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1960" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1961" s="28"/>
+      <c r="B1961" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1961" s="28" t="s">
+        <v>693</v>
+      </c>
+      <c r="D1961" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1961" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1962" s="28"/>
+      <c r="B1962" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1962" s="28" t="s">
+        <v>694</v>
+      </c>
+      <c r="D1962" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1962" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1963" s="28"/>
+      <c r="B1963" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1963" s="28" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1963" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1963" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1964" s="28"/>
+      <c r="B1964" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1964" s="28" t="s">
+        <v>691</v>
+      </c>
+      <c r="D1964" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1964" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1965" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1965" s="28"/>
+      <c r="B1965" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1965" s="28" t="s">
+        <v>692</v>
+      </c>
+      <c r="D1965" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1965" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1966" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1966" s="28"/>
+      <c r="B1966" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1966" s="28" t="s">
+        <v>693</v>
+      </c>
+      <c r="D1966" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1966" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1967" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1967" s="28"/>
+      <c r="B1967" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1967" s="28" t="s">
+        <v>694</v>
+      </c>
+      <c r="D1967" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1967" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1968" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1968" s="28"/>
+      <c r="B1968" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1968" s="28" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1968" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1968" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1969" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1969" s="33"/>
+      <c r="B1969" s="33" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1969" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1969" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1969" s="33" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="1970" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1970" s="33"/>
+      <c r="B1970" s="33" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1970" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1970" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1970" s="33" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="1971" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1971" s="33"/>
+      <c r="B1971" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1971" s="33" t="s">
+        <v>697</v>
+      </c>
+      <c r="D1971" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1971" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1972" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1972" s="33"/>
+      <c r="B1972" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1972" s="33" t="s">
+        <v>698</v>
+      </c>
+      <c r="D1972" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1972" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1973" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1973" s="33"/>
+      <c r="B1973" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1973" s="33" t="s">
+        <v>699</v>
+      </c>
+      <c r="D1973" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1973" s="33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1974" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1974" s="33"/>
+      <c r="B1974" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1974" s="33" t="s">
+        <v>700</v>
+      </c>
+      <c r="D1974" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1974" s="33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1975" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1975" s="33"/>
+      <c r="B1975" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1975" s="33" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1975" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1975" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1976" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1976" s="33"/>
+      <c r="B1976" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1976" s="33" t="s">
+        <v>702</v>
+      </c>
+      <c r="D1976" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1976" s="33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1977" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1977" s="33"/>
+      <c r="B1977" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1977" s="33" t="s">
+        <v>703</v>
+      </c>
+      <c r="D1977" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1977" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1978" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1978" s="33"/>
+      <c r="B1978" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1978" s="33" t="s">
+        <v>704</v>
+      </c>
+      <c r="D1978" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1978" s="33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1979" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1979" s="33"/>
+      <c r="B1979" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1979" s="33" t="s">
+        <v>705</v>
+      </c>
+      <c r="D1979" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1979" s="33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1980" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1980" s="33"/>
+      <c r="B1980" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1980" s="33" t="s">
+        <v>706</v>
+      </c>
+      <c r="D1980" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1980" s="33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1981" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1981" s="33"/>
+      <c r="B1981" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1981" s="33" t="s">
+        <v>707</v>
+      </c>
+      <c r="D1981" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1981" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1982" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1982" s="33"/>
+      <c r="B1982" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1982" s="33" t="s">
+        <v>708</v>
+      </c>
+      <c r="D1982" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1982" s="33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1983" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1983" s="33"/>
+      <c r="B1983" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1983" s="33" t="s">
+        <v>709</v>
+      </c>
+      <c r="D1983" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1983" s="33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1984" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1984" s="33"/>
+      <c r="B1984" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1984" s="33" t="s">
+        <v>710</v>
+      </c>
+      <c r="D1984" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1984" s="33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1985" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1985" s="33"/>
+      <c r="B1985" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1985" s="33" t="s">
+        <v>711</v>
+      </c>
+      <c r="D1985" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1985" s="33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1986" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1986" s="33"/>
+      <c r="B1986" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1986" s="33" t="s">
+        <v>712</v>
+      </c>
+      <c r="D1986" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1986" s="33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="1987" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1987" s="33"/>
+      <c r="B1987" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1987" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="D1987" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1987" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1988" s="33"/>
+      <c r="B1988" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1988" s="33" t="s">
+        <v>714</v>
+      </c>
+      <c r="D1988" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1988" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1989" s="33"/>
+      <c r="B1989" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1989" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="D1989" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1989" s="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1990" s="33"/>
+      <c r="B1990" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1990" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="D1990" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1990" s="33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1991" s="33"/>
+      <c r="B1991" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1991" s="33" t="s">
+        <v>717</v>
+      </c>
+      <c r="D1991" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1991" s="33" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1992" s="33"/>
+      <c r="B1992" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1992" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="D1992" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1992" s="33" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1993" s="33"/>
+      <c r="B1993" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1993" s="33" t="s">
+        <v>676</v>
+      </c>
+      <c r="D1993" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1993" s="33" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1994" s="33"/>
+      <c r="B1994" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1994" s="33" t="s">
+        <v>697</v>
+      </c>
+      <c r="D1994" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1994" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1995" s="33"/>
+      <c r="B1995" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1995" s="33" t="s">
+        <v>698</v>
+      </c>
+      <c r="D1995" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1995" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1996" s="33"/>
+      <c r="B1996" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1996" s="33" t="s">
+        <v>699</v>
+      </c>
+      <c r="D1996" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1996" s="33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1997" s="33"/>
+      <c r="B1997" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1997" s="33" t="s">
+        <v>700</v>
+      </c>
+      <c r="D1997" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1997" s="33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1998" s="33"/>
+      <c r="B1998" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1998" s="33" t="s">
+        <v>701</v>
+      </c>
+      <c r="D1998" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1998" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1999" s="33"/>
+      <c r="B1999" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1999" s="33" t="s">
+        <v>702</v>
+      </c>
+      <c r="D1999" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1999" s="33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2000" s="33"/>
+      <c r="B2000" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2000" s="33" t="s">
+        <v>703</v>
+      </c>
+      <c r="D2000" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2000" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2001" s="33"/>
+      <c r="B2001" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2001" s="33" t="s">
+        <v>704</v>
+      </c>
+      <c r="D2001" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2001" s="33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2002" s="33"/>
+      <c r="B2002" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2002" s="33" t="s">
+        <v>705</v>
+      </c>
+      <c r="D2002" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2002" s="33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2003" s="33"/>
+      <c r="B2003" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2003" s="33" t="s">
+        <v>706</v>
+      </c>
+      <c r="D2003" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2003" s="33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2004" s="33"/>
+      <c r="B2004" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2004" s="33" t="s">
+        <v>707</v>
+      </c>
+      <c r="D2004" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2004" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2005" s="33"/>
+      <c r="B2005" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2005" s="33" t="s">
+        <v>708</v>
+      </c>
+      <c r="D2005" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2005" s="33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2006" s="33"/>
+      <c r="B2006" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2006" s="33" t="s">
+        <v>709</v>
+      </c>
+      <c r="D2006" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2006" s="33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2007" s="33"/>
+      <c r="B2007" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2007" s="33" t="s">
+        <v>710</v>
+      </c>
+      <c r="D2007" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2007" s="33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2008" s="33"/>
+      <c r="B2008" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2008" s="33" t="s">
+        <v>711</v>
+      </c>
+      <c r="D2008" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2008" s="33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2009" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2009" s="33"/>
+      <c r="B2009" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2009" s="33" t="s">
+        <v>712</v>
+      </c>
+      <c r="D2009" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2009" s="33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2010" s="33"/>
+      <c r="B2010" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2010" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="D2010" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2010" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2011" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2011" s="33"/>
+      <c r="B2011" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2011" s="33" t="s">
+        <v>714</v>
+      </c>
+      <c r="D2011" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2011" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2012" s="33"/>
+      <c r="B2012" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2012" s="33" t="s">
+        <v>715</v>
+      </c>
+      <c r="D2012" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2012" s="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2013" s="33"/>
+      <c r="B2013" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2013" s="33" t="s">
+        <v>716</v>
+      </c>
+      <c r="D2013" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2013" s="33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2014" s="33"/>
+      <c r="B2014" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2014" s="33" t="s">
+        <v>717</v>
+      </c>
+      <c r="D2014" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2014" s="33" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="2015" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2015" s="33"/>
+      <c r="B2015" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2015" s="33" t="s">
+        <v>718</v>
+      </c>
+      <c r="D2015" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2015" s="33" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="2016" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2016" s="33"/>
+      <c r="B2016" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2016" s="33" t="s">
+        <v>676</v>
+      </c>
+      <c r="D2016" s="33" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2016" s="33" t="s">
         <v>654</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished Marin first pass - need to test now
</commit_message>
<xml_diff>
--- a/make-uniform/production/Dictionary for Standard Database.xlsx
+++ b/make-uniform/production/Dictionary for Standard Database.xlsx
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8760" uniqueCount="769">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8764" uniqueCount="784">
   <si>
     <t>Survey_Variable</t>
   </si>
@@ -2559,7 +2559,52 @@
     <t>Mode</t>
   </si>
   <si>
-    <t>START HERE COMPUTE THIS IN EXCEL</t>
+    <t>ONBUS-LAT1</t>
+  </si>
+  <si>
+    <t>ONBUS-LONG1</t>
+  </si>
+  <si>
+    <t>boarding_lat</t>
+  </si>
+  <si>
+    <t>boarding_lon</t>
+  </si>
+  <si>
+    <t>alighting_lat</t>
+  </si>
+  <si>
+    <t>alighting_lon</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>TUE</t>
+  </si>
+  <si>
+    <t>WED</t>
+  </si>
+  <si>
+    <t>THUR</t>
+  </si>
+  <si>
+    <t>FRI</t>
+  </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>SUN</t>
+  </si>
+  <si>
+    <t>Hometime_c1</t>
+  </si>
+  <si>
+    <t>Hometime_c2</t>
   </si>
 </sst>
 </file>
@@ -2660,7 +2705,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2701,12 +2746,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2727,7 +2766,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2805,9 +2844,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -3161,11 +3197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2008"/>
+  <dimension ref="A1:E2004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1925" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1930" sqref="B1930"/>
+      <pane ySplit="1" topLeftCell="A1958" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -36101,11 +36137,11 @@
       </c>
     </row>
     <row r="1938" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1938" s="35" t="s">
+      <c r="A1938" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1938" s="28" t="s">
         <v>768</v>
-      </c>
-      <c r="B1938" s="28" t="s">
-        <v>110</v>
       </c>
       <c r="C1938" s="28" t="s">
         <v>4</v>
@@ -36118,9 +36154,11 @@
       </c>
     </row>
     <row r="1939" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1939" s="28"/>
+      <c r="A1939" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1939" s="28" t="s">
-        <v>111</v>
+        <v>769</v>
       </c>
       <c r="C1939" s="28" t="s">
         <v>4</v>
@@ -36133,7 +36171,9 @@
       </c>
     </row>
     <row r="1940" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1940" s="28"/>
+      <c r="A1940" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1940" s="28" t="s">
         <v>108</v>
       </c>
@@ -36148,7 +36188,9 @@
       </c>
     </row>
     <row r="1941" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1941" s="28"/>
+      <c r="A1941" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1941" s="28" t="s">
         <v>109</v>
       </c>
@@ -36163,9 +36205,11 @@
       </c>
     </row>
     <row r="1942" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1942" s="28"/>
+      <c r="A1942" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1942" s="28" t="s">
-        <v>634</v>
+        <v>522</v>
       </c>
       <c r="C1942" s="28" t="s">
         <v>4</v>
@@ -36178,9 +36222,11 @@
       </c>
     </row>
     <row r="1943" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1943" s="28"/>
+      <c r="A1943" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1943" s="28" t="s">
-        <v>602</v>
+        <v>770</v>
       </c>
       <c r="C1943" s="28" t="s">
         <v>4</v>
@@ -36193,9 +36239,11 @@
       </c>
     </row>
     <row r="1944" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1944" s="28"/>
+      <c r="A1944" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1944" s="28" t="s">
-        <v>603</v>
+        <v>771</v>
       </c>
       <c r="C1944" s="28" t="s">
         <v>4</v>
@@ -36208,9 +36256,11 @@
       </c>
     </row>
     <row r="1945" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1945" s="28"/>
+      <c r="A1945" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1945" s="29" t="s">
-        <v>601</v>
+        <v>772</v>
       </c>
       <c r="C1945" s="28" t="s">
         <v>4</v>
@@ -36223,9 +36273,11 @@
       </c>
     </row>
     <row r="1946" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1946" s="28"/>
+      <c r="A1946" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1946" s="29" t="s">
-        <v>645</v>
+        <v>773</v>
       </c>
       <c r="C1946" s="28" t="s">
         <v>4</v>
@@ -36238,237 +36290,269 @@
       </c>
     </row>
     <row r="1947" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1947" s="28"/>
+      <c r="A1947" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1947" s="28" t="s">
-        <v>470</v>
+        <v>344</v>
       </c>
       <c r="C1947" s="28" t="s">
-        <v>688</v>
+        <v>4</v>
       </c>
       <c r="D1947" s="28" t="s">
-        <v>470</v>
+        <v>345</v>
       </c>
       <c r="E1947" s="28" t="s">
-        <v>144</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1948" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1948" s="28"/>
+      <c r="A1948" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1948" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1948" s="28" t="s">
-        <v>689</v>
+        <v>136</v>
+      </c>
+      <c r="C1948" s="28">
+        <v>0</v>
       </c>
       <c r="D1948" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1948" s="28" t="s">
-        <v>471</v>
+        <v>136</v>
+      </c>
+      <c r="E1948" s="28">
+        <v>0</v>
       </c>
     </row>
     <row r="1949" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1949" s="28"/>
+      <c r="A1949" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1949" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="C1949" s="28" t="s">
-        <v>690</v>
+        <v>136</v>
+      </c>
+      <c r="C1949" s="28">
+        <v>1</v>
       </c>
       <c r="D1949" s="28" t="s">
-        <v>470</v>
-      </c>
-      <c r="E1949" s="28" t="s">
-        <v>471</v>
+        <v>136</v>
+      </c>
+      <c r="E1949" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="1950" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1950" s="28"/>
+      <c r="A1950" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1950" s="28" t="s">
-        <v>604</v>
-      </c>
-      <c r="C1950" s="28" t="s">
-        <v>4</v>
+        <v>136</v>
+      </c>
+      <c r="C1950" s="28">
+        <v>2</v>
       </c>
       <c r="D1950" s="28" t="s">
-        <v>345</v>
-      </c>
-      <c r="E1950" s="28" t="s">
-        <v>4</v>
+        <v>136</v>
+      </c>
+      <c r="E1950" s="28">
+        <v>2</v>
       </c>
     </row>
     <row r="1951" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1951" s="28"/>
+      <c r="A1951" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1951" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="C1951" s="28" t="s">
-        <v>691</v>
+      <c r="C1951" s="28">
+        <v>3</v>
       </c>
       <c r="D1951" s="28" t="s">
         <v>136</v>
       </c>
       <c r="E1951" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1952" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1952" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1952" s="28">
         <v>0</v>
       </c>
-    </row>
-    <row r="1952" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1952" s="28"/>
-      <c r="B1952" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1952" s="28" t="s">
-        <v>692</v>
-      </c>
       <c r="D1952" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1952" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1953" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1953" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1953" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1953" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="1953" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1953" s="28"/>
-      <c r="B1953" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1953" s="28" t="s">
-        <v>693</v>
-      </c>
       <c r="D1953" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1953" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1954" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1954" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1954" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1954" s="28">
         <v>2</v>
       </c>
-    </row>
-    <row r="1954" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1954" s="28"/>
-      <c r="B1954" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1954" s="28" t="s">
-        <v>694</v>
-      </c>
       <c r="D1954" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1954" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1955" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1955" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1955" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1955" s="28">
         <v>3</v>
       </c>
-    </row>
-    <row r="1955" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1955" s="28"/>
-      <c r="B1955" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1955" s="28" t="s">
-        <v>695</v>
-      </c>
       <c r="D1955" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E1955" s="28">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="1956" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1956" s="28"/>
-      <c r="B1956" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1956" s="28" t="s">
-        <v>691</v>
-      </c>
-      <c r="D1956" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1956" s="28">
-        <v>0</v>
+      <c r="A1956" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1956" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1956" s="33" t="s">
+        <v>775</v>
+      </c>
+      <c r="D1956" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1956" s="33" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="1957" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1957" s="28"/>
-      <c r="B1957" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1957" s="28" t="s">
-        <v>692</v>
-      </c>
-      <c r="D1957" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1957" s="28">
-        <v>1</v>
+      <c r="A1957" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1957" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1957" s="33" t="s">
+        <v>776</v>
+      </c>
+      <c r="D1957" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1957" s="33" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="1958" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1958" s="28"/>
-      <c r="B1958" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1958" s="28" t="s">
-        <v>693</v>
-      </c>
-      <c r="D1958" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1958" s="28">
-        <v>2</v>
+      <c r="A1958" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1958" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1958" s="33" t="s">
+        <v>777</v>
+      </c>
+      <c r="D1958" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1958" s="33" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="1959" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1959" s="28"/>
-      <c r="B1959" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1959" s="28" t="s">
-        <v>694</v>
-      </c>
-      <c r="D1959" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1959" s="28">
-        <v>3</v>
+      <c r="A1959" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1959" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1959" s="33" t="s">
+        <v>778</v>
+      </c>
+      <c r="D1959" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1959" s="33" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="1960" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1960" s="28"/>
-      <c r="B1960" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1960" s="28" t="s">
-        <v>695</v>
-      </c>
-      <c r="D1960" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1960" s="28">
-        <v>4</v>
+      <c r="A1960" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1960" s="33" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1960" s="33" t="s">
+        <v>779</v>
+      </c>
+      <c r="D1960" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1960" s="33" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="1961" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1961" s="33"/>
+      <c r="A1961" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1961" s="33" t="s">
-        <v>696</v>
+        <v>774</v>
       </c>
       <c r="C1961" s="33" t="s">
-        <v>349</v>
+        <v>780</v>
       </c>
       <c r="D1961" s="33" t="s">
         <v>350</v>
       </c>
       <c r="E1961" s="33" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="1962" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1962" s="33"/>
+      <c r="A1962" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1962" s="33" t="s">
-        <v>696</v>
+        <v>774</v>
       </c>
       <c r="C1962" s="33" t="s">
-        <v>352</v>
+        <v>781</v>
       </c>
       <c r="D1962" s="33" t="s">
         <v>350</v>
@@ -36478,12 +36562,14 @@
       </c>
     </row>
     <row r="1963" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1963" s="33"/>
+      <c r="A1963" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1963" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1963" s="33" t="s">
-        <v>697</v>
+        <v>782</v>
+      </c>
+      <c r="C1963" s="33">
+        <v>1</v>
       </c>
       <c r="D1963" s="33" t="s">
         <v>251</v>
@@ -36493,12 +36579,14 @@
       </c>
     </row>
     <row r="1964" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1964" s="33"/>
+      <c r="A1964" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1964" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1964" s="33" t="s">
-        <v>698</v>
+        <v>782</v>
+      </c>
+      <c r="C1964" s="33">
+        <v>2</v>
       </c>
       <c r="D1964" s="33" t="s">
         <v>251</v>
@@ -36508,12 +36596,14 @@
       </c>
     </row>
     <row r="1965" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1965" s="33"/>
+      <c r="A1965" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1965" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1965" s="33" t="s">
-        <v>699</v>
+        <v>782</v>
+      </c>
+      <c r="C1965" s="33">
+        <v>3</v>
       </c>
       <c r="D1965" s="33" t="s">
         <v>251</v>
@@ -36523,12 +36613,14 @@
       </c>
     </row>
     <row r="1966" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1966" s="33"/>
+      <c r="A1966" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1966" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1966" s="33" t="s">
-        <v>700</v>
+        <v>782</v>
+      </c>
+      <c r="C1966" s="33">
+        <v>4</v>
       </c>
       <c r="D1966" s="33" t="s">
         <v>251</v>
@@ -36538,12 +36630,14 @@
       </c>
     </row>
     <row r="1967" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1967" s="33"/>
+      <c r="A1967" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1967" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1967" s="33" t="s">
-        <v>701</v>
+        <v>782</v>
+      </c>
+      <c r="C1967" s="33">
+        <v>5</v>
       </c>
       <c r="D1967" s="33" t="s">
         <v>251</v>
@@ -36553,12 +36647,14 @@
       </c>
     </row>
     <row r="1968" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1968" s="33"/>
+      <c r="A1968" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1968" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1968" s="33" t="s">
-        <v>702</v>
+        <v>782</v>
+      </c>
+      <c r="C1968" s="33">
+        <v>6</v>
       </c>
       <c r="D1968" s="33" t="s">
         <v>251</v>
@@ -36568,12 +36664,14 @@
       </c>
     </row>
     <row r="1969" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1969" s="33"/>
+      <c r="A1969" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1969" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1969" s="33" t="s">
-        <v>703</v>
+        <v>782</v>
+      </c>
+      <c r="C1969" s="33">
+        <v>7</v>
       </c>
       <c r="D1969" s="33" t="s">
         <v>251</v>
@@ -36583,12 +36681,14 @@
       </c>
     </row>
     <row r="1970" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1970" s="33"/>
+      <c r="A1970" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1970" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1970" s="33" t="s">
-        <v>704</v>
+        <v>782</v>
+      </c>
+      <c r="C1970" s="33">
+        <v>8</v>
       </c>
       <c r="D1970" s="33" t="s">
         <v>251</v>
@@ -36598,12 +36698,14 @@
       </c>
     </row>
     <row r="1971" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1971" s="33"/>
+      <c r="A1971" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1971" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1971" s="33" t="s">
-        <v>705</v>
+        <v>782</v>
+      </c>
+      <c r="C1971" s="33">
+        <v>9</v>
       </c>
       <c r="D1971" s="33" t="s">
         <v>251</v>
@@ -36613,12 +36715,14 @@
       </c>
     </row>
     <row r="1972" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1972" s="33"/>
+      <c r="A1972" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1972" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1972" s="33" t="s">
-        <v>706</v>
+        <v>782</v>
+      </c>
+      <c r="C1972" s="33">
+        <v>10</v>
       </c>
       <c r="D1972" s="33" t="s">
         <v>251</v>
@@ -36628,12 +36732,14 @@
       </c>
     </row>
     <row r="1973" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1973" s="33"/>
+      <c r="A1973" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1973" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1973" s="33" t="s">
-        <v>707</v>
+        <v>782</v>
+      </c>
+      <c r="C1973" s="33">
+        <v>11</v>
       </c>
       <c r="D1973" s="33" t="s">
         <v>251</v>
@@ -36643,12 +36749,14 @@
       </c>
     </row>
     <row r="1974" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1974" s="33"/>
+      <c r="A1974" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1974" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1974" s="33" t="s">
-        <v>708</v>
+        <v>782</v>
+      </c>
+      <c r="C1974" s="33">
+        <v>12</v>
       </c>
       <c r="D1974" s="33" t="s">
         <v>251</v>
@@ -36658,12 +36766,14 @@
       </c>
     </row>
     <row r="1975" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1975" s="33"/>
+      <c r="A1975" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1975" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1975" s="33" t="s">
-        <v>709</v>
+        <v>782</v>
+      </c>
+      <c r="C1975" s="33">
+        <v>13</v>
       </c>
       <c r="D1975" s="33" t="s">
         <v>251</v>
@@ -36673,12 +36783,14 @@
       </c>
     </row>
     <row r="1976" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1976" s="33"/>
+      <c r="A1976" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1976" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1976" s="33" t="s">
-        <v>710</v>
+        <v>782</v>
+      </c>
+      <c r="C1976" s="33">
+        <v>14</v>
       </c>
       <c r="D1976" s="33" t="s">
         <v>251</v>
@@ -36688,12 +36800,14 @@
       </c>
     </row>
     <row r="1977" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1977" s="33"/>
+      <c r="A1977" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1977" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1977" s="33" t="s">
-        <v>711</v>
+        <v>782</v>
+      </c>
+      <c r="C1977" s="33">
+        <v>15</v>
       </c>
       <c r="D1977" s="33" t="s">
         <v>251</v>
@@ -36703,12 +36817,14 @@
       </c>
     </row>
     <row r="1978" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1978" s="33"/>
+      <c r="A1978" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1978" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1978" s="33" t="s">
-        <v>712</v>
+        <v>782</v>
+      </c>
+      <c r="C1978" s="33">
+        <v>16</v>
       </c>
       <c r="D1978" s="33" t="s">
         <v>251</v>
@@ -36718,12 +36834,14 @@
       </c>
     </row>
     <row r="1979" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1979" s="33"/>
+      <c r="A1979" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1979" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1979" s="33" t="s">
-        <v>713</v>
+        <v>782</v>
+      </c>
+      <c r="C1979" s="33">
+        <v>17</v>
       </c>
       <c r="D1979" s="33" t="s">
         <v>251</v>
@@ -36733,12 +36851,14 @@
       </c>
     </row>
     <row r="1980" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1980" s="33"/>
+      <c r="A1980" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1980" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1980" s="33" t="s">
-        <v>714</v>
+        <v>782</v>
+      </c>
+      <c r="C1980" s="33">
+        <v>18</v>
       </c>
       <c r="D1980" s="33" t="s">
         <v>251</v>
@@ -36748,12 +36868,14 @@
       </c>
     </row>
     <row r="1981" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1981" s="33"/>
+      <c r="A1981" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1981" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1981" s="33" t="s">
-        <v>715</v>
+        <v>782</v>
+      </c>
+      <c r="C1981" s="33">
+        <v>19</v>
       </c>
       <c r="D1981" s="33" t="s">
         <v>251</v>
@@ -36763,27 +36885,31 @@
       </c>
     </row>
     <row r="1982" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1982" s="33"/>
+      <c r="A1982" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1982" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1982" s="33" t="s">
-        <v>716</v>
+        <v>782</v>
+      </c>
+      <c r="C1982" s="33">
+        <v>20</v>
       </c>
       <c r="D1982" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="E1982" s="33">
-        <v>23</v>
+      <c r="E1982" s="33" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="1983" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1983" s="33"/>
+      <c r="A1983" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1983" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1983" s="33" t="s">
-        <v>717</v>
+        <v>782</v>
+      </c>
+      <c r="C1983" s="33">
+        <v>21</v>
       </c>
       <c r="D1983" s="33" t="s">
         <v>251</v>
@@ -36793,377 +36919,359 @@
       </c>
     </row>
     <row r="1984" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1984" s="33"/>
+      <c r="A1984" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1984" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1984" s="33" t="s">
-        <v>718</v>
+        <v>783</v>
+      </c>
+      <c r="C1984" s="33">
+        <v>1</v>
       </c>
       <c r="D1984" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1984" s="33" t="s">
-        <v>654</v>
+        <v>253</v>
+      </c>
+      <c r="E1984" s="33">
+        <v>4</v>
       </c>
     </row>
     <row r="1985" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1985" s="33"/>
+      <c r="A1985" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1985" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1985" s="33" t="s">
-        <v>676</v>
+        <v>783</v>
+      </c>
+      <c r="C1985" s="33">
+        <v>2</v>
       </c>
       <c r="D1985" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="E1985" s="33" t="s">
-        <v>654</v>
+        <v>253</v>
+      </c>
+      <c r="E1985" s="33">
+        <v>5</v>
       </c>
     </row>
     <row r="1986" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1986" s="33"/>
+      <c r="A1986" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1986" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1986" s="33" t="s">
-        <v>697</v>
+        <v>783</v>
+      </c>
+      <c r="C1986" s="33">
+        <v>3</v>
       </c>
       <c r="D1986" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1986" s="33">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="1987" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1987" s="33"/>
+      <c r="A1987" s="28" t="s">
+        <v>720</v>
+      </c>
       <c r="B1987" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1987" s="33" t="s">
-        <v>698</v>
+        <v>783</v>
+      </c>
+      <c r="C1987" s="33">
+        <v>4</v>
       </c>
       <c r="D1987" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1987" s="33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1988" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1988" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1988" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1988" s="33">
         <v>5</v>
-      </c>
-    </row>
-    <row r="1988" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1988" s="33"/>
-      <c r="B1988" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1988" s="33" t="s">
-        <v>699</v>
       </c>
       <c r="D1988" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1988" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1989" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1989" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1989" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1989" s="33">
         <v>6</v>
-      </c>
-    </row>
-    <row r="1989" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1989" s="33"/>
-      <c r="B1989" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1989" s="33" t="s">
-        <v>700</v>
       </c>
       <c r="D1989" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1989" s="33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1990" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1990" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1990" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1990" s="33">
         <v>7</v>
-      </c>
-    </row>
-    <row r="1990" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1990" s="33"/>
-      <c r="B1990" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1990" s="33" t="s">
-        <v>701</v>
       </c>
       <c r="D1990" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1990" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1991" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1991" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1991" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1991" s="33">
         <v>8</v>
-      </c>
-    </row>
-    <row r="1991" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1991" s="33"/>
-      <c r="B1991" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1991" s="33" t="s">
-        <v>702</v>
       </c>
       <c r="D1991" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1991" s="33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1992" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1992" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1992" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1992" s="33">
         <v>9</v>
-      </c>
-    </row>
-    <row r="1992" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1992" s="33"/>
-      <c r="B1992" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1992" s="33" t="s">
-        <v>703</v>
       </c>
       <c r="D1992" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1992" s="33">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1993" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1993" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1993" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1993" s="33">
         <v>10</v>
-      </c>
-    </row>
-    <row r="1993" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1993" s="33"/>
-      <c r="B1993" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1993" s="33" t="s">
-        <v>704</v>
       </c>
       <c r="D1993" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1993" s="33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1994" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1994" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1994" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1994" s="33">
         <v>11</v>
-      </c>
-    </row>
-    <row r="1994" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1994" s="33"/>
-      <c r="B1994" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1994" s="33" t="s">
-        <v>705</v>
       </c>
       <c r="D1994" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1994" s="33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1995" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1995" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1995" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1995" s="33">
         <v>12</v>
-      </c>
-    </row>
-    <row r="1995" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1995" s="33"/>
-      <c r="B1995" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1995" s="33" t="s">
-        <v>706</v>
       </c>
       <c r="D1995" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1995" s="33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1996" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1996" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1996" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1996" s="33">
         <v>13</v>
-      </c>
-    </row>
-    <row r="1996" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1996" s="33"/>
-      <c r="B1996" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1996" s="33" t="s">
-        <v>707</v>
       </c>
       <c r="D1996" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1996" s="33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1997" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1997" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1997" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1997" s="33">
         <v>14</v>
-      </c>
-    </row>
-    <row r="1997" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1997" s="33"/>
-      <c r="B1997" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1997" s="33" t="s">
-        <v>708</v>
       </c>
       <c r="D1997" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1997" s="33">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1998" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1998" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1998" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1998" s="33">
         <v>15</v>
-      </c>
-    </row>
-    <row r="1998" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1998" s="33"/>
-      <c r="B1998" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1998" s="33" t="s">
-        <v>709</v>
       </c>
       <c r="D1998" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1998" s="33">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1999" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1999" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B1999" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C1999" s="33">
         <v>16</v>
-      </c>
-    </row>
-    <row r="1999" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1999" s="33"/>
-      <c r="B1999" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1999" s="33" t="s">
-        <v>710</v>
       </c>
       <c r="D1999" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E1999" s="33">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2000" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2000" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B2000" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2000" s="33">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2000" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2000" s="33"/>
-      <c r="B2000" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2000" s="33" t="s">
-        <v>711</v>
       </c>
       <c r="D2000" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E2000" s="33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2001" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2001" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B2001" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2001" s="33">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2001" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2001" s="33"/>
-      <c r="B2001" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2001" s="33" t="s">
-        <v>712</v>
       </c>
       <c r="D2001" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E2001" s="33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2002" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2002" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B2002" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2002" s="33">
         <v>19</v>
-      </c>
-    </row>
-    <row r="2002" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2002" s="33"/>
-      <c r="B2002" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2002" s="33" t="s">
-        <v>713</v>
       </c>
       <c r="D2002" s="33" t="s">
         <v>253</v>
       </c>
       <c r="E2002" s="33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2003" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B2003" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2003" s="33">
         <v>20</v>
-      </c>
-    </row>
-    <row r="2003" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2003" s="33"/>
-      <c r="B2003" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2003" s="33" t="s">
-        <v>714</v>
       </c>
       <c r="D2003" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E2003" s="33">
+      <c r="E2003" s="33" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2004" s="28" t="s">
+        <v>720</v>
+      </c>
+      <c r="B2004" s="33" t="s">
+        <v>783</v>
+      </c>
+      <c r="C2004" s="33">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2004" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2004" s="33"/>
-      <c r="B2004" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2004" s="33" t="s">
-        <v>715</v>
       </c>
       <c r="D2004" s="33" t="s">
         <v>253</v>
       </c>
-      <c r="E2004" s="33">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2005" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2005" s="33"/>
-      <c r="B2005" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2005" s="33" t="s">
-        <v>716</v>
-      </c>
-      <c r="D2005" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2005" s="33">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2006" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2006" s="33"/>
-      <c r="B2006" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2006" s="33" t="s">
-        <v>717</v>
-      </c>
-      <c r="D2006" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2006" s="33" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="2007" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2007" s="33"/>
-      <c r="B2007" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2007" s="33" t="s">
-        <v>718</v>
-      </c>
-      <c r="D2007" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2007" s="33" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="2008" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2008" s="33"/>
-      <c r="B2008" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2008" s="33" t="s">
-        <v>676</v>
-      </c>
-      <c r="D2008" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2008" s="33" t="s">
+      <c r="E2004" s="33" t="s">
         <v>654</v>
       </c>
     </row>

</xml_diff>